<commit_message>
final update to trcability matrix
final update to trcability matrix
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -384,10 +384,11 @@
     <t>BANK_SYS_SRS_Reg_R010</t>
   </si>
   <si>
-    <t>BANK_SYS_SIQ_Q8</t>
-  </si>
-  <si>
     <t>BANK_SYS_SIQ_Q45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK_SYS_SIQ_Q29
+</t>
   </si>
 </sst>
 </file>
@@ -1071,8 +1072,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A57" sqref="A57:XFD57"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A49" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E57" sqref="E57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1839,7 +1840,7 @@
         <v>86</v>
       </c>
       <c r="E55" s="23" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
@@ -1861,7 +1862,7 @@
       <c r="H56" s="11"/>
       <c r="I56" s="13"/>
     </row>
-    <row r="57" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="21" t="s">
         <v>19</v>
       </c>
@@ -1869,7 +1870,7 @@
         <v>90</v>
       </c>
       <c r="E57" s="23" t="s">
-        <v>91</v>
+        <v>92</v>
       </c>
       <c r="F57" s="22"/>
       <c r="G57" s="22"/>

</xml_diff>

<commit_message>
Adding BANK_SYS_SRS_NF_R005 and BANK_SYS_SRS_NF_R005
 Adding BANK_SYS_SRS_NF_R005 and BANK_SYS_SRS_NF_R005
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\sondos\CM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="93">
   <si>
     <t>Author</t>
   </si>
@@ -378,7 +378,16 @@
   </si>
   <si>
     <t>Introduction: requirements traceability matrix (RTM) is a simple and effective document that
-                          allows to establish and maintain bidirectional traceability for a project.</t>
+                           allows to establish and maintain bidirectional traceability for a project.</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> bank_sys_Q8</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Reg_R010</t>
+  </si>
+  <si>
+    <t>bank_sys_Q45</t>
   </si>
 </sst>
 </file>
@@ -1060,10 +1069,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L56"/>
+  <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A52" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B68" sqref="B68"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D55" sqref="D55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1829,7 +1838,9 @@
       <c r="D55" s="22" t="s">
         <v>86</v>
       </c>
-      <c r="E55" s="23"/>
+      <c r="E55" s="23" t="s">
+        <v>92</v>
+      </c>
       <c r="F55" s="22"/>
       <c r="G55" s="22"/>
       <c r="H55" s="11"/>
@@ -1849,6 +1860,21 @@
       <c r="G56" s="22"/>
       <c r="H56" s="11"/>
       <c r="I56" s="13"/>
+    </row>
+    <row r="57" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C57" s="21" t="s">
+        <v>19</v>
+      </c>
+      <c r="D57" s="22" t="s">
+        <v>91</v>
+      </c>
+      <c r="E57" s="23" t="s">
+        <v>90</v>
+      </c>
+      <c r="F57" s="22"/>
+      <c r="G57" s="22"/>
+      <c r="H57" s="11"/>
+      <c r="I57" s="13"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Update Requirements Trcability Matrix.xlsx
1- Recover the updates in SIQ sheet with traceability matrix
2- Link the following SRS
BANK_SYS_SRS_PT_R020
BANK_SYS_SRS_PT_R021
BANK_SYS_SRS_PT_R022
with Customer requirements
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\PM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Documents\GitHub\Internet-Banking-System\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7755"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="95">
   <si>
     <t>Author</t>
   </si>
@@ -388,6 +388,18 @@
   </si>
   <si>
     <t>bank_sys_Q45</t>
+  </si>
+  <si>
+    <t>Ahmed Hamdy</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1- Recover the updates in SIQ sheet with traceability matrix 
+2- Link the following SRS 
+BANK_SYS_SRS_PT_R020
+BANK_SYS_SRS_PT_R021
+BANK_SYS_SRS_PT_R022
+with Customer requirements
+</t>
   </si>
 </sst>
 </file>
@@ -687,7 +699,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -707,9 +719,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -761,6 +770,9 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
@@ -786,6 +798,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="4" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1071,8 +1086,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L57"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A48" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D55" sqref="D55"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B7" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1213,7 +1228,7 @@
       </c>
       <c r="J8" s="31"/>
     </row>
-    <row r="9" spans="1:12" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" ht="144.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="4" t="s">
         <v>12</v>
       </c>
@@ -1227,19 +1242,25 @@
         <v>14</v>
       </c>
       <c r="F9" s="32"/>
-      <c r="G9" s="7"/>
-      <c r="H9" s="7"/>
-      <c r="I9" s="32"/>
+      <c r="G9" s="24" t="s">
+        <v>93</v>
+      </c>
+      <c r="H9" s="34">
+        <v>43529</v>
+      </c>
+      <c r="I9" s="32" t="s">
+        <v>94</v>
+      </c>
       <c r="J9" s="33"/>
     </row>
     <row r="10" spans="1:12" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B10" s="8"/>
-      <c r="C10" s="9"/>
-      <c r="D10" s="9"/>
+      <c r="B10" s="7"/>
+      <c r="C10" s="8"/>
+      <c r="D10" s="8"/>
       <c r="E10" s="25"/>
       <c r="F10" s="25"/>
-      <c r="G10" s="9"/>
-      <c r="H10" s="9"/>
+      <c r="G10" s="8"/>
+      <c r="H10" s="8"/>
       <c r="I10" s="25"/>
       <c r="J10" s="26"/>
     </row>
@@ -1335,546 +1356,546 @@
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="22" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D22" s="14" t="s">
+      <c r="D22" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="E22" s="15" t="s">
+      <c r="E22" s="14" t="s">
         <v>3</v>
       </c>
-      <c r="F22" s="15" t="s">
+      <c r="F22" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="G22" s="15" t="s">
+      <c r="G22" s="14" t="s">
         <v>4</v>
       </c>
-      <c r="H22" s="16" t="s">
+      <c r="H22" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="I22" s="12"/>
+      <c r="I22" s="11"/>
     </row>
     <row r="23" spans="2:10" ht="105" x14ac:dyDescent="0.25">
-      <c r="C23" s="17" t="s">
+      <c r="C23" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D23" s="18" t="s">
+      <c r="D23" s="17" t="s">
         <v>28</v>
       </c>
-      <c r="E23" s="19" t="s">
+      <c r="E23" s="18" t="s">
         <v>29</v>
       </c>
-      <c r="F23" s="20"/>
-      <c r="G23" s="20"/>
-      <c r="H23" s="10"/>
-      <c r="I23" s="13"/>
+      <c r="F23" s="19"/>
+      <c r="G23" s="19"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="12"/>
     </row>
     <row r="24" spans="2:10" ht="135.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="21" t="s">
+      <c r="C24" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="22" t="s">
+      <c r="D24" s="21" t="s">
         <v>30</v>
       </c>
-      <c r="E24" s="23" t="s">
+      <c r="E24" s="22" t="s">
         <v>31</v>
       </c>
-      <c r="F24" s="22"/>
-      <c r="G24" s="22"/>
-      <c r="H24" s="11"/>
-      <c r="I24" s="13"/>
+      <c r="F24" s="21"/>
+      <c r="G24" s="21"/>
+      <c r="H24" s="10"/>
+      <c r="I24" s="12"/>
     </row>
     <row r="25" spans="2:10" ht="75" x14ac:dyDescent="0.25">
-      <c r="C25" s="17" t="s">
+      <c r="C25" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D25" s="18" t="s">
+      <c r="D25" s="17" t="s">
         <v>32</v>
       </c>
-      <c r="E25" s="19" t="s">
+      <c r="E25" s="18" t="s">
         <v>33</v>
       </c>
-      <c r="F25" s="20"/>
-      <c r="G25" s="20"/>
-      <c r="H25" s="10"/>
-      <c r="I25" s="13"/>
+      <c r="F25" s="19"/>
+      <c r="G25" s="19"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="12"/>
     </row>
     <row r="26" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="21" t="s">
+      <c r="C26" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="21" t="s">
         <v>34</v>
       </c>
-      <c r="E26" s="23"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="22"/>
-      <c r="H26" s="11"/>
-      <c r="I26" s="13"/>
+      <c r="E26" s="22"/>
+      <c r="F26" s="21"/>
+      <c r="G26" s="21"/>
+      <c r="H26" s="10"/>
+      <c r="I26" s="12"/>
     </row>
     <row r="27" spans="2:10" ht="45" x14ac:dyDescent="0.25">
-      <c r="C27" s="17" t="s">
+      <c r="C27" s="16" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="18" t="s">
+      <c r="D27" s="17" t="s">
         <v>35</v>
       </c>
-      <c r="E27" s="19" t="s">
+      <c r="E27" s="18" t="s">
         <v>36</v>
       </c>
-      <c r="F27" s="20"/>
-      <c r="G27" s="20"/>
-      <c r="H27" s="10"/>
-      <c r="I27" s="13"/>
+      <c r="F27" s="19"/>
+      <c r="G27" s="19"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="12"/>
     </row>
     <row r="28" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="21" t="s">
+      <c r="C28" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D28" s="22" t="s">
+      <c r="D28" s="21" t="s">
         <v>37</v>
       </c>
-      <c r="E28" s="23" t="s">
+      <c r="E28" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="F28" s="22"/>
-      <c r="G28" s="22"/>
-      <c r="H28" s="11"/>
-      <c r="I28" s="13"/>
+      <c r="F28" s="21"/>
+      <c r="G28" s="21"/>
+      <c r="H28" s="10"/>
+      <c r="I28" s="12"/>
     </row>
     <row r="29" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="21" t="s">
+      <c r="C29" s="20" t="s">
         <v>17</v>
       </c>
-      <c r="D29" s="22" t="s">
+      <c r="D29" s="21" t="s">
         <v>39</v>
       </c>
-      <c r="E29" s="23" t="s">
+      <c r="E29" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="F29" s="22"/>
-      <c r="G29" s="22"/>
-      <c r="H29" s="11"/>
-      <c r="I29" s="13"/>
+      <c r="F29" s="21"/>
+      <c r="G29" s="21"/>
+      <c r="H29" s="10"/>
+      <c r="I29" s="12"/>
     </row>
     <row r="30" spans="2:10" ht="60.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C30" s="21" t="s">
+      <c r="C30" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D30" s="22" t="s">
+      <c r="D30" s="21" t="s">
         <v>41</v>
       </c>
-      <c r="E30" s="23" t="s">
+      <c r="E30" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="F30" s="22"/>
-      <c r="G30" s="22"/>
-      <c r="H30" s="11"/>
-      <c r="I30" s="13"/>
+      <c r="F30" s="21"/>
+      <c r="G30" s="21"/>
+      <c r="H30" s="10"/>
+      <c r="I30" s="12"/>
     </row>
     <row r="31" spans="2:10" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C31" s="21" t="s">
+      <c r="C31" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D31" s="22" t="s">
+      <c r="D31" s="21" t="s">
         <v>44</v>
       </c>
-      <c r="E31" s="23" t="s">
+      <c r="E31" s="22" t="s">
         <v>43</v>
       </c>
-      <c r="F31" s="22"/>
-      <c r="G31" s="22"/>
-      <c r="H31" s="11"/>
-      <c r="I31" s="13"/>
+      <c r="F31" s="21"/>
+      <c r="G31" s="21"/>
+      <c r="H31" s="10"/>
+      <c r="I31" s="12"/>
     </row>
     <row r="32" spans="2:10" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C32" s="21" t="s">
+      <c r="C32" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="22" t="s">
+      <c r="D32" s="21" t="s">
         <v>45</v>
       </c>
-      <c r="E32" s="23" t="s">
+      <c r="E32" s="22" t="s">
         <v>46</v>
       </c>
-      <c r="F32" s="22"/>
-      <c r="G32" s="22"/>
-      <c r="H32" s="11"/>
-      <c r="I32" s="13"/>
+      <c r="F32" s="21"/>
+      <c r="G32" s="21"/>
+      <c r="H32" s="10"/>
+      <c r="I32" s="12"/>
     </row>
     <row r="33" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C33" s="21" t="s">
+      <c r="C33" s="20" t="s">
         <v>18</v>
       </c>
-      <c r="D33" s="22" t="s">
+      <c r="D33" s="21" t="s">
         <v>47</v>
       </c>
-      <c r="E33" s="23" t="s">
+      <c r="E33" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="F33" s="22"/>
-      <c r="G33" s="22"/>
-      <c r="H33" s="11"/>
-      <c r="I33" s="13"/>
+      <c r="F33" s="21"/>
+      <c r="G33" s="21"/>
+      <c r="H33" s="10"/>
+      <c r="I33" s="12"/>
     </row>
     <row r="34" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C34" s="21" t="s">
+      <c r="C34" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D34" s="22" t="s">
+      <c r="D34" s="21" t="s">
         <v>50</v>
       </c>
-      <c r="E34" s="23" t="s">
+      <c r="E34" s="22" t="s">
         <v>51</v>
       </c>
-      <c r="F34" s="22"/>
-      <c r="G34" s="22"/>
-      <c r="H34" s="11"/>
-      <c r="I34" s="13"/>
+      <c r="F34" s="21"/>
+      <c r="G34" s="21"/>
+      <c r="H34" s="10"/>
+      <c r="I34" s="12"/>
     </row>
     <row r="35" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C35" s="21" t="s">
+      <c r="C35" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="22" t="s">
+      <c r="D35" s="21" t="s">
         <v>52</v>
       </c>
-      <c r="E35" s="23" t="s">
+      <c r="E35" s="22" t="s">
         <v>53</v>
       </c>
-      <c r="F35" s="22"/>
-      <c r="G35" s="22"/>
-      <c r="H35" s="11"/>
-      <c r="I35" s="13"/>
+      <c r="F35" s="21"/>
+      <c r="G35" s="21"/>
+      <c r="H35" s="10"/>
+      <c r="I35" s="12"/>
     </row>
     <row r="36" spans="3:9" ht="105.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D36" s="22" t="s">
+      <c r="D36" s="21" t="s">
         <v>56</v>
       </c>
-      <c r="E36" s="23" t="s">
+      <c r="E36" s="22" t="s">
         <v>54</v>
       </c>
-      <c r="F36" s="22"/>
-      <c r="G36" s="22"/>
-      <c r="H36" s="11"/>
-      <c r="I36" s="13"/>
+      <c r="F36" s="21"/>
+      <c r="G36" s="21"/>
+      <c r="H36" s="10"/>
+      <c r="I36" s="12"/>
     </row>
     <row r="37" spans="3:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C37" s="21" t="s">
+      <c r="C37" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D37" s="22" t="s">
+      <c r="D37" s="21" t="s">
         <v>55</v>
       </c>
-      <c r="E37" s="23" t="s">
+      <c r="E37" s="22" t="s">
         <v>57</v>
       </c>
-      <c r="F37" s="22"/>
-      <c r="G37" s="22"/>
-      <c r="H37" s="11"/>
-      <c r="I37" s="13"/>
+      <c r="F37" s="21"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="10"/>
+      <c r="I37" s="12"/>
     </row>
     <row r="38" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C38" s="21" t="s">
+      <c r="C38" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D38" s="22" t="s">
+      <c r="D38" s="21" t="s">
         <v>58</v>
       </c>
-      <c r="E38" s="23" t="s">
+      <c r="E38" s="22" t="s">
         <v>59</v>
       </c>
-      <c r="F38" s="22"/>
-      <c r="G38" s="22"/>
-      <c r="H38" s="11"/>
-      <c r="I38" s="13"/>
+      <c r="F38" s="21"/>
+      <c r="G38" s="21"/>
+      <c r="H38" s="10"/>
+      <c r="I38" s="12"/>
     </row>
     <row r="39" spans="3:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C39" s="21" t="s">
+      <c r="C39" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D39" s="22" t="s">
+      <c r="D39" s="21" t="s">
         <v>60</v>
       </c>
-      <c r="E39" s="23" t="s">
+      <c r="E39" s="22" t="s">
         <v>61</v>
       </c>
-      <c r="F39" s="22"/>
-      <c r="G39" s="22"/>
-      <c r="H39" s="11"/>
-      <c r="I39" s="13"/>
+      <c r="F39" s="21"/>
+      <c r="G39" s="21"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="12"/>
     </row>
     <row r="40" spans="3:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C40" s="21" t="s">
+      <c r="C40" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D40" s="22" t="s">
+      <c r="D40" s="21" t="s">
         <v>63</v>
       </c>
-      <c r="E40" s="23" t="s">
+      <c r="E40" s="22" t="s">
         <v>62</v>
       </c>
-      <c r="F40" s="22"/>
-      <c r="G40" s="22"/>
-      <c r="H40" s="11"/>
-      <c r="I40" s="13"/>
+      <c r="F40" s="21"/>
+      <c r="G40" s="21"/>
+      <c r="H40" s="10"/>
+      <c r="I40" s="12"/>
     </row>
     <row r="41" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C41" s="21" t="s">
+      <c r="C41" s="20" t="s">
         <v>49</v>
       </c>
-      <c r="D41" s="22" t="s">
+      <c r="D41" s="21" t="s">
         <v>64</v>
       </c>
-      <c r="E41" s="23" t="s">
+      <c r="E41" s="22" t="s">
         <v>65</v>
       </c>
-      <c r="F41" s="22"/>
-      <c r="G41" s="22"/>
-      <c r="H41" s="11"/>
-      <c r="I41" s="13"/>
+      <c r="F41" s="21"/>
+      <c r="G41" s="21"/>
+      <c r="H41" s="10"/>
+      <c r="I41" s="12"/>
     </row>
     <row r="42" spans="3:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C42" s="21"/>
-      <c r="D42" s="22" t="s">
+      <c r="C42" s="20"/>
+      <c r="D42" s="21" t="s">
         <v>66</v>
       </c>
-      <c r="E42" s="23" t="s">
+      <c r="E42" s="22" t="s">
         <v>67</v>
       </c>
-      <c r="F42" s="22"/>
-      <c r="G42" s="22"/>
-      <c r="H42" s="11"/>
-      <c r="I42" s="13"/>
+      <c r="F42" s="21"/>
+      <c r="G42" s="21"/>
+      <c r="H42" s="10"/>
+      <c r="I42" s="12"/>
     </row>
     <row r="43" spans="3:9" ht="90.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C43" s="21" t="s">
+      <c r="C43" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D43" s="22" t="s">
+      <c r="D43" s="21" t="s">
         <v>69</v>
       </c>
-      <c r="E43" s="23" t="s">
+      <c r="E43" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="22"/>
-      <c r="G43" s="22"/>
-      <c r="H43" s="11"/>
-      <c r="I43" s="13"/>
+      <c r="F43" s="21"/>
+      <c r="G43" s="21"/>
+      <c r="H43" s="10"/>
+      <c r="I43" s="12"/>
     </row>
     <row r="44" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C44" s="21" t="s">
+      <c r="C44" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D44" s="22" t="s">
+      <c r="D44" s="21" t="s">
         <v>70</v>
       </c>
-      <c r="E44" s="23" t="s">
+      <c r="E44" s="22" t="s">
         <v>27</v>
       </c>
-      <c r="F44" s="22"/>
-      <c r="G44" s="22"/>
-      <c r="H44" s="11"/>
-      <c r="I44" s="13"/>
+      <c r="F44" s="21"/>
+      <c r="G44" s="21"/>
+      <c r="H44" s="10"/>
+      <c r="I44" s="12"/>
     </row>
     <row r="45" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C45" s="21" t="s">
+      <c r="C45" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D45" s="22" t="s">
+      <c r="D45" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E45" s="23" t="s">
+      <c r="E45" s="22" t="s">
         <v>26</v>
       </c>
-      <c r="F45" s="22"/>
-      <c r="G45" s="22"/>
-      <c r="H45" s="11"/>
-      <c r="I45" s="13"/>
+      <c r="F45" s="21"/>
+      <c r="G45" s="21"/>
+      <c r="H45" s="10"/>
+      <c r="I45" s="12"/>
     </row>
     <row r="46" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C46" s="21" t="s">
+      <c r="C46" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D46" s="22" t="s">
+      <c r="D46" s="21" t="s">
         <v>72</v>
       </c>
-      <c r="E46" s="23" t="s">
+      <c r="E46" s="22" t="s">
         <v>21</v>
       </c>
-      <c r="F46" s="22"/>
-      <c r="G46" s="22"/>
-      <c r="H46" s="11"/>
-      <c r="I46" s="13"/>
+      <c r="F46" s="21"/>
+      <c r="G46" s="21"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="12"/>
     </row>
     <row r="47" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C47" s="21" t="s">
+      <c r="C47" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D47" s="22" t="s">
+      <c r="D47" s="21" t="s">
         <v>73</v>
       </c>
-      <c r="E47" s="23" t="s">
+      <c r="E47" s="22" t="s">
         <v>22</v>
       </c>
-      <c r="F47" s="22"/>
-      <c r="G47" s="22"/>
-      <c r="H47" s="11"/>
-      <c r="I47" s="13"/>
+      <c r="F47" s="21"/>
+      <c r="G47" s="21"/>
+      <c r="H47" s="10"/>
+      <c r="I47" s="12"/>
     </row>
     <row r="48" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C48" s="21" t="s">
+      <c r="C48" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D48" s="22" t="s">
+      <c r="D48" s="21" t="s">
         <v>74</v>
       </c>
-      <c r="E48" s="23" t="s">
+      <c r="E48" s="22" t="s">
         <v>24</v>
       </c>
-      <c r="F48" s="22"/>
-      <c r="G48" s="22"/>
-      <c r="H48" s="11"/>
-      <c r="I48" s="13"/>
+      <c r="F48" s="21"/>
+      <c r="G48" s="21"/>
+      <c r="H48" s="10"/>
+      <c r="I48" s="12"/>
     </row>
     <row r="49" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C49" s="21" t="s">
+      <c r="C49" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="D49" s="22" t="s">
+      <c r="D49" s="21" t="s">
         <v>75</v>
       </c>
-      <c r="E49" s="23" t="s">
+      <c r="E49" s="22" t="s">
         <v>23</v>
       </c>
-      <c r="F49" s="22"/>
-      <c r="G49" s="22"/>
-      <c r="H49" s="11"/>
-      <c r="I49" s="13"/>
+      <c r="F49" s="21"/>
+      <c r="G49" s="21"/>
+      <c r="H49" s="10"/>
+      <c r="I49" s="12"/>
     </row>
     <row r="50" spans="3:9" ht="45.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C50" s="21" t="s">
+      <c r="C50" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D50" s="22" t="s">
+      <c r="D50" s="21" t="s">
         <v>76</v>
       </c>
-      <c r="E50" s="23" t="s">
+      <c r="E50" s="22" t="s">
         <v>77</v>
       </c>
-      <c r="F50" s="22"/>
-      <c r="G50" s="22"/>
-      <c r="H50" s="11"/>
-      <c r="I50" s="13"/>
+      <c r="F50" s="21"/>
+      <c r="G50" s="21"/>
+      <c r="H50" s="10"/>
+      <c r="I50" s="12"/>
     </row>
     <row r="51" spans="3:9" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C51" s="21" t="s">
+      <c r="C51" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D51" s="22" t="s">
+      <c r="D51" s="21" t="s">
         <v>78</v>
       </c>
-      <c r="E51" s="23" t="s">
+      <c r="E51" s="22" t="s">
         <v>79</v>
       </c>
-      <c r="F51" s="22"/>
-      <c r="G51" s="22"/>
-      <c r="H51" s="11"/>
-      <c r="I51" s="13"/>
+      <c r="F51" s="21"/>
+      <c r="G51" s="21"/>
+      <c r="H51" s="10"/>
+      <c r="I51" s="12"/>
     </row>
     <row r="52" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C52" s="21" t="s">
+      <c r="C52" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D52" s="22" t="s">
+      <c r="D52" s="21" t="s">
         <v>80</v>
       </c>
-      <c r="E52" s="23" t="s">
+      <c r="E52" s="22" t="s">
         <v>81</v>
       </c>
-      <c r="F52" s="22"/>
-      <c r="G52" s="22"/>
-      <c r="H52" s="11"/>
-      <c r="I52" s="13"/>
+      <c r="F52" s="21"/>
+      <c r="G52" s="21"/>
+      <c r="H52" s="10"/>
+      <c r="I52" s="12"/>
     </row>
     <row r="53" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="21" t="s">
+      <c r="C53" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D53" s="22" t="s">
+      <c r="D53" s="21" t="s">
         <v>83</v>
       </c>
-      <c r="E53" s="23" t="s">
+      <c r="E53" s="22" t="s">
         <v>82</v>
       </c>
-      <c r="F53" s="22"/>
-      <c r="G53" s="22"/>
-      <c r="H53" s="11"/>
-      <c r="I53" s="13"/>
+      <c r="F53" s="21"/>
+      <c r="G53" s="21"/>
+      <c r="H53" s="10"/>
+      <c r="I53" s="12"/>
     </row>
     <row r="54" spans="3:9" ht="30.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C54" s="21" t="s">
+      <c r="C54" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D54" s="22" t="s">
+      <c r="D54" s="21" t="s">
         <v>84</v>
       </c>
-      <c r="E54" s="23" t="s">
+      <c r="E54" s="22" t="s">
         <v>85</v>
       </c>
-      <c r="F54" s="22"/>
-      <c r="G54" s="22"/>
-      <c r="H54" s="11"/>
-      <c r="I54" s="13"/>
+      <c r="F54" s="21"/>
+      <c r="G54" s="21"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="12"/>
     </row>
     <row r="55" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C55" s="21" t="s">
+      <c r="C55" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D55" s="22" t="s">
+      <c r="D55" s="21" t="s">
         <v>86</v>
       </c>
-      <c r="E55" s="23" t="s">
+      <c r="E55" s="22" t="s">
         <v>92</v>
       </c>
-      <c r="F55" s="22"/>
-      <c r="G55" s="22"/>
-      <c r="H55" s="11"/>
-      <c r="I55" s="13"/>
+      <c r="F55" s="21"/>
+      <c r="G55" s="21"/>
+      <c r="H55" s="10"/>
+      <c r="I55" s="12"/>
     </row>
     <row r="56" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C56" s="21" t="s">
+      <c r="C56" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D56" s="22" t="s">
+      <c r="D56" s="21" t="s">
         <v>87</v>
       </c>
-      <c r="E56" s="23" t="s">
+      <c r="E56" s="22" t="s">
         <v>88</v>
       </c>
-      <c r="F56" s="22"/>
-      <c r="G56" s="22"/>
-      <c r="H56" s="11"/>
-      <c r="I56" s="13"/>
+      <c r="F56" s="21"/>
+      <c r="G56" s="21"/>
+      <c r="H56" s="10"/>
+      <c r="I56" s="12"/>
     </row>
     <row r="57" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C57" s="21" t="s">
+      <c r="C57" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="D57" s="22" t="s">
+      <c r="D57" s="21" t="s">
         <v>91</v>
       </c>
-      <c r="E57" s="23" t="s">
+      <c r="E57" s="22" t="s">
         <v>90</v>
       </c>
-      <c r="F57" s="22"/>
-      <c r="G57" s="22"/>
-      <c r="H57" s="11"/>
-      <c r="I57" s="13"/>
+      <c r="F57" s="21"/>
+      <c r="G57" s="21"/>
+      <c r="H57" s="10"/>
+      <c r="I57" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>

<commit_message>
Add Data Flow Design IDs
Add Data Flow Design IDs
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="368" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="215">
   <si>
     <t>Author</t>
   </si>
@@ -32,13 +32,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>Test Case ID</t>
-  </si>
-  <si>
     <t>SIQ ID</t>
-  </si>
-  <si>
-    <t>Design ID</t>
   </si>
   <si>
     <t>Comment</t>
@@ -660,6 +654,64 @@
   </si>
   <si>
     <t>BANK_SYS_SIQ_Q45</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Test Case ID</t>
+  </si>
+  <si>
+    <t>Data Flow Design ID</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_003</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_ADMIN_003
+</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_008
+Bank_Sys_DM_ADMIN_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005
+Bank_Sys_DM_ADMIN_007</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_001
+Bank_Sys_DM_CST_001</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_004</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_005
+Bank_Sys_DM_CST_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_006
+Bank_Sys_DM_CST_007</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_005</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008</t>
   </si>
 </sst>
 </file>
@@ -971,7 +1023,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="44">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -1033,36 +1085,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1098,6 +1120,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1381,8 +1436,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A130" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F94" sqref="F94"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1390,9 +1445,9 @@
     <col min="1" max="1" width="9" customWidth="1"/>
     <col min="2" max="2" width="18.7109375" customWidth="1"/>
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
-    <col min="4" max="4" width="26.28515625" style="43" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="43" customWidth="1"/>
-    <col min="6" max="6" width="24.85546875" customWidth="1"/>
+    <col min="4" max="4" width="26.28515625" style="33" customWidth="1"/>
+    <col min="5" max="5" width="27.7109375" style="33" customWidth="1"/>
+    <col min="6" max="6" width="33.28515625" style="33" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
@@ -1400,103 +1455,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="22" t="s">
-        <v>13</v>
-      </c>
-      <c r="B1" s="22"/>
-      <c r="C1" s="22"/>
-      <c r="D1" s="22"/>
-      <c r="E1" s="22"/>
-      <c r="F1" s="22"/>
-      <c r="G1" s="22"/>
-      <c r="H1" s="22"/>
-      <c r="I1" s="22"/>
-      <c r="J1" s="22"/>
-      <c r="K1" s="22"/>
-      <c r="L1" s="22"/>
+      <c r="A1" s="34" t="s">
+        <v>11</v>
+      </c>
+      <c r="B1" s="34"/>
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34"/>
+      <c r="K1" s="34"/>
+      <c r="L1" s="34"/>
     </row>
     <row r="2" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="22"/>
-      <c r="B2" s="22"/>
-      <c r="C2" s="22"/>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="22"/>
-      <c r="G2" s="22"/>
-      <c r="H2" s="22"/>
-      <c r="I2" s="22"/>
-      <c r="J2" s="22"/>
-      <c r="K2" s="22"/>
-      <c r="L2" s="22"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="34"/>
+      <c r="C2" s="34"/>
+      <c r="D2" s="34"/>
+      <c r="E2" s="34"/>
+      <c r="F2" s="34"/>
+      <c r="G2" s="34"/>
+      <c r="H2" s="34"/>
+      <c r="I2" s="34"/>
+      <c r="J2" s="34"/>
+      <c r="K2" s="34"/>
+      <c r="L2" s="34"/>
     </row>
     <row r="3" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="22"/>
-      <c r="B3" s="22"/>
-      <c r="C3" s="22"/>
-      <c r="D3" s="22"/>
-      <c r="E3" s="22"/>
-      <c r="F3" s="22"/>
-      <c r="G3" s="22"/>
-      <c r="H3" s="22"/>
-      <c r="I3" s="22"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="22"/>
-      <c r="L3" s="22"/>
+      <c r="A3" s="34"/>
+      <c r="B3" s="34"/>
+      <c r="C3" s="34"/>
+      <c r="D3" s="34"/>
+      <c r="E3" s="34"/>
+      <c r="F3" s="34"/>
+      <c r="G3" s="34"/>
+      <c r="H3" s="34"/>
+      <c r="I3" s="34"/>
+      <c r="J3" s="34"/>
+      <c r="K3" s="34"/>
+      <c r="L3" s="34"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22"/>
-      <c r="B4" s="22"/>
-      <c r="C4" s="22"/>
-      <c r="D4" s="22"/>
-      <c r="E4" s="22"/>
-      <c r="F4" s="22"/>
-      <c r="G4" s="22"/>
-      <c r="H4" s="22"/>
-      <c r="I4" s="22"/>
-      <c r="J4" s="22"/>
-      <c r="K4" s="22"/>
-      <c r="L4" s="22"/>
+      <c r="A4" s="34"/>
+      <c r="B4" s="34"/>
+      <c r="C4" s="34"/>
+      <c r="D4" s="34"/>
+      <c r="E4" s="34"/>
+      <c r="F4" s="34"/>
+      <c r="G4" s="34"/>
+      <c r="H4" s="34"/>
+      <c r="I4" s="34"/>
+      <c r="J4" s="34"/>
+      <c r="K4" s="34"/>
+      <c r="L4" s="34"/>
     </row>
     <row r="5" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="22"/>
-      <c r="B5" s="22"/>
-      <c r="C5" s="22"/>
-      <c r="D5" s="22"/>
-      <c r="E5" s="22"/>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22"/>
-      <c r="H5" s="22"/>
-      <c r="I5" s="22"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="22"/>
-      <c r="L5" s="22"/>
+      <c r="A5" s="34"/>
+      <c r="B5" s="34"/>
+      <c r="C5" s="34"/>
+      <c r="D5" s="34"/>
+      <c r="E5" s="34"/>
+      <c r="F5" s="34"/>
+      <c r="G5" s="34"/>
+      <c r="H5" s="34"/>
+      <c r="I5" s="34"/>
+      <c r="J5" s="34"/>
+      <c r="K5" s="34"/>
+      <c r="L5" s="34"/>
     </row>
     <row r="6" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="22"/>
-      <c r="D6" s="22"/>
-      <c r="E6" s="22"/>
-      <c r="F6" s="22"/>
-      <c r="G6" s="22"/>
-      <c r="H6" s="22"/>
-      <c r="I6" s="22"/>
-      <c r="J6" s="22"/>
-      <c r="K6" s="22"/>
-      <c r="L6" s="22"/>
+      <c r="A6" s="34"/>
+      <c r="B6" s="34"/>
+      <c r="C6" s="34"/>
+      <c r="D6" s="34"/>
+      <c r="E6" s="34"/>
+      <c r="F6" s="34"/>
+      <c r="G6" s="34"/>
+      <c r="H6" s="34"/>
+      <c r="I6" s="34"/>
+      <c r="J6" s="34"/>
+      <c r="K6" s="34"/>
+      <c r="L6" s="34"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="23" t="s">
-        <v>7</v>
-      </c>
-      <c r="C7" s="23"/>
-      <c r="D7" s="23"/>
-      <c r="E7" s="23"/>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
+      <c r="B7" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="C7" s="35"/>
+      <c r="D7" s="35"/>
+      <c r="E7" s="35"/>
+      <c r="F7" s="35"/>
+      <c r="G7" s="35"/>
+      <c r="H7" s="35"/>
+      <c r="I7" s="35"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1504,1973 +1559,2179 @@
         <v>0</v>
       </c>
       <c r="C8" s="19" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="24" t="s">
-        <v>5</v>
-      </c>
-      <c r="F8" s="24"/>
+      <c r="E8" s="36" t="s">
+        <v>3</v>
+      </c>
+      <c r="F8" s="36"/>
       <c r="G8" s="19" t="s">
+        <v>7</v>
+      </c>
+      <c r="H8" s="19" t="s">
+        <v>8</v>
+      </c>
+      <c r="I8" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="H8" s="19" t="s">
-        <v>10</v>
-      </c>
-      <c r="I8" s="24" t="s">
-        <v>11</v>
-      </c>
-      <c r="J8" s="25"/>
+      <c r="J8" s="37"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C9" s="4">
         <v>1</v>
       </c>
-      <c r="D9" s="31" t="s">
-        <v>6</v>
-      </c>
-      <c r="E9" s="26" t="s">
-        <v>14</v>
-      </c>
-      <c r="F9" s="26"/>
+      <c r="D9" s="21" t="s">
+        <v>4</v>
+      </c>
+      <c r="E9" s="38" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="38"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="26"/>
-      <c r="J9" s="27"/>
+      <c r="I9" s="38"/>
+      <c r="J9" s="39"/>
     </row>
     <row r="10" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
-        <v>12</v>
+        <v>10</v>
       </c>
       <c r="C10" s="4">
         <v>2</v>
       </c>
-      <c r="D10" s="32">
+      <c r="D10" s="22">
         <v>43529</v>
       </c>
-      <c r="E10" s="28" t="s">
-        <v>66</v>
-      </c>
-      <c r="F10" s="29"/>
+      <c r="E10" s="40" t="s">
+        <v>64</v>
+      </c>
+      <c r="F10" s="41"/>
       <c r="G10" s="17" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="H10" s="18">
         <v>43529</v>
       </c>
-      <c r="I10" s="28" t="s">
-        <v>67</v>
-      </c>
-      <c r="J10" s="30"/>
+      <c r="I10" s="40" t="s">
+        <v>65</v>
+      </c>
+      <c r="J10" s="42"/>
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="21" t="s">
-        <v>68</v>
-      </c>
-      <c r="C13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="21"/>
-      <c r="F13" s="21"/>
-      <c r="G13" s="21"/>
-      <c r="H13" s="21"/>
-      <c r="I13" s="21"/>
-      <c r="J13" s="21"/>
+      <c r="B13" s="43" t="s">
+        <v>66</v>
+      </c>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
+      <c r="G13" s="43"/>
+      <c r="H13" s="43"/>
+      <c r="I13" s="43"/>
+      <c r="J13" s="43"/>
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="21"/>
-      <c r="C14" s="21"/>
-      <c r="D14" s="21"/>
-      <c r="E14" s="21"/>
-      <c r="F14" s="21"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
-      <c r="I14" s="21"/>
-      <c r="J14" s="21"/>
+      <c r="B14" s="43"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
+      <c r="G14" s="43"/>
+      <c r="H14" s="43"/>
+      <c r="I14" s="43"/>
+      <c r="J14" s="43"/>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="21"/>
-      <c r="C15" s="21"/>
-      <c r="D15" s="21"/>
-      <c r="E15" s="21"/>
-      <c r="F15" s="21"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="21"/>
-      <c r="J15" s="21"/>
+      <c r="B15" s="43"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
+      <c r="G15" s="43"/>
+      <c r="H15" s="43"/>
+      <c r="I15" s="43"/>
+      <c r="J15" s="43"/>
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="21"/>
-      <c r="C16" s="21"/>
-      <c r="D16" s="21"/>
-      <c r="E16" s="21"/>
-      <c r="F16" s="21"/>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="21"/>
-      <c r="J16" s="21"/>
+      <c r="B16" s="43"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
+      <c r="G16" s="43"/>
+      <c r="H16" s="43"/>
+      <c r="I16" s="43"/>
+      <c r="J16" s="43"/>
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="21"/>
-      <c r="C17" s="21"/>
-      <c r="D17" s="21"/>
-      <c r="E17" s="21"/>
-      <c r="F17" s="21"/>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="21"/>
-      <c r="J17" s="21"/>
+      <c r="B17" s="43"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
+      <c r="G17" s="43"/>
+      <c r="H17" s="43"/>
+      <c r="I17" s="43"/>
+      <c r="J17" s="43"/>
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="21"/>
-      <c r="C18" s="21"/>
-      <c r="D18" s="21"/>
-      <c r="E18" s="21"/>
-      <c r="F18" s="21"/>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="21"/>
-      <c r="J18" s="21"/>
+      <c r="B18" s="43"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
+      <c r="G18" s="43"/>
+      <c r="H18" s="43"/>
+      <c r="I18" s="43"/>
+      <c r="J18" s="43"/>
     </row>
     <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="21"/>
-      <c r="C19" s="21"/>
-      <c r="D19" s="21"/>
-      <c r="E19" s="21"/>
-      <c r="F19" s="21"/>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="21"/>
-      <c r="J19" s="21"/>
+      <c r="B19" s="43"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
+      <c r="G19" s="43"/>
+      <c r="H19" s="43"/>
+      <c r="I19" s="43"/>
+      <c r="J19" s="43"/>
     </row>
     <row r="20" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="21"/>
-      <c r="C20" s="21"/>
-      <c r="D20" s="21"/>
-      <c r="E20" s="21"/>
-      <c r="F20" s="21"/>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="21"/>
-      <c r="J20" s="21"/>
+      <c r="B20" s="43"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
+      <c r="G20" s="43"/>
+      <c r="H20" s="43"/>
+      <c r="I20" s="43"/>
+      <c r="J20" s="43"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="21"/>
-      <c r="C21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="21"/>
-      <c r="F21" s="21"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="21"/>
-      <c r="J21" s="21"/>
+      <c r="B21" s="43"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
+      <c r="G21" s="43"/>
+      <c r="H21" s="43"/>
+      <c r="I21" s="43"/>
+      <c r="J21" s="43"/>
     </row>
     <row r="22" spans="2:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="16" t="s">
+        <v>68</v>
+      </c>
+      <c r="D22" s="9" t="s">
+        <v>69</v>
+      </c>
+      <c r="E22" s="10" t="s">
+        <v>2</v>
+      </c>
+      <c r="F22" s="10" t="s">
+        <v>199</v>
+      </c>
+      <c r="G22" s="10" t="s">
+        <v>198</v>
+      </c>
+      <c r="H22" s="11" t="s">
+        <v>13</v>
+      </c>
+      <c r="I22" s="7"/>
+    </row>
+    <row r="23" spans="2:10" s="23" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="12" t="s">
         <v>70</v>
       </c>
-      <c r="D22" s="9" t="s">
-        <v>71</v>
-      </c>
-      <c r="E22" s="10" t="s">
-        <v>3</v>
-      </c>
-      <c r="F22" s="10" t="s">
-        <v>2</v>
-      </c>
-      <c r="G22" s="10" t="s">
-        <v>4</v>
-      </c>
-      <c r="H22" s="11" t="s">
-        <v>15</v>
-      </c>
-      <c r="I22" s="7"/>
-    </row>
-    <row r="23" spans="2:10" s="33" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C23" s="12" t="s">
-        <v>72</v>
-      </c>
-      <c r="D23" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="E23" s="35" t="s">
-        <v>25</v>
-      </c>
-      <c r="F23" s="13"/>
+      <c r="D23" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E23" s="25" t="s">
+        <v>23</v>
+      </c>
+      <c r="F23" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G23" s="13"/>
       <c r="H23" s="5"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="2:10" s="36" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C24" s="37" t="s">
+    <row r="24" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="27" t="s">
+        <v>71</v>
+      </c>
+      <c r="D24" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E24" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F24" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="G24" s="29"/>
+      <c r="H24" s="30"/>
+      <c r="I24" s="7"/>
+    </row>
+    <row r="25" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C25" s="27" t="s">
         <v>73</v>
       </c>
-      <c r="D24" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E24" s="39" t="s">
+      <c r="D25" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E25" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F25" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="G25" s="29"/>
+      <c r="H25" s="30"/>
+      <c r="I25" s="7"/>
+    </row>
+    <row r="26" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C26" s="27" t="s">
         <v>74</v>
       </c>
-      <c r="F24" s="39"/>
-      <c r="G24" s="39"/>
-      <c r="H24" s="40"/>
-      <c r="I24" s="7"/>
-    </row>
-    <row r="25" spans="2:10" s="36" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="37" t="s">
+      <c r="D26" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E26" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F26" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="G26" s="29"/>
+      <c r="H26" s="30"/>
+      <c r="I26" s="7"/>
+    </row>
+    <row r="27" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C27" s="27" t="s">
         <v>75</v>
       </c>
-      <c r="D25" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E25" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="F25" s="39"/>
-      <c r="G25" s="39"/>
-      <c r="H25" s="40"/>
-      <c r="I25" s="7"/>
-    </row>
-    <row r="26" spans="2:10" s="36" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="37" t="s">
+      <c r="D27" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E27" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F27" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="G27" s="29"/>
+      <c r="H27" s="30"/>
+      <c r="I27" s="7"/>
+    </row>
+    <row r="28" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C28" s="27" t="s">
         <v>76</v>
       </c>
-      <c r="D26" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E26" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="F26" s="39"/>
-      <c r="G26" s="39"/>
-      <c r="H26" s="40"/>
-      <c r="I26" s="7"/>
-    </row>
-    <row r="27" spans="2:10" s="36" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C27" s="37" t="s">
+      <c r="D28" s="28" t="s">
+        <v>14</v>
+      </c>
+      <c r="E28" s="29" t="s">
+        <v>72</v>
+      </c>
+      <c r="F28" s="44" t="s">
+        <v>207</v>
+      </c>
+      <c r="G28" s="29"/>
+      <c r="H28" s="30"/>
+      <c r="I28" s="7"/>
+    </row>
+    <row r="29" spans="2:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C29" s="14" t="s">
         <v>77</v>
       </c>
-      <c r="D27" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E27" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="F27" s="39"/>
-      <c r="G27" s="39"/>
-      <c r="H27" s="40"/>
-      <c r="I27" s="7"/>
-    </row>
-    <row r="28" spans="2:10" s="36" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C28" s="37" t="s">
-        <v>78</v>
-      </c>
-      <c r="D28" s="38" t="s">
-        <v>16</v>
-      </c>
-      <c r="E28" s="39" t="s">
-        <v>74</v>
-      </c>
-      <c r="F28" s="39"/>
-      <c r="G28" s="39"/>
-      <c r="H28" s="40"/>
-      <c r="I28" s="7"/>
-    </row>
-    <row r="29" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C29" s="14" t="s">
-        <v>79</v>
-      </c>
-      <c r="D29" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E29" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F29" s="15"/>
+      <c r="D29" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E29" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F29" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G29" s="15"/>
       <c r="H29" s="6"/>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="37.5" x14ac:dyDescent="0.25">
       <c r="C30" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="D30" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="E30" s="35" t="s">
-        <v>26</v>
-      </c>
-      <c r="F30" s="13"/>
+        <v>78</v>
+      </c>
+      <c r="D30" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E30" s="25" t="s">
+        <v>24</v>
+      </c>
+      <c r="F30" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G30" s="13"/>
       <c r="H30" s="5"/>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="14" t="s">
-        <v>69</v>
-      </c>
-      <c r="D31" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E31" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F31" s="15"/>
+        <v>67</v>
+      </c>
+      <c r="D31" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F31" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G31" s="15"/>
       <c r="H31" s="6"/>
       <c r="I31" s="8"/>
     </row>
-    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" ht="37.5" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
-        <v>81</v>
-      </c>
-      <c r="D32" s="34" t="s">
-        <v>16</v>
-      </c>
-      <c r="E32" s="35" t="s">
-        <v>82</v>
-      </c>
-      <c r="F32" s="13"/>
+        <v>79</v>
+      </c>
+      <c r="D32" s="24" t="s">
+        <v>14</v>
+      </c>
+      <c r="E32" s="25" t="s">
+        <v>80</v>
+      </c>
+      <c r="F32" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G32" s="13"/>
       <c r="H32" s="5"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="14" t="s">
-        <v>83</v>
-      </c>
-      <c r="D33" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E33" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F33" s="15"/>
+        <v>81</v>
+      </c>
+      <c r="D33" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E33" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F33" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G33" s="15"/>
       <c r="H33" s="6"/>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="14" t="s">
-        <v>84</v>
-      </c>
-      <c r="D34" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E34" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F34" s="15"/>
+        <v>82</v>
+      </c>
+      <c r="D34" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E34" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F34" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G34" s="15"/>
       <c r="H34" s="6"/>
       <c r="I34" s="8"/>
     </row>
-    <row r="35" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="14" t="s">
-        <v>85</v>
-      </c>
-      <c r="D35" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E35" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F35" s="15"/>
+        <v>83</v>
+      </c>
+      <c r="D35" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E35" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F35" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G35" s="15"/>
       <c r="H35" s="6"/>
       <c r="I35" s="8"/>
     </row>
-    <row r="36" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="14" t="s">
-        <v>86</v>
-      </c>
-      <c r="D36" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E36" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F36" s="15"/>
+        <v>84</v>
+      </c>
+      <c r="D36" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E36" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F36" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G36" s="15"/>
       <c r="H36" s="6"/>
       <c r="I36" s="8"/>
     </row>
-    <row r="37" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="14" t="s">
-        <v>87</v>
-      </c>
-      <c r="D37" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E37" s="42" t="s">
-        <v>26</v>
-      </c>
-      <c r="F37" s="15"/>
+        <v>85</v>
+      </c>
+      <c r="D37" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E37" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="F37" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G37" s="15"/>
       <c r="H37" s="6"/>
       <c r="I37" s="8"/>
     </row>
-    <row r="38" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="14" t="s">
-        <v>88</v>
-      </c>
-      <c r="D38" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E38" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="F38" s="15"/>
+        <v>86</v>
+      </c>
+      <c r="D38" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E38" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F38" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G38" s="15"/>
       <c r="H38" s="6"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="14" t="s">
-        <v>89</v>
-      </c>
-      <c r="D39" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E39" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="F39" s="15"/>
+        <v>87</v>
+      </c>
+      <c r="D39" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E39" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F39" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G39" s="15"/>
       <c r="H39" s="6"/>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="14" t="s">
-        <v>90</v>
-      </c>
-      <c r="D40" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E40" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="F40" s="15"/>
+        <v>88</v>
+      </c>
+      <c r="D40" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E40" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F40" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G40" s="15"/>
       <c r="H40" s="6"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="14" t="s">
-        <v>91</v>
-      </c>
-      <c r="D41" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E41" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="F41" s="15"/>
+        <v>89</v>
+      </c>
+      <c r="D41" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E41" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F41" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G41" s="15"/>
       <c r="H41" s="6"/>
       <c r="I41" s="8"/>
     </row>
     <row r="42" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="14" t="s">
-        <v>27</v>
-      </c>
-      <c r="D42" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E42" s="42" t="s">
-        <v>93</v>
-      </c>
-      <c r="F42" s="15"/>
+        <v>25</v>
+      </c>
+      <c r="D42" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E42" s="32" t="s">
+        <v>91</v>
+      </c>
+      <c r="F42" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G42" s="15"/>
       <c r="H42" s="6"/>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="14" t="s">
-        <v>28</v>
-      </c>
-      <c r="D43" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E43" s="42" t="s">
-        <v>29</v>
-      </c>
-      <c r="F43" s="15"/>
+        <v>26</v>
+      </c>
+      <c r="D43" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E43" s="32" t="s">
+        <v>27</v>
+      </c>
+      <c r="F43" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G43" s="15"/>
       <c r="H43" s="6"/>
       <c r="I43" s="8"/>
     </row>
     <row r="44" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="14" t="s">
-        <v>30</v>
-      </c>
-      <c r="D44" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E44" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="F44" s="15"/>
+        <v>28</v>
+      </c>
+      <c r="D44" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E44" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F44" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G44" s="15"/>
       <c r="H44" s="6"/>
       <c r="I44" s="8"/>
     </row>
     <row r="45" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="14" t="s">
-        <v>95</v>
-      </c>
-      <c r="D45" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E45" s="42" t="s">
-        <v>94</v>
-      </c>
-      <c r="F45" s="15"/>
+        <v>93</v>
+      </c>
+      <c r="D45" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E45" s="32" t="s">
+        <v>92</v>
+      </c>
+      <c r="F45" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G45" s="15"/>
       <c r="H45" s="6"/>
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="D46" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E46" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="F46" s="15"/>
+        <v>94</v>
+      </c>
+      <c r="D46" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E46" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F46" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G46" s="15"/>
       <c r="H46" s="6"/>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="14" t="s">
-        <v>98</v>
-      </c>
-      <c r="D47" s="41" t="s">
-        <v>16</v>
-      </c>
-      <c r="E47" s="42" t="s">
-        <v>92</v>
-      </c>
-      <c r="F47" s="15"/>
+        <v>96</v>
+      </c>
+      <c r="D47" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="E47" s="32" t="s">
+        <v>90</v>
+      </c>
+      <c r="F47" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G47" s="15"/>
       <c r="H47" s="6"/>
       <c r="I47" s="8"/>
     </row>
     <row r="48" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="D48" s="31" t="s">
+        <v>98</v>
+      </c>
+      <c r="E48" s="32" t="s">
         <v>99</v>
       </c>
-      <c r="D48" s="41" t="s">
-        <v>100</v>
-      </c>
-      <c r="E48" s="42" t="s">
-        <v>101</v>
-      </c>
-      <c r="F48" s="15"/>
+      <c r="F48" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G48" s="15"/>
       <c r="H48" s="6"/>
       <c r="I48" s="8"/>
     </row>
-    <row r="49" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="14" t="s">
-        <v>102</v>
-      </c>
-      <c r="D49" s="41" t="s">
-        <v>103</v>
-      </c>
-      <c r="E49" s="42"/>
-      <c r="F49" s="15"/>
+        <v>100</v>
+      </c>
+      <c r="D49" s="31" t="s">
+        <v>101</v>
+      </c>
+      <c r="E49" s="32"/>
+      <c r="F49" s="44" t="s">
+        <v>207</v>
+      </c>
       <c r="G49" s="15"/>
       <c r="H49" s="6"/>
       <c r="I49" s="8"/>
     </row>
-    <row r="50" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="D50" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E50" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="F50" s="15"/>
+        <v>102</v>
+      </c>
+      <c r="D50" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E50" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F50" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G50" s="15"/>
       <c r="H50" s="6"/>
       <c r="I50" s="8"/>
     </row>
-    <row r="51" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="14" t="s">
-        <v>105</v>
-      </c>
-      <c r="D51" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E51" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="F51" s="15"/>
+        <v>103</v>
+      </c>
+      <c r="D51" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E51" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F51" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G51" s="15"/>
       <c r="H51" s="6"/>
       <c r="I51" s="8"/>
     </row>
-    <row r="52" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="14" t="s">
-        <v>106</v>
-      </c>
-      <c r="D52" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E52" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="F52" s="15"/>
+        <v>104</v>
+      </c>
+      <c r="D52" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E52" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F52" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G52" s="15"/>
       <c r="H52" s="6"/>
       <c r="I52" s="8"/>
     </row>
-    <row r="53" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="14" t="s">
-        <v>107</v>
-      </c>
-      <c r="D53" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E53" s="42" t="s">
-        <v>31</v>
-      </c>
-      <c r="F53" s="15"/>
+        <v>105</v>
+      </c>
+      <c r="D53" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E53" s="32" t="s">
+        <v>29</v>
+      </c>
+      <c r="F53" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G53" s="15"/>
       <c r="H53" s="6"/>
       <c r="I53" s="8"/>
     </row>
-    <row r="54" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="14" t="s">
-        <v>108</v>
-      </c>
-      <c r="D54" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E54" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F54" s="15"/>
+        <v>106</v>
+      </c>
+      <c r="D54" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E54" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F54" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G54" s="15"/>
       <c r="H54" s="6"/>
       <c r="I54" s="8"/>
     </row>
-    <row r="55" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="14" t="s">
-        <v>109</v>
-      </c>
-      <c r="D55" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E55" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F55" s="15"/>
+        <v>107</v>
+      </c>
+      <c r="D55" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E55" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F55" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G55" s="15"/>
       <c r="H55" s="6"/>
       <c r="I55" s="8"/>
     </row>
-    <row r="56" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="14" t="s">
-        <v>110</v>
-      </c>
-      <c r="D56" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E56" s="42" t="s">
-        <v>32</v>
-      </c>
-      <c r="F56" s="15"/>
+        <v>108</v>
+      </c>
+      <c r="D56" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E56" s="32" t="s">
+        <v>30</v>
+      </c>
+      <c r="F56" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G56" s="15"/>
       <c r="H56" s="6"/>
       <c r="I56" s="8"/>
     </row>
-    <row r="57" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D57" s="41" t="s">
-        <v>17</v>
-      </c>
-      <c r="E57" s="42" t="s">
-        <v>33</v>
-      </c>
-      <c r="F57" s="15"/>
+        <v>109</v>
+      </c>
+      <c r="D57" s="31" t="s">
+        <v>15</v>
+      </c>
+      <c r="E57" s="32" t="s">
+        <v>31</v>
+      </c>
+      <c r="F57" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G57" s="15"/>
       <c r="H57" s="6"/>
       <c r="I57" s="8"/>
     </row>
-    <row r="58" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="14" t="s">
-        <v>112</v>
-      </c>
-      <c r="D58" s="41"/>
-      <c r="E58" s="42" t="s">
-        <v>35</v>
-      </c>
-      <c r="F58" s="15"/>
+        <v>110</v>
+      </c>
+      <c r="D58" s="31"/>
+      <c r="E58" s="32" t="s">
+        <v>33</v>
+      </c>
+      <c r="F58" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G58" s="15"/>
       <c r="H58" s="6"/>
       <c r="I58" s="8"/>
     </row>
-    <row r="59" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="14" t="s">
-        <v>34</v>
-      </c>
-      <c r="D59" s="41"/>
-      <c r="E59" s="42" t="s">
-        <v>97</v>
-      </c>
-      <c r="F59" s="15"/>
+        <v>32</v>
+      </c>
+      <c r="D59" s="31"/>
+      <c r="E59" s="32" t="s">
+        <v>95</v>
+      </c>
+      <c r="F59" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G59" s="15"/>
       <c r="H59" s="6"/>
       <c r="I59" s="8"/>
     </row>
-    <row r="60" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="14" t="s">
-        <v>113</v>
-      </c>
-      <c r="D60" s="41" t="s">
-        <v>114</v>
-      </c>
-      <c r="E60" s="42"/>
-      <c r="F60" s="15"/>
+        <v>111</v>
+      </c>
+      <c r="D60" s="31" t="s">
+        <v>112</v>
+      </c>
+      <c r="E60" s="32"/>
+      <c r="F60" s="31" t="s">
+        <v>206</v>
+      </c>
       <c r="G60" s="15"/>
       <c r="H60" s="6"/>
       <c r="I60" s="8"/>
     </row>
     <row r="61" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D61" s="41" t="s">
+        <v>35</v>
+      </c>
+      <c r="D61" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E61" s="32" t="s">
         <v>36</v>
       </c>
-      <c r="E61" s="42" t="s">
-        <v>38</v>
-      </c>
-      <c r="F61" s="15"/>
+      <c r="F61" s="31" t="s">
+        <v>208</v>
+      </c>
       <c r="G61" s="15"/>
       <c r="H61" s="6"/>
       <c r="I61" s="8"/>
     </row>
     <row r="62" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="14" t="s">
-        <v>39</v>
-      </c>
-      <c r="D62" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E62" s="42" t="s">
-        <v>40</v>
-      </c>
-      <c r="F62" s="15"/>
+        <v>37</v>
+      </c>
+      <c r="D62" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E62" s="32" t="s">
+        <v>38</v>
+      </c>
+      <c r="F62" s="31"/>
       <c r="G62" s="15"/>
       <c r="H62" s="6"/>
       <c r="I62" s="8"/>
     </row>
-    <row r="63" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C63" s="14" t="s">
-        <v>115</v>
-      </c>
-      <c r="D63" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E63" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F63" s="15"/>
+        <v>113</v>
+      </c>
+      <c r="D63" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E63" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F63" s="31" t="s">
+        <v>209</v>
+      </c>
       <c r="G63" s="15"/>
       <c r="H63" s="6"/>
       <c r="I63" s="8"/>
     </row>
     <row r="64" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="14" t="s">
-        <v>116</v>
-      </c>
-      <c r="D64" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E64" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F64" s="15"/>
+        <v>114</v>
+      </c>
+      <c r="D64" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E64" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F64" s="31" t="s">
+        <v>210</v>
+      </c>
       <c r="G64" s="15"/>
       <c r="H64" s="6"/>
       <c r="I64" s="8"/>
     </row>
     <row r="65" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="14" t="s">
-        <v>117</v>
-      </c>
-      <c r="D65" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E65" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F65" s="15"/>
+        <v>115</v>
+      </c>
+      <c r="D65" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E65" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F65" s="31" t="s">
+        <v>210</v>
+      </c>
       <c r="G65" s="15"/>
       <c r="H65" s="6"/>
       <c r="I65" s="8"/>
     </row>
-    <row r="66" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="14" t="s">
-        <v>118</v>
-      </c>
-      <c r="D66" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E66" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F66" s="15"/>
+        <v>116</v>
+      </c>
+      <c r="D66" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E66" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F66" s="31" t="s">
+        <v>211</v>
+      </c>
       <c r="G66" s="15"/>
       <c r="H66" s="6"/>
       <c r="I66" s="8"/>
     </row>
     <row r="67" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="14" t="s">
-        <v>119</v>
-      </c>
-      <c r="D67" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E67" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F67" s="15"/>
+        <v>117</v>
+      </c>
+      <c r="D67" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E67" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F67" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G67" s="15"/>
       <c r="H67" s="6"/>
       <c r="I67" s="8"/>
     </row>
     <row r="68" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="14" t="s">
-        <v>120</v>
-      </c>
-      <c r="D68" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E68" s="42" t="s">
-        <v>41</v>
-      </c>
-      <c r="F68" s="15"/>
+        <v>118</v>
+      </c>
+      <c r="D68" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E68" s="32" t="s">
+        <v>39</v>
+      </c>
+      <c r="F68" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G68" s="15"/>
       <c r="H68" s="6"/>
       <c r="I68" s="8"/>
     </row>
     <row r="69" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="14" t="s">
-        <v>42</v>
-      </c>
-      <c r="D69" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E69" s="42" t="s">
-        <v>43</v>
-      </c>
-      <c r="F69" s="15"/>
+        <v>40</v>
+      </c>
+      <c r="D69" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E69" s="32" t="s">
+        <v>41</v>
+      </c>
+      <c r="F69" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G69" s="15"/>
       <c r="H69" s="6"/>
       <c r="I69" s="8"/>
     </row>
     <row r="70" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C70" s="14" t="s">
-        <v>44</v>
-      </c>
-      <c r="D70" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E70" s="42" t="s">
-        <v>45</v>
-      </c>
-      <c r="F70" s="15"/>
+        <v>42</v>
+      </c>
+      <c r="D70" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E70" s="32" t="s">
+        <v>43</v>
+      </c>
+      <c r="F70" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G70" s="15"/>
       <c r="H70" s="6"/>
       <c r="I70" s="8"/>
     </row>
     <row r="71" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C71" s="14" t="s">
-        <v>121</v>
-      </c>
-      <c r="D71" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E71" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F71" s="15"/>
+        <v>119</v>
+      </c>
+      <c r="D71" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E71" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F71" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G71" s="15"/>
       <c r="H71" s="6"/>
       <c r="I71" s="8"/>
     </row>
     <row r="72" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C72" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D72" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E72" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F72" s="15"/>
+        <v>120</v>
+      </c>
+      <c r="D72" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E72" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F72" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G72" s="15"/>
       <c r="H72" s="6"/>
       <c r="I72" s="8"/>
     </row>
     <row r="73" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="14" t="s">
-        <v>123</v>
-      </c>
-      <c r="D73" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E73" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F73" s="15"/>
+        <v>121</v>
+      </c>
+      <c r="D73" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E73" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F73" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G73" s="15"/>
       <c r="H73" s="6"/>
       <c r="I73" s="8"/>
     </row>
     <row r="74" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C74" s="14" t="s">
-        <v>48</v>
-      </c>
-      <c r="D74" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E74" s="42" t="s">
-        <v>47</v>
-      </c>
-      <c r="F74" s="15"/>
+        <v>46</v>
+      </c>
+      <c r="D74" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E74" s="32" t="s">
+        <v>45</v>
+      </c>
+      <c r="F74" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G74" s="15"/>
       <c r="H74" s="6"/>
       <c r="I74" s="8"/>
     </row>
     <row r="75" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="14" t="s">
-        <v>124</v>
-      </c>
-      <c r="D75" s="41" t="s">
-        <v>125</v>
-      </c>
-      <c r="E75" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F75" s="15"/>
+        <v>122</v>
+      </c>
+      <c r="D75" s="31" t="s">
+        <v>123</v>
+      </c>
+      <c r="E75" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F75" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G75" s="15"/>
       <c r="H75" s="6"/>
       <c r="I75" s="8"/>
     </row>
     <row r="76" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C76" s="14" t="s">
-        <v>126</v>
-      </c>
-      <c r="D76" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E76" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F76" s="15"/>
+        <v>124</v>
+      </c>
+      <c r="D76" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E76" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F76" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G76" s="15"/>
       <c r="H76" s="6"/>
       <c r="I76" s="8"/>
     </row>
     <row r="77" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C77" s="14" t="s">
-        <v>127</v>
-      </c>
-      <c r="D77" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E77" s="42" t="s">
-        <v>46</v>
-      </c>
-      <c r="F77" s="15"/>
+        <v>125</v>
+      </c>
+      <c r="D77" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E77" s="32" t="s">
+        <v>44</v>
+      </c>
+      <c r="F77" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G77" s="15"/>
       <c r="H77" s="6"/>
       <c r="I77" s="8"/>
     </row>
     <row r="78" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C78" s="14" t="s">
-        <v>128</v>
-      </c>
-      <c r="D78" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E78" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="F78" s="15"/>
+        <v>126</v>
+      </c>
+      <c r="D78" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E78" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="F78" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G78" s="15"/>
       <c r="H78" s="6"/>
       <c r="I78" s="8"/>
     </row>
     <row r="79" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="14" t="s">
-        <v>129</v>
-      </c>
-      <c r="D79" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E79" s="42" t="s">
-        <v>49</v>
-      </c>
-      <c r="F79" s="15"/>
+        <v>127</v>
+      </c>
+      <c r="D79" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E79" s="32" t="s">
+        <v>47</v>
+      </c>
+      <c r="F79" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G79" s="15"/>
       <c r="H79" s="6"/>
       <c r="I79" s="8"/>
     </row>
     <row r="80" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C80" s="14" t="s">
-        <v>130</v>
-      </c>
-      <c r="D80" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E80" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="F80" s="15"/>
+        <v>128</v>
+      </c>
+      <c r="D80" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E80" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F80" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G80" s="15"/>
       <c r="H80" s="6"/>
       <c r="I80" s="8"/>
     </row>
     <row r="81" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="14" t="s">
-        <v>131</v>
-      </c>
-      <c r="D81" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E81" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="F81" s="15"/>
+        <v>129</v>
+      </c>
+      <c r="D81" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E81" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F81" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G81" s="15"/>
       <c r="H81" s="6"/>
       <c r="I81" s="8"/>
     </row>
     <row r="82" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C82" s="14" t="s">
-        <v>132</v>
-      </c>
-      <c r="D82" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E82" s="42" t="s">
-        <v>50</v>
-      </c>
-      <c r="F82" s="15"/>
+        <v>130</v>
+      </c>
+      <c r="D82" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E82" s="32" t="s">
+        <v>48</v>
+      </c>
+      <c r="F82" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G82" s="15"/>
       <c r="H82" s="6"/>
       <c r="I82" s="8"/>
     </row>
     <row r="83" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C83" s="14" t="s">
-        <v>133</v>
-      </c>
-      <c r="D83" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E83" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="F83" s="15"/>
+        <v>131</v>
+      </c>
+      <c r="D83" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E83" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="F83" s="31" t="s">
+        <v>213</v>
+      </c>
       <c r="G83" s="15"/>
       <c r="H83" s="6"/>
       <c r="I83" s="8"/>
     </row>
     <row r="84" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C84" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="D84" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E84" s="42" t="s">
-        <v>134</v>
-      </c>
-      <c r="F84" s="15"/>
+        <v>133</v>
+      </c>
+      <c r="D84" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E84" s="32" t="s">
+        <v>132</v>
+      </c>
+      <c r="F84" s="31" t="s">
+        <v>213</v>
+      </c>
       <c r="G84" s="15"/>
       <c r="H84" s="6"/>
       <c r="I84" s="8"/>
     </row>
     <row r="85" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C85" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="D85" s="41" t="s">
-        <v>36</v>
-      </c>
-      <c r="E85" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="F85" s="15"/>
+        <v>134</v>
+      </c>
+      <c r="D85" s="31" t="s">
+        <v>34</v>
+      </c>
+      <c r="E85" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F85" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G85" s="15"/>
       <c r="H85" s="6"/>
       <c r="I85" s="8"/>
     </row>
     <row r="86" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C86" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D86" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E86" s="42"/>
-      <c r="F86" s="15"/>
+        <v>136</v>
+      </c>
+      <c r="D86" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="E86" s="32"/>
+      <c r="F86" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G86" s="15"/>
       <c r="H86" s="6"/>
       <c r="I86" s="8"/>
     </row>
     <row r="87" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C87" s="14" t="s">
-        <v>140</v>
-      </c>
-      <c r="D87" s="41" t="s">
-        <v>139</v>
-      </c>
-      <c r="E87" s="42"/>
-      <c r="F87" s="15"/>
+        <v>138</v>
+      </c>
+      <c r="D87" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="E87" s="32"/>
+      <c r="F87" s="31"/>
       <c r="G87" s="15"/>
       <c r="H87" s="6"/>
       <c r="I87" s="8"/>
     </row>
     <row r="88" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C88" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D88" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="E88" s="42"/>
-      <c r="F88" s="15"/>
+        <v>139</v>
+      </c>
+      <c r="D88" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E88" s="32"/>
+      <c r="F88" s="31"/>
       <c r="G88" s="15"/>
       <c r="H88" s="6"/>
       <c r="I88" s="8"/>
     </row>
     <row r="89" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C89" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="D89" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="E89" s="42"/>
-      <c r="F89" s="15"/>
+        <v>141</v>
+      </c>
+      <c r="D89" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E89" s="32"/>
+      <c r="F89" s="31"/>
       <c r="G89" s="15"/>
       <c r="H89" s="6"/>
       <c r="I89" s="8"/>
     </row>
     <row r="90" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D90" s="41" t="s">
         <v>142</v>
       </c>
-      <c r="E90" s="42"/>
-      <c r="F90" s="15"/>
+      <c r="D90" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E90" s="32"/>
+      <c r="F90" s="31"/>
       <c r="G90" s="15"/>
       <c r="H90" s="6"/>
       <c r="I90" s="8"/>
     </row>
     <row r="91" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C91" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D91" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="E91" s="42"/>
-      <c r="F91" s="15"/>
+        <v>143</v>
+      </c>
+      <c r="D91" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E91" s="32"/>
+      <c r="F91" s="31"/>
       <c r="G91" s="15"/>
       <c r="H91" s="6"/>
       <c r="I91" s="8"/>
     </row>
     <row r="92" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C92" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="D92" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="E92" s="42"/>
-      <c r="F92" s="15"/>
+        <v>144</v>
+      </c>
+      <c r="D92" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E92" s="32"/>
+      <c r="F92" s="31"/>
       <c r="G92" s="15"/>
       <c r="H92" s="6"/>
       <c r="I92" s="8"/>
     </row>
     <row r="93" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C93" s="14" t="s">
-        <v>147</v>
-      </c>
-      <c r="D93" s="41" t="s">
-        <v>142</v>
-      </c>
-      <c r="E93" s="42"/>
-      <c r="F93" s="15"/>
+        <v>145</v>
+      </c>
+      <c r="D93" s="31" t="s">
+        <v>140</v>
+      </c>
+      <c r="E93" s="32"/>
+      <c r="F93" s="31"/>
       <c r="G93" s="15"/>
       <c r="H93" s="6"/>
       <c r="I93" s="8"/>
     </row>
     <row r="94" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C94" s="14" t="s">
-        <v>148</v>
-      </c>
-      <c r="D94" s="41" t="s">
-        <v>149</v>
-      </c>
-      <c r="E94" s="42"/>
-      <c r="F94" s="15"/>
+        <v>146</v>
+      </c>
+      <c r="D94" s="31" t="s">
+        <v>147</v>
+      </c>
+      <c r="E94" s="32"/>
+      <c r="F94" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G94" s="15"/>
       <c r="H94" s="6"/>
       <c r="I94" s="8"/>
     </row>
     <row r="95" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C95" s="14" t="s">
-        <v>150</v>
-      </c>
-      <c r="D95" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E95" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F95" s="15"/>
+        <v>148</v>
+      </c>
+      <c r="D95" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E95" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F95" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G95" s="15"/>
       <c r="H95" s="6"/>
       <c r="I95" s="8"/>
     </row>
     <row r="96" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C96" s="14" t="s">
-        <v>151</v>
-      </c>
-      <c r="D96" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E96" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F96" s="15"/>
+        <v>149</v>
+      </c>
+      <c r="D96" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E96" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F96" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G96" s="15"/>
       <c r="H96" s="6"/>
       <c r="I96" s="8"/>
     </row>
     <row r="97" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C97" s="14" t="s">
-        <v>152</v>
-      </c>
-      <c r="D97" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E97" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F97" s="15"/>
+        <v>150</v>
+      </c>
+      <c r="D97" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E97" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F97" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G97" s="15"/>
       <c r="H97" s="6"/>
       <c r="I97" s="8"/>
     </row>
     <row r="98" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C98" s="14" t="s">
-        <v>153</v>
-      </c>
-      <c r="D98" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E98" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F98" s="15"/>
+        <v>151</v>
+      </c>
+      <c r="D98" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E98" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F98" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G98" s="15"/>
       <c r="H98" s="6"/>
       <c r="I98" s="8"/>
     </row>
     <row r="99" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C99" s="14" t="s">
-        <v>154</v>
-      </c>
-      <c r="D99" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E99" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F99" s="15"/>
+        <v>152</v>
+      </c>
+      <c r="D99" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E99" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F99" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G99" s="15"/>
       <c r="H99" s="6"/>
       <c r="I99" s="8"/>
     </row>
     <row r="100" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C100" s="14" t="s">
-        <v>155</v>
-      </c>
-      <c r="D100" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E100" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F100" s="15"/>
+        <v>153</v>
+      </c>
+      <c r="D100" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E100" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F100" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G100" s="15"/>
       <c r="H100" s="6"/>
       <c r="I100" s="8"/>
     </row>
     <row r="101" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C101" s="14" t="s">
-        <v>52</v>
-      </c>
-      <c r="D101" s="41" t="s">
-        <v>156</v>
-      </c>
-      <c r="E101" s="42" t="s">
-        <v>24</v>
-      </c>
-      <c r="F101" s="15"/>
+        <v>50</v>
+      </c>
+      <c r="D101" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E101" s="32" t="s">
+        <v>22</v>
+      </c>
+      <c r="F101" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G101" s="15"/>
       <c r="H101" s="6"/>
       <c r="I101" s="8"/>
     </row>
     <row r="102" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C102" s="14" t="s">
-        <v>53</v>
-      </c>
-      <c r="D102" s="41" t="s">
-        <v>156</v>
-      </c>
-      <c r="E102" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="F102" s="15"/>
+        <v>51</v>
+      </c>
+      <c r="D102" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E102" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F102" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G102" s="15"/>
       <c r="H102" s="6"/>
       <c r="I102" s="8"/>
     </row>
     <row r="103" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C103" s="14" t="s">
-        <v>54</v>
-      </c>
-      <c r="D103" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E103" s="42" t="s">
-        <v>19</v>
-      </c>
-      <c r="F103" s="15"/>
+        <v>52</v>
+      </c>
+      <c r="D103" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E103" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="F103" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G103" s="15"/>
       <c r="H103" s="6"/>
       <c r="I103" s="8"/>
     </row>
     <row r="104" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C104" s="14" t="s">
-        <v>157</v>
-      </c>
-      <c r="D104" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E104" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F104" s="15"/>
+        <v>155</v>
+      </c>
+      <c r="D104" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E104" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F104" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G104" s="15"/>
       <c r="H104" s="6"/>
       <c r="I104" s="8"/>
     </row>
     <row r="105" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C105" s="14" t="s">
-        <v>158</v>
-      </c>
-      <c r="D105" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E105" s="42" t="s">
-        <v>20</v>
-      </c>
-      <c r="F105" s="15"/>
+        <v>156</v>
+      </c>
+      <c r="D105" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E105" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F105" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G105" s="15"/>
       <c r="H105" s="6"/>
       <c r="I105" s="8"/>
     </row>
     <row r="106" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C106" s="14" t="s">
-        <v>159</v>
-      </c>
-      <c r="D106" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E106" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="F106" s="15"/>
+        <v>157</v>
+      </c>
+      <c r="D106" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E106" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F106" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G106" s="15"/>
       <c r="H106" s="6"/>
       <c r="I106" s="8"/>
     </row>
     <row r="107" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C107" s="14" t="s">
-        <v>160</v>
-      </c>
-      <c r="D107" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E107" s="42" t="s">
-        <v>21</v>
-      </c>
-      <c r="F107" s="15"/>
+        <v>158</v>
+      </c>
+      <c r="D107" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E107" s="32" t="s">
+        <v>19</v>
+      </c>
+      <c r="F107" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G107" s="15"/>
       <c r="H107" s="6"/>
       <c r="I107" s="8"/>
     </row>
     <row r="108" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C108" s="14" t="s">
-        <v>55</v>
-      </c>
-      <c r="D108" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E108" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="F108" s="15"/>
+        <v>53</v>
+      </c>
+      <c r="D108" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E108" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="F108" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G108" s="15"/>
       <c r="H108" s="6"/>
       <c r="I108" s="8"/>
     </row>
     <row r="109" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C109" s="14" t="s">
-        <v>162</v>
-      </c>
-      <c r="D109" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E109" s="42" t="s">
-        <v>161</v>
-      </c>
-      <c r="F109" s="15"/>
+        <v>160</v>
+      </c>
+      <c r="D109" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E109" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="F109" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G109" s="15"/>
       <c r="H109" s="6"/>
       <c r="I109" s="8"/>
     </row>
     <row r="110" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C110" s="14" t="s">
-        <v>163</v>
-      </c>
-      <c r="D110" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E110" s="42" t="s">
         <v>161</v>
       </c>
-      <c r="F110" s="15"/>
+      <c r="D110" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E110" s="32" t="s">
+        <v>159</v>
+      </c>
+      <c r="F110" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G110" s="15"/>
       <c r="H110" s="6"/>
       <c r="I110" s="8"/>
     </row>
     <row r="111" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="14" t="s">
-        <v>164</v>
-      </c>
-      <c r="D111" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E111" s="42" t="s">
-        <v>165</v>
-      </c>
-      <c r="F111" s="15"/>
+        <v>162</v>
+      </c>
+      <c r="D111" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E111" s="32" t="s">
+        <v>163</v>
+      </c>
+      <c r="F111" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G111" s="15"/>
       <c r="H111" s="6"/>
       <c r="I111" s="8"/>
     </row>
     <row r="112" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C112" s="14" t="s">
-        <v>166</v>
-      </c>
-      <c r="D112" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E112" s="42" t="s">
-        <v>167</v>
-      </c>
-      <c r="F112" s="15"/>
+        <v>164</v>
+      </c>
+      <c r="D112" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E112" s="32" t="s">
+        <v>165</v>
+      </c>
+      <c r="F112" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G112" s="15"/>
       <c r="H112" s="6"/>
       <c r="I112" s="8"/>
     </row>
     <row r="113" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C113" s="14" t="s">
-        <v>168</v>
-      </c>
-      <c r="D113" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E113" s="42" t="s">
-        <v>169</v>
-      </c>
-      <c r="F113" s="15"/>
+        <v>166</v>
+      </c>
+      <c r="D113" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E113" s="32" t="s">
+        <v>167</v>
+      </c>
+      <c r="F113" s="31" t="s">
+        <v>212</v>
+      </c>
       <c r="G113" s="15"/>
       <c r="H113" s="6"/>
       <c r="I113" s="8"/>
     </row>
     <row r="114" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C114" s="14" t="s">
-        <v>170</v>
-      </c>
-      <c r="D114" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E114" s="42" t="s">
-        <v>171</v>
-      </c>
-      <c r="F114" s="15"/>
+        <v>168</v>
+      </c>
+      <c r="D114" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E114" s="32" t="s">
+        <v>169</v>
+      </c>
+      <c r="F114" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G114" s="15"/>
       <c r="H114" s="6"/>
       <c r="I114" s="8"/>
     </row>
     <row r="115" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C115" s="14" t="s">
-        <v>172</v>
-      </c>
-      <c r="D115" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E115" s="42" t="s">
-        <v>137</v>
-      </c>
-      <c r="F115" s="15"/>
+        <v>170</v>
+      </c>
+      <c r="D115" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E115" s="32" t="s">
+        <v>135</v>
+      </c>
+      <c r="F115" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G115" s="15"/>
       <c r="H115" s="6"/>
       <c r="I115" s="8"/>
     </row>
     <row r="116" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C116" s="14" t="s">
-        <v>173</v>
-      </c>
-      <c r="D116" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E116" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="F116" s="15"/>
+        <v>171</v>
+      </c>
+      <c r="D116" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E116" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="F116" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G116" s="15"/>
       <c r="H116" s="6"/>
       <c r="I116" s="8"/>
     </row>
     <row r="117" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C117" s="14" t="s">
-        <v>175</v>
-      </c>
-      <c r="D117" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E117" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="F117" s="15"/>
+        <v>173</v>
+      </c>
+      <c r="D117" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E117" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="F117" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G117" s="15"/>
       <c r="H117" s="6"/>
       <c r="I117" s="8"/>
     </row>
     <row r="118" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C118" s="14" t="s">
-        <v>176</v>
-      </c>
-      <c r="D118" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E118" s="42" t="s">
         <v>174</v>
       </c>
-      <c r="F118" s="15"/>
+      <c r="D118" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E118" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="F118" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G118" s="15"/>
       <c r="H118" s="6"/>
       <c r="I118" s="8"/>
     </row>
     <row r="119" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C119" s="14" t="s">
-        <v>177</v>
-      </c>
-      <c r="D119" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E119" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="F119" s="15"/>
+        <v>175</v>
+      </c>
+      <c r="D119" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E119" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="F119" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G119" s="15"/>
       <c r="H119" s="6"/>
       <c r="I119" s="8"/>
     </row>
     <row r="120" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C120" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="D120" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E120" s="42" t="s">
-        <v>174</v>
-      </c>
-      <c r="F120" s="15"/>
+        <v>176</v>
+      </c>
+      <c r="D120" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E120" s="32" t="s">
+        <v>172</v>
+      </c>
+      <c r="F120" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G120" s="15"/>
       <c r="H120" s="6"/>
       <c r="I120" s="8"/>
     </row>
     <row r="121" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C121" s="14" t="s">
-        <v>179</v>
-      </c>
-      <c r="D121" s="41" t="s">
-        <v>156</v>
-      </c>
-      <c r="E121" s="42" t="s">
-        <v>23</v>
-      </c>
-      <c r="F121" s="15"/>
+        <v>177</v>
+      </c>
+      <c r="D121" s="31" t="s">
+        <v>154</v>
+      </c>
+      <c r="E121" s="32" t="s">
+        <v>21</v>
+      </c>
+      <c r="F121" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G121" s="15"/>
       <c r="H121" s="6"/>
       <c r="I121" s="8"/>
     </row>
     <row r="122" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C122" s="14" t="s">
-        <v>180</v>
-      </c>
-      <c r="D122" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E122" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F122" s="15"/>
+        <v>178</v>
+      </c>
+      <c r="D122" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E122" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F122" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G122" s="15"/>
       <c r="H122" s="6"/>
       <c r="I122" s="8"/>
     </row>
     <row r="123" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C123" s="14" t="s">
-        <v>181</v>
-      </c>
-      <c r="D123" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E123" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F123" s="15"/>
+        <v>179</v>
+      </c>
+      <c r="D123" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E123" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F123" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G123" s="15"/>
       <c r="H123" s="6"/>
       <c r="I123" s="8"/>
     </row>
     <row r="124" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C124" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="D124" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E124" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F124" s="15"/>
+        <v>180</v>
+      </c>
+      <c r="D124" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E124" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F124" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G124" s="15"/>
       <c r="H124" s="6"/>
       <c r="I124" s="8"/>
     </row>
     <row r="125" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C125" s="14" t="s">
-        <v>183</v>
-      </c>
-      <c r="D125" s="41" t="s">
-        <v>51</v>
-      </c>
-      <c r="E125" s="42" t="s">
-        <v>22</v>
-      </c>
-      <c r="F125" s="15"/>
+        <v>181</v>
+      </c>
+      <c r="D125" s="31" t="s">
+        <v>49</v>
+      </c>
+      <c r="E125" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="F125" s="31" t="s">
+        <v>214</v>
+      </c>
       <c r="G125" s="15"/>
       <c r="H125" s="6"/>
       <c r="I125" s="8"/>
     </row>
     <row r="126" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C126" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="D126" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="E126" s="42"/>
-      <c r="F126" s="15"/>
+        <v>182</v>
+      </c>
+      <c r="D126" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E126" s="32"/>
+      <c r="F126" s="31"/>
       <c r="G126" s="15"/>
       <c r="H126" s="6"/>
       <c r="I126" s="8"/>
     </row>
     <row r="127" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C127" s="14" t="s">
-        <v>186</v>
-      </c>
-      <c r="D127" s="41" t="s">
-        <v>185</v>
-      </c>
-      <c r="E127" s="42"/>
-      <c r="F127" s="15"/>
+        <v>184</v>
+      </c>
+      <c r="D127" s="31" t="s">
+        <v>183</v>
+      </c>
+      <c r="E127" s="32"/>
+      <c r="F127" s="31"/>
       <c r="G127" s="15"/>
       <c r="H127" s="6"/>
       <c r="I127" s="8"/>
     </row>
     <row r="128" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C128" s="14" t="s">
-        <v>187</v>
-      </c>
-      <c r="D128" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E128" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="F128" s="15"/>
+        <v>185</v>
+      </c>
+      <c r="D128" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E128" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F128" s="31"/>
       <c r="G128" s="15"/>
       <c r="H128" s="6"/>
       <c r="I128" s="8"/>
     </row>
-    <row r="129" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C129" s="14" t="s">
-        <v>188</v>
-      </c>
-      <c r="D129" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E129" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="F129" s="15"/>
+        <v>186</v>
+      </c>
+      <c r="D129" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E129" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F129" s="31" t="s">
+        <v>204</v>
+      </c>
       <c r="G129" s="15"/>
       <c r="H129" s="6"/>
       <c r="I129" s="8"/>
     </row>
-    <row r="130" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C130" s="14" t="s">
-        <v>189</v>
-      </c>
-      <c r="D130" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E130" s="42" t="s">
-        <v>56</v>
-      </c>
-      <c r="F130" s="15"/>
+        <v>187</v>
+      </c>
+      <c r="D130" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E130" s="32" t="s">
+        <v>54</v>
+      </c>
+      <c r="F130" s="31" t="s">
+        <v>203</v>
+      </c>
       <c r="G130" s="15"/>
       <c r="H130" s="6"/>
       <c r="I130" s="8"/>
     </row>
     <row r="131" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C131" s="14" t="s">
-        <v>190</v>
-      </c>
-      <c r="D131" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E131" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="F131" s="15"/>
+        <v>188</v>
+      </c>
+      <c r="D131" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E131" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F131" s="31" t="s">
+        <v>201</v>
+      </c>
       <c r="G131" s="15"/>
       <c r="H131" s="6"/>
       <c r="I131" s="8"/>
     </row>
-    <row r="132" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C132" s="14" t="s">
-        <v>191</v>
-      </c>
-      <c r="D132" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E132" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="F132" s="15"/>
+        <v>189</v>
+      </c>
+      <c r="D132" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E132" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F132" s="31" t="s">
+        <v>205</v>
+      </c>
       <c r="G132" s="15"/>
       <c r="H132" s="6"/>
       <c r="I132" s="8"/>
     </row>
     <row r="133" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C133" s="14" t="s">
-        <v>192</v>
-      </c>
-      <c r="D133" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E133" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="F133" s="15"/>
+        <v>190</v>
+      </c>
+      <c r="D133" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E133" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F133" s="31" t="s">
+        <v>200</v>
+      </c>
       <c r="G133" s="15"/>
       <c r="H133" s="6"/>
       <c r="I133" s="8"/>
     </row>
     <row r="134" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C134" s="14" t="s">
-        <v>193</v>
-      </c>
-      <c r="D134" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E134" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="F134" s="15"/>
+        <v>191</v>
+      </c>
+      <c r="D134" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E134" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F134" s="31" t="s">
+        <v>202</v>
+      </c>
       <c r="G134" s="15"/>
       <c r="H134" s="6"/>
       <c r="I134" s="8"/>
     </row>
     <row r="135" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C135" s="14" t="s">
-        <v>194</v>
-      </c>
-      <c r="D135" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E135" s="42" t="s">
-        <v>57</v>
-      </c>
-      <c r="F135" s="15"/>
+        <v>192</v>
+      </c>
+      <c r="D135" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E135" s="32" t="s">
+        <v>55</v>
+      </c>
+      <c r="F135" s="31" t="s">
+        <v>201</v>
+      </c>
       <c r="G135" s="15"/>
       <c r="H135" s="6"/>
       <c r="I135" s="8"/>
     </row>
     <row r="136" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C136" s="14" t="s">
-        <v>58</v>
-      </c>
-      <c r="D136" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E136" s="42" t="s">
-        <v>59</v>
-      </c>
-      <c r="F136" s="15"/>
+        <v>56</v>
+      </c>
+      <c r="D136" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E136" s="32" t="s">
+        <v>57</v>
+      </c>
+      <c r="F136" s="31" t="s">
+        <v>202</v>
+      </c>
       <c r="G136" s="15"/>
       <c r="H136" s="6"/>
       <c r="I136" s="8"/>
     </row>
     <row r="137" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C137" s="14" t="s">
-        <v>195</v>
-      </c>
-      <c r="D137" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E137" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="F137" s="15"/>
+        <v>193</v>
+      </c>
+      <c r="D137" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E137" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F137" s="31"/>
       <c r="G137" s="15"/>
       <c r="H137" s="6"/>
       <c r="I137" s="8"/>
     </row>
     <row r="138" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C138" s="14" t="s">
-        <v>196</v>
-      </c>
-      <c r="D138" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E138" s="42" t="s">
-        <v>60</v>
-      </c>
-      <c r="F138" s="15"/>
+        <v>194</v>
+      </c>
+      <c r="D138" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E138" s="32" t="s">
+        <v>58</v>
+      </c>
+      <c r="F138" s="31"/>
       <c r="G138" s="15"/>
       <c r="H138" s="6"/>
       <c r="I138" s="8"/>
     </row>
     <row r="139" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C139" s="14" t="s">
-        <v>197</v>
-      </c>
-      <c r="D139" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E139" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="F139" s="15"/>
+        <v>195</v>
+      </c>
+      <c r="D139" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E139" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F139" s="31"/>
       <c r="G139" s="15"/>
       <c r="H139" s="6"/>
       <c r="I139" s="8"/>
     </row>
     <row r="140" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C140" s="14" t="s">
-        <v>198</v>
-      </c>
-      <c r="D140" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E140" s="42" t="s">
-        <v>61</v>
-      </c>
-      <c r="F140" s="15"/>
+        <v>196</v>
+      </c>
+      <c r="D140" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E140" s="32" t="s">
+        <v>59</v>
+      </c>
+      <c r="F140" s="31"/>
       <c r="G140" s="15"/>
       <c r="H140" s="6"/>
       <c r="I140" s="8"/>
     </row>
     <row r="141" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C141" s="14" t="s">
-        <v>62</v>
-      </c>
-      <c r="D141" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E141" s="42" t="s">
-        <v>199</v>
-      </c>
-      <c r="F141" s="15"/>
+        <v>60</v>
+      </c>
+      <c r="D141" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E141" s="32" t="s">
+        <v>197</v>
+      </c>
+      <c r="F141" s="31"/>
       <c r="G141" s="15"/>
       <c r="H141" s="6"/>
       <c r="I141" s="8"/>
     </row>
     <row r="142" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C142" s="14" t="s">
-        <v>63</v>
-      </c>
-      <c r="D142" s="41" t="s">
-        <v>18</v>
-      </c>
-      <c r="E142" s="42" t="s">
-        <v>64</v>
-      </c>
-      <c r="F142" s="15"/>
+        <v>61</v>
+      </c>
+      <c r="D142" s="31" t="s">
+        <v>16</v>
+      </c>
+      <c r="E142" s="32" t="s">
+        <v>62</v>
+      </c>
+      <c r="F142" s="31"/>
       <c r="G142" s="15"/>
       <c r="H142" s="6"/>
       <c r="I142" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="9">
+    <mergeCell ref="E10:F10"/>
+    <mergeCell ref="I10:J10"/>
+    <mergeCell ref="B13:J21"/>
     <mergeCell ref="A1:L6"/>
     <mergeCell ref="B7:I7"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="E9:F9"/>
     <mergeCell ref="I9:J9"/>
-    <mergeCell ref="E10:F10"/>
-    <mergeCell ref="I10:J10"/>
-    <mergeCell ref="B13:J21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added low level design,component and GUI  diagram,class diagram ,
Added low level design,component and GUI  diagram,class diagram ,
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="471" uniqueCount="217">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="255">
   <si>
     <t>Author</t>
   </si>
@@ -659,69 +659,321 @@
     <t xml:space="preserve"> Test Case ID</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_ADMIN_003</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_005</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_ADMIN_003
-</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_008
-Bank_Sys_DM_ADMIN_009</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_005
-Bank_Sys_DM_ADMIN_007</t>
+    <t>Bank_Sys_DM_CST_007</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008</t>
+  </si>
+  <si>
+    <t>Design ID</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_006
+Bank_SYS_HLD_admin_003</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_003
+Bank_SYS_HLD_admin_004
+BANK_SYS_DD_ Admin _007</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_005
+BANK_SYS_DD_account_001</t>
   </si>
   <si>
     <t>Bank_Sys_DM_ADMIN_001
-Bank_Sys_DM_CST_001</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_004</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_005
-Bank_Sys_DM_CST_006</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_006</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_006
-Bank_Sys_DM_CST_007</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_005</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_008</t>
+Bank_Sys_DM_CST_001
+Bank_SYS_HLD_client_002
+Bank_SYS_HLD_admin_002
+BANK_SYS_DD_CST_001
+BANK_SYS_DD_Admin_001
+Bank_SYS_DSN_001</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_001
+Bank_Sys_DM_CST_001
+Bank_SYS_HLD_client_002
+Bank_SYS_HLD_admin_002
+Bank_SYS_DSN_001</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_001
+Bank_Sys_DM_CST_001
+Bank_SYS_HLD_client_002
+Bank_SYS_HLD_admin_002
+BANK_SYS_DD_ CST _002
+BANK_SYS_DD_ Admin _002
+Bank_SYS_DSN_001</t>
   </si>
   <si>
     <t>Bank_Sys_DM_ADMIN_002
 Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001</t>
-  </si>
-  <si>
-    <t>Design ID</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_001
-Bank_Sys_DM_CST_001
-Bank_SYS_HLD_client_002</t>
+Bank_SYS_HLD_client_001
+Bank_SYS_HLD_admin_001
+BANK_SYS_DD_CST_001
+BANK_SYS_DD_Admin_001
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_HLD_admin_001
+BANK_SYS_DD_ CST _002
+BANK_SYS_DD_ Admin _002
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_HLD_admin_001
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_HLD_admin_001
+BANK_SYS_DD_ CST _003
+BANK_SYS_DD_ Admin _005
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_HLD_admin_001
+BANK_SYS_DD_ CST _004
+BANK_SYS_DD_ Admin _004
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_HLD_admin_001
+BANK_SYS_DD_ Admin _003
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_HLD_admin_001
+Bank_SYS_DSN_003</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_HLD_admin_001
+Bank_SYS_DSN_004</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_DSN_004</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_002
+Bank_SYS_HLD_client_001
+Bank_SYS_HLD_admin_001
+Bank_SYS_DSN_004
+Bank_SYS_DSN_005</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_004
+Bank_SYS_DSN_005</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008
+Bank_SYS_DSN_005</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_005</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_005
+Bank_Sys_DM_CST_006
+Bank_SYS_DSN_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_006
+Bank_SYS_HLD_client_003
+Bank_SYS_DSN_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_006
+Bank_SYS_DSN_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_006
+Bank_Sys_DM_CST_007
+Bank_SYS_HLD_client_004
+BANK_SYS_DD_TR_001
+Bank_SYS_DSN_006</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_006</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_005
+Bank_SYS_DSN_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
+Bank_SYS_HLD_client_004
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
+Bank_SYS_HLD_client_005
+Bank_SYS_HLD_client_006
+BANK_SYS_DD_ TR _002
+BANK_SYS_DD_ PR _002
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
+Bank_SYS_HLD_client_003
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_007
+</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_005
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
+BANK_SYS_DD_ PR _002
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008
+Bank_SYS_DSN_010</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008
+BANK_SYS_DD_ Trans _003
+Bank_SYS_DSN_010</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008
+BANK_SYS_DD_ account _003
+BANK_SYS_DD_Trans_001
+BANK_SYS_DD_PR_001
+Bank_SYS_DSN_010</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008
+BANK_SYS_DD_ Trans _002
+Bank_SYS_DSN_010</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_005
+Bank_SYS_DSN_010</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_010</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008
+Bank_SYS_DSN_012</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008
+Bank_SYS_DSN_013</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_008
+BANK_SYS_DD_ account _002
+Bank_SYS_DSN_011</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
+Bank_SYS_HLD_client_006
+BANK_SYS_DD_ PR _003
+Bank_SYS_DSN_014</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
+Bank_SYS_DSN_014</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_admin_003
+BANK_SYS_DD_ Admin _006
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_008
+Bank_Sys_DM_ADMIN_009
+Bank_SYS_HLD_admin_006
+Bank_SYS_HLD_admin_005
+BANK_SYS_DD_ Admin _008
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_003
+Bank_SYS_HLD_admin_004
+BANK_SYS_DD_ Admin _007
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005
+Bank_Sys_DM_ADMIN_007
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_006
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005
+BANK_SYS_DD_ Admin _006
+Bank_SYS_DSN_015</t>
   </si>
 </sst>
 </file>
@@ -1446,8 +1698,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A58" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F60" sqref="F60"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1457,7 +1709,7 @@
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" style="33" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" style="33" customWidth="1"/>
-    <col min="6" max="6" width="33.28515625" style="33" customWidth="1"/>
+    <col min="6" max="6" width="35" style="33" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
@@ -1745,7 +1997,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>198</v>
@@ -1755,7 +2007,7 @@
       </c>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:10" s="23" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" s="23" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="12" t="s">
         <v>70</v>
       </c>
@@ -1766,13 +2018,13 @@
         <v>23</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="5"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="2:10" s="26" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" s="26" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="27" t="s">
         <v>71</v>
       </c>
@@ -1783,13 +2035,13 @@
         <v>72</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="G24" s="29"/>
       <c r="H24" s="30"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="2:10" s="26" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" s="26" customFormat="1" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="27" t="s">
         <v>73</v>
       </c>
@@ -1800,13 +2052,13 @@
         <v>72</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G25" s="29"/>
       <c r="H25" s="30"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" s="26" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="27" t="s">
         <v>74</v>
       </c>
@@ -1817,13 +2069,13 @@
         <v>72</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>206</v>
+        <v>211</v>
       </c>
       <c r="G26" s="29"/>
       <c r="H26" s="30"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="2:10" s="26" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" s="26" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="27" t="s">
         <v>75</v>
       </c>
@@ -1834,13 +2086,13 @@
         <v>72</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
       <c r="G27" s="29"/>
       <c r="H27" s="30"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" s="26" customFormat="1" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="27" t="s">
         <v>76</v>
       </c>
@@ -1851,13 +2103,13 @@
         <v>72</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="G28" s="29"/>
       <c r="H28" s="30"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="2:10" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="14" t="s">
         <v>77</v>
       </c>
@@ -1868,13 +2120,13 @@
         <v>24</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="6"/>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="2:10" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" ht="93.75" x14ac:dyDescent="0.25">
       <c r="C30" s="12" t="s">
         <v>78</v>
       </c>
@@ -1885,13 +2137,13 @@
         <v>24</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="5"/>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="2:10" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="14" t="s">
         <v>67</v>
       </c>
@@ -1902,13 +2154,13 @@
         <v>24</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="6"/>
       <c r="I31" s="8"/>
     </row>
-    <row r="32" spans="2:10" ht="56.25" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" ht="93.75" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>79</v>
       </c>
@@ -1919,13 +2171,13 @@
         <v>80</v>
       </c>
       <c r="F32" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="5"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="14" t="s">
         <v>81</v>
       </c>
@@ -1936,13 +2188,13 @@
         <v>24</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>206</v>
+        <v>210</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="6"/>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="14" t="s">
         <v>82</v>
       </c>
@@ -1953,13 +2205,13 @@
         <v>24</v>
       </c>
       <c r="F34" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="6"/>
       <c r="I34" s="8"/>
     </row>
-    <row r="35" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="14" t="s">
         <v>83</v>
       </c>
@@ -1970,13 +2222,13 @@
         <v>24</v>
       </c>
       <c r="F35" s="34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="6"/>
       <c r="I35" s="8"/>
     </row>
-    <row r="36" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="14" t="s">
         <v>84</v>
       </c>
@@ -1987,13 +2239,13 @@
         <v>24</v>
       </c>
       <c r="F36" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="6"/>
       <c r="I36" s="8"/>
     </row>
-    <row r="37" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="14" t="s">
         <v>85</v>
       </c>
@@ -2004,13 +2256,13 @@
         <v>24</v>
       </c>
       <c r="F37" s="34" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="6"/>
       <c r="I37" s="8"/>
     </row>
-    <row r="38" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="14" t="s">
         <v>86</v>
       </c>
@@ -2021,13 +2273,13 @@
         <v>31</v>
       </c>
       <c r="F38" s="34" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="6"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="14" t="s">
         <v>87</v>
       </c>
@@ -2038,13 +2290,13 @@
         <v>31</v>
       </c>
       <c r="F39" s="34" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="6"/>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="14" t="s">
         <v>88</v>
       </c>
@@ -2055,13 +2307,13 @@
         <v>31</v>
       </c>
       <c r="F40" s="34" t="s">
-        <v>214</v>
+        <v>216</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="6"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="14" t="s">
         <v>89</v>
       </c>
@@ -2072,13 +2324,13 @@
         <v>90</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="6"/>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="14" t="s">
         <v>25</v>
       </c>
@@ -2095,7 +2347,7 @@
       <c r="H42" s="6"/>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="14" t="s">
         <v>26</v>
       </c>
@@ -2106,13 +2358,13 @@
         <v>27</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G43" s="15"/>
       <c r="H43" s="6"/>
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="14" t="s">
         <v>28</v>
       </c>
@@ -2123,13 +2375,13 @@
         <v>92</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G44" s="15"/>
       <c r="H44" s="6"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="14" t="s">
         <v>93</v>
       </c>
@@ -2140,13 +2392,13 @@
         <v>92</v>
       </c>
       <c r="F45" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G45" s="15"/>
       <c r="H45" s="6"/>
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="14" t="s">
         <v>94</v>
       </c>
@@ -2157,13 +2409,13 @@
         <v>95</v>
       </c>
       <c r="F46" s="34" t="s">
-        <v>214</v>
+        <v>215</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="6"/>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="14" t="s">
         <v>96</v>
       </c>
@@ -2174,13 +2426,13 @@
         <v>90</v>
       </c>
       <c r="F47" s="34" t="s">
-        <v>214</v>
+        <v>218</v>
       </c>
       <c r="G47" s="15"/>
       <c r="H47" s="6"/>
       <c r="I47" s="8"/>
     </row>
-    <row r="48" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="14" t="s">
         <v>97</v>
       </c>
@@ -2191,13 +2443,13 @@
         <v>99</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="G48" s="15"/>
       <c r="H48" s="6"/>
       <c r="I48" s="8"/>
     </row>
-    <row r="49" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="14" t="s">
         <v>100</v>
       </c>
@@ -2206,13 +2458,13 @@
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="34" t="s">
-        <v>214</v>
+        <v>210</v>
       </c>
       <c r="G49" s="15"/>
       <c r="H49" s="6"/>
       <c r="I49" s="8"/>
     </row>
-    <row r="50" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="3:9" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="14" t="s">
         <v>102</v>
       </c>
@@ -2223,13 +2475,13 @@
         <v>29</v>
       </c>
       <c r="F50" s="31" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="G50" s="15"/>
       <c r="H50" s="6"/>
       <c r="I50" s="8"/>
     </row>
-    <row r="51" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="3:9" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="14" t="s">
         <v>103</v>
       </c>
@@ -2240,13 +2492,13 @@
         <v>29</v>
       </c>
       <c r="F51" s="31" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="6"/>
       <c r="I51" s="8"/>
     </row>
-    <row r="52" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="14" t="s">
         <v>104</v>
       </c>
@@ -2257,13 +2509,13 @@
         <v>29</v>
       </c>
       <c r="F52" s="31" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G52" s="15"/>
       <c r="H52" s="6"/>
       <c r="I52" s="8"/>
     </row>
-    <row r="53" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="14" t="s">
         <v>105</v>
       </c>
@@ -2274,13 +2526,13 @@
         <v>29</v>
       </c>
       <c r="F53" s="31" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G53" s="15"/>
       <c r="H53" s="6"/>
       <c r="I53" s="8"/>
     </row>
-    <row r="54" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="14" t="s">
         <v>106</v>
       </c>
@@ -2291,13 +2543,13 @@
         <v>30</v>
       </c>
       <c r="F54" s="31" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="6"/>
       <c r="I54" s="8"/>
     </row>
-    <row r="55" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="14" t="s">
         <v>107</v>
       </c>
@@ -2308,13 +2560,13 @@
         <v>30</v>
       </c>
       <c r="F55" s="31" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G55" s="15"/>
       <c r="H55" s="6"/>
       <c r="I55" s="8"/>
     </row>
-    <row r="56" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="14" t="s">
         <v>108</v>
       </c>
@@ -2325,13 +2577,13 @@
         <v>30</v>
       </c>
       <c r="F56" s="31" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G56" s="15"/>
       <c r="H56" s="6"/>
       <c r="I56" s="8"/>
     </row>
-    <row r="57" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="14" t="s">
         <v>109</v>
       </c>
@@ -2342,13 +2594,13 @@
         <v>31</v>
       </c>
       <c r="F57" s="31" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G57" s="15"/>
       <c r="H57" s="6"/>
       <c r="I57" s="8"/>
     </row>
-    <row r="58" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="14" t="s">
         <v>110</v>
       </c>
@@ -2357,13 +2609,13 @@
         <v>33</v>
       </c>
       <c r="F58" s="31" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G58" s="15"/>
       <c r="H58" s="6"/>
       <c r="I58" s="8"/>
     </row>
-    <row r="59" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="14" t="s">
         <v>32</v>
       </c>
@@ -2372,13 +2624,13 @@
         <v>95</v>
       </c>
       <c r="F59" s="31" t="s">
-        <v>205</v>
+        <v>206</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="6"/>
       <c r="I59" s="8"/>
     </row>
-    <row r="60" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="14" t="s">
         <v>111</v>
       </c>
@@ -2387,13 +2639,13 @@
       </c>
       <c r="E60" s="32"/>
       <c r="F60" s="31" t="s">
-        <v>216</v>
+        <v>206</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="6"/>
       <c r="I60" s="8"/>
     </row>
-    <row r="61" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="14" t="s">
         <v>35</v>
       </c>
@@ -2404,7 +2656,7 @@
         <v>36</v>
       </c>
       <c r="F61" s="31" t="s">
-        <v>207</v>
+        <v>219</v>
       </c>
       <c r="G61" s="15"/>
       <c r="H61" s="6"/>
@@ -2425,7 +2677,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="8"/>
     </row>
-    <row r="63" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C63" s="14" t="s">
         <v>113</v>
       </c>
@@ -2436,13 +2688,13 @@
         <v>39</v>
       </c>
       <c r="F63" s="31" t="s">
-        <v>208</v>
+        <v>222</v>
       </c>
       <c r="G63" s="15"/>
       <c r="H63" s="6"/>
       <c r="I63" s="8"/>
     </row>
-    <row r="64" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="14" t="s">
         <v>114</v>
       </c>
@@ -2453,13 +2705,13 @@
         <v>39</v>
       </c>
       <c r="F64" s="31" t="s">
-        <v>209</v>
+        <v>223</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="6"/>
       <c r="I64" s="8"/>
     </row>
-    <row r="65" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="14" t="s">
         <v>115</v>
       </c>
@@ -2470,13 +2722,13 @@
         <v>39</v>
       </c>
       <c r="F65" s="31" t="s">
-        <v>209</v>
+        <v>224</v>
       </c>
       <c r="G65" s="15"/>
       <c r="H65" s="6"/>
       <c r="I65" s="8"/>
     </row>
-    <row r="66" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="14" t="s">
         <v>116</v>
       </c>
@@ -2487,13 +2739,13 @@
         <v>39</v>
       </c>
       <c r="F66" s="31" t="s">
-        <v>210</v>
+        <v>225</v>
       </c>
       <c r="G66" s="15"/>
       <c r="H66" s="6"/>
       <c r="I66" s="8"/>
     </row>
-    <row r="67" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="14" t="s">
         <v>117</v>
       </c>
@@ -2504,13 +2756,13 @@
         <v>39</v>
       </c>
       <c r="F67" s="31" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G67" s="15"/>
       <c r="H67" s="6"/>
       <c r="I67" s="8"/>
     </row>
-    <row r="68" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="14" t="s">
         <v>118</v>
       </c>
@@ -2521,13 +2773,13 @@
         <v>39</v>
       </c>
       <c r="F68" s="31" t="s">
-        <v>211</v>
+        <v>228</v>
       </c>
       <c r="G68" s="15"/>
       <c r="H68" s="6"/>
       <c r="I68" s="8"/>
     </row>
-    <row r="69" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:9" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="14" t="s">
         <v>40</v>
       </c>
@@ -2538,13 +2790,13 @@
         <v>41</v>
       </c>
       <c r="F69" s="31" t="s">
-        <v>211</v>
+        <v>229</v>
       </c>
       <c r="G69" s="15"/>
       <c r="H69" s="6"/>
       <c r="I69" s="8"/>
     </row>
-    <row r="70" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C70" s="14" t="s">
         <v>42</v>
       </c>
@@ -2555,13 +2807,13 @@
         <v>43</v>
       </c>
       <c r="F70" s="31" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="G70" s="15"/>
       <c r="H70" s="6"/>
       <c r="I70" s="8"/>
     </row>
-    <row r="71" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C71" s="14" t="s">
         <v>119</v>
       </c>
@@ -2572,13 +2824,13 @@
         <v>44</v>
       </c>
       <c r="F71" s="31" t="s">
-        <v>211</v>
+        <v>232</v>
       </c>
       <c r="G71" s="15"/>
       <c r="H71" s="6"/>
       <c r="I71" s="8"/>
     </row>
-    <row r="72" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C72" s="14" t="s">
         <v>120</v>
       </c>
@@ -2589,13 +2841,13 @@
         <v>44</v>
       </c>
       <c r="F72" s="31" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="G72" s="15"/>
       <c r="H72" s="6"/>
       <c r="I72" s="8"/>
     </row>
-    <row r="73" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="14" t="s">
         <v>121</v>
       </c>
@@ -2606,13 +2858,13 @@
         <v>44</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="G73" s="15"/>
       <c r="H73" s="6"/>
       <c r="I73" s="8"/>
     </row>
-    <row r="74" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C74" s="14" t="s">
         <v>46</v>
       </c>
@@ -2623,7 +2875,7 @@
         <v>45</v>
       </c>
       <c r="F74" s="31" t="s">
-        <v>211</v>
+        <v>231</v>
       </c>
       <c r="G74" s="15"/>
       <c r="H74" s="6"/>
@@ -2640,13 +2892,13 @@
         <v>44</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="6"/>
       <c r="I75" s="8"/>
     </row>
-    <row r="76" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C76" s="14" t="s">
         <v>124</v>
       </c>
@@ -2657,13 +2909,13 @@
         <v>44</v>
       </c>
       <c r="F76" s="31" t="s">
-        <v>211</v>
+        <v>246</v>
       </c>
       <c r="G76" s="15"/>
       <c r="H76" s="6"/>
       <c r="I76" s="8"/>
     </row>
-    <row r="77" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C77" s="14" t="s">
         <v>125</v>
       </c>
@@ -2674,13 +2926,13 @@
         <v>44</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="G77" s="15"/>
       <c r="H77" s="6"/>
       <c r="I77" s="8"/>
     </row>
-    <row r="78" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C78" s="14" t="s">
         <v>126</v>
       </c>
@@ -2691,13 +2943,13 @@
         <v>47</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="G78" s="15"/>
       <c r="H78" s="6"/>
       <c r="I78" s="8"/>
     </row>
-    <row r="79" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="14" t="s">
         <v>127</v>
       </c>
@@ -2708,7 +2960,7 @@
         <v>47</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>211</v>
+        <v>247</v>
       </c>
       <c r="G79" s="15"/>
       <c r="H79" s="6"/>
@@ -2725,7 +2977,7 @@
         <v>48</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G80" s="15"/>
       <c r="H80" s="6"/>
@@ -2742,7 +2994,7 @@
         <v>48</v>
       </c>
       <c r="F81" s="31" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G81" s="15"/>
       <c r="H81" s="6"/>
@@ -2759,13 +3011,13 @@
         <v>48</v>
       </c>
       <c r="F82" s="31" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G82" s="15"/>
       <c r="H82" s="6"/>
       <c r="I82" s="8"/>
     </row>
-    <row r="83" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C83" s="14" t="s">
         <v>131</v>
       </c>
@@ -2776,13 +3028,13 @@
         <v>132</v>
       </c>
       <c r="F83" s="31" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="6"/>
       <c r="I83" s="8"/>
     </row>
-    <row r="84" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C84" s="14" t="s">
         <v>133</v>
       </c>
@@ -2793,13 +3045,13 @@
         <v>132</v>
       </c>
       <c r="F84" s="31" t="s">
-        <v>212</v>
+        <v>204</v>
       </c>
       <c r="G84" s="15"/>
       <c r="H84" s="6"/>
       <c r="I84" s="8"/>
     </row>
-    <row r="85" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C85" s="14" t="s">
         <v>134</v>
       </c>
@@ -2810,13 +3062,13 @@
         <v>135</v>
       </c>
       <c r="F85" s="31" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G85" s="15"/>
       <c r="H85" s="6"/>
       <c r="I85" s="8"/>
     </row>
-    <row r="86" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C86" s="14" t="s">
         <v>136</v>
       </c>
@@ -2825,7 +3077,7 @@
       </c>
       <c r="E86" s="32"/>
       <c r="F86" s="31" t="s">
-        <v>213</v>
+        <v>220</v>
       </c>
       <c r="G86" s="15"/>
       <c r="H86" s="6"/>
@@ -2839,7 +3091,9 @@
         <v>137</v>
       </c>
       <c r="E87" s="32"/>
-      <c r="F87" s="31"/>
+      <c r="F87" s="31" t="s">
+        <v>221</v>
+      </c>
       <c r="G87" s="15"/>
       <c r="H87" s="6"/>
       <c r="I87" s="8"/>
@@ -2852,12 +3106,14 @@
         <v>140</v>
       </c>
       <c r="E88" s="32"/>
-      <c r="F88" s="31"/>
+      <c r="F88" s="31" t="s">
+        <v>226</v>
+      </c>
       <c r="G88" s="15"/>
       <c r="H88" s="6"/>
       <c r="I88" s="8"/>
     </row>
-    <row r="89" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C89" s="14" t="s">
         <v>141</v>
       </c>
@@ -2865,12 +3121,14 @@
         <v>140</v>
       </c>
       <c r="E89" s="32"/>
-      <c r="F89" s="31"/>
+      <c r="F89" s="31" t="s">
+        <v>227</v>
+      </c>
       <c r="G89" s="15"/>
       <c r="H89" s="6"/>
       <c r="I89" s="8"/>
     </row>
-    <row r="90" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="14" t="s">
         <v>142</v>
       </c>
@@ -2878,12 +3136,14 @@
         <v>140</v>
       </c>
       <c r="E90" s="32"/>
-      <c r="F90" s="31"/>
+      <c r="F90" s="31" t="s">
+        <v>233</v>
+      </c>
       <c r="G90" s="15"/>
       <c r="H90" s="6"/>
       <c r="I90" s="8"/>
     </row>
-    <row r="91" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C91" s="14" t="s">
         <v>143</v>
       </c>
@@ -2891,12 +3151,14 @@
         <v>140</v>
       </c>
       <c r="E91" s="32"/>
-      <c r="F91" s="31"/>
+      <c r="F91" s="31" t="s">
+        <v>233</v>
+      </c>
       <c r="G91" s="15"/>
       <c r="H91" s="6"/>
       <c r="I91" s="8"/>
     </row>
-    <row r="92" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C92" s="14" t="s">
         <v>144</v>
       </c>
@@ -2904,7 +3166,9 @@
         <v>140</v>
       </c>
       <c r="E92" s="32"/>
-      <c r="F92" s="31"/>
+      <c r="F92" s="31" t="s">
+        <v>234</v>
+      </c>
       <c r="G92" s="15"/>
       <c r="H92" s="6"/>
       <c r="I92" s="8"/>
@@ -2917,7 +3181,9 @@
         <v>140</v>
       </c>
       <c r="E93" s="32"/>
-      <c r="F93" s="31"/>
+      <c r="F93" s="31" t="s">
+        <v>221</v>
+      </c>
       <c r="G93" s="15"/>
       <c r="H93" s="6"/>
       <c r="I93" s="8"/>
@@ -2931,13 +3197,13 @@
       </c>
       <c r="E94" s="32"/>
       <c r="F94" s="31" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G94" s="15"/>
       <c r="H94" s="6"/>
       <c r="I94" s="8"/>
     </row>
-    <row r="95" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C95" s="14" t="s">
         <v>148</v>
       </c>
@@ -2948,7 +3214,7 @@
         <v>20</v>
       </c>
       <c r="F95" s="31" t="s">
-        <v>213</v>
+        <v>238</v>
       </c>
       <c r="G95" s="15"/>
       <c r="H95" s="6"/>
@@ -2965,13 +3231,13 @@
         <v>20</v>
       </c>
       <c r="F96" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G96" s="15"/>
       <c r="H96" s="6"/>
       <c r="I96" s="8"/>
     </row>
-    <row r="97" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C97" s="14" t="s">
         <v>150</v>
       </c>
@@ -2982,7 +3248,7 @@
         <v>20</v>
       </c>
       <c r="F97" s="31" t="s">
-        <v>213</v>
+        <v>239</v>
       </c>
       <c r="G97" s="15"/>
       <c r="H97" s="6"/>
@@ -2999,13 +3265,13 @@
         <v>20</v>
       </c>
       <c r="F98" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G98" s="15"/>
       <c r="H98" s="6"/>
       <c r="I98" s="8"/>
     </row>
-    <row r="99" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C99" s="14" t="s">
         <v>152</v>
       </c>
@@ -3016,13 +3282,13 @@
         <v>20</v>
       </c>
       <c r="F99" s="31" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="G99" s="15"/>
       <c r="H99" s="6"/>
       <c r="I99" s="8"/>
     </row>
-    <row r="100" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C100" s="14" t="s">
         <v>153</v>
       </c>
@@ -3033,7 +3299,7 @@
         <v>20</v>
       </c>
       <c r="F100" s="31" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G100" s="15"/>
       <c r="H100" s="6"/>
@@ -3050,7 +3316,7 @@
         <v>22</v>
       </c>
       <c r="F101" s="31" t="s">
-        <v>213</v>
+        <v>243</v>
       </c>
       <c r="G101" s="15"/>
       <c r="H101" s="6"/>
@@ -3067,7 +3333,7 @@
         <v>21</v>
       </c>
       <c r="F102" s="31" t="s">
-        <v>213</v>
+        <v>244</v>
       </c>
       <c r="G102" s="15"/>
       <c r="H102" s="6"/>
@@ -3084,7 +3350,7 @@
         <v>17</v>
       </c>
       <c r="F103" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G103" s="15"/>
       <c r="H103" s="6"/>
@@ -3101,7 +3367,7 @@
         <v>18</v>
       </c>
       <c r="F104" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G104" s="15"/>
       <c r="H104" s="6"/>
@@ -3118,7 +3384,7 @@
         <v>18</v>
       </c>
       <c r="F105" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G105" s="15"/>
       <c r="H105" s="6"/>
@@ -3135,7 +3401,7 @@
         <v>19</v>
       </c>
       <c r="F106" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G106" s="15"/>
       <c r="H106" s="6"/>
@@ -3152,13 +3418,13 @@
         <v>19</v>
       </c>
       <c r="F107" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G107" s="15"/>
       <c r="H107" s="6"/>
       <c r="I107" s="8"/>
     </row>
-    <row r="108" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C108" s="14" t="s">
         <v>53</v>
       </c>
@@ -3169,13 +3435,13 @@
         <v>159</v>
       </c>
       <c r="F108" s="31" t="s">
-        <v>213</v>
+        <v>245</v>
       </c>
       <c r="G108" s="15"/>
       <c r="H108" s="6"/>
       <c r="I108" s="8"/>
     </row>
-    <row r="109" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C109" s="14" t="s">
         <v>160</v>
       </c>
@@ -3186,7 +3452,7 @@
         <v>159</v>
       </c>
       <c r="F109" s="31" t="s">
-        <v>213</v>
+        <v>235</v>
       </c>
       <c r="G109" s="15"/>
       <c r="H109" s="6"/>
@@ -3203,13 +3469,13 @@
         <v>159</v>
       </c>
       <c r="F110" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G110" s="15"/>
       <c r="H110" s="6"/>
       <c r="I110" s="8"/>
     </row>
-    <row r="111" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="14" t="s">
         <v>162</v>
       </c>
@@ -3220,13 +3486,13 @@
         <v>163</v>
       </c>
       <c r="F111" s="31" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="G111" s="15"/>
       <c r="H111" s="6"/>
       <c r="I111" s="8"/>
     </row>
-    <row r="112" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C112" s="14" t="s">
         <v>164</v>
       </c>
@@ -3237,13 +3503,13 @@
         <v>165</v>
       </c>
       <c r="F112" s="31" t="s">
-        <v>211</v>
+        <v>236</v>
       </c>
       <c r="G112" s="15"/>
       <c r="H112" s="6"/>
       <c r="I112" s="8"/>
     </row>
-    <row r="113" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C113" s="14" t="s">
         <v>166</v>
       </c>
@@ -3254,7 +3520,7 @@
         <v>167</v>
       </c>
       <c r="F113" s="31" t="s">
-        <v>211</v>
+        <v>230</v>
       </c>
       <c r="G113" s="15"/>
       <c r="H113" s="6"/>
@@ -3271,13 +3537,13 @@
         <v>169</v>
       </c>
       <c r="F114" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G114" s="15"/>
       <c r="H114" s="6"/>
       <c r="I114" s="8"/>
     </row>
-    <row r="115" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C115" s="14" t="s">
         <v>170</v>
       </c>
@@ -3288,13 +3554,13 @@
         <v>135</v>
       </c>
       <c r="F115" s="31" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G115" s="15"/>
       <c r="H115" s="6"/>
       <c r="I115" s="8"/>
     </row>
-    <row r="116" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C116" s="14" t="s">
         <v>171</v>
       </c>
@@ -3305,13 +3571,13 @@
         <v>172</v>
       </c>
       <c r="F116" s="31" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G116" s="15"/>
       <c r="H116" s="6"/>
       <c r="I116" s="8"/>
     </row>
-    <row r="117" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C117" s="14" t="s">
         <v>173</v>
       </c>
@@ -3322,13 +3588,13 @@
         <v>172</v>
       </c>
       <c r="F117" s="31" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G117" s="15"/>
       <c r="H117" s="6"/>
       <c r="I117" s="8"/>
     </row>
-    <row r="118" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C118" s="14" t="s">
         <v>174</v>
       </c>
@@ -3339,13 +3605,13 @@
         <v>172</v>
       </c>
       <c r="F118" s="31" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G118" s="15"/>
       <c r="H118" s="6"/>
       <c r="I118" s="8"/>
     </row>
-    <row r="119" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C119" s="14" t="s">
         <v>175</v>
       </c>
@@ -3356,13 +3622,13 @@
         <v>172</v>
       </c>
       <c r="F119" s="31" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G119" s="15"/>
       <c r="H119" s="6"/>
       <c r="I119" s="8"/>
     </row>
-    <row r="120" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C120" s="14" t="s">
         <v>176</v>
       </c>
@@ -3373,7 +3639,7 @@
         <v>172</v>
       </c>
       <c r="F120" s="31" t="s">
-        <v>213</v>
+        <v>237</v>
       </c>
       <c r="G120" s="15"/>
       <c r="H120" s="6"/>
@@ -3390,13 +3656,13 @@
         <v>21</v>
       </c>
       <c r="F121" s="31" t="s">
-        <v>213</v>
+        <v>200</v>
       </c>
       <c r="G121" s="15"/>
       <c r="H121" s="6"/>
       <c r="I121" s="8"/>
     </row>
-    <row r="122" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C122" s="14" t="s">
         <v>178</v>
       </c>
@@ -3407,13 +3673,13 @@
         <v>20</v>
       </c>
       <c r="F122" s="31" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="G122" s="15"/>
       <c r="H122" s="6"/>
       <c r="I122" s="8"/>
     </row>
-    <row r="123" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C123" s="14" t="s">
         <v>179</v>
       </c>
@@ -3424,13 +3690,13 @@
         <v>20</v>
       </c>
       <c r="F123" s="31" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="G123" s="15"/>
       <c r="H123" s="6"/>
       <c r="I123" s="8"/>
     </row>
-    <row r="124" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C124" s="14" t="s">
         <v>180</v>
       </c>
@@ -3441,13 +3707,13 @@
         <v>20</v>
       </c>
       <c r="F124" s="31" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="G124" s="15"/>
       <c r="H124" s="6"/>
       <c r="I124" s="8"/>
     </row>
-    <row r="125" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C125" s="14" t="s">
         <v>181</v>
       </c>
@@ -3458,13 +3724,13 @@
         <v>20</v>
       </c>
       <c r="F125" s="31" t="s">
-        <v>213</v>
+        <v>240</v>
       </c>
       <c r="G125" s="15"/>
       <c r="H125" s="6"/>
       <c r="I125" s="8"/>
     </row>
-    <row r="126" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C126" s="14" t="s">
         <v>182</v>
       </c>
@@ -3472,7 +3738,9 @@
         <v>183</v>
       </c>
       <c r="E126" s="32"/>
-      <c r="F126" s="31"/>
+      <c r="F126" s="31" t="s">
+        <v>241</v>
+      </c>
       <c r="G126" s="15"/>
       <c r="H126" s="6"/>
       <c r="I126" s="8"/>
@@ -3485,12 +3753,14 @@
         <v>183</v>
       </c>
       <c r="E127" s="32"/>
-      <c r="F127" s="31"/>
+      <c r="F127" s="31" t="s">
+        <v>242</v>
+      </c>
       <c r="G127" s="15"/>
       <c r="H127" s="6"/>
       <c r="I127" s="8"/>
     </row>
-    <row r="128" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C128" s="14" t="s">
         <v>185</v>
       </c>
@@ -3500,12 +3770,14 @@
       <c r="E128" s="32" t="s">
         <v>54</v>
       </c>
-      <c r="F128" s="31"/>
+      <c r="F128" s="31" t="s">
+        <v>248</v>
+      </c>
       <c r="G128" s="15"/>
       <c r="H128" s="6"/>
       <c r="I128" s="8"/>
     </row>
-    <row r="129" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C129" s="14" t="s">
         <v>186</v>
       </c>
@@ -3516,13 +3788,13 @@
         <v>54</v>
       </c>
       <c r="F129" s="31" t="s">
-        <v>203</v>
+        <v>249</v>
       </c>
       <c r="G129" s="15"/>
       <c r="H129" s="6"/>
       <c r="I129" s="8"/>
     </row>
-    <row r="130" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C130" s="14" t="s">
         <v>187</v>
       </c>
@@ -3533,13 +3805,13 @@
         <v>54</v>
       </c>
       <c r="F130" s="31" t="s">
-        <v>202</v>
+        <v>250</v>
       </c>
       <c r="G130" s="15"/>
       <c r="H130" s="6"/>
       <c r="I130" s="8"/>
     </row>
-    <row r="131" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C131" s="14" t="s">
         <v>188</v>
       </c>
@@ -3550,13 +3822,13 @@
         <v>55</v>
       </c>
       <c r="F131" s="31" t="s">
-        <v>200</v>
+        <v>251</v>
       </c>
       <c r="G131" s="15"/>
       <c r="H131" s="6"/>
       <c r="I131" s="8"/>
     </row>
-    <row r="132" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C132" s="14" t="s">
         <v>189</v>
       </c>
@@ -3567,13 +3839,13 @@
         <v>55</v>
       </c>
       <c r="F132" s="31" t="s">
-        <v>204</v>
+        <v>252</v>
       </c>
       <c r="G132" s="15"/>
       <c r="H132" s="6"/>
       <c r="I132" s="8"/>
     </row>
-    <row r="133" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C133" s="14" t="s">
         <v>190</v>
       </c>
@@ -3584,13 +3856,13 @@
         <v>55</v>
       </c>
       <c r="F133" s="31" t="s">
-        <v>199</v>
+        <v>203</v>
       </c>
       <c r="G133" s="15"/>
       <c r="H133" s="6"/>
       <c r="I133" s="8"/>
     </row>
-    <row r="134" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C134" s="14" t="s">
         <v>191</v>
       </c>
@@ -3601,13 +3873,13 @@
         <v>55</v>
       </c>
       <c r="F134" s="31" t="s">
-        <v>201</v>
+        <v>253</v>
       </c>
       <c r="G134" s="15"/>
       <c r="H134" s="6"/>
       <c r="I134" s="8"/>
     </row>
-    <row r="135" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C135" s="14" t="s">
         <v>192</v>
       </c>
@@ -3618,13 +3890,13 @@
         <v>55</v>
       </c>
       <c r="F135" s="31" t="s">
-        <v>200</v>
+        <v>254</v>
       </c>
       <c r="G135" s="15"/>
       <c r="H135" s="6"/>
       <c r="I135" s="8"/>
     </row>
-    <row r="136" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C136" s="14" t="s">
         <v>56</v>
       </c>
@@ -3635,7 +3907,7 @@
         <v>57</v>
       </c>
       <c r="F136" s="31" t="s">
-        <v>201</v>
+        <v>202</v>
       </c>
       <c r="G136" s="15"/>
       <c r="H136" s="6"/>

</xml_diff>

<commit_message>
Edit Flow diagram  Design ID based on updates which based on review comments
Edit Flow diagram  Design ID based on updates which based on review comments
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="255">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="258">
   <si>
     <t>Author</t>
   </si>
@@ -662,23 +662,11 @@
     <t>Bank_Sys_DM_CST_007</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_008</t>
-  </si>
-  <si>
     <t>Design ID</t>
   </si>
   <si>
     <t>Bank_Sys_DM_ADMIN_006
 Bank_SYS_HLD_admin_003</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_003
-Bank_SYS_HLD_admin_004
-BANK_SYS_DD_ Admin _007</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_005
-BANK_SYS_DD_account_001</t>
   </si>
   <si>
     <t>Bank_Sys_DM_ADMIN_001
@@ -783,61 +771,130 @@
 Bank_SYS_DSN_004</t>
   </si>
   <si>
+    <t>Bank_SYS_DSN_005</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_006</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_005
+Bank_SYS_DSN_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_005
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_005
+Bank_SYS_DSN_010</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_010</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005
+BANK_SYS_DD_ Admin _006
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_003                                                   
+Bank_SYS_HLD_admin_004
+BANK_SYS_DD_ Admin _007
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">     Bank_Sys_DM_ADMIN_003                                              
+Bank_SYS_HLD_admin_004
+BANK_SYS_DD_ Admin _007</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_004
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_004
+Bank_Sys_DM_ADMIN_007
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005
+Bank_Sys_DM_ADMIN_006
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_008
+Bank_SYS_HLD_admin_006
+Bank_SYS_HLD_admin_005
+BANK_SYS_DD_ Admin _008
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_009
+Bank_SYS_HLD_admin_003
+BANK_SYS_DD_ Admin _006
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
     <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
+Bank_Sys_DM_CST_003
 Bank_SYS_HLD_client_001
 Bank_SYS_HLD_admin_001
 Bank_SYS_DSN_004
 Bank_SYS_DSN_005</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_004
+    <t xml:space="preserve">                                                      
 Bank_SYS_DSN_005</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_008
-Bank_SYS_DSN_005</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_005</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_005
-Bank_Sys_DM_CST_006
+    <t xml:space="preserve">                                                      
+BANK_SYS_DD_account_001</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_006
+Bank_Sys_DM_CST_004
 Bank_SYS_DSN_006</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_006
+    <t>Bank_Sys_DM_ADMIN_006
+Bank_Sys_DM_CST_005
 Bank_SYS_HLD_client_003
 Bank_SYS_DSN_006</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_006
+    <t>Bank_Sys_DM_ADMIN_006
+Bank_Sys_DM_CST_005
 Bank_SYS_DSN_006</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_006
-Bank_Sys_DM_CST_007
+    <t>Bank_Sys_DM_CST_005
 Bank_SYS_HLD_client_004
 BANK_SYS_DD_TR_001
 Bank_SYS_DSN_006</t>
   </si>
   <si>
-    <t>Bank_SYS_DSN_006</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_005
-Bank_SYS_DSN_006</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
+    <t xml:space="preserve">                                                      
+Bank_Sys_DM_CST_006
 Bank_SYS_HLD_client_004
 Bank_SYS_DSN_007
 Bank_SYS_DSN_008
 Bank_SYS_DSN_009</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_007
+    <t xml:space="preserve">                                                      
 Bank_SYS_HLD_client_005
 Bank_SYS_HLD_client_006
 BANK_SYS_DD_ TR _002
@@ -847,133 +904,98 @@
 Bank_SYS_DSN_009</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_007
+    <t xml:space="preserve">                                                      
 Bank_SYS_DSN_007
 Bank_SYS_DSN_008
 Bank_SYS_DSN_009</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_007
+    <t xml:space="preserve">                                                      
+</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
 Bank_SYS_HLD_client_003
 Bank_SYS_DSN_007
 Bank_SYS_DSN_008
 Bank_SYS_DSN_009</t>
   </si>
   <si>
-    <t xml:space="preserve">Bank_Sys_DM_CST_007
-</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_005
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_008
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
+    <t xml:space="preserve">                                                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+Bank_SYS_HLD_client_006
+BANK_SYS_DD_ PR _003
+Bank_SYS_DSN_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+Bank_SYS_DSN_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+Bank_Sys_DM_CST_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_006
 BANK_SYS_DD_ PR _002
 Bank_SYS_DSN_007
 Bank_SYS_DSN_008
 Bank_SYS_DSN_009</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_008
+    <t>Bank_Sys_DM_CST_006                                                      
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_006
+Bank_Sys_DM_ADMIN_007                                                      
+BANK_SYS_DD_ PR _002
+Bank_SYS_DSN_007
+Bank_SYS_DSN_008
+Bank_SYS_DSN_009</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
 Bank_SYS_DSN_010</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_008
+    <t>Bank_Sys_DM_CST_007
+Bank_SYS_DSN_005</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
 BANK_SYS_DD_ Trans _003
 Bank_SYS_DSN_010</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_008
+    <t>Bank_Sys_DM_CST_007
 BANK_SYS_DD_ account _003
 BANK_SYS_DD_Trans_001
 BANK_SYS_DD_PR_001
 Bank_SYS_DSN_010</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_008
+    <t>Bank_Sys_DM_CST_007
 BANK_SYS_DD_ Trans _002
 Bank_SYS_DSN_010</t>
   </si>
   <si>
-    <t>Bank_SYS_DSN_005
-Bank_SYS_DSN_010</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_010</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_008
+    <t>Bank_Sys_DM_CST_007
 Bank_SYS_DSN_012</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_008
+    <t>Bank_Sys_DM_CST_007
 Bank_SYS_DSN_013</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_008
+    <t>Bank_Sys_DM_CST_007
+Bank_Sys_DM_CST_007
 BANK_SYS_DD_ account _002
 Bank_SYS_DSN_011</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-Bank_SYS_HLD_client_006
-BANK_SYS_DD_ PR _003
-Bank_SYS_DSN_014</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-Bank_SYS_DSN_014</t>
-  </si>
-  <si>
-    <t>Bank_SYS_HLD_admin_003
-BANK_SYS_DD_ Admin _006
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_008
-Bank_Sys_DM_ADMIN_009
-Bank_SYS_HLD_admin_006
-Bank_SYS_HLD_admin_005
-BANK_SYS_DD_ Admin _008
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_003
-Bank_SYS_HLD_admin_004
-BANK_SYS_DD_ Admin _007
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_005
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_005
-Bank_Sys_DM_ADMIN_007
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_006
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_005
-BANK_SYS_DD_ Admin _006
-Bank_SYS_DSN_015</t>
   </si>
 </sst>
 </file>
@@ -1698,8 +1720,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B18" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B53" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E54" sqref="E54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1997,7 +2019,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>198</v>
@@ -2018,7 +2040,7 @@
         <v>23</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>208</v>
+        <v>205</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="5"/>
@@ -2035,7 +2057,7 @@
         <v>72</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>209</v>
+        <v>206</v>
       </c>
       <c r="G24" s="29"/>
       <c r="H24" s="30"/>
@@ -2052,7 +2074,7 @@
         <v>72</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G25" s="29"/>
       <c r="H25" s="30"/>
@@ -2069,7 +2091,7 @@
         <v>72</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>211</v>
+        <v>208</v>
       </c>
       <c r="G26" s="29"/>
       <c r="H26" s="30"/>
@@ -2086,7 +2108,7 @@
         <v>72</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>212</v>
+        <v>209</v>
       </c>
       <c r="G27" s="29"/>
       <c r="H27" s="30"/>
@@ -2103,7 +2125,7 @@
         <v>72</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G28" s="29"/>
       <c r="H28" s="30"/>
@@ -2120,7 +2142,7 @@
         <v>24</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="6"/>
@@ -2137,7 +2159,7 @@
         <v>24</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="5"/>
@@ -2154,7 +2176,7 @@
         <v>24</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="6"/>
@@ -2171,7 +2193,7 @@
         <v>80</v>
       </c>
       <c r="F32" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="5"/>
@@ -2188,7 +2210,7 @@
         <v>24</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="6"/>
@@ -2205,7 +2227,7 @@
         <v>24</v>
       </c>
       <c r="F34" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="6"/>
@@ -2222,7 +2244,7 @@
         <v>24</v>
       </c>
       <c r="F35" s="34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="6"/>
@@ -2239,7 +2261,7 @@
         <v>24</v>
       </c>
       <c r="F36" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="6"/>
@@ -2256,7 +2278,7 @@
         <v>24</v>
       </c>
       <c r="F37" s="34" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="6"/>
@@ -2273,7 +2295,7 @@
         <v>31</v>
       </c>
       <c r="F38" s="34" t="s">
-        <v>217</v>
+        <v>214</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="6"/>
@@ -2290,7 +2312,7 @@
         <v>31</v>
       </c>
       <c r="F39" s="34" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="6"/>
@@ -2307,7 +2329,7 @@
         <v>31</v>
       </c>
       <c r="F40" s="34" t="s">
-        <v>216</v>
+        <v>213</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="6"/>
@@ -2324,7 +2346,7 @@
         <v>90</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="6"/>
@@ -2341,7 +2363,7 @@
         <v>91</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>214</v>
+        <v>211</v>
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="6"/>
@@ -2358,7 +2380,7 @@
         <v>27</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G43" s="15"/>
       <c r="H43" s="6"/>
@@ -2375,7 +2397,7 @@
         <v>92</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G44" s="15"/>
       <c r="H44" s="6"/>
@@ -2392,7 +2414,7 @@
         <v>92</v>
       </c>
       <c r="F45" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G45" s="15"/>
       <c r="H45" s="6"/>
@@ -2409,7 +2431,7 @@
         <v>95</v>
       </c>
       <c r="F46" s="34" t="s">
-        <v>215</v>
+        <v>212</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="6"/>
@@ -2426,7 +2448,7 @@
         <v>90</v>
       </c>
       <c r="F47" s="34" t="s">
-        <v>218</v>
+        <v>231</v>
       </c>
       <c r="G47" s="15"/>
       <c r="H47" s="6"/>
@@ -2443,7 +2465,7 @@
         <v>99</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>213</v>
+        <v>210</v>
       </c>
       <c r="G48" s="15"/>
       <c r="H48" s="6"/>
@@ -2458,7 +2480,7 @@
       </c>
       <c r="E49" s="32"/>
       <c r="F49" s="34" t="s">
-        <v>210</v>
+        <v>207</v>
       </c>
       <c r="G49" s="15"/>
       <c r="H49" s="6"/>
@@ -2475,7 +2497,7 @@
         <v>29</v>
       </c>
       <c r="F50" s="31" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
       <c r="G50" s="15"/>
       <c r="H50" s="6"/>
@@ -2492,7 +2514,7 @@
         <v>29</v>
       </c>
       <c r="F51" s="31" t="s">
-        <v>207</v>
+        <v>204</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="6"/>
@@ -2509,7 +2531,7 @@
         <v>29</v>
       </c>
       <c r="F52" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G52" s="15"/>
       <c r="H52" s="6"/>
@@ -2526,7 +2548,7 @@
         <v>29</v>
       </c>
       <c r="F53" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G53" s="15"/>
       <c r="H53" s="6"/>
@@ -2543,7 +2565,7 @@
         <v>30</v>
       </c>
       <c r="F54" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="6"/>
@@ -2560,7 +2582,7 @@
         <v>30</v>
       </c>
       <c r="F55" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G55" s="15"/>
       <c r="H55" s="6"/>
@@ -2577,7 +2599,7 @@
         <v>30</v>
       </c>
       <c r="F56" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G56" s="15"/>
       <c r="H56" s="6"/>
@@ -2594,7 +2616,7 @@
         <v>31</v>
       </c>
       <c r="F57" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G57" s="15"/>
       <c r="H57" s="6"/>
@@ -2609,7 +2631,7 @@
         <v>33</v>
       </c>
       <c r="F58" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G58" s="15"/>
       <c r="H58" s="6"/>
@@ -2624,7 +2646,7 @@
         <v>95</v>
       </c>
       <c r="F59" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="6"/>
@@ -2639,7 +2661,7 @@
       </c>
       <c r="E60" s="32"/>
       <c r="F60" s="31" t="s">
-        <v>206</v>
+        <v>203</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="6"/>
@@ -2656,7 +2678,7 @@
         <v>36</v>
       </c>
       <c r="F61" s="31" t="s">
-        <v>219</v>
+        <v>232</v>
       </c>
       <c r="G61" s="15"/>
       <c r="H61" s="6"/>
@@ -2677,7 +2699,7 @@
       <c r="H62" s="6"/>
       <c r="I62" s="8"/>
     </row>
-    <row r="63" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C63" s="14" t="s">
         <v>113</v>
       </c>
@@ -2688,13 +2710,13 @@
         <v>39</v>
       </c>
       <c r="F63" s="31" t="s">
-        <v>222</v>
+        <v>234</v>
       </c>
       <c r="G63" s="15"/>
       <c r="H63" s="6"/>
       <c r="I63" s="8"/>
     </row>
-    <row r="64" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="14" t="s">
         <v>114</v>
       </c>
@@ -2705,13 +2727,13 @@
         <v>39</v>
       </c>
       <c r="F64" s="31" t="s">
-        <v>223</v>
+        <v>235</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="6"/>
       <c r="I64" s="8"/>
     </row>
-    <row r="65" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="14" t="s">
         <v>115</v>
       </c>
@@ -2722,13 +2744,13 @@
         <v>39</v>
       </c>
       <c r="F65" s="31" t="s">
-        <v>224</v>
+        <v>236</v>
       </c>
       <c r="G65" s="15"/>
       <c r="H65" s="6"/>
       <c r="I65" s="8"/>
     </row>
-    <row r="66" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="14" t="s">
         <v>116</v>
       </c>
@@ -2739,7 +2761,7 @@
         <v>39</v>
       </c>
       <c r="F66" s="31" t="s">
-        <v>225</v>
+        <v>237</v>
       </c>
       <c r="G66" s="15"/>
       <c r="H66" s="6"/>
@@ -2756,13 +2778,13 @@
         <v>39</v>
       </c>
       <c r="F67" s="31" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G67" s="15"/>
       <c r="H67" s="6"/>
       <c r="I67" s="8"/>
     </row>
-    <row r="68" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="14" t="s">
         <v>118</v>
       </c>
@@ -2773,7 +2795,7 @@
         <v>39</v>
       </c>
       <c r="F68" s="31" t="s">
-        <v>228</v>
+        <v>238</v>
       </c>
       <c r="G68" s="15"/>
       <c r="H68" s="6"/>
@@ -2790,7 +2812,7 @@
         <v>41</v>
       </c>
       <c r="F69" s="31" t="s">
-        <v>229</v>
+        <v>239</v>
       </c>
       <c r="G69" s="15"/>
       <c r="H69" s="6"/>
@@ -2807,7 +2829,7 @@
         <v>43</v>
       </c>
       <c r="F70" s="31" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="G70" s="15"/>
       <c r="H70" s="6"/>
@@ -2824,7 +2846,7 @@
         <v>44</v>
       </c>
       <c r="F71" s="31" t="s">
-        <v>232</v>
+        <v>241</v>
       </c>
       <c r="G71" s="15"/>
       <c r="H71" s="6"/>
@@ -2841,7 +2863,7 @@
         <v>44</v>
       </c>
       <c r="F72" s="31" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="G72" s="15"/>
       <c r="H72" s="6"/>
@@ -2858,7 +2880,7 @@
         <v>44</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="G73" s="15"/>
       <c r="H73" s="6"/>
@@ -2875,7 +2897,7 @@
         <v>45</v>
       </c>
       <c r="F74" s="31" t="s">
-        <v>231</v>
+        <v>242</v>
       </c>
       <c r="G74" s="15"/>
       <c r="H74" s="6"/>
@@ -2892,7 +2914,7 @@
         <v>44</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="6"/>
@@ -2909,7 +2931,7 @@
         <v>44</v>
       </c>
       <c r="F76" s="31" t="s">
-        <v>246</v>
+        <v>244</v>
       </c>
       <c r="G76" s="15"/>
       <c r="H76" s="6"/>
@@ -2926,7 +2948,7 @@
         <v>44</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>230</v>
+        <v>240</v>
       </c>
       <c r="G77" s="15"/>
       <c r="H77" s="6"/>
@@ -2943,7 +2965,7 @@
         <v>47</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G78" s="15"/>
       <c r="H78" s="6"/>
@@ -2960,7 +2982,7 @@
         <v>47</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>247</v>
+        <v>245</v>
       </c>
       <c r="G79" s="15"/>
       <c r="H79" s="6"/>
@@ -2977,13 +2999,13 @@
         <v>48</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
       <c r="G80" s="15"/>
       <c r="H80" s="6"/>
       <c r="I80" s="8"/>
     </row>
-    <row r="81" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="14" t="s">
         <v>129</v>
       </c>
@@ -2994,13 +3016,13 @@
         <v>48</v>
       </c>
       <c r="F81" s="31" t="s">
-        <v>199</v>
+        <v>246</v>
       </c>
       <c r="G81" s="15"/>
       <c r="H81" s="6"/>
       <c r="I81" s="8"/>
     </row>
-    <row r="82" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C82" s="14" t="s">
         <v>130</v>
       </c>
@@ -3011,13 +3033,13 @@
         <v>48</v>
       </c>
       <c r="F82" s="31" t="s">
-        <v>199</v>
+        <v>246</v>
       </c>
       <c r="G82" s="15"/>
       <c r="H82" s="6"/>
       <c r="I82" s="8"/>
     </row>
-    <row r="83" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C83" s="14" t="s">
         <v>131</v>
       </c>
@@ -3028,13 +3050,13 @@
         <v>132</v>
       </c>
       <c r="F83" s="31" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="6"/>
       <c r="I83" s="8"/>
     </row>
-    <row r="84" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C84" s="14" t="s">
         <v>133</v>
       </c>
@@ -3045,7 +3067,7 @@
         <v>132</v>
       </c>
       <c r="F84" s="31" t="s">
-        <v>204</v>
+        <v>233</v>
       </c>
       <c r="G84" s="15"/>
       <c r="H84" s="6"/>
@@ -3062,7 +3084,7 @@
         <v>135</v>
       </c>
       <c r="F85" s="31" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G85" s="15"/>
       <c r="H85" s="6"/>
@@ -3077,7 +3099,7 @@
       </c>
       <c r="E86" s="32"/>
       <c r="F86" s="31" t="s">
-        <v>220</v>
+        <v>251</v>
       </c>
       <c r="G86" s="15"/>
       <c r="H86" s="6"/>
@@ -3092,7 +3114,7 @@
       </c>
       <c r="E87" s="32"/>
       <c r="F87" s="31" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G87" s="15"/>
       <c r="H87" s="6"/>
@@ -3107,7 +3129,7 @@
       </c>
       <c r="E88" s="32"/>
       <c r="F88" s="31" t="s">
-        <v>226</v>
+        <v>216</v>
       </c>
       <c r="G88" s="15"/>
       <c r="H88" s="6"/>
@@ -3122,7 +3144,7 @@
       </c>
       <c r="E89" s="32"/>
       <c r="F89" s="31" t="s">
-        <v>227</v>
+        <v>217</v>
       </c>
       <c r="G89" s="15"/>
       <c r="H89" s="6"/>
@@ -3137,7 +3159,7 @@
       </c>
       <c r="E90" s="32"/>
       <c r="F90" s="31" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="G90" s="15"/>
       <c r="H90" s="6"/>
@@ -3152,7 +3174,7 @@
       </c>
       <c r="E91" s="32"/>
       <c r="F91" s="31" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="G91" s="15"/>
       <c r="H91" s="6"/>
@@ -3167,7 +3189,7 @@
       </c>
       <c r="E92" s="32"/>
       <c r="F92" s="31" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="G92" s="15"/>
       <c r="H92" s="6"/>
@@ -3182,7 +3204,7 @@
       </c>
       <c r="E93" s="32"/>
       <c r="F93" s="31" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="G93" s="15"/>
       <c r="H93" s="6"/>
@@ -3197,7 +3219,7 @@
       </c>
       <c r="E94" s="32"/>
       <c r="F94" s="31" t="s">
-        <v>199</v>
+        <v>243</v>
       </c>
       <c r="G94" s="15"/>
       <c r="H94" s="6"/>
@@ -3214,7 +3236,7 @@
         <v>20</v>
       </c>
       <c r="F95" s="31" t="s">
-        <v>238</v>
+        <v>252</v>
       </c>
       <c r="G95" s="15"/>
       <c r="H95" s="6"/>
@@ -3231,7 +3253,7 @@
         <v>20</v>
       </c>
       <c r="F96" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G96" s="15"/>
       <c r="H96" s="6"/>
@@ -3248,7 +3270,7 @@
         <v>20</v>
       </c>
       <c r="F97" s="31" t="s">
-        <v>239</v>
+        <v>253</v>
       </c>
       <c r="G97" s="15"/>
       <c r="H97" s="6"/>
@@ -3265,7 +3287,7 @@
         <v>20</v>
       </c>
       <c r="F98" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G98" s="15"/>
       <c r="H98" s="6"/>
@@ -3282,7 +3304,7 @@
         <v>20</v>
       </c>
       <c r="F99" s="31" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="G99" s="15"/>
       <c r="H99" s="6"/>
@@ -3299,7 +3321,7 @@
         <v>20</v>
       </c>
       <c r="F100" s="31" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G100" s="15"/>
       <c r="H100" s="6"/>
@@ -3316,7 +3338,7 @@
         <v>22</v>
       </c>
       <c r="F101" s="31" t="s">
-        <v>243</v>
+        <v>255</v>
       </c>
       <c r="G101" s="15"/>
       <c r="H101" s="6"/>
@@ -3333,7 +3355,7 @@
         <v>21</v>
       </c>
       <c r="F102" s="31" t="s">
-        <v>244</v>
+        <v>256</v>
       </c>
       <c r="G102" s="15"/>
       <c r="H102" s="6"/>
@@ -3350,7 +3372,7 @@
         <v>17</v>
       </c>
       <c r="F103" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G103" s="15"/>
       <c r="H103" s="6"/>
@@ -3367,7 +3389,7 @@
         <v>18</v>
       </c>
       <c r="F104" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G104" s="15"/>
       <c r="H104" s="6"/>
@@ -3384,7 +3406,7 @@
         <v>18</v>
       </c>
       <c r="F105" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G105" s="15"/>
       <c r="H105" s="6"/>
@@ -3401,7 +3423,7 @@
         <v>19</v>
       </c>
       <c r="F106" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G106" s="15"/>
       <c r="H106" s="6"/>
@@ -3418,13 +3440,13 @@
         <v>19</v>
       </c>
       <c r="F107" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G107" s="15"/>
       <c r="H107" s="6"/>
       <c r="I107" s="8"/>
     </row>
-    <row r="108" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C108" s="14" t="s">
         <v>53</v>
       </c>
@@ -3435,7 +3457,7 @@
         <v>159</v>
       </c>
       <c r="F108" s="31" t="s">
-        <v>245</v>
+        <v>257</v>
       </c>
       <c r="G108" s="15"/>
       <c r="H108" s="6"/>
@@ -3452,7 +3474,7 @@
         <v>159</v>
       </c>
       <c r="F109" s="31" t="s">
-        <v>235</v>
+        <v>218</v>
       </c>
       <c r="G109" s="15"/>
       <c r="H109" s="6"/>
@@ -3469,13 +3491,13 @@
         <v>159</v>
       </c>
       <c r="F110" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G110" s="15"/>
       <c r="H110" s="6"/>
       <c r="I110" s="8"/>
     </row>
-    <row r="111" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="14" t="s">
         <v>162</v>
       </c>
@@ -3486,13 +3508,13 @@
         <v>163</v>
       </c>
       <c r="F111" s="31" t="s">
-        <v>236</v>
+        <v>247</v>
       </c>
       <c r="G111" s="15"/>
       <c r="H111" s="6"/>
       <c r="I111" s="8"/>
     </row>
-    <row r="112" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C112" s="14" t="s">
         <v>164</v>
       </c>
@@ -3503,7 +3525,7 @@
         <v>165</v>
       </c>
       <c r="F112" s="31" t="s">
-        <v>236</v>
+        <v>249</v>
       </c>
       <c r="G112" s="15"/>
       <c r="H112" s="6"/>
@@ -3520,7 +3542,7 @@
         <v>167</v>
       </c>
       <c r="F113" s="31" t="s">
-        <v>230</v>
+        <v>248</v>
       </c>
       <c r="G113" s="15"/>
       <c r="H113" s="6"/>
@@ -3537,7 +3559,7 @@
         <v>169</v>
       </c>
       <c r="F114" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G114" s="15"/>
       <c r="H114" s="6"/>
@@ -3554,7 +3576,7 @@
         <v>135</v>
       </c>
       <c r="F115" s="31" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G115" s="15"/>
       <c r="H115" s="6"/>
@@ -3571,7 +3593,7 @@
         <v>172</v>
       </c>
       <c r="F116" s="31" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G116" s="15"/>
       <c r="H116" s="6"/>
@@ -3588,7 +3610,7 @@
         <v>172</v>
       </c>
       <c r="F117" s="31" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G117" s="15"/>
       <c r="H117" s="6"/>
@@ -3605,7 +3627,7 @@
         <v>172</v>
       </c>
       <c r="F118" s="31" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G118" s="15"/>
       <c r="H118" s="6"/>
@@ -3622,7 +3644,7 @@
         <v>172</v>
       </c>
       <c r="F119" s="31" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G119" s="15"/>
       <c r="H119" s="6"/>
@@ -3639,7 +3661,7 @@
         <v>172</v>
       </c>
       <c r="F120" s="31" t="s">
-        <v>237</v>
+        <v>250</v>
       </c>
       <c r="G120" s="15"/>
       <c r="H120" s="6"/>
@@ -3656,7 +3678,7 @@
         <v>21</v>
       </c>
       <c r="F121" s="31" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G121" s="15"/>
       <c r="H121" s="6"/>
@@ -3673,7 +3695,7 @@
         <v>20</v>
       </c>
       <c r="F122" s="31" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="G122" s="15"/>
       <c r="H122" s="6"/>
@@ -3690,7 +3712,7 @@
         <v>20</v>
       </c>
       <c r="F123" s="31" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="G123" s="15"/>
       <c r="H123" s="6"/>
@@ -3707,7 +3729,7 @@
         <v>20</v>
       </c>
       <c r="F124" s="31" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="G124" s="15"/>
       <c r="H124" s="6"/>
@@ -3724,7 +3746,7 @@
         <v>20</v>
       </c>
       <c r="F125" s="31" t="s">
-        <v>240</v>
+        <v>254</v>
       </c>
       <c r="G125" s="15"/>
       <c r="H125" s="6"/>
@@ -3739,7 +3761,7 @@
       </c>
       <c r="E126" s="32"/>
       <c r="F126" s="31" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="G126" s="15"/>
       <c r="H126" s="6"/>
@@ -3754,13 +3776,13 @@
       </c>
       <c r="E127" s="32"/>
       <c r="F127" s="31" t="s">
-        <v>242</v>
+        <v>222</v>
       </c>
       <c r="G127" s="15"/>
       <c r="H127" s="6"/>
       <c r="I127" s="8"/>
     </row>
-    <row r="128" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C128" s="14" t="s">
         <v>185</v>
       </c>
@@ -3771,13 +3793,13 @@
         <v>54</v>
       </c>
       <c r="F128" s="31" t="s">
-        <v>248</v>
+        <v>230</v>
       </c>
       <c r="G128" s="15"/>
       <c r="H128" s="6"/>
       <c r="I128" s="8"/>
     </row>
-    <row r="129" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C129" s="14" t="s">
         <v>186</v>
       </c>
@@ -3788,7 +3810,7 @@
         <v>54</v>
       </c>
       <c r="F129" s="31" t="s">
-        <v>249</v>
+        <v>229</v>
       </c>
       <c r="G129" s="15"/>
       <c r="H129" s="6"/>
@@ -3805,7 +3827,7 @@
         <v>54</v>
       </c>
       <c r="F130" s="31" t="s">
-        <v>250</v>
+        <v>224</v>
       </c>
       <c r="G130" s="15"/>
       <c r="H130" s="6"/>
@@ -3822,7 +3844,7 @@
         <v>55</v>
       </c>
       <c r="F131" s="31" t="s">
-        <v>251</v>
+        <v>226</v>
       </c>
       <c r="G131" s="15"/>
       <c r="H131" s="6"/>
@@ -3839,13 +3861,13 @@
         <v>55</v>
       </c>
       <c r="F132" s="31" t="s">
-        <v>252</v>
+        <v>227</v>
       </c>
       <c r="G132" s="15"/>
       <c r="H132" s="6"/>
       <c r="I132" s="8"/>
     </row>
-    <row r="133" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C133" s="14" t="s">
         <v>190</v>
       </c>
@@ -3856,13 +3878,13 @@
         <v>55</v>
       </c>
       <c r="F133" s="31" t="s">
-        <v>203</v>
+        <v>225</v>
       </c>
       <c r="G133" s="15"/>
       <c r="H133" s="6"/>
       <c r="I133" s="8"/>
     </row>
-    <row r="134" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C134" s="14" t="s">
         <v>191</v>
       </c>
@@ -3873,7 +3895,7 @@
         <v>55</v>
       </c>
       <c r="F134" s="31" t="s">
-        <v>253</v>
+        <v>228</v>
       </c>
       <c r="G134" s="15"/>
       <c r="H134" s="6"/>
@@ -3890,7 +3912,7 @@
         <v>55</v>
       </c>
       <c r="F135" s="31" t="s">
-        <v>254</v>
+        <v>223</v>
       </c>
       <c r="G135" s="15"/>
       <c r="H135" s="6"/>
@@ -3907,7 +3929,7 @@
         <v>57</v>
       </c>
       <c r="F136" s="31" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="G136" s="15"/>
       <c r="H136" s="6"/>

</xml_diff>

<commit_message>
replace BANK_SYS_CR_Q[5-6-7-8-9] WITH BANK_SYS_SIQ_Q[46,47,48,49,50]
replace BANK_SYS_CR_Q[5-6-7-8-9] WITH BANK_SYS_SIQ_Q[46,47,48,49,50]
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="481" uniqueCount="258">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="480" uniqueCount="256">
   <si>
     <t>Author</t>
   </si>
@@ -109,12 +109,6 @@
     <t>BANK_SYS_SIQ_Q20</t>
   </si>
   <si>
-    <t>BANK_SYS_SIQ_Q43</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q44</t>
-  </si>
-  <si>
     <t xml:space="preserve">BANK_SYS_SIQ_Q29
 BANK_SYS_SIQ_Q08
 </t>
@@ -353,19 +347,9 @@
     <t>BANK_SYS_SRS_Reg_R026</t>
   </si>
   <si>
-    <t>BANK_SYS_CR_001
-Bank_Sys_CR_006</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q40</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_Reg_R027</t>
   </si>
   <si>
-    <t>BANK_SYS_CR_008</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_Log_R001</t>
   </si>
   <si>
@@ -396,9 +380,6 @@
     <t>BANK_SYS_SRS_Log_R011</t>
   </si>
   <si>
-    <t>Bank_Sys_CR_007</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_PT_R003</t>
   </si>
   <si>
@@ -429,9 +410,6 @@
     <t>BANK_SYS_SRS_PT_R015</t>
   </si>
   <si>
-    <t>BANK_SYS_CR_006</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_PT_R016</t>
   </si>
   <si>
@@ -471,18 +449,12 @@
     <t>BANK_SYS_SRS_PT_R026</t>
   </si>
   <si>
-    <t>BANK_SYS_CR_009</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_PT_R027</t>
   </si>
   <si>
     <t>BANK_SYS_SRS_PT_R028</t>
   </si>
   <si>
-    <t>Bank_Sys_CR_005</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_PT_R029</t>
   </si>
   <si>
@@ -501,9 +473,6 @@
     <t>BANK_SYS_SRS_PT_R034</t>
   </si>
   <si>
-    <t>Bank_Sys_CR_009</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_TR_R001</t>
   </si>
   <si>
@@ -522,11 +491,6 @@
     <t>BANK_SYS_SRS_TR_R006</t>
   </si>
   <si>
-    <t xml:space="preserve">BANK_SYS_CR_004
-BANK_SYS_CR_006
-</t>
-  </si>
-  <si>
     <t>BANK_SYS_SRS_TR_R010</t>
   </si>
   <si>
@@ -609,9 +573,6 @@
   </si>
   <si>
     <t>BANK_SYS_SRS_TR_R032</t>
-  </si>
-  <si>
-    <t>BANK_SYS_CR_005</t>
   </si>
   <si>
     <t>BANK_SYS_SRS_TR_R033</t>
@@ -996,6 +957,42 @@
 Bank_Sys_DM_CST_007
 BANK_SYS_DD_ account _002
 Bank_SYS_DSN_011</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q46</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q48</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q49</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK_SYS_CR_001
+</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q40
+BANK_SYS_SIQ_Q47</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q22
+BANK_SYS_SIQ_Q47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK_SYS_CR_004
+</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q44
+BANK_SYS_SIQ_Q47</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q43
+BANK_SYS_SIQ_Q47</t>
   </si>
 </sst>
 </file>
@@ -1720,8 +1717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L142"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B53" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E54" sqref="E54"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B134" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E144" sqref="E144"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1893,23 +1890,23 @@
         <v>43529</v>
       </c>
       <c r="E10" s="35" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F10" s="36"/>
       <c r="G10" s="17" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="H10" s="18">
         <v>43529</v>
       </c>
       <c r="I10" s="35" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="J10" s="37"/>
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="B13" s="38" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C13" s="38"/>
       <c r="D13" s="38"/>
@@ -2010,19 +2007,19 @@
     </row>
     <row r="22" spans="2:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="16" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="D22" s="9" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="E22" s="10" t="s">
         <v>2</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>200</v>
+        <v>188</v>
       </c>
       <c r="G22" s="10" t="s">
-        <v>198</v>
+        <v>186</v>
       </c>
       <c r="H22" s="11" t="s">
         <v>13</v>
@@ -2031,16 +2028,16 @@
     </row>
     <row r="23" spans="2:10" s="23" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="12" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="D23" s="24" t="s">
         <v>14</v>
       </c>
       <c r="E23" s="25" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>205</v>
+        <v>193</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="5"/>
@@ -2048,16 +2045,16 @@
     </row>
     <row r="24" spans="2:10" s="26" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="27" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="D24" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E24" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>206</v>
+        <v>194</v>
       </c>
       <c r="G24" s="29"/>
       <c r="H24" s="30"/>
@@ -2065,16 +2062,16 @@
     </row>
     <row r="25" spans="2:10" s="26" customFormat="1" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="27" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="D25" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E25" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G25" s="29"/>
       <c r="H25" s="30"/>
@@ -2082,16 +2079,16 @@
     </row>
     <row r="26" spans="2:10" s="26" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="27" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="D26" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E26" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="G26" s="29"/>
       <c r="H26" s="30"/>
@@ -2099,16 +2096,16 @@
     </row>
     <row r="27" spans="2:10" s="26" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="27" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="D27" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E27" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
       <c r="G27" s="29"/>
       <c r="H27" s="30"/>
@@ -2116,16 +2113,16 @@
     </row>
     <row r="28" spans="2:10" s="26" customFormat="1" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="27" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="D28" s="28" t="s">
         <v>14</v>
       </c>
       <c r="E28" s="29" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G28" s="29"/>
       <c r="H28" s="30"/>
@@ -2133,16 +2130,16 @@
     </row>
     <row r="29" spans="2:10" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="14" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="D29" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E29" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="6"/>
@@ -2150,16 +2147,16 @@
     </row>
     <row r="30" spans="2:10" ht="93.75" x14ac:dyDescent="0.25">
       <c r="C30" s="12" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="D30" s="24" t="s">
         <v>14</v>
       </c>
       <c r="E30" s="25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="5"/>
@@ -2167,16 +2164,16 @@
     </row>
     <row r="31" spans="2:10" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="14" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="D31" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E31" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="6"/>
@@ -2184,16 +2181,16 @@
     </row>
     <row r="32" spans="2:10" ht="93.75" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="D32" s="24" t="s">
         <v>14</v>
       </c>
       <c r="E32" s="25" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="F32" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="5"/>
@@ -2201,16 +2198,16 @@
     </row>
     <row r="33" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="14" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="D33" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E33" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="6"/>
@@ -2218,16 +2215,16 @@
     </row>
     <row r="34" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="14" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="D34" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E34" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F34" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="6"/>
@@ -2235,16 +2232,16 @@
     </row>
     <row r="35" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="14" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="D35" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E35" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F35" s="34" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="6"/>
@@ -2252,16 +2249,16 @@
     </row>
     <row r="36" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="14" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="D36" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E36" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F36" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="6"/>
@@ -2269,16 +2266,16 @@
     </row>
     <row r="37" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="14" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="D37" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E37" s="32" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="F37" s="34" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="6"/>
@@ -2286,16 +2283,16 @@
     </row>
     <row r="38" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="14" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="D38" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E38" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F38" s="34" t="s">
-        <v>214</v>
+        <v>202</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="6"/>
@@ -2303,16 +2300,16 @@
     </row>
     <row r="39" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="14" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="D39" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E39" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F39" s="34" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="6"/>
@@ -2320,16 +2317,16 @@
     </row>
     <row r="40" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="14" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="D40" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E40" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F40" s="34" t="s">
-        <v>213</v>
+        <v>201</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="6"/>
@@ -2337,16 +2334,16 @@
     </row>
     <row r="41" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="14" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="D41" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E41" s="32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="6"/>
@@ -2354,16 +2351,16 @@
     </row>
     <row r="42" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="14" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="D42" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E42" s="32" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>211</v>
+        <v>199</v>
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="6"/>
@@ -2371,16 +2368,16 @@
     </row>
     <row r="43" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="14" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="D43" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E43" s="32" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G43" s="15"/>
       <c r="H43" s="6"/>
@@ -2388,16 +2385,16 @@
     </row>
     <row r="44" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="14" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="D44" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E44" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G44" s="15"/>
       <c r="H44" s="6"/>
@@ -2405,16 +2402,16 @@
     </row>
     <row r="45" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="14" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="D45" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E45" s="32" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="F45" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G45" s="15"/>
       <c r="H45" s="6"/>
@@ -2422,16 +2419,16 @@
     </row>
     <row r="46" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="14" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="D46" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E46" s="32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F46" s="34" t="s">
-        <v>212</v>
+        <v>200</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="6"/>
@@ -2439,16 +2436,16 @@
     </row>
     <row r="47" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="14" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="D47" s="31" t="s">
         <v>14</v>
       </c>
       <c r="E47" s="32" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="F47" s="34" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="G47" s="15"/>
       <c r="H47" s="6"/>
@@ -2456,16 +2453,16 @@
     </row>
     <row r="48" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="14" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>98</v>
+        <v>250</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>99</v>
+        <v>251</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="G48" s="15"/>
       <c r="H48" s="6"/>
@@ -2473,14 +2470,14 @@
     </row>
     <row r="49" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C49" s="14" t="s">
-        <v>100</v>
-      </c>
-      <c r="D49" s="31" t="s">
-        <v>101</v>
-      </c>
-      <c r="E49" s="32"/>
+        <v>96</v>
+      </c>
+      <c r="D49" s="31"/>
+      <c r="E49" s="32" t="s">
+        <v>248</v>
+      </c>
       <c r="F49" s="34" t="s">
-        <v>207</v>
+        <v>195</v>
       </c>
       <c r="G49" s="15"/>
       <c r="H49" s="6"/>
@@ -2488,16 +2485,16 @@
     </row>
     <row r="50" spans="3:9" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C50" s="14" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
       <c r="D50" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E50" s="32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F50" s="31" t="s">
-        <v>202</v>
+        <v>190</v>
       </c>
       <c r="G50" s="15"/>
       <c r="H50" s="6"/>
@@ -2505,16 +2502,16 @@
     </row>
     <row r="51" spans="3:9" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C51" s="14" t="s">
-        <v>103</v>
+        <v>98</v>
       </c>
       <c r="D51" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E51" s="32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F51" s="31" t="s">
-        <v>204</v>
+        <v>192</v>
       </c>
       <c r="G51" s="15"/>
       <c r="H51" s="6"/>
@@ -2522,16 +2519,16 @@
     </row>
     <row r="52" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C52" s="14" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="D52" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E52" s="32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F52" s="31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G52" s="15"/>
       <c r="H52" s="6"/>
@@ -2539,16 +2536,16 @@
     </row>
     <row r="53" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="14" t="s">
-        <v>105</v>
+        <v>100</v>
       </c>
       <c r="D53" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E53" s="32" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F53" s="31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G53" s="15"/>
       <c r="H53" s="6"/>
@@ -2556,16 +2553,16 @@
     </row>
     <row r="54" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="14" t="s">
-        <v>106</v>
+        <v>101</v>
       </c>
       <c r="D54" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E54" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F54" s="31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="6"/>
@@ -2573,16 +2570,16 @@
     </row>
     <row r="55" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="14" t="s">
-        <v>107</v>
+        <v>102</v>
       </c>
       <c r="D55" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E55" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F55" s="31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G55" s="15"/>
       <c r="H55" s="6"/>
@@ -2590,16 +2587,16 @@
     </row>
     <row r="56" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="14" t="s">
-        <v>108</v>
+        <v>103</v>
       </c>
       <c r="D56" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E56" s="32" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="F56" s="31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G56" s="15"/>
       <c r="H56" s="6"/>
@@ -2607,16 +2604,16 @@
     </row>
     <row r="57" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="14" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
       <c r="D57" s="31" t="s">
         <v>15</v>
       </c>
       <c r="E57" s="32" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="F57" s="31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G57" s="15"/>
       <c r="H57" s="6"/>
@@ -2624,14 +2621,14 @@
     </row>
     <row r="58" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="14" t="s">
-        <v>110</v>
+        <v>105</v>
       </c>
       <c r="D58" s="31"/>
       <c r="E58" s="32" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="F58" s="31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G58" s="15"/>
       <c r="H58" s="6"/>
@@ -2639,14 +2636,14 @@
     </row>
     <row r="59" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="14" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="D59" s="31"/>
       <c r="E59" s="32" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="F59" s="31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G59" s="15"/>
       <c r="H59" s="6"/>
@@ -2654,14 +2651,14 @@
     </row>
     <row r="60" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="14" t="s">
-        <v>111</v>
-      </c>
-      <c r="D60" s="31" t="s">
-        <v>112</v>
-      </c>
-      <c r="E60" s="32"/>
+        <v>106</v>
+      </c>
+      <c r="D60" s="31"/>
+      <c r="E60" s="32" t="s">
+        <v>247</v>
+      </c>
       <c r="F60" s="31" t="s">
-        <v>203</v>
+        <v>191</v>
       </c>
       <c r="G60" s="15"/>
       <c r="H60" s="6"/>
@@ -2669,16 +2666,16 @@
     </row>
     <row r="61" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="14" t="s">
-        <v>35</v>
+        <v>33</v>
       </c>
       <c r="D61" s="31" t="s">
+        <v>32</v>
+      </c>
+      <c r="E61" s="32" t="s">
         <v>34</v>
       </c>
-      <c r="E61" s="32" t="s">
-        <v>36</v>
-      </c>
       <c r="F61" s="31" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="G61" s="15"/>
       <c r="H61" s="6"/>
@@ -2686,13 +2683,13 @@
     </row>
     <row r="62" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="14" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E62" s="32" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="F62" s="31"/>
       <c r="G62" s="15"/>
@@ -2701,16 +2698,16 @@
     </row>
     <row r="63" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C63" s="14" t="s">
-        <v>113</v>
+        <v>107</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E63" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F63" s="31" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="G63" s="15"/>
       <c r="H63" s="6"/>
@@ -2718,16 +2715,16 @@
     </row>
     <row r="64" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="14" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="D64" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E64" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F64" s="31" t="s">
-        <v>235</v>
+        <v>223</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="6"/>
@@ -2735,16 +2732,16 @@
     </row>
     <row r="65" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="14" t="s">
-        <v>115</v>
+        <v>109</v>
       </c>
       <c r="D65" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E65" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F65" s="31" t="s">
-        <v>236</v>
+        <v>224</v>
       </c>
       <c r="G65" s="15"/>
       <c r="H65" s="6"/>
@@ -2752,16 +2749,16 @@
     </row>
     <row r="66" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="14" t="s">
-        <v>116</v>
+        <v>110</v>
       </c>
       <c r="D66" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E66" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F66" s="31" t="s">
-        <v>237</v>
+        <v>225</v>
       </c>
       <c r="G66" s="15"/>
       <c r="H66" s="6"/>
@@ -2769,16 +2766,16 @@
     </row>
     <row r="67" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="14" t="s">
-        <v>117</v>
+        <v>111</v>
       </c>
       <c r="D67" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E67" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F67" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="G67" s="15"/>
       <c r="H67" s="6"/>
@@ -2786,16 +2783,16 @@
     </row>
     <row r="68" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="14" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="D68" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E68" s="32" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="F68" s="31" t="s">
-        <v>238</v>
+        <v>226</v>
       </c>
       <c r="G68" s="15"/>
       <c r="H68" s="6"/>
@@ -2803,16 +2800,16 @@
     </row>
     <row r="69" spans="3:9" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="14" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D69" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E69" s="32" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="F69" s="31" t="s">
-        <v>239</v>
+        <v>227</v>
       </c>
       <c r="G69" s="15"/>
       <c r="H69" s="6"/>
@@ -2820,16 +2817,16 @@
     </row>
     <row r="70" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C70" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D70" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E70" s="32" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="F70" s="31" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="G70" s="15"/>
       <c r="H70" s="6"/>
@@ -2837,16 +2834,16 @@
     </row>
     <row r="71" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C71" s="14" t="s">
-        <v>119</v>
+        <v>113</v>
       </c>
       <c r="D71" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E71" s="32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F71" s="31" t="s">
-        <v>241</v>
+        <v>229</v>
       </c>
       <c r="G71" s="15"/>
       <c r="H71" s="6"/>
@@ -2854,16 +2851,16 @@
     </row>
     <row r="72" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C72" s="14" t="s">
-        <v>120</v>
+        <v>114</v>
       </c>
       <c r="D72" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E72" s="32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F72" s="31" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="G72" s="15"/>
       <c r="H72" s="6"/>
@@ -2871,16 +2868,16 @@
     </row>
     <row r="73" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="14" t="s">
-        <v>121</v>
+        <v>115</v>
       </c>
       <c r="D73" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E73" s="32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="G73" s="15"/>
       <c r="H73" s="6"/>
@@ -2888,33 +2885,31 @@
     </row>
     <row r="74" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C74" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D74" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E74" s="32" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="F74" s="31" t="s">
-        <v>242</v>
+        <v>230</v>
       </c>
       <c r="G74" s="15"/>
       <c r="H74" s="6"/>
       <c r="I74" s="8"/>
     </row>
-    <row r="75" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="14" t="s">
-        <v>122</v>
-      </c>
-      <c r="D75" s="31" t="s">
-        <v>123</v>
-      </c>
+        <v>116</v>
+      </c>
+      <c r="D75" s="31"/>
       <c r="E75" s="32" t="s">
-        <v>44</v>
+        <v>252</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="6"/>
@@ -2922,16 +2917,16 @@
     </row>
     <row r="76" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C76" s="14" t="s">
-        <v>124</v>
+        <v>117</v>
       </c>
       <c r="D76" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E76" s="32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F76" s="31" t="s">
-        <v>244</v>
+        <v>232</v>
       </c>
       <c r="G76" s="15"/>
       <c r="H76" s="6"/>
@@ -2939,16 +2934,16 @@
     </row>
     <row r="77" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C77" s="14" t="s">
-        <v>125</v>
+        <v>118</v>
       </c>
       <c r="D77" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E77" s="32" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>240</v>
+        <v>228</v>
       </c>
       <c r="G77" s="15"/>
       <c r="H77" s="6"/>
@@ -2956,16 +2951,16 @@
     </row>
     <row r="78" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C78" s="14" t="s">
-        <v>126</v>
+        <v>119</v>
       </c>
       <c r="D78" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E78" s="32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="G78" s="15"/>
       <c r="H78" s="6"/>
@@ -2973,16 +2968,16 @@
     </row>
     <row r="79" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="14" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="D79" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E79" s="32" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>245</v>
+        <v>233</v>
       </c>
       <c r="G79" s="15"/>
       <c r="H79" s="6"/>
@@ -2990,16 +2985,16 @@
     </row>
     <row r="80" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C80" s="14" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="D80" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E80" s="32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G80" s="15"/>
       <c r="H80" s="6"/>
@@ -3007,16 +3002,16 @@
     </row>
     <row r="81" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C81" s="14" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="D81" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E81" s="32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F81" s="31" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="G81" s="15"/>
       <c r="H81" s="6"/>
@@ -3024,16 +3019,16 @@
     </row>
     <row r="82" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C82" s="14" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="D82" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E82" s="32" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F82" s="31" t="s">
-        <v>246</v>
+        <v>234</v>
       </c>
       <c r="G82" s="15"/>
       <c r="H82" s="6"/>
@@ -3041,16 +3036,16 @@
     </row>
     <row r="83" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C83" s="14" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="D83" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E83" s="32" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F83" s="31" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="6"/>
@@ -3058,16 +3053,16 @@
     </row>
     <row r="84" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C84" s="14" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="D84" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E84" s="32" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="F84" s="31" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="G84" s="15"/>
       <c r="H84" s="6"/>
@@ -3075,16 +3070,16 @@
     </row>
     <row r="85" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C85" s="14" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="D85" s="31" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="E85" s="32" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F85" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="G85" s="15"/>
       <c r="H85" s="6"/>
@@ -3092,14 +3087,14 @@
     </row>
     <row r="86" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C86" s="14" t="s">
-        <v>136</v>
-      </c>
-      <c r="D86" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="E86" s="32"/>
+        <v>129</v>
+      </c>
+      <c r="D86" s="31"/>
+      <c r="E86" s="32" t="s">
+        <v>249</v>
+      </c>
       <c r="F86" s="31" t="s">
-        <v>251</v>
+        <v>239</v>
       </c>
       <c r="G86" s="15"/>
       <c r="H86" s="6"/>
@@ -3107,14 +3102,14 @@
     </row>
     <row r="87" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C87" s="14" t="s">
-        <v>138</v>
-      </c>
-      <c r="D87" s="31" t="s">
-        <v>137</v>
-      </c>
-      <c r="E87" s="32"/>
+        <v>130</v>
+      </c>
+      <c r="D87" s="31"/>
+      <c r="E87" s="32" t="s">
+        <v>249</v>
+      </c>
       <c r="F87" s="31" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="G87" s="15"/>
       <c r="H87" s="6"/>
@@ -3122,14 +3117,14 @@
     </row>
     <row r="88" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C88" s="14" t="s">
-        <v>139</v>
-      </c>
-      <c r="D88" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="E88" s="32"/>
+        <v>131</v>
+      </c>
+      <c r="D88" s="31"/>
+      <c r="E88" s="32" t="s">
+        <v>246</v>
+      </c>
       <c r="F88" s="31" t="s">
-        <v>216</v>
+        <v>204</v>
       </c>
       <c r="G88" s="15"/>
       <c r="H88" s="6"/>
@@ -3137,14 +3132,14 @@
     </row>
     <row r="89" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C89" s="14" t="s">
-        <v>141</v>
-      </c>
-      <c r="D89" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="E89" s="32"/>
+        <v>132</v>
+      </c>
+      <c r="D89" s="31"/>
+      <c r="E89" s="32" t="s">
+        <v>246</v>
+      </c>
       <c r="F89" s="31" t="s">
-        <v>217</v>
+        <v>205</v>
       </c>
       <c r="G89" s="15"/>
       <c r="H89" s="6"/>
@@ -3152,14 +3147,14 @@
     </row>
     <row r="90" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C90" s="14" t="s">
-        <v>142</v>
-      </c>
-      <c r="D90" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="E90" s="32"/>
+        <v>133</v>
+      </c>
+      <c r="D90" s="31"/>
+      <c r="E90" s="32" t="s">
+        <v>246</v>
+      </c>
       <c r="F90" s="31" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="G90" s="15"/>
       <c r="H90" s="6"/>
@@ -3167,14 +3162,14 @@
     </row>
     <row r="91" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C91" s="14" t="s">
-        <v>143</v>
-      </c>
-      <c r="D91" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="E91" s="32"/>
+        <v>134</v>
+      </c>
+      <c r="D91" s="31"/>
+      <c r="E91" s="32" t="s">
+        <v>246</v>
+      </c>
       <c r="F91" s="31" t="s">
-        <v>219</v>
+        <v>207</v>
       </c>
       <c r="G91" s="15"/>
       <c r="H91" s="6"/>
@@ -3182,14 +3177,14 @@
     </row>
     <row r="92" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C92" s="14" t="s">
-        <v>144</v>
-      </c>
-      <c r="D92" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="E92" s="32"/>
+        <v>135</v>
+      </c>
+      <c r="D92" s="31"/>
+      <c r="E92" s="32" t="s">
+        <v>246</v>
+      </c>
       <c r="F92" s="31" t="s">
-        <v>220</v>
+        <v>208</v>
       </c>
       <c r="G92" s="15"/>
       <c r="H92" s="6"/>
@@ -3197,14 +3192,14 @@
     </row>
     <row r="93" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C93" s="14" t="s">
-        <v>145</v>
-      </c>
-      <c r="D93" s="31" t="s">
-        <v>140</v>
-      </c>
-      <c r="E93" s="32"/>
+        <v>136</v>
+      </c>
+      <c r="D93" s="31"/>
+      <c r="E93" s="32" t="s">
+        <v>246</v>
+      </c>
       <c r="F93" s="31" t="s">
-        <v>215</v>
+        <v>203</v>
       </c>
       <c r="G93" s="15"/>
       <c r="H93" s="6"/>
@@ -3212,14 +3207,14 @@
     </row>
     <row r="94" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C94" s="14" t="s">
-        <v>146</v>
-      </c>
-      <c r="D94" s="31" t="s">
-        <v>147</v>
-      </c>
-      <c r="E94" s="32"/>
+        <v>137</v>
+      </c>
+      <c r="D94" s="31"/>
+      <c r="E94" s="32" t="s">
+        <v>249</v>
+      </c>
       <c r="F94" s="31" t="s">
-        <v>243</v>
+        <v>231</v>
       </c>
       <c r="G94" s="15"/>
       <c r="H94" s="6"/>
@@ -3227,16 +3222,16 @@
     </row>
     <row r="95" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C95" s="14" t="s">
-        <v>148</v>
+        <v>138</v>
       </c>
       <c r="D95" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E95" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F95" s="31" t="s">
-        <v>252</v>
+        <v>240</v>
       </c>
       <c r="G95" s="15"/>
       <c r="H95" s="6"/>
@@ -3244,16 +3239,16 @@
     </row>
     <row r="96" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C96" s="14" t="s">
-        <v>149</v>
+        <v>139</v>
       </c>
       <c r="D96" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E96" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F96" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G96" s="15"/>
       <c r="H96" s="6"/>
@@ -3261,16 +3256,16 @@
     </row>
     <row r="97" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C97" s="14" t="s">
-        <v>150</v>
+        <v>140</v>
       </c>
       <c r="D97" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E97" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F97" s="31" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="G97" s="15"/>
       <c r="H97" s="6"/>
@@ -3278,16 +3273,16 @@
     </row>
     <row r="98" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C98" s="14" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="D98" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E98" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F98" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G98" s="15"/>
       <c r="H98" s="6"/>
@@ -3295,16 +3290,16 @@
     </row>
     <row r="99" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C99" s="14" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="D99" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E99" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F99" s="31" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="G99" s="15"/>
       <c r="H99" s="6"/>
@@ -3312,16 +3307,16 @@
     </row>
     <row r="100" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C100" s="14" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="D100" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E100" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F100" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="G100" s="15"/>
       <c r="H100" s="6"/>
@@ -3329,16 +3324,16 @@
     </row>
     <row r="101" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C101" s="14" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="D101" s="31" t="s">
-        <v>154</v>
+        <v>253</v>
       </c>
       <c r="E101" s="32" t="s">
-        <v>22</v>
+        <v>254</v>
       </c>
       <c r="F101" s="31" t="s">
-        <v>255</v>
+        <v>243</v>
       </c>
       <c r="G101" s="15"/>
       <c r="H101" s="6"/>
@@ -3346,16 +3341,16 @@
     </row>
     <row r="102" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C102" s="14" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="D102" s="31" t="s">
-        <v>154</v>
+        <v>253</v>
       </c>
       <c r="E102" s="32" t="s">
-        <v>21</v>
+        <v>255</v>
       </c>
       <c r="F102" s="31" t="s">
-        <v>256</v>
+        <v>244</v>
       </c>
       <c r="G102" s="15"/>
       <c r="H102" s="6"/>
@@ -3363,16 +3358,16 @@
     </row>
     <row r="103" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C103" s="14" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="D103" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E103" s="32" t="s">
         <v>17</v>
       </c>
       <c r="F103" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G103" s="15"/>
       <c r="H103" s="6"/>
@@ -3380,16 +3375,16 @@
     </row>
     <row r="104" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C104" s="14" t="s">
-        <v>155</v>
+        <v>144</v>
       </c>
       <c r="D104" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E104" s="32" t="s">
         <v>18</v>
       </c>
       <c r="F104" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G104" s="15"/>
       <c r="H104" s="6"/>
@@ -3397,16 +3392,16 @@
     </row>
     <row r="105" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C105" s="14" t="s">
-        <v>156</v>
+        <v>145</v>
       </c>
       <c r="D105" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E105" s="32" t="s">
         <v>18</v>
       </c>
       <c r="F105" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G105" s="15"/>
       <c r="H105" s="6"/>
@@ -3414,16 +3409,16 @@
     </row>
     <row r="106" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C106" s="14" t="s">
-        <v>157</v>
+        <v>146</v>
       </c>
       <c r="D106" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E106" s="32" t="s">
         <v>19</v>
       </c>
       <c r="F106" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G106" s="15"/>
       <c r="H106" s="6"/>
@@ -3431,16 +3426,16 @@
     </row>
     <row r="107" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C107" s="14" t="s">
-        <v>158</v>
+        <v>147</v>
       </c>
       <c r="D107" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E107" s="32" t="s">
         <v>19</v>
       </c>
       <c r="F107" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G107" s="15"/>
       <c r="H107" s="6"/>
@@ -3448,16 +3443,16 @@
     </row>
     <row r="108" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C108" s="14" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="D108" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E108" s="32" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F108" s="31" t="s">
-        <v>257</v>
+        <v>245</v>
       </c>
       <c r="G108" s="15"/>
       <c r="H108" s="6"/>
@@ -3465,16 +3460,16 @@
     </row>
     <row r="109" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C109" s="14" t="s">
-        <v>160</v>
+        <v>149</v>
       </c>
       <c r="D109" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E109" s="32" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F109" s="31" t="s">
-        <v>218</v>
+        <v>206</v>
       </c>
       <c r="G109" s="15"/>
       <c r="H109" s="6"/>
@@ -3482,16 +3477,16 @@
     </row>
     <row r="110" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C110" s="14" t="s">
-        <v>161</v>
+        <v>150</v>
       </c>
       <c r="D110" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E110" s="32" t="s">
-        <v>159</v>
+        <v>148</v>
       </c>
       <c r="F110" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G110" s="15"/>
       <c r="H110" s="6"/>
@@ -3499,16 +3494,16 @@
     </row>
     <row r="111" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="14" t="s">
-        <v>162</v>
+        <v>151</v>
       </c>
       <c r="D111" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E111" s="32" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="F111" s="31" t="s">
-        <v>247</v>
+        <v>235</v>
       </c>
       <c r="G111" s="15"/>
       <c r="H111" s="6"/>
@@ -3516,16 +3511,16 @@
     </row>
     <row r="112" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C112" s="14" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="D112" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E112" s="32" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="F112" s="31" t="s">
-        <v>249</v>
+        <v>237</v>
       </c>
       <c r="G112" s="15"/>
       <c r="H112" s="6"/>
@@ -3533,16 +3528,16 @@
     </row>
     <row r="113" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C113" s="14" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
       <c r="D113" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E113" s="32" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="F113" s="31" t="s">
-        <v>248</v>
+        <v>236</v>
       </c>
       <c r="G113" s="15"/>
       <c r="H113" s="6"/>
@@ -3550,16 +3545,16 @@
     </row>
     <row r="114" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C114" s="14" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
       <c r="D114" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E114" s="32" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="F114" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G114" s="15"/>
       <c r="H114" s="6"/>
@@ -3567,16 +3562,16 @@
     </row>
     <row r="115" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C115" s="14" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
       <c r="D115" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E115" s="32" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="F115" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="G115" s="15"/>
       <c r="H115" s="6"/>
@@ -3584,16 +3579,16 @@
     </row>
     <row r="116" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C116" s="14" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="D116" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E116" s="32" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="F116" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="G116" s="15"/>
       <c r="H116" s="6"/>
@@ -3601,16 +3596,16 @@
     </row>
     <row r="117" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C117" s="14" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="D117" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E117" s="32" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="F117" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="G117" s="15"/>
       <c r="H117" s="6"/>
@@ -3618,16 +3613,16 @@
     </row>
     <row r="118" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C118" s="14" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="D118" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E118" s="32" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="F118" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="G118" s="15"/>
       <c r="H118" s="6"/>
@@ -3635,16 +3630,16 @@
     </row>
     <row r="119" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C119" s="14" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="D119" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E119" s="32" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="F119" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="G119" s="15"/>
       <c r="H119" s="6"/>
@@ -3652,16 +3647,16 @@
     </row>
     <row r="120" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C120" s="14" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="D120" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E120" s="32" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
       <c r="F120" s="31" t="s">
-        <v>250</v>
+        <v>238</v>
       </c>
       <c r="G120" s="15"/>
       <c r="H120" s="6"/>
@@ -3669,16 +3664,16 @@
     </row>
     <row r="121" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C121" s="14" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="D121" s="31" t="s">
-        <v>154</v>
+        <v>253</v>
       </c>
       <c r="E121" s="32" t="s">
-        <v>21</v>
+        <v>255</v>
       </c>
       <c r="F121" s="31" t="s">
-        <v>199</v>
+        <v>187</v>
       </c>
       <c r="G121" s="15"/>
       <c r="H121" s="6"/>
@@ -3686,16 +3681,16 @@
     </row>
     <row r="122" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C122" s="14" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="D122" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E122" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F122" s="31" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="G122" s="15"/>
       <c r="H122" s="6"/>
@@ -3703,16 +3698,16 @@
     </row>
     <row r="123" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C123" s="14" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="D123" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E123" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F123" s="31" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="G123" s="15"/>
       <c r="H123" s="6"/>
@@ -3720,16 +3715,16 @@
     </row>
     <row r="124" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C124" s="14" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="D124" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E124" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F124" s="31" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="G124" s="15"/>
       <c r="H124" s="6"/>
@@ -3737,16 +3732,16 @@
     </row>
     <row r="125" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C125" s="14" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="D125" s="31" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="E125" s="32" t="s">
         <v>20</v>
       </c>
       <c r="F125" s="31" t="s">
-        <v>254</v>
+        <v>242</v>
       </c>
       <c r="G125" s="15"/>
       <c r="H125" s="6"/>
@@ -3754,14 +3749,14 @@
     </row>
     <row r="126" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C126" s="14" t="s">
-        <v>182</v>
-      </c>
-      <c r="D126" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="E126" s="32"/>
+        <v>171</v>
+      </c>
+      <c r="D126" s="31"/>
+      <c r="E126" s="32" t="s">
+        <v>246</v>
+      </c>
       <c r="F126" s="31" t="s">
-        <v>221</v>
+        <v>209</v>
       </c>
       <c r="G126" s="15"/>
       <c r="H126" s="6"/>
@@ -3769,14 +3764,14 @@
     </row>
     <row r="127" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C127" s="14" t="s">
-        <v>184</v>
-      </c>
-      <c r="D127" s="31" t="s">
-        <v>183</v>
-      </c>
-      <c r="E127" s="32"/>
+        <v>172</v>
+      </c>
+      <c r="D127" s="31"/>
+      <c r="E127" s="32" t="s">
+        <v>246</v>
+      </c>
       <c r="F127" s="31" t="s">
-        <v>222</v>
+        <v>210</v>
       </c>
       <c r="G127" s="15"/>
       <c r="H127" s="6"/>
@@ -3784,16 +3779,16 @@
     </row>
     <row r="128" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C128" s="14" t="s">
-        <v>185</v>
+        <v>173</v>
       </c>
       <c r="D128" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E128" s="32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F128" s="31" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G128" s="15"/>
       <c r="H128" s="6"/>
@@ -3801,16 +3796,16 @@
     </row>
     <row r="129" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C129" s="14" t="s">
-        <v>186</v>
+        <v>174</v>
       </c>
       <c r="D129" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E129" s="32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F129" s="31" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="G129" s="15"/>
       <c r="H129" s="6"/>
@@ -3818,16 +3813,16 @@
     </row>
     <row r="130" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C130" s="14" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="D130" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E130" s="32" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="F130" s="31" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="G130" s="15"/>
       <c r="H130" s="6"/>
@@ -3835,16 +3830,16 @@
     </row>
     <row r="131" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C131" s="14" t="s">
-        <v>188</v>
+        <v>176</v>
       </c>
       <c r="D131" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E131" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F131" s="31" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
       <c r="G131" s="15"/>
       <c r="H131" s="6"/>
@@ -3852,16 +3847,16 @@
     </row>
     <row r="132" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C132" s="14" t="s">
-        <v>189</v>
+        <v>177</v>
       </c>
       <c r="D132" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E132" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F132" s="31" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="G132" s="15"/>
       <c r="H132" s="6"/>
@@ -3869,16 +3864,16 @@
     </row>
     <row r="133" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C133" s="14" t="s">
-        <v>190</v>
+        <v>178</v>
       </c>
       <c r="D133" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E133" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F133" s="31" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="G133" s="15"/>
       <c r="H133" s="6"/>
@@ -3886,16 +3881,16 @@
     </row>
     <row r="134" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C134" s="14" t="s">
-        <v>191</v>
+        <v>179</v>
       </c>
       <c r="D134" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F134" s="31" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="G134" s="15"/>
       <c r="H134" s="6"/>
@@ -3903,16 +3898,16 @@
     </row>
     <row r="135" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C135" s="14" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="D135" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E135" s="32" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="F135" s="31" t="s">
-        <v>223</v>
+        <v>211</v>
       </c>
       <c r="G135" s="15"/>
       <c r="H135" s="6"/>
@@ -3920,16 +3915,16 @@
     </row>
     <row r="136" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C136" s="14" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="D136" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E136" s="32" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="F136" s="31" t="s">
-        <v>201</v>
+        <v>189</v>
       </c>
       <c r="G136" s="15"/>
       <c r="H136" s="6"/>
@@ -3937,13 +3932,13 @@
     </row>
     <row r="137" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C137" s="14" t="s">
-        <v>193</v>
+        <v>181</v>
       </c>
       <c r="D137" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E137" s="32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F137" s="31"/>
       <c r="G137" s="15"/>
@@ -3952,13 +3947,13 @@
     </row>
     <row r="138" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C138" s="14" t="s">
-        <v>194</v>
+        <v>182</v>
       </c>
       <c r="D138" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E138" s="32" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="F138" s="31"/>
       <c r="G138" s="15"/>
@@ -3967,13 +3962,13 @@
     </row>
     <row r="139" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C139" s="14" t="s">
-        <v>195</v>
+        <v>183</v>
       </c>
       <c r="D139" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E139" s="32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F139" s="31"/>
       <c r="G139" s="15"/>
@@ -3982,13 +3977,13 @@
     </row>
     <row r="140" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C140" s="14" t="s">
-        <v>196</v>
+        <v>184</v>
       </c>
       <c r="D140" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E140" s="32" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="F140" s="31"/>
       <c r="G140" s="15"/>
@@ -3997,13 +3992,13 @@
     </row>
     <row r="141" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C141" s="14" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="D141" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E141" s="32" t="s">
-        <v>197</v>
+        <v>185</v>
       </c>
       <c r="F141" s="31"/>
       <c r="G141" s="15"/>
@@ -4012,13 +4007,13 @@
     </row>
     <row r="142" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C142" s="14" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="D142" s="31" t="s">
         <v>16</v>
       </c>
       <c r="E142" s="32" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="F142" s="31"/>
       <c r="G142" s="15"/>

</xml_diff>

<commit_message>
Modifiey design id u on quality assurance demand
Modifiey design id u on quality assurance demand
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="520" uniqueCount="273">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="275">
   <si>
     <t>Author</t>
   </si>
@@ -630,71 +630,10 @@
 Bank_SYS_HLD_admin_003</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_ADMIN_001
-Bank_Sys_DM_CST_001
-Bank_SYS_HLD_client_002
-Bank_SYS_HLD_admin_002
-BANK_SYS_DD_CST_001
-BANK_SYS_DD_Admin_001
-Bank_SYS_DSN_001</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_001
-Bank_Sys_DM_CST_001
-Bank_SYS_HLD_client_002
-Bank_SYS_HLD_admin_002
-Bank_SYS_DSN_001</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_001
-Bank_Sys_DM_CST_001
-Bank_SYS_HLD_client_002
-Bank_SYS_HLD_admin_002
-BANK_SYS_DD_ CST _002
-BANK_SYS_DD_ Admin _002
-Bank_SYS_DSN_001</t>
-  </si>
-  <si>
     <t>Bank_Sys_DM_ADMIN_002
 Bank_Sys_DM_CST_002
 Bank_SYS_HLD_client_001
 Bank_SYS_HLD_admin_001
-BANK_SYS_DD_CST_001
-BANK_SYS_DD_Admin_001
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_HLD_admin_001
-BANK_SYS_DD_ CST _002
-BANK_SYS_DD_ Admin _002
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_HLD_admin_001
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_HLD_admin_001
-BANK_SYS_DD_ CST _003
-BANK_SYS_DD_ Admin _005
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_HLD_admin_001
-BANK_SYS_DD_ CST _004
-BANK_SYS_DD_ Admin _004
 Bank_SYS_DSN_002</t>
   </si>
   <si>
@@ -716,65 +655,10 @@
 Bank_Sys_DM_CST_002
 Bank_SYS_HLD_client_001
 Bank_SYS_HLD_admin_001
-Bank_SYS_DSN_003</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_HLD_admin_001
 Bank_SYS_DSN_004</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_DSN_004</t>
-  </si>
-  <si>
     <t>Bank_SYS_DSN_005</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_006</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_005
-Bank_SYS_DSN_006</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_005
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_005
-Bank_SYS_DSN_010</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_010</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_005
-BANK_SYS_DD_ Admin _006
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_003                                                   
-Bank_SYS_HLD_admin_004
-BANK_SYS_DD_ Admin _007
-Bank_SYS_DSN_015</t>
   </si>
   <si>
     <t xml:space="preserve">     Bank_Sys_DM_ADMIN_003                                              
@@ -782,57 +666,281 @@
 BANK_SYS_DD_ Admin _007</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_ADMIN_004
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_004
-Bank_Sys_DM_ADMIN_007
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_005
-Bank_Sys_DM_ADMIN_006
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_008
-Bank_SYS_HLD_admin_006
-Bank_SYS_HLD_admin_005
-BANK_SYS_DD_ Admin _008
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_009
-Bank_SYS_HLD_admin_003
-BANK_SYS_DD_ Admin _006
-Bank_SYS_DSN_015</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_003
-Bank_SYS_HLD_client_001
-Bank_SYS_HLD_admin_001
-Bank_SYS_DSN_004
-Bank_SYS_DSN_005</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                      
 Bank_SYS_DSN_005</t>
   </si>
   <si>
+    <t xml:space="preserve">                                                      </t>
+  </si>
+  <si>
     <t xml:space="preserve">                                                      
-BANK_SYS_DD_account_001</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_006
-Bank_Sys_DM_CST_004
-Bank_SYS_DSN_006</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_006
+Bank_Sys_DM_CST_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_007
+Bank_SYS_DSN_005</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q46</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q48</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q49</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK_SYS_CR_001
+</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q40
+BANK_SYS_SIQ_Q47</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q22
+BANK_SYS_SIQ_Q47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BANK_SYS_CR_004
+</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q44
+BANK_SYS_SIQ_Q47</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q43
+BANK_SYS_SIQ_Q47</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Reg_R028</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Reg_R029</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_Reg_R030</t>
+  </si>
+  <si>
+    <t>BANK_SYS_CR_001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_CR_002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q56</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q57</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R035</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R036</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R037</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R038</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SRS_PT_R039</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q51</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q52</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q53</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q54</t>
+  </si>
+  <si>
+    <t>BANK_SYS_SIQ_Q55</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_004</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_005</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_admin_005
+Bank_SYS_HLD_admin_006
+Bank_Sys_DM_ADMIN_007
+Bank_Sys_DM_ADMIN_008</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_002
+Bank_Sys_DM_CST_003</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_004</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_004
+Bank_Sys_DM_CST_006</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_006
+Bank_Sys_DM_CST_007</t>
+  </si>
+  <si>
+    <t>BANK_SYS_ ERD _ CST _005</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+BANK_SYS_DD_account_001
+BANK_SYS_ ERD _ account_001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_ ERD _ account_002</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_admin_003
+Bank_Sys_DM_ADMIN_009
+BANK_SYS_ ERD _ account_004
+BANK_SYS_ ERD _ Admin _006</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_admin_004
+Bank_Sys_DM_ADMIN_003
+BANK_SYS_ ERD _ Admin _007
+BANK_SYS_ ERD _ account_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">       BANK_SYS_ ERD _ TR _004                                               </t>
+  </si>
+  <si>
+    <t>BANK_SYS_ERD_CST_001
+Bank_SYS_DSN_001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_ ERD _ CST _002
+Bank_SYS_DSN_001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_ ERD _ CST _005Bank_SYS_DSN_001</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_ERD_CST_001
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_ ERD _ CST _002
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_ ERD _ CST _003
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_ ERD _ CST _004
+Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_003</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_007
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_006
+BANK_SYS_DD_ PR _002
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_006
+Bank_Sys_DM_ADMIN_007                                                      
+BANK_SYS_DD_ PR _002
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_006                                                      
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_007
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_007
+BANK_SYS_DD_ Trans _003
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_007
+BANK_SYS_DD_ account _003
+BANK_SYS_DD_Trans_001
+BANK_SYS_DD_PR_001
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_007
+BANK_SYS_DD_ Trans _002
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_SYS_DSN_005
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+Bank_SYS_HLD_client_006
+BANK_SYS_DD_ PR _003
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_ADMIN_004
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_ADMIN_004
+Bank_Sys_DM_ADMIN_007
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_ADMIN_005
+BANK_SYS_DD_ Admin _006
+                                                 </t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_003
+Bank_Sys_DM_ADMIN_006
 Bank_Sys_DM_CST_005
-Bank_SYS_HLD_client_003
 Bank_SYS_DSN_006</t>
   </si>
   <si>
@@ -841,209 +949,23 @@
 Bank_SYS_DSN_006</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_005
-Bank_SYS_HLD_client_004
-BANK_SYS_DD_TR_001
-Bank_SYS_DSN_006</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-Bank_Sys_DM_CST_006
-Bank_SYS_HLD_client_004
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-Bank_SYS_HLD_client_005
-Bank_SYS_HLD_client_006
-BANK_SYS_DD_ TR _002
-BANK_SYS_DD_ PR _002
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                      
 Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">             Bank_SYS_HLD_client_007                                         
+                                                 </t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Bank_SYS_DSN_006                                       </t>
   </si>
   <si>
     <t xml:space="preserve">                                                      
-</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-Bank_SYS_HLD_client_003
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-Bank_SYS_HLD_client_006
-BANK_SYS_DD_ PR _003
-Bank_SYS_DSN_014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-Bank_SYS_DSN_014</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-Bank_Sys_DM_CST_006</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_006
-BANK_SYS_DD_ PR _002
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_006                                                      
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_006
-Bank_Sys_DM_ADMIN_007                                                      
-BANK_SYS_DD_ PR _002
-Bank_SYS_DSN_007
-Bank_SYS_DSN_008
-Bank_SYS_DSN_009</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-Bank_SYS_DSN_010</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-Bank_SYS_DSN_005</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-BANK_SYS_DD_ Trans _003
-Bank_SYS_DSN_010</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-BANK_SYS_DD_ account _003
-BANK_SYS_DD_Trans_001
-BANK_SYS_DD_PR_001
-Bank_SYS_DSN_010</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-BANK_SYS_DD_ Trans _002
-Bank_SYS_DSN_010</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-Bank_SYS_DSN_012</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-Bank_SYS_DSN_013</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-Bank_Sys_DM_CST_007
-BANK_SYS_DD_ account _002
-Bank_SYS_DSN_011</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q46</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q48</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q49</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BANK_SYS_CR_001
-</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q40
-BANK_SYS_SIQ_Q47</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q22
-BANK_SYS_SIQ_Q47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BANK_SYS_CR_004
-</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q44
-BANK_SYS_SIQ_Q47</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q43
-BANK_SYS_SIQ_Q47</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Reg_R028</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Reg_R029</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_Reg_R030</t>
-  </si>
-  <si>
-    <t>BANK_SYS_CR_001</t>
-  </si>
-  <si>
-    <t>BANK_SYS_CR_002</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q56</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q57</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_PT_R035</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_PT_R036</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_PT_R037</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_PT_R038</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SRS_PT_R039</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q51</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q52</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q53</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q54</t>
-  </si>
-  <si>
-    <t>BANK_SYS_SIQ_Q55</t>
+Bank_SYS_HLD_client_008</t>
   </si>
 </sst>
 </file>
@@ -1577,36 +1499,6 @@
     <xf numFmtId="0" fontId="7" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="7" fillId="2" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1645,6 +1537,36 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1930,8 +1852,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L150"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A95" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="E98" sqref="E98:E102"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F75" sqref="F75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -1941,7 +1863,7 @@
     <col min="3" max="3" width="34.28515625" customWidth="1"/>
     <col min="4" max="4" width="26.28515625" style="33" customWidth="1"/>
     <col min="5" max="5" width="27.7109375" style="33" customWidth="1"/>
-    <col min="6" max="6" width="35" style="33" customWidth="1"/>
+    <col min="6" max="6" width="38.42578125" style="33" customWidth="1"/>
     <col min="7" max="7" width="25.5703125" customWidth="1"/>
     <col min="8" max="8" width="20.28515625" customWidth="1"/>
     <col min="9" max="9" width="18.28515625" customWidth="1"/>
@@ -1949,103 +1871,103 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="39" t="s">
+      <c r="A1" s="53" t="s">
         <v>11</v>
       </c>
-      <c r="B1" s="39"/>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="39"/>
-      <c r="F1" s="39"/>
-      <c r="G1" s="39"/>
-      <c r="H1" s="39"/>
-      <c r="I1" s="39"/>
-      <c r="J1" s="39"/>
-      <c r="K1" s="39"/>
-      <c r="L1" s="39"/>
+      <c r="B1" s="53"/>
+      <c r="C1" s="53"/>
+      <c r="D1" s="53"/>
+      <c r="E1" s="53"/>
+      <c r="F1" s="53"/>
+      <c r="G1" s="53"/>
+      <c r="H1" s="53"/>
+      <c r="I1" s="53"/>
+      <c r="J1" s="53"/>
+      <c r="K1" s="53"/>
+      <c r="L1" s="53"/>
     </row>
     <row r="2" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="39"/>
-      <c r="B2" s="39"/>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
+      <c r="A2" s="53"/>
+      <c r="B2" s="53"/>
+      <c r="C2" s="53"/>
+      <c r="D2" s="53"/>
+      <c r="E2" s="53"/>
+      <c r="F2" s="53"/>
+      <c r="G2" s="53"/>
+      <c r="H2" s="53"/>
+      <c r="I2" s="53"/>
+      <c r="J2" s="53"/>
+      <c r="K2" s="53"/>
+      <c r="L2" s="53"/>
     </row>
     <row r="3" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="39"/>
-      <c r="B3" s="39"/>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
-      <c r="G3" s="39"/>
-      <c r="H3" s="39"/>
-      <c r="I3" s="39"/>
-      <c r="J3" s="39"/>
-      <c r="K3" s="39"/>
-      <c r="L3" s="39"/>
+      <c r="A3" s="53"/>
+      <c r="B3" s="53"/>
+      <c r="C3" s="53"/>
+      <c r="D3" s="53"/>
+      <c r="E3" s="53"/>
+      <c r="F3" s="53"/>
+      <c r="G3" s="53"/>
+      <c r="H3" s="53"/>
+      <c r="I3" s="53"/>
+      <c r="J3" s="53"/>
+      <c r="K3" s="53"/>
+      <c r="L3" s="53"/>
     </row>
     <row r="4" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="39"/>
-      <c r="B4" s="39"/>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
-      <c r="G4" s="39"/>
-      <c r="H4" s="39"/>
-      <c r="I4" s="39"/>
-      <c r="J4" s="39"/>
-      <c r="K4" s="39"/>
-      <c r="L4" s="39"/>
+      <c r="A4" s="53"/>
+      <c r="B4" s="53"/>
+      <c r="C4" s="53"/>
+      <c r="D4" s="53"/>
+      <c r="E4" s="53"/>
+      <c r="F4" s="53"/>
+      <c r="G4" s="53"/>
+      <c r="H4" s="53"/>
+      <c r="I4" s="53"/>
+      <c r="J4" s="53"/>
+      <c r="K4" s="53"/>
+      <c r="L4" s="53"/>
     </row>
     <row r="5" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="39"/>
-      <c r="B5" s="39"/>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
-      <c r="G5" s="39"/>
-      <c r="H5" s="39"/>
-      <c r="I5" s="39"/>
-      <c r="J5" s="39"/>
-      <c r="K5" s="39"/>
-      <c r="L5" s="39"/>
+      <c r="A5" s="53"/>
+      <c r="B5" s="53"/>
+      <c r="C5" s="53"/>
+      <c r="D5" s="53"/>
+      <c r="E5" s="53"/>
+      <c r="F5" s="53"/>
+      <c r="G5" s="53"/>
+      <c r="H5" s="53"/>
+      <c r="I5" s="53"/>
+      <c r="J5" s="53"/>
+      <c r="K5" s="53"/>
+      <c r="L5" s="53"/>
     </row>
     <row r="6" spans="1:12" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="39"/>
-      <c r="B6" s="39"/>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
-      <c r="G6" s="39"/>
-      <c r="H6" s="39"/>
-      <c r="I6" s="39"/>
-      <c r="J6" s="39"/>
-      <c r="K6" s="39"/>
-      <c r="L6" s="39"/>
+      <c r="A6" s="53"/>
+      <c r="B6" s="53"/>
+      <c r="C6" s="53"/>
+      <c r="D6" s="53"/>
+      <c r="E6" s="53"/>
+      <c r="F6" s="53"/>
+      <c r="G6" s="53"/>
+      <c r="H6" s="53"/>
+      <c r="I6" s="53"/>
+      <c r="J6" s="53"/>
+      <c r="K6" s="53"/>
+      <c r="L6" s="53"/>
     </row>
     <row r="7" spans="1:12" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A7" s="1"/>
-      <c r="B7" s="40" t="s">
+      <c r="B7" s="54" t="s">
         <v>5</v>
       </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
-      <c r="G7" s="40"/>
-      <c r="H7" s="40"/>
-      <c r="I7" s="40"/>
+      <c r="C7" s="54"/>
+      <c r="D7" s="54"/>
+      <c r="E7" s="54"/>
+      <c r="F7" s="54"/>
+      <c r="G7" s="54"/>
+      <c r="H7" s="54"/>
+      <c r="I7" s="54"/>
       <c r="J7" s="1"/>
     </row>
     <row r="8" spans="1:12" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2058,20 +1980,20 @@
       <c r="D8" s="10" t="s">
         <v>1</v>
       </c>
-      <c r="E8" s="41" t="s">
+      <c r="E8" s="55" t="s">
         <v>3</v>
       </c>
-      <c r="F8" s="41"/>
+      <c r="F8" s="55"/>
       <c r="G8" s="19" t="s">
         <v>7</v>
       </c>
       <c r="H8" s="19" t="s">
         <v>8</v>
       </c>
-      <c r="I8" s="41" t="s">
+      <c r="I8" s="55" t="s">
         <v>9</v>
       </c>
-      <c r="J8" s="42"/>
+      <c r="J8" s="56"/>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="3" t="s">
@@ -2083,14 +2005,14 @@
       <c r="D9" s="21" t="s">
         <v>4</v>
       </c>
-      <c r="E9" s="43" t="s">
+      <c r="E9" s="57" t="s">
         <v>12</v>
       </c>
-      <c r="F9" s="43"/>
+      <c r="F9" s="57"/>
       <c r="G9" s="20"/>
       <c r="H9" s="20"/>
-      <c r="I9" s="43"/>
-      <c r="J9" s="44"/>
+      <c r="I9" s="57"/>
+      <c r="J9" s="58"/>
     </row>
     <row r="10" spans="1:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="3" t="s">
@@ -2102,121 +2024,121 @@
       <c r="D10" s="22">
         <v>43529</v>
       </c>
-      <c r="E10" s="35" t="s">
+      <c r="E10" s="49" t="s">
         <v>62</v>
       </c>
-      <c r="F10" s="36"/>
+      <c r="F10" s="50"/>
       <c r="G10" s="17" t="s">
         <v>61</v>
       </c>
       <c r="H10" s="18">
         <v>43529</v>
       </c>
-      <c r="I10" s="35" t="s">
+      <c r="I10" s="49" t="s">
         <v>63</v>
       </c>
-      <c r="J10" s="37"/>
+      <c r="J10" s="51"/>
     </row>
     <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B13" s="38" t="s">
+      <c r="B13" s="52" t="s">
         <v>64</v>
       </c>
-      <c r="C13" s="38"/>
-      <c r="D13" s="38"/>
-      <c r="E13" s="38"/>
-      <c r="F13" s="38"/>
-      <c r="G13" s="38"/>
-      <c r="H13" s="38"/>
-      <c r="I13" s="38"/>
-      <c r="J13" s="38"/>
+      <c r="C13" s="52"/>
+      <c r="D13" s="52"/>
+      <c r="E13" s="52"/>
+      <c r="F13" s="52"/>
+      <c r="G13" s="52"/>
+      <c r="H13" s="52"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="52"/>
     </row>
     <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B14" s="38"/>
-      <c r="C14" s="38"/>
-      <c r="D14" s="38"/>
-      <c r="E14" s="38"/>
-      <c r="F14" s="38"/>
-      <c r="G14" s="38"/>
-      <c r="H14" s="38"/>
-      <c r="I14" s="38"/>
-      <c r="J14" s="38"/>
+      <c r="B14" s="52"/>
+      <c r="C14" s="52"/>
+      <c r="D14" s="52"/>
+      <c r="E14" s="52"/>
+      <c r="F14" s="52"/>
+      <c r="G14" s="52"/>
+      <c r="H14" s="52"/>
+      <c r="I14" s="52"/>
+      <c r="J14" s="52"/>
     </row>
     <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B15" s="38"/>
-      <c r="C15" s="38"/>
-      <c r="D15" s="38"/>
-      <c r="E15" s="38"/>
-      <c r="F15" s="38"/>
-      <c r="G15" s="38"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="38"/>
-      <c r="J15" s="38"/>
+      <c r="B15" s="52"/>
+      <c r="C15" s="52"/>
+      <c r="D15" s="52"/>
+      <c r="E15" s="52"/>
+      <c r="F15" s="52"/>
+      <c r="G15" s="52"/>
+      <c r="H15" s="52"/>
+      <c r="I15" s="52"/>
+      <c r="J15" s="52"/>
     </row>
     <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="B16" s="38"/>
-      <c r="C16" s="38"/>
-      <c r="D16" s="38"/>
-      <c r="E16" s="38"/>
-      <c r="F16" s="38"/>
-      <c r="G16" s="38"/>
-      <c r="H16" s="38"/>
-      <c r="I16" s="38"/>
-      <c r="J16" s="38"/>
+      <c r="B16" s="52"/>
+      <c r="C16" s="52"/>
+      <c r="D16" s="52"/>
+      <c r="E16" s="52"/>
+      <c r="F16" s="52"/>
+      <c r="G16" s="52"/>
+      <c r="H16" s="52"/>
+      <c r="I16" s="52"/>
+      <c r="J16" s="52"/>
     </row>
     <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B17" s="38"/>
-      <c r="C17" s="38"/>
-      <c r="D17" s="38"/>
-      <c r="E17" s="38"/>
-      <c r="F17" s="38"/>
-      <c r="G17" s="38"/>
-      <c r="H17" s="38"/>
-      <c r="I17" s="38"/>
-      <c r="J17" s="38"/>
+      <c r="B17" s="52"/>
+      <c r="C17" s="52"/>
+      <c r="D17" s="52"/>
+      <c r="E17" s="52"/>
+      <c r="F17" s="52"/>
+      <c r="G17" s="52"/>
+      <c r="H17" s="52"/>
+      <c r="I17" s="52"/>
+      <c r="J17" s="52"/>
     </row>
     <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B18" s="38"/>
-      <c r="C18" s="38"/>
-      <c r="D18" s="38"/>
-      <c r="E18" s="38"/>
-      <c r="F18" s="38"/>
-      <c r="G18" s="38"/>
-      <c r="H18" s="38"/>
-      <c r="I18" s="38"/>
-      <c r="J18" s="38"/>
+      <c r="B18" s="52"/>
+      <c r="C18" s="52"/>
+      <c r="D18" s="52"/>
+      <c r="E18" s="52"/>
+      <c r="F18" s="52"/>
+      <c r="G18" s="52"/>
+      <c r="H18" s="52"/>
+      <c r="I18" s="52"/>
+      <c r="J18" s="52"/>
     </row>
     <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B19" s="38"/>
-      <c r="C19" s="38"/>
-      <c r="D19" s="38"/>
-      <c r="E19" s="38"/>
-      <c r="F19" s="38"/>
-      <c r="G19" s="38"/>
-      <c r="H19" s="38"/>
-      <c r="I19" s="38"/>
-      <c r="J19" s="38"/>
+      <c r="B19" s="52"/>
+      <c r="C19" s="52"/>
+      <c r="D19" s="52"/>
+      <c r="E19" s="52"/>
+      <c r="F19" s="52"/>
+      <c r="G19" s="52"/>
+      <c r="H19" s="52"/>
+      <c r="I19" s="52"/>
+      <c r="J19" s="52"/>
     </row>
     <row r="20" spans="2:10" ht="15" x14ac:dyDescent="0.25">
-      <c r="B20" s="38"/>
-      <c r="C20" s="38"/>
-      <c r="D20" s="38"/>
-      <c r="E20" s="38"/>
-      <c r="F20" s="38"/>
-      <c r="G20" s="38"/>
-      <c r="H20" s="38"/>
-      <c r="I20" s="38"/>
-      <c r="J20" s="38"/>
+      <c r="B20" s="52"/>
+      <c r="C20" s="52"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="52"/>
+      <c r="F20" s="52"/>
+      <c r="G20" s="52"/>
+      <c r="H20" s="52"/>
+      <c r="I20" s="52"/>
+      <c r="J20" s="52"/>
     </row>
     <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B21" s="38"/>
-      <c r="C21" s="38"/>
-      <c r="D21" s="38"/>
-      <c r="E21" s="38"/>
-      <c r="F21" s="38"/>
-      <c r="G21" s="38"/>
-      <c r="H21" s="38"/>
-      <c r="I21" s="38"/>
-      <c r="J21" s="38"/>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="52"/>
+      <c r="E21" s="52"/>
+      <c r="F21" s="52"/>
+      <c r="G21" s="52"/>
+      <c r="H21" s="52"/>
+      <c r="I21" s="52"/>
+      <c r="J21" s="52"/>
     </row>
     <row r="22" spans="2:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C22" s="16" t="s">
@@ -2239,7 +2161,7 @@
       </c>
       <c r="I22" s="7"/>
     </row>
-    <row r="23" spans="2:10" s="23" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:10" s="23" customFormat="1" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C23" s="12" t="s">
         <v>68</v>
       </c>
@@ -2250,13 +2172,13 @@
         <v>21</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>193</v>
+        <v>245</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="5"/>
       <c r="I23" s="8"/>
     </row>
-    <row r="24" spans="2:10" s="26" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C24" s="27" t="s">
         <v>69</v>
       </c>
@@ -2267,13 +2189,13 @@
         <v>70</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>194</v>
+        <v>246</v>
       </c>
       <c r="G24" s="29"/>
       <c r="H24" s="30"/>
       <c r="I24" s="7"/>
     </row>
-    <row r="25" spans="2:10" s="26" customFormat="1" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C25" s="27" t="s">
         <v>71</v>
       </c>
@@ -2284,13 +2206,13 @@
         <v>70</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
       <c r="G25" s="29"/>
       <c r="H25" s="30"/>
       <c r="I25" s="7"/>
     </row>
-    <row r="26" spans="2:10" s="26" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="26" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C26" s="27" t="s">
         <v>72</v>
       </c>
@@ -2301,13 +2223,13 @@
         <v>70</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>196</v>
+        <v>248</v>
       </c>
       <c r="G26" s="29"/>
       <c r="H26" s="30"/>
       <c r="I26" s="7"/>
     </row>
-    <row r="27" spans="2:10" s="26" customFormat="1" ht="132" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="27" t="s">
         <v>73</v>
       </c>
@@ -2318,13 +2240,13 @@
         <v>70</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>197</v>
+        <v>249</v>
       </c>
       <c r="G27" s="29"/>
       <c r="H27" s="30"/>
       <c r="I27" s="7"/>
     </row>
-    <row r="28" spans="2:10" s="26" customFormat="1" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="2:10" s="26" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C28" s="27" t="s">
         <v>74</v>
       </c>
@@ -2335,7 +2257,7 @@
         <v>70</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>195</v>
+        <v>247</v>
       </c>
       <c r="G28" s="29"/>
       <c r="H28" s="30"/>
@@ -2352,7 +2274,7 @@
         <v>22</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="6"/>
@@ -2369,7 +2291,7 @@
         <v>22</v>
       </c>
       <c r="F30" s="34" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G30" s="13"/>
       <c r="H30" s="5"/>
@@ -2386,7 +2308,7 @@
         <v>22</v>
       </c>
       <c r="F31" s="34" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G31" s="15"/>
       <c r="H31" s="6"/>
@@ -2403,13 +2325,13 @@
         <v>78</v>
       </c>
       <c r="F32" s="34" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G32" s="13"/>
       <c r="H32" s="5"/>
       <c r="I32" s="8"/>
     </row>
-    <row r="33" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C33" s="14" t="s">
         <v>79</v>
       </c>
@@ -2420,13 +2342,13 @@
         <v>22</v>
       </c>
       <c r="F33" s="34" t="s">
-        <v>195</v>
+        <v>235</v>
       </c>
       <c r="G33" s="15"/>
       <c r="H33" s="6"/>
       <c r="I33" s="8"/>
     </row>
-    <row r="34" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C34" s="14" t="s">
         <v>80</v>
       </c>
@@ -2437,7 +2359,7 @@
         <v>22</v>
       </c>
       <c r="F34" s="34" t="s">
-        <v>195</v>
+        <v>235</v>
       </c>
       <c r="G34" s="15"/>
       <c r="H34" s="6"/>
@@ -2454,7 +2376,7 @@
         <v>22</v>
       </c>
       <c r="F35" s="34" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G35" s="15"/>
       <c r="H35" s="6"/>
@@ -2471,7 +2393,7 @@
         <v>22</v>
       </c>
       <c r="F36" s="34" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G36" s="15"/>
       <c r="H36" s="6"/>
@@ -2488,13 +2410,13 @@
         <v>22</v>
       </c>
       <c r="F37" s="34" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="6"/>
       <c r="I37" s="8"/>
     </row>
-    <row r="38" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C38" s="14" t="s">
         <v>84</v>
       </c>
@@ -2505,7 +2427,7 @@
         <v>29</v>
       </c>
       <c r="F38" s="34" t="s">
-        <v>202</v>
+        <v>251</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="6"/>
@@ -2522,7 +2444,7 @@
         <v>29</v>
       </c>
       <c r="F39" s="34" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="6"/>
@@ -2539,7 +2461,7 @@
         <v>29</v>
       </c>
       <c r="F40" s="34" t="s">
-        <v>201</v>
+        <v>193</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="6"/>
@@ -2556,7 +2478,7 @@
         <v>88</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="6"/>
@@ -2573,7 +2495,7 @@
         <v>89</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>199</v>
+        <v>192</v>
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="6"/>
@@ -2590,7 +2512,7 @@
         <v>25</v>
       </c>
       <c r="F43" s="34" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G43" s="15"/>
       <c r="H43" s="6"/>
@@ -2607,7 +2529,7 @@
         <v>90</v>
       </c>
       <c r="F44" s="34" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G44" s="15"/>
       <c r="H44" s="6"/>
@@ -2624,13 +2546,13 @@
         <v>90</v>
       </c>
       <c r="F45" s="34" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="G45" s="15"/>
       <c r="H45" s="6"/>
       <c r="I45" s="8"/>
     </row>
-    <row r="46" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C46" s="14" t="s">
         <v>92</v>
       </c>
@@ -2641,13 +2563,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="34" t="s">
-        <v>200</v>
+        <v>250</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="6"/>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="14" t="s">
         <v>94</v>
       </c>
@@ -2658,7 +2580,7 @@
         <v>88</v>
       </c>
       <c r="F47" s="34" t="s">
-        <v>219</v>
+        <v>231</v>
       </c>
       <c r="G47" s="15"/>
       <c r="H47" s="6"/>
@@ -2669,98 +2591,98 @@
         <v>95</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>250</v>
+        <v>204</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>251</v>
+        <v>205</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>198</v>
+        <v>191</v>
       </c>
       <c r="G48" s="15"/>
       <c r="H48" s="6"/>
       <c r="I48" s="8"/>
     </row>
     <row r="49" spans="3:9" ht="93.75" x14ac:dyDescent="0.25">
-      <c r="C49" s="46" t="s">
+      <c r="C49" s="36" t="s">
         <v>96</v>
       </c>
-      <c r="D49" s="47" t="s">
-        <v>259</v>
-      </c>
-      <c r="E49" s="48" t="s">
-        <v>248</v>
-      </c>
-      <c r="F49" s="45" t="s">
-        <v>195</v>
-      </c>
-      <c r="G49" s="49"/>
-      <c r="H49" s="50"/>
+      <c r="D49" s="37" t="s">
+        <v>213</v>
+      </c>
+      <c r="E49" s="38" t="s">
+        <v>202</v>
+      </c>
+      <c r="F49" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="G49" s="39"/>
+      <c r="H49" s="40"/>
       <c r="I49" s="8"/>
     </row>
-    <row r="50" spans="3:9" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C50" s="57" t="s">
-        <v>256</v>
-      </c>
-      <c r="D50" s="57" t="s">
-        <v>259</v>
-      </c>
-      <c r="E50" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="F50" s="57"/>
-      <c r="G50" s="58"/>
-      <c r="H50" s="58"/>
-      <c r="I50" s="58"/>
-    </row>
-    <row r="51" spans="3:9" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C51" s="57" t="s">
-        <v>257</v>
-      </c>
-      <c r="D51" s="57" t="s">
-        <v>259</v>
-      </c>
-      <c r="E51" s="57" t="s">
-        <v>261</v>
-      </c>
-      <c r="F51" s="57"/>
-      <c r="G51" s="58"/>
-      <c r="H51" s="58"/>
-      <c r="I51" s="58"/>
-    </row>
-    <row r="52" spans="3:9" s="56" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="C52" s="57" t="s">
-        <v>258</v>
-      </c>
-      <c r="D52" s="57" t="s">
-        <v>259</v>
-      </c>
-      <c r="E52" s="57" t="s">
-        <v>262</v>
-      </c>
-      <c r="F52" s="57"/>
-      <c r="G52" s="58"/>
-      <c r="H52" s="58"/>
-      <c r="I52" s="58"/>
-    </row>
-    <row r="53" spans="3:9" ht="132" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C53" s="51" t="s">
+    <row r="50" spans="3:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C50" s="47" t="s">
+        <v>210</v>
+      </c>
+      <c r="D50" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="E50" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="F50" s="47"/>
+      <c r="G50" s="48"/>
+      <c r="H50" s="48"/>
+      <c r="I50" s="48"/>
+    </row>
+    <row r="51" spans="3:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C51" s="47" t="s">
+        <v>211</v>
+      </c>
+      <c r="D51" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="E51" s="47" t="s">
+        <v>215</v>
+      </c>
+      <c r="F51" s="47"/>
+      <c r="G51" s="48"/>
+      <c r="H51" s="48"/>
+      <c r="I51" s="48"/>
+    </row>
+    <row r="52" spans="3:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="C52" s="47" t="s">
+        <v>212</v>
+      </c>
+      <c r="D52" s="47" t="s">
+        <v>213</v>
+      </c>
+      <c r="E52" s="47" t="s">
+        <v>216</v>
+      </c>
+      <c r="F52" s="47"/>
+      <c r="G52" s="48"/>
+      <c r="H52" s="48"/>
+      <c r="I52" s="48"/>
+    </row>
+    <row r="53" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C53" s="41" t="s">
         <v>97</v>
       </c>
-      <c r="D53" s="52" t="s">
+      <c r="D53" s="42" t="s">
         <v>15</v>
       </c>
-      <c r="E53" s="53" t="s">
+      <c r="E53" s="43" t="s">
         <v>27</v>
       </c>
-      <c r="F53" s="52" t="s">
-        <v>190</v>
-      </c>
-      <c r="G53" s="54"/>
-      <c r="H53" s="55"/>
+      <c r="F53" s="42" t="s">
+        <v>241</v>
+      </c>
+      <c r="G53" s="44"/>
+      <c r="H53" s="45"/>
       <c r="I53" s="8"/>
     </row>
-    <row r="54" spans="3:9" ht="132" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="14" t="s">
         <v>98</v>
       </c>
@@ -2771,13 +2693,13 @@
         <v>27</v>
       </c>
       <c r="F54" s="31" t="s">
-        <v>192</v>
+        <v>242</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="6"/>
       <c r="I54" s="8"/>
     </row>
-    <row r="55" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="14" t="s">
         <v>99</v>
       </c>
@@ -2788,13 +2710,13 @@
         <v>27</v>
       </c>
       <c r="F55" s="31" t="s">
-        <v>191</v>
+        <v>243</v>
       </c>
       <c r="G55" s="15"/>
       <c r="H55" s="6"/>
       <c r="I55" s="8"/>
     </row>
-    <row r="56" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C56" s="14" t="s">
         <v>100</v>
       </c>
@@ -2805,13 +2727,13 @@
         <v>27</v>
       </c>
       <c r="F56" s="31" t="s">
-        <v>191</v>
+        <v>244</v>
       </c>
       <c r="G56" s="15"/>
       <c r="H56" s="6"/>
       <c r="I56" s="8"/>
     </row>
-    <row r="57" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C57" s="14" t="s">
         <v>101</v>
       </c>
@@ -2821,14 +2743,12 @@
       <c r="E57" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F57" s="31" t="s">
-        <v>191</v>
-      </c>
+      <c r="F57" s="31"/>
       <c r="G57" s="15"/>
       <c r="H57" s="6"/>
       <c r="I57" s="8"/>
     </row>
-    <row r="58" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="14" t="s">
         <v>102</v>
       </c>
@@ -2838,14 +2758,12 @@
       <c r="E58" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F58" s="31" t="s">
-        <v>191</v>
-      </c>
+      <c r="F58" s="31"/>
       <c r="G58" s="15"/>
       <c r="H58" s="6"/>
       <c r="I58" s="8"/>
     </row>
-    <row r="59" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C59" s="14" t="s">
         <v>103</v>
       </c>
@@ -2855,14 +2773,12 @@
       <c r="E59" s="32" t="s">
         <v>28</v>
       </c>
-      <c r="F59" s="31" t="s">
-        <v>191</v>
-      </c>
+      <c r="F59" s="31"/>
       <c r="G59" s="15"/>
       <c r="H59" s="6"/>
       <c r="I59" s="8"/>
     </row>
-    <row r="60" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C60" s="14" t="s">
         <v>104</v>
       </c>
@@ -2872,59 +2788,53 @@
       <c r="E60" s="32" t="s">
         <v>29</v>
       </c>
-      <c r="F60" s="31" t="s">
-        <v>191</v>
-      </c>
+      <c r="F60" s="31"/>
       <c r="G60" s="15"/>
       <c r="H60" s="6"/>
       <c r="I60" s="8"/>
     </row>
-    <row r="61" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C61" s="14" t="s">
         <v>105</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>260</v>
+        <v>214</v>
       </c>
       <c r="E61" s="32" t="s">
         <v>31</v>
       </c>
-      <c r="F61" s="31" t="s">
-        <v>191</v>
-      </c>
+      <c r="F61" s="31"/>
       <c r="G61" s="15"/>
       <c r="H61" s="6"/>
       <c r="I61" s="8"/>
     </row>
-    <row r="62" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="14" t="s">
         <v>30</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>260</v>
+        <v>214</v>
       </c>
       <c r="E62" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="F62" s="31" t="s">
-        <v>191</v>
-      </c>
+      <c r="F62" s="31"/>
       <c r="G62" s="15"/>
       <c r="H62" s="6"/>
       <c r="I62" s="8"/>
     </row>
-    <row r="63" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C63" s="14" t="s">
         <v>106</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>260</v>
+        <v>214</v>
       </c>
       <c r="E63" s="32" t="s">
-        <v>247</v>
+        <v>201</v>
       </c>
       <c r="F63" s="31" t="s">
-        <v>191</v>
+        <v>244</v>
       </c>
       <c r="G63" s="15"/>
       <c r="H63" s="6"/>
@@ -2941,7 +2851,7 @@
         <v>34</v>
       </c>
       <c r="F64" s="31" t="s">
-        <v>220</v>
+        <v>196</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="6"/>
@@ -2962,7 +2872,7 @@
       <c r="H65" s="6"/>
       <c r="I65" s="8"/>
     </row>
-    <row r="66" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="14" t="s">
         <v>107</v>
       </c>
@@ -2973,13 +2883,13 @@
         <v>37</v>
       </c>
       <c r="F66" s="31" t="s">
-        <v>222</v>
+        <v>232</v>
       </c>
       <c r="G66" s="15"/>
       <c r="H66" s="6"/>
       <c r="I66" s="8"/>
     </row>
-    <row r="67" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="14" t="s">
         <v>108</v>
       </c>
@@ -2990,13 +2900,13 @@
         <v>37</v>
       </c>
       <c r="F67" s="31" t="s">
-        <v>223</v>
+        <v>268</v>
       </c>
       <c r="G67" s="15"/>
       <c r="H67" s="6"/>
       <c r="I67" s="8"/>
     </row>
-    <row r="68" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="14" t="s">
         <v>109</v>
       </c>
@@ -3007,13 +2917,13 @@
         <v>37</v>
       </c>
       <c r="F68" s="31" t="s">
-        <v>224</v>
+        <v>269</v>
       </c>
       <c r="G68" s="15"/>
       <c r="H68" s="6"/>
       <c r="I68" s="8"/>
     </row>
-    <row r="69" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="14" t="s">
         <v>110</v>
       </c>
@@ -3024,7 +2934,7 @@
         <v>37</v>
       </c>
       <c r="F69" s="31" t="s">
-        <v>225</v>
+        <v>269</v>
       </c>
       <c r="G69" s="15"/>
       <c r="H69" s="6"/>
@@ -3041,13 +2951,13 @@
         <v>37</v>
       </c>
       <c r="F70" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G70" s="15"/>
       <c r="H70" s="6"/>
       <c r="I70" s="8"/>
     </row>
-    <row r="71" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C71" s="14" t="s">
         <v>112</v>
       </c>
@@ -3058,13 +2968,13 @@
         <v>37</v>
       </c>
       <c r="F71" s="31" t="s">
-        <v>226</v>
+        <v>233</v>
       </c>
       <c r="G71" s="15"/>
       <c r="H71" s="6"/>
       <c r="I71" s="8"/>
     </row>
-    <row r="72" spans="3:9" ht="150.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C72" s="14" t="s">
         <v>38</v>
       </c>
@@ -3075,13 +2985,13 @@
         <v>39</v>
       </c>
       <c r="F72" s="31" t="s">
-        <v>227</v>
+        <v>270</v>
       </c>
       <c r="G72" s="15"/>
       <c r="H72" s="6"/>
       <c r="I72" s="8"/>
     </row>
-    <row r="73" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="14" t="s">
         <v>40</v>
       </c>
@@ -3092,7 +3002,7 @@
         <v>41</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>228</v>
+        <v>271</v>
       </c>
       <c r="G73" s="15"/>
       <c r="H73" s="6"/>
@@ -3109,13 +3019,13 @@
         <v>42</v>
       </c>
       <c r="F74" s="31" t="s">
-        <v>229</v>
+        <v>274</v>
       </c>
       <c r="G74" s="15"/>
       <c r="H74" s="6"/>
       <c r="I74" s="8"/>
     </row>
-    <row r="75" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="14" t="s">
         <v>114</v>
       </c>
@@ -3126,7 +3036,7 @@
         <v>42</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="6"/>
@@ -3143,13 +3053,13 @@
         <v>42</v>
       </c>
       <c r="F76" s="31" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="G76" s="15"/>
       <c r="H76" s="6"/>
       <c r="I76" s="8"/>
     </row>
-    <row r="77" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C77" s="14" t="s">
         <v>44</v>
       </c>
@@ -3160,7 +3070,7 @@
         <v>43</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>230</v>
+        <v>227</v>
       </c>
       <c r="G77" s="15"/>
       <c r="H77" s="6"/>
@@ -3174,10 +3084,10 @@
         <v>32</v>
       </c>
       <c r="E78" s="32" t="s">
-        <v>252</v>
+        <v>206</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="G78" s="15"/>
       <c r="H78" s="6"/>
@@ -3194,7 +3104,7 @@
         <v>42</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>232</v>
+        <v>263</v>
       </c>
       <c r="G79" s="15"/>
       <c r="H79" s="6"/>
@@ -3211,7 +3121,7 @@
         <v>42</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>228</v>
+        <v>253</v>
       </c>
       <c r="G80" s="15"/>
       <c r="H80" s="6"/>
@@ -3228,7 +3138,7 @@
         <v>45</v>
       </c>
       <c r="F81" s="31" t="s">
-        <v>233</v>
+        <v>264</v>
       </c>
       <c r="G81" s="15"/>
       <c r="H81" s="6"/>
@@ -3245,7 +3155,7 @@
         <v>45</v>
       </c>
       <c r="F82" s="31" t="s">
-        <v>233</v>
+        <v>264</v>
       </c>
       <c r="G82" s="15"/>
       <c r="H82" s="6"/>
@@ -3262,7 +3172,7 @@
         <v>46</v>
       </c>
       <c r="F83" s="31" t="s">
-        <v>231</v>
+        <v>240</v>
       </c>
       <c r="G83" s="15"/>
       <c r="H83" s="6"/>
@@ -3279,7 +3189,7 @@
         <v>46</v>
       </c>
       <c r="F84" s="31" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="G84" s="15"/>
       <c r="H84" s="6"/>
@@ -3296,13 +3206,13 @@
         <v>46</v>
       </c>
       <c r="F85" s="31" t="s">
-        <v>234</v>
+        <v>198</v>
       </c>
       <c r="G85" s="15"/>
       <c r="H85" s="6"/>
       <c r="I85" s="8"/>
     </row>
-    <row r="86" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C86" s="14" t="s">
         <v>124</v>
       </c>
@@ -3313,13 +3223,13 @@
         <v>125</v>
       </c>
       <c r="F86" s="31" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="G86" s="15"/>
       <c r="H86" s="6"/>
       <c r="I86" s="8"/>
     </row>
-    <row r="87" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C87" s="14" t="s">
         <v>126</v>
       </c>
@@ -3330,7 +3240,7 @@
         <v>125</v>
       </c>
       <c r="F87" s="31" t="s">
-        <v>221</v>
+        <v>236</v>
       </c>
       <c r="G87" s="15"/>
       <c r="H87" s="6"/>
@@ -3347,7 +3257,7 @@
         <v>128</v>
       </c>
       <c r="F88" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G88" s="15"/>
       <c r="H88" s="6"/>
@@ -3361,10 +3271,10 @@
         <v>32</v>
       </c>
       <c r="E89" s="32" t="s">
-        <v>249</v>
+        <v>203</v>
       </c>
       <c r="F89" s="31" t="s">
-        <v>239</v>
+        <v>199</v>
       </c>
       <c r="G89" s="15"/>
       <c r="H89" s="6"/>
@@ -3378,10 +3288,10 @@
         <v>32</v>
       </c>
       <c r="E90" s="32" t="s">
-        <v>249</v>
+        <v>203</v>
       </c>
       <c r="F90" s="31" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="G90" s="15"/>
       <c r="H90" s="6"/>
@@ -3395,16 +3305,16 @@
         <v>32</v>
       </c>
       <c r="E91" s="32" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="F91" s="31" t="s">
-        <v>204</v>
+        <v>273</v>
       </c>
       <c r="G91" s="15"/>
       <c r="H91" s="6"/>
       <c r="I91" s="8"/>
     </row>
-    <row r="92" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C92" s="14" t="s">
         <v>132</v>
       </c>
@@ -3412,16 +3322,14 @@
         <v>32</v>
       </c>
       <c r="E92" s="32" t="s">
-        <v>246</v>
-      </c>
-      <c r="F92" s="31" t="s">
-        <v>205</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="F92" s="31"/>
       <c r="G92" s="15"/>
       <c r="H92" s="6"/>
       <c r="I92" s="8"/>
     </row>
-    <row r="93" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C93" s="14" t="s">
         <v>133</v>
       </c>
@@ -3429,16 +3337,16 @@
         <v>32</v>
       </c>
       <c r="E93" s="32" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="F93" s="31" t="s">
-        <v>207</v>
+        <v>272</v>
       </c>
       <c r="G93" s="15"/>
       <c r="H93" s="6"/>
       <c r="I93" s="8"/>
     </row>
-    <row r="94" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C94" s="14" t="s">
         <v>134</v>
       </c>
@@ -3446,16 +3354,14 @@
         <v>32</v>
       </c>
       <c r="E94" s="32" t="s">
-        <v>246</v>
-      </c>
-      <c r="F94" s="31" t="s">
-        <v>207</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="F94" s="31"/>
       <c r="G94" s="15"/>
       <c r="H94" s="6"/>
       <c r="I94" s="8"/>
     </row>
-    <row r="95" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C95" s="14" t="s">
         <v>135</v>
       </c>
@@ -3463,11 +3369,9 @@
         <v>32</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>246</v>
-      </c>
-      <c r="F95" s="31" t="s">
-        <v>208</v>
-      </c>
+        <v>200</v>
+      </c>
+      <c r="F95" s="31"/>
       <c r="G95" s="15"/>
       <c r="H95" s="6"/>
       <c r="I95" s="8"/>
@@ -3480,10 +3384,10 @@
         <v>32</v>
       </c>
       <c r="E96" s="32" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="F96" s="31" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="G96" s="15"/>
       <c r="H96" s="6"/>
@@ -3497,10 +3401,10 @@
         <v>32</v>
       </c>
       <c r="E97" s="32" t="s">
-        <v>249</v>
+        <v>203</v>
       </c>
       <c r="F97" s="31" t="s">
-        <v>231</v>
+        <v>197</v>
       </c>
       <c r="G97" s="15"/>
       <c r="H97" s="6"/>
@@ -3508,13 +3412,13 @@
     </row>
     <row r="98" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C98" s="14" t="s">
-        <v>263</v>
+        <v>217</v>
       </c>
       <c r="D98" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E98" s="32" t="s">
-        <v>268</v>
+        <v>222</v>
       </c>
       <c r="F98" s="31"/>
       <c r="G98" s="15"/>
@@ -3523,13 +3427,13 @@
     </row>
     <row r="99" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C99" s="14" t="s">
-        <v>264</v>
+        <v>218</v>
       </c>
       <c r="D99" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E99" s="32" t="s">
-        <v>269</v>
+        <v>223</v>
       </c>
       <c r="F99" s="31"/>
       <c r="G99" s="15"/>
@@ -3538,13 +3442,13 @@
     </row>
     <row r="100" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C100" s="14" t="s">
-        <v>265</v>
+        <v>219</v>
       </c>
       <c r="D100" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E100" s="32" t="s">
-        <v>270</v>
+        <v>224</v>
       </c>
       <c r="F100" s="31"/>
       <c r="G100" s="15"/>
@@ -3553,13 +3457,13 @@
     </row>
     <row r="101" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C101" s="14" t="s">
-        <v>266</v>
+        <v>220</v>
       </c>
       <c r="D101" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E101" s="32" t="s">
-        <v>271</v>
+        <v>225</v>
       </c>
       <c r="F101" s="31"/>
       <c r="G101" s="15"/>
@@ -3568,13 +3472,13 @@
     </row>
     <row r="102" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C102" s="14" t="s">
-        <v>267</v>
+        <v>221</v>
       </c>
       <c r="D102" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E102" s="32" t="s">
-        <v>272</v>
+        <v>226</v>
       </c>
       <c r="F102" s="31"/>
       <c r="G102" s="15"/>
@@ -3592,7 +3496,7 @@
         <v>20</v>
       </c>
       <c r="F103" s="31" t="s">
-        <v>240</v>
+        <v>259</v>
       </c>
       <c r="G103" s="15"/>
       <c r="H103" s="6"/>
@@ -3626,7 +3530,7 @@
         <v>20</v>
       </c>
       <c r="F105" s="31" t="s">
-        <v>241</v>
+        <v>260</v>
       </c>
       <c r="G105" s="15"/>
       <c r="H105" s="6"/>
@@ -3660,7 +3564,7 @@
         <v>20</v>
       </c>
       <c r="F107" s="31" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="G107" s="15"/>
       <c r="H107" s="6"/>
@@ -3677,7 +3581,7 @@
         <v>20</v>
       </c>
       <c r="F108" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G108" s="15"/>
       <c r="H108" s="6"/>
@@ -3688,13 +3592,13 @@
         <v>48</v>
       </c>
       <c r="D109" s="31" t="s">
-        <v>253</v>
+        <v>207</v>
       </c>
       <c r="E109" s="32" t="s">
-        <v>254</v>
+        <v>208</v>
       </c>
       <c r="F109" s="31" t="s">
-        <v>243</v>
+        <v>258</v>
       </c>
       <c r="G109" s="15"/>
       <c r="H109" s="6"/>
@@ -3705,13 +3609,13 @@
         <v>49</v>
       </c>
       <c r="D110" s="31" t="s">
-        <v>253</v>
+        <v>207</v>
       </c>
       <c r="E110" s="32" t="s">
-        <v>255</v>
+        <v>209</v>
       </c>
       <c r="F110" s="31" t="s">
-        <v>244</v>
+        <v>258</v>
       </c>
       <c r="G110" s="15"/>
       <c r="H110" s="6"/>
@@ -3728,7 +3632,7 @@
         <v>17</v>
       </c>
       <c r="F111" s="31" t="s">
-        <v>187</v>
+        <v>228</v>
       </c>
       <c r="G111" s="15"/>
       <c r="H111" s="6"/>
@@ -3802,7 +3706,7 @@
       <c r="H115" s="6"/>
       <c r="I115" s="8"/>
     </row>
-    <row r="116" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C116" s="14" t="s">
         <v>51</v>
       </c>
@@ -3813,7 +3717,7 @@
         <v>148</v>
       </c>
       <c r="F116" s="31" t="s">
-        <v>245</v>
+        <v>237</v>
       </c>
       <c r="G116" s="15"/>
       <c r="H116" s="6"/>
@@ -3830,13 +3734,13 @@
         <v>148</v>
       </c>
       <c r="F117" s="31" t="s">
-        <v>206</v>
+        <v>254</v>
       </c>
       <c r="G117" s="15"/>
       <c r="H117" s="6"/>
       <c r="I117" s="8"/>
     </row>
-    <row r="118" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C118" s="14" t="s">
         <v>150</v>
       </c>
@@ -3847,7 +3751,7 @@
         <v>148</v>
       </c>
       <c r="F118" s="31" t="s">
-        <v>187</v>
+        <v>234</v>
       </c>
       <c r="G118" s="15"/>
       <c r="H118" s="6"/>
@@ -3864,7 +3768,7 @@
         <v>152</v>
       </c>
       <c r="F119" s="31" t="s">
-        <v>235</v>
+        <v>255</v>
       </c>
       <c r="G119" s="15"/>
       <c r="H119" s="6"/>
@@ -3881,7 +3785,7 @@
         <v>154</v>
       </c>
       <c r="F120" s="31" t="s">
-        <v>237</v>
+        <v>256</v>
       </c>
       <c r="G120" s="15"/>
       <c r="H120" s="6"/>
@@ -3898,7 +3802,7 @@
         <v>156</v>
       </c>
       <c r="F121" s="31" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="G121" s="15"/>
       <c r="H121" s="6"/>
@@ -3932,7 +3836,7 @@
         <v>128</v>
       </c>
       <c r="F123" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G123" s="15"/>
       <c r="H123" s="6"/>
@@ -3949,7 +3853,7 @@
         <v>161</v>
       </c>
       <c r="F124" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G124" s="15"/>
       <c r="H124" s="6"/>
@@ -3966,7 +3870,7 @@
         <v>161</v>
       </c>
       <c r="F125" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G125" s="15"/>
       <c r="H125" s="6"/>
@@ -3983,7 +3887,7 @@
         <v>161</v>
       </c>
       <c r="F126" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G126" s="15"/>
       <c r="H126" s="6"/>
@@ -4000,7 +3904,7 @@
         <v>161</v>
       </c>
       <c r="F127" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G127" s="15"/>
       <c r="H127" s="6"/>
@@ -4017,7 +3921,7 @@
         <v>161</v>
       </c>
       <c r="F128" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G128" s="15"/>
       <c r="H128" s="6"/>
@@ -4028,10 +3932,10 @@
         <v>166</v>
       </c>
       <c r="D129" s="31" t="s">
-        <v>253</v>
+        <v>207</v>
       </c>
       <c r="E129" s="32" t="s">
-        <v>255</v>
+        <v>209</v>
       </c>
       <c r="F129" s="31" t="s">
         <v>187</v>
@@ -4051,7 +3955,7 @@
         <v>20</v>
       </c>
       <c r="F130" s="31" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="G130" s="15"/>
       <c r="H130" s="6"/>
@@ -4068,7 +3972,7 @@
         <v>20</v>
       </c>
       <c r="F131" s="31" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="G131" s="15"/>
       <c r="H131" s="6"/>
@@ -4085,7 +3989,7 @@
         <v>20</v>
       </c>
       <c r="F132" s="31" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="G132" s="15"/>
       <c r="H132" s="6"/>
@@ -4102,7 +4006,7 @@
         <v>20</v>
       </c>
       <c r="F133" s="31" t="s">
-        <v>242</v>
+        <v>261</v>
       </c>
       <c r="G133" s="15"/>
       <c r="H133" s="6"/>
@@ -4116,10 +4020,10 @@
         <v>47</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="F134" s="31" t="s">
-        <v>209</v>
+        <v>262</v>
       </c>
       <c r="G134" s="15"/>
       <c r="H134" s="6"/>
@@ -4133,10 +4037,10 @@
         <v>47</v>
       </c>
       <c r="E135" s="32" t="s">
-        <v>246</v>
+        <v>200</v>
       </c>
       <c r="F135" s="31" t="s">
-        <v>210</v>
+        <v>252</v>
       </c>
       <c r="G135" s="15"/>
       <c r="H135" s="6"/>
@@ -4153,13 +4057,13 @@
         <v>52</v>
       </c>
       <c r="F136" s="31" t="s">
-        <v>218</v>
+        <v>238</v>
       </c>
       <c r="G136" s="15"/>
       <c r="H136" s="6"/>
       <c r="I136" s="8"/>
     </row>
-    <row r="137" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C137" s="14" t="s">
         <v>174</v>
       </c>
@@ -4170,7 +4074,7 @@
         <v>52</v>
       </c>
       <c r="F137" s="31" t="s">
-        <v>217</v>
+        <v>230</v>
       </c>
       <c r="G137" s="15"/>
       <c r="H137" s="6"/>
@@ -4187,7 +4091,7 @@
         <v>52</v>
       </c>
       <c r="F138" s="31" t="s">
-        <v>212</v>
+        <v>239</v>
       </c>
       <c r="G138" s="15"/>
       <c r="H138" s="6"/>
@@ -4204,7 +4108,7 @@
         <v>53</v>
       </c>
       <c r="F139" s="31" t="s">
-        <v>214</v>
+        <v>265</v>
       </c>
       <c r="G139" s="15"/>
       <c r="H139" s="6"/>
@@ -4221,7 +4125,7 @@
         <v>53</v>
       </c>
       <c r="F140" s="31" t="s">
-        <v>215</v>
+        <v>266</v>
       </c>
       <c r="G140" s="15"/>
       <c r="H140" s="6"/>
@@ -4238,13 +4142,13 @@
         <v>53</v>
       </c>
       <c r="F141" s="31" t="s">
-        <v>213</v>
+        <v>195</v>
       </c>
       <c r="G141" s="15"/>
       <c r="H141" s="6"/>
       <c r="I141" s="8"/>
     </row>
-    <row r="142" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C142" s="14" t="s">
         <v>179</v>
       </c>
@@ -4255,7 +4159,7 @@
         <v>53</v>
       </c>
       <c r="F142" s="31" t="s">
-        <v>216</v>
+        <v>229</v>
       </c>
       <c r="G142" s="15"/>
       <c r="H142" s="6"/>
@@ -4272,7 +4176,7 @@
         <v>53</v>
       </c>
       <c r="F143" s="31" t="s">
-        <v>211</v>
+        <v>267</v>
       </c>
       <c r="G143" s="15"/>
       <c r="H143" s="6"/>

</xml_diff>

<commit_message>
adding Design id up on quality assurance demand
adding Design id up on quality assurance demand
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="511" uniqueCount="275">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="488" uniqueCount="264">
   <si>
     <t>Author</t>
   </si>
@@ -620,50 +620,10 @@
     <t xml:space="preserve"> Test Case ID</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_CST_007</t>
-  </si>
-  <si>
     <t>Design ID</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_ADMIN_006
-Bank_SYS_HLD_admin_003</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_HLD_admin_001
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_HLD_admin_001
-BANK_SYS_DD_ Admin _003
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_002
-Bank_SYS_HLD_client_001
-Bank_SYS_HLD_admin_001
-Bank_SYS_DSN_004</t>
-  </si>
-  <si>
     <t>Bank_SYS_DSN_005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">     Bank_Sys_DM_ADMIN_003                                              
-Bank_SYS_HLD_admin_004
-BANK_SYS_DD_ Admin _007</t>
   </si>
   <si>
     <t xml:space="preserve">                                                      
@@ -673,14 +633,6 @@
     <t xml:space="preserve">                                                      </t>
   </si>
   <si>
-    <t xml:space="preserve">                                                      
-Bank_Sys_DM_CST_006</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_CST_007
-Bank_SYS_DSN_005</t>
-  </si>
-  <si>
     <t>BANK_SYS_SIQ_Q46</t>
   </si>
   <si>
@@ -766,15 +718,6 @@
   </si>
   <si>
     <t>BANK_SYS_SIQ_Q55</t>
-  </si>
-  <si>
-    <t>Bank_SYS_HLD_client_004</t>
-  </si>
-  <si>
-    <t>Bank_SYS_HLD_client_005</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_005</t>
   </si>
   <si>
     <t>Bank_SYS_HLD_admin_005
@@ -783,36 +726,7 @@
 Bank_Sys_DM_ADMIN_008</t>
   </si>
   <si>
-    <t>Bank_Sys_DM_ADMIN_002
-Bank_Sys_DM_CST_003</t>
-  </si>
-  <si>
     <t>Bank_Sys_DM_CST_004</t>
-  </si>
-  <si>
-    <t>Bank_SYS_HLD_client_004
-Bank_Sys_DM_CST_006</t>
-  </si>
-  <si>
-    <t>Bank_SYS_HLD_client_006
-Bank_Sys_DM_CST_007</t>
-  </si>
-  <si>
-    <t>BANK_SYS_ ERD _ CST _005</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-BANK_SYS_DD_account_001
-BANK_SYS_ ERD _ account_001</t>
-  </si>
-  <si>
-    <t>BANK_SYS_ ERD _ account_002</t>
-  </si>
-  <si>
-    <t>Bank_SYS_HLD_admin_003
-Bank_Sys_DM_ADMIN_009
-BANK_SYS_ ERD _ account_004
-BANK_SYS_ ERD _ Admin _006</t>
   </si>
   <si>
     <t>Bank_SYS_HLD_admin_004
@@ -821,132 +735,47 @@
 BANK_SYS_ ERD _ account_008</t>
   </si>
   <si>
-    <t xml:space="preserve">       BANK_SYS_ ERD _ TR _004                                               </t>
-  </si>
-  <si>
-    <t>BANK_SYS_ERD_CST_001
-Bank_SYS_DSN_001</t>
-  </si>
-  <si>
-    <t>BANK_SYS_ ERD _ CST _002
-Bank_SYS_DSN_001</t>
-  </si>
-  <si>
-    <t>BANK_SYS_ ERD _ CST _005Bank_SYS_DSN_001</t>
-  </si>
-  <si>
     <t>Bank_SYS_DSN_001</t>
   </si>
   <si>
-    <t>BANK_SYS_ERD_CST_001
+    <t>Bank_SYS_DSN_002</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_003</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                 </t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">          Bank_SYS_DSN_006                                       </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
 Bank_SYS_DSN_002</t>
   </si>
   <si>
-    <t>BANK_SYS_ ERD _ CST _002
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>BANK_SYS_ ERD _ CST _003
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>BANK_SYS_ ERD _ CST _004
-Bank_SYS_DSN_002</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_003</t>
-  </si>
-  <si>
-    <t>Bank_SYS_DSN_004</t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_CST_007
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_CST_006
-BANK_SYS_DD_ PR _002
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_CST_006
-Bank_Sys_DM_ADMIN_007                                                      
-BANK_SYS_DD_ PR _002
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_CST_006                                                      
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_CST_007
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_CST_007
-BANK_SYS_DD_ Trans _003
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_CST_007
-BANK_SYS_DD_ account _003
-BANK_SYS_DD_Trans_001
-BANK_SYS_DD_PR_001
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_CST_007
-BANK_SYS_DD_ Trans _002
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_SYS_DSN_005
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-Bank_SYS_HLD_client_006
-BANK_SYS_DD_ PR _003
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">                                                      
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_ADMIN_004
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_ADMIN_004
-Bank_Sys_DM_ADMIN_007
-                                                 </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Bank_Sys_DM_ADMIN_005
-BANK_SYS_DD_ Admin _006
-                                                 </t>
-  </si>
-  <si>
-    <t>Bank_SYS_HLD_client_003
-Bank_Sys_DM_ADMIN_006
-Bank_Sys_DM_CST_005
-Bank_SYS_DSN_006</t>
-  </si>
-  <si>
-    <t>Bank_Sys_DM_ADMIN_006
-Bank_Sys_DM_CST_005
-Bank_SYS_DSN_006</t>
+    <t>Bank_Sys_DM_CST_001</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_002</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_003</t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_006</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_Sys_DM_CST_007                                                 </t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_006</t>
   </si>
   <si>
     <t xml:space="preserve">                                                      
@@ -954,18 +783,117 @@
                                                  </t>
   </si>
   <si>
-    <t xml:space="preserve">             Bank_SYS_HLD_client_007                                         
+    <t xml:space="preserve">           Bank_SYS_DSN_007                                                                                                                                           
                                                  </t>
   </si>
   <si>
-    <t>Bank_SYS_HLD_client_007</t>
-  </si>
-  <si>
-    <t xml:space="preserve">          Bank_SYS_DSN_006                                       </t>
-  </si>
-  <si>
     <t xml:space="preserve">                                                      
-Bank_SYS_HLD_client_008</t>
+Bank_SYS_DSN_008</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+Bank_SYS_DSN_007                                                 
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+                 Bank_SYS_DSN_009                                
+                                                 </t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+Bank_SYS_DSN_014                                                 
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_SYS_DSN_014                                                      
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+Bank_SYS_DSN_014                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                      
+Bank_Sys_DM_CST_006
+Bank_SYS_DSN_014</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_SYS_DSN_010                      </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+                              Bank_SYS_DSN_010
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+      Bank_SYS_DSN_010                                          </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_SYS_DSN_010
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_SYS_DSN_012
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_SYS_DSN_013
+                                                 </t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_005
+Bank_SYS_HLD_client_006</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_CST_005</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_client_006
+Bank_Sys_DM_CST_005
+Bank_Sys_DM_CST_007</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                     Bank_SYS_DSN_009                                   
+                                                                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                                                                                   Bank_SYS_DSN_009                                                        
+                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_SYS_DSN_014                                                   
+                                                                                                                                                   </t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_010</t>
+  </si>
+  <si>
+    <t>Bank_SYS_HLD_admin_003
+Bank_Sys_DM_ADMIN_009
+BANK_SYS_ ERD _ account_004</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_SYS_DSN_015
+                                                 </t>
+  </si>
+  <si>
+    <t>Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t>Bank_Sys_DM_ADMIN_005
+Bank_SYS_DSN_015</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Bank_SYS_DSN_015                                                 </t>
+  </si>
+  <si>
+    <t xml:space="preserve">
+Bank_Sys_DM_ADMIN_009</t>
   </si>
 </sst>
 </file>
@@ -1852,8 +1780,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L150"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A74" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="F75" sqref="F75"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A145" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="F159" sqref="F159"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.3"/>
@@ -2039,7 +1967,7 @@
       </c>
       <c r="J10" s="51"/>
     </row>
-    <row r="13" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="52" t="s">
         <v>64</v>
       </c>
@@ -2052,7 +1980,7 @@
       <c r="I13" s="52"/>
       <c r="J13" s="52"/>
     </row>
-    <row r="14" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B14" s="52"/>
       <c r="C14" s="52"/>
       <c r="D14" s="52"/>
@@ -2063,7 +1991,7 @@
       <c r="I14" s="52"/>
       <c r="J14" s="52"/>
     </row>
-    <row r="15" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B15" s="52"/>
       <c r="C15" s="52"/>
       <c r="D15" s="52"/>
@@ -2074,7 +2002,7 @@
       <c r="I15" s="52"/>
       <c r="J15" s="52"/>
     </row>
-    <row r="16" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="52"/>
       <c r="C16" s="52"/>
       <c r="D16" s="52"/>
@@ -2085,7 +2013,7 @@
       <c r="I16" s="52"/>
       <c r="J16" s="52"/>
     </row>
-    <row r="17" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="52"/>
       <c r="C17" s="52"/>
       <c r="D17" s="52"/>
@@ -2096,7 +2024,7 @@
       <c r="I17" s="52"/>
       <c r="J17" s="52"/>
     </row>
-    <row r="18" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="52"/>
       <c r="C18" s="52"/>
       <c r="D18" s="52"/>
@@ -2107,7 +2035,7 @@
       <c r="I18" s="52"/>
       <c r="J18" s="52"/>
     </row>
-    <row r="19" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B19" s="52"/>
       <c r="C19" s="52"/>
       <c r="D19" s="52"/>
@@ -2118,7 +2046,7 @@
       <c r="I19" s="52"/>
       <c r="J19" s="52"/>
     </row>
-    <row r="20" spans="2:10" ht="15" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="52"/>
       <c r="C20" s="52"/>
       <c r="D20" s="52"/>
@@ -2129,7 +2057,7 @@
       <c r="I20" s="52"/>
       <c r="J20" s="52"/>
     </row>
-    <row r="21" spans="2:10" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:10" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B21" s="52"/>
       <c r="C21" s="52"/>
       <c r="D21" s="52"/>
@@ -2151,7 +2079,7 @@
         <v>2</v>
       </c>
       <c r="F22" s="10" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G22" s="10" t="s">
         <v>186</v>
@@ -2172,7 +2100,7 @@
         <v>21</v>
       </c>
       <c r="F23" s="34" t="s">
-        <v>245</v>
+        <v>222</v>
       </c>
       <c r="G23" s="13"/>
       <c r="H23" s="5"/>
@@ -2189,7 +2117,7 @@
         <v>70</v>
       </c>
       <c r="F24" s="34" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="G24" s="29"/>
       <c r="H24" s="30"/>
@@ -2206,7 +2134,7 @@
         <v>70</v>
       </c>
       <c r="F25" s="34" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="G25" s="29"/>
       <c r="H25" s="30"/>
@@ -2223,7 +2151,7 @@
         <v>70</v>
       </c>
       <c r="F26" s="34" t="s">
-        <v>248</v>
+        <v>222</v>
       </c>
       <c r="G26" s="29"/>
       <c r="H26" s="30"/>
@@ -2240,7 +2168,7 @@
         <v>70</v>
       </c>
       <c r="F27" s="34" t="s">
-        <v>249</v>
+        <v>222</v>
       </c>
       <c r="G27" s="29"/>
       <c r="H27" s="30"/>
@@ -2257,13 +2185,13 @@
         <v>70</v>
       </c>
       <c r="F28" s="34" t="s">
-        <v>247</v>
+        <v>222</v>
       </c>
       <c r="G28" s="29"/>
       <c r="H28" s="30"/>
       <c r="I28" s="7"/>
     </row>
-    <row r="29" spans="2:10" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="2:10" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C29" s="14" t="s">
         <v>75</v>
       </c>
@@ -2274,13 +2202,13 @@
         <v>22</v>
       </c>
       <c r="F29" s="34" t="s">
-        <v>190</v>
+        <v>228</v>
       </c>
       <c r="G29" s="15"/>
       <c r="H29" s="6"/>
       <c r="I29" s="8"/>
     </row>
-    <row r="30" spans="2:10" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C30" s="12" t="s">
         <v>76</v>
       </c>
@@ -2290,14 +2218,12 @@
       <c r="E30" s="25" t="s">
         <v>22</v>
       </c>
-      <c r="F30" s="34" t="s">
-        <v>190</v>
-      </c>
+      <c r="F30" s="34"/>
       <c r="G30" s="13"/>
       <c r="H30" s="5"/>
       <c r="I30" s="8"/>
     </row>
-    <row r="31" spans="2:10" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:10" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C31" s="14" t="s">
         <v>65</v>
       </c>
@@ -2307,14 +2233,12 @@
       <c r="E31" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F31" s="34" t="s">
-        <v>190</v>
-      </c>
+      <c r="F31" s="34"/>
       <c r="G31" s="15"/>
       <c r="H31" s="6"/>
       <c r="I31" s="8"/>
     </row>
-    <row r="32" spans="2:10" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" x14ac:dyDescent="0.25">
       <c r="C32" s="12" t="s">
         <v>77</v>
       </c>
@@ -2324,9 +2248,7 @@
       <c r="E32" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="F32" s="34" t="s">
-        <v>190</v>
-      </c>
+      <c r="F32" s="34"/>
       <c r="G32" s="13"/>
       <c r="H32" s="5"/>
       <c r="I32" s="8"/>
@@ -2341,9 +2263,7 @@
       <c r="E33" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F33" s="34" t="s">
-        <v>235</v>
-      </c>
+      <c r="F33" s="34"/>
       <c r="G33" s="15"/>
       <c r="H33" s="6"/>
       <c r="I33" s="8"/>
@@ -2358,14 +2278,12 @@
       <c r="E34" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F34" s="34" t="s">
-        <v>235</v>
-      </c>
+      <c r="F34" s="34"/>
       <c r="G34" s="15"/>
       <c r="H34" s="6"/>
       <c r="I34" s="8"/>
     </row>
-    <row r="35" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="14" t="s">
         <v>81</v>
       </c>
@@ -2375,14 +2293,12 @@
       <c r="E35" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F35" s="34" t="s">
-        <v>191</v>
-      </c>
+      <c r="F35" s="34"/>
       <c r="G35" s="15"/>
       <c r="H35" s="6"/>
       <c r="I35" s="8"/>
     </row>
-    <row r="36" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C36" s="14" t="s">
         <v>82</v>
       </c>
@@ -2392,14 +2308,12 @@
       <c r="E36" s="32" t="s">
         <v>22</v>
       </c>
-      <c r="F36" s="34" t="s">
-        <v>190</v>
-      </c>
+      <c r="F36" s="34"/>
       <c r="G36" s="15"/>
       <c r="H36" s="6"/>
       <c r="I36" s="8"/>
     </row>
-    <row r="37" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C37" s="14" t="s">
         <v>83</v>
       </c>
@@ -2410,7 +2324,7 @@
         <v>22</v>
       </c>
       <c r="F37" s="34" t="s">
-        <v>193</v>
+        <v>229</v>
       </c>
       <c r="G37" s="15"/>
       <c r="H37" s="6"/>
@@ -2427,13 +2341,13 @@
         <v>29</v>
       </c>
       <c r="F38" s="34" t="s">
-        <v>251</v>
+        <v>224</v>
       </c>
       <c r="G38" s="15"/>
       <c r="H38" s="6"/>
       <c r="I38" s="8"/>
     </row>
-    <row r="39" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="14" t="s">
         <v>85</v>
       </c>
@@ -2444,13 +2358,13 @@
         <v>29</v>
       </c>
       <c r="F39" s="34" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="G39" s="15"/>
       <c r="H39" s="6"/>
       <c r="I39" s="8"/>
     </row>
-    <row r="40" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C40" s="14" t="s">
         <v>86</v>
       </c>
@@ -2461,13 +2375,13 @@
         <v>29</v>
       </c>
       <c r="F40" s="34" t="s">
-        <v>193</v>
+        <v>224</v>
       </c>
       <c r="G40" s="15"/>
       <c r="H40" s="6"/>
       <c r="I40" s="8"/>
     </row>
-    <row r="41" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C41" s="14" t="s">
         <v>87</v>
       </c>
@@ -2478,13 +2392,13 @@
         <v>88</v>
       </c>
       <c r="F41" s="34" t="s">
-        <v>191</v>
+        <v>230</v>
       </c>
       <c r="G41" s="15"/>
       <c r="H41" s="6"/>
       <c r="I41" s="8"/>
     </row>
-    <row r="42" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C42" s="14" t="s">
         <v>23</v>
       </c>
@@ -2495,13 +2409,13 @@
         <v>89</v>
       </c>
       <c r="F42" s="34" t="s">
-        <v>192</v>
+        <v>222</v>
       </c>
       <c r="G42" s="15"/>
       <c r="H42" s="6"/>
       <c r="I42" s="8"/>
     </row>
-    <row r="43" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C43" s="14" t="s">
         <v>24</v>
       </c>
@@ -2511,14 +2425,12 @@
       <c r="E43" s="32" t="s">
         <v>25</v>
       </c>
-      <c r="F43" s="34" t="s">
-        <v>190</v>
-      </c>
+      <c r="F43" s="34"/>
       <c r="G43" s="15"/>
       <c r="H43" s="6"/>
       <c r="I43" s="8"/>
     </row>
-    <row r="44" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C44" s="14" t="s">
         <v>26</v>
       </c>
@@ -2528,14 +2440,12 @@
       <c r="E44" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F44" s="34" t="s">
-        <v>190</v>
-      </c>
+      <c r="F44" s="34"/>
       <c r="G44" s="15"/>
       <c r="H44" s="6"/>
       <c r="I44" s="8"/>
     </row>
-    <row r="45" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C45" s="14" t="s">
         <v>91</v>
       </c>
@@ -2545,9 +2455,7 @@
       <c r="E45" s="32" t="s">
         <v>90</v>
       </c>
-      <c r="F45" s="34" t="s">
-        <v>190</v>
-      </c>
+      <c r="F45" s="34"/>
       <c r="G45" s="15"/>
       <c r="H45" s="6"/>
       <c r="I45" s="8"/>
@@ -2563,13 +2471,13 @@
         <v>93</v>
       </c>
       <c r="F46" s="34" t="s">
-        <v>250</v>
+        <v>223</v>
       </c>
       <c r="G46" s="15"/>
       <c r="H46" s="6"/>
       <c r="I46" s="8"/>
     </row>
-    <row r="47" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C47" s="14" t="s">
         <v>94</v>
       </c>
@@ -2586,35 +2494,35 @@
       <c r="H47" s="6"/>
       <c r="I47" s="8"/>
     </row>
-    <row r="48" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C48" s="14" t="s">
         <v>95</v>
       </c>
       <c r="D48" s="31" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="E48" s="32" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="F48" s="34" t="s">
-        <v>191</v>
+        <v>223</v>
       </c>
       <c r="G48" s="15"/>
       <c r="H48" s="6"/>
       <c r="I48" s="8"/>
     </row>
-    <row r="49" spans="3:9" ht="93.75" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:9" x14ac:dyDescent="0.25">
       <c r="C49" s="36" t="s">
         <v>96</v>
       </c>
       <c r="D49" s="37" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E49" s="38" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="F49" s="35" t="s">
-        <v>190</v>
+        <v>222</v>
       </c>
       <c r="G49" s="39"/>
       <c r="H49" s="40"/>
@@ -2622,13 +2530,13 @@
     </row>
     <row r="50" spans="3:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C50" s="47" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="D50" s="47" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E50" s="47" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="F50" s="47"/>
       <c r="G50" s="48"/>
@@ -2637,13 +2545,13 @@
     </row>
     <row r="51" spans="3:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C51" s="47" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="D51" s="47" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E51" s="47" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="F51" s="47"/>
       <c r="G51" s="48"/>
@@ -2652,20 +2560,20 @@
     </row>
     <row r="52" spans="3:9" s="46" customFormat="1" x14ac:dyDescent="0.25">
       <c r="C52" s="47" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="D52" s="47" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="E52" s="47" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="F52" s="47"/>
       <c r="G52" s="48"/>
       <c r="H52" s="48"/>
       <c r="I52" s="48"/>
     </row>
-    <row r="53" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C53" s="41" t="s">
         <v>97</v>
       </c>
@@ -2676,13 +2584,13 @@
         <v>27</v>
       </c>
       <c r="F53" s="42" t="s">
-        <v>241</v>
+        <v>221</v>
       </c>
       <c r="G53" s="44"/>
       <c r="H53" s="45"/>
       <c r="I53" s="8"/>
     </row>
-    <row r="54" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C54" s="14" t="s">
         <v>98</v>
       </c>
@@ -2693,13 +2601,13 @@
         <v>27</v>
       </c>
       <c r="F54" s="31" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="G54" s="15"/>
       <c r="H54" s="6"/>
       <c r="I54" s="8"/>
     </row>
-    <row r="55" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C55" s="14" t="s">
         <v>99</v>
       </c>
@@ -2710,7 +2618,7 @@
         <v>27</v>
       </c>
       <c r="F55" s="31" t="s">
-        <v>243</v>
+        <v>221</v>
       </c>
       <c r="G55" s="15"/>
       <c r="H55" s="6"/>
@@ -2727,7 +2635,7 @@
         <v>27</v>
       </c>
       <c r="F56" s="31" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="G56" s="15"/>
       <c r="H56" s="6"/>
@@ -2798,7 +2706,7 @@
         <v>105</v>
       </c>
       <c r="D61" s="31" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E61" s="32" t="s">
         <v>31</v>
@@ -2813,12 +2721,14 @@
         <v>30</v>
       </c>
       <c r="D62" s="31" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E62" s="32" t="s">
         <v>93</v>
       </c>
-      <c r="F62" s="31"/>
+      <c r="F62" s="31" t="s">
+        <v>223</v>
+      </c>
       <c r="G62" s="15"/>
       <c r="H62" s="6"/>
       <c r="I62" s="8"/>
@@ -2828,13 +2738,13 @@
         <v>106</v>
       </c>
       <c r="D63" s="31" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="E63" s="32" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="F63" s="31" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="G63" s="15"/>
       <c r="H63" s="6"/>
@@ -2851,7 +2761,7 @@
         <v>34</v>
       </c>
       <c r="F64" s="31" t="s">
-        <v>196</v>
+        <v>189</v>
       </c>
       <c r="G64" s="15"/>
       <c r="H64" s="6"/>
@@ -2883,13 +2793,13 @@
         <v>37</v>
       </c>
       <c r="F66" s="31" t="s">
-        <v>232</v>
+        <v>219</v>
       </c>
       <c r="G66" s="15"/>
       <c r="H66" s="6"/>
       <c r="I66" s="8"/>
     </row>
-    <row r="67" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="14" t="s">
         <v>108</v>
       </c>
@@ -2900,13 +2810,13 @@
         <v>37</v>
       </c>
       <c r="F67" s="31" t="s">
-        <v>268</v>
+        <v>232</v>
       </c>
       <c r="G67" s="15"/>
       <c r="H67" s="6"/>
       <c r="I67" s="8"/>
     </row>
-    <row r="68" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C68" s="14" t="s">
         <v>109</v>
       </c>
@@ -2917,13 +2827,13 @@
         <v>37</v>
       </c>
       <c r="F68" s="31" t="s">
-        <v>269</v>
+        <v>232</v>
       </c>
       <c r="G68" s="15"/>
       <c r="H68" s="6"/>
       <c r="I68" s="8"/>
     </row>
-    <row r="69" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C69" s="14" t="s">
         <v>110</v>
       </c>
@@ -2934,13 +2844,13 @@
         <v>37</v>
       </c>
       <c r="F69" s="31" t="s">
-        <v>269</v>
+        <v>232</v>
       </c>
       <c r="G69" s="15"/>
       <c r="H69" s="6"/>
       <c r="I69" s="8"/>
     </row>
-    <row r="70" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C70" s="14" t="s">
         <v>111</v>
       </c>
@@ -2951,13 +2861,13 @@
         <v>37</v>
       </c>
       <c r="F70" s="31" t="s">
-        <v>258</v>
+        <v>233</v>
       </c>
       <c r="G70" s="15"/>
       <c r="H70" s="6"/>
       <c r="I70" s="8"/>
     </row>
-    <row r="71" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C71" s="14" t="s">
         <v>112</v>
       </c>
@@ -2968,7 +2878,7 @@
         <v>37</v>
       </c>
       <c r="F71" s="31" t="s">
-        <v>233</v>
+        <v>234</v>
       </c>
       <c r="G71" s="15"/>
       <c r="H71" s="6"/>
@@ -2985,13 +2895,13 @@
         <v>39</v>
       </c>
       <c r="F72" s="31" t="s">
-        <v>270</v>
+        <v>235</v>
       </c>
       <c r="G72" s="15"/>
       <c r="H72" s="6"/>
       <c r="I72" s="8"/>
     </row>
-    <row r="73" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C73" s="14" t="s">
         <v>40</v>
       </c>
@@ -3002,7 +2912,7 @@
         <v>41</v>
       </c>
       <c r="F73" s="31" t="s">
-        <v>271</v>
+        <v>236</v>
       </c>
       <c r="G73" s="15"/>
       <c r="H73" s="6"/>
@@ -3019,13 +2929,13 @@
         <v>42</v>
       </c>
       <c r="F74" s="31" t="s">
-        <v>274</v>
+        <v>237</v>
       </c>
       <c r="G74" s="15"/>
       <c r="H74" s="6"/>
       <c r="I74" s="8"/>
     </row>
-    <row r="75" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C75" s="14" t="s">
         <v>114</v>
       </c>
@@ -3036,7 +2946,7 @@
         <v>42</v>
       </c>
       <c r="F75" s="31" t="s">
-        <v>253</v>
+        <v>238</v>
       </c>
       <c r="G75" s="15"/>
       <c r="H75" s="6"/>
@@ -3053,7 +2963,7 @@
         <v>42</v>
       </c>
       <c r="F76" s="31" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="G76" s="15"/>
       <c r="H76" s="6"/>
@@ -3070,7 +2980,7 @@
         <v>43</v>
       </c>
       <c r="F77" s="31" t="s">
-        <v>227</v>
+        <v>240</v>
       </c>
       <c r="G77" s="15"/>
       <c r="H77" s="6"/>
@@ -3084,16 +2994,16 @@
         <v>32</v>
       </c>
       <c r="E78" s="32" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="F78" s="31" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G78" s="15"/>
       <c r="H78" s="6"/>
       <c r="I78" s="8"/>
     </row>
-    <row r="79" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C79" s="14" t="s">
         <v>117</v>
       </c>
@@ -3104,7 +3014,7 @@
         <v>42</v>
       </c>
       <c r="F79" s="31" t="s">
-        <v>263</v>
+        <v>240</v>
       </c>
       <c r="G79" s="15"/>
       <c r="H79" s="6"/>
@@ -3121,7 +3031,7 @@
         <v>42</v>
       </c>
       <c r="F80" s="31" t="s">
-        <v>253</v>
+        <v>241</v>
       </c>
       <c r="G80" s="15"/>
       <c r="H80" s="6"/>
@@ -3138,7 +3048,7 @@
         <v>45</v>
       </c>
       <c r="F81" s="31" t="s">
-        <v>264</v>
+        <v>242</v>
       </c>
       <c r="G81" s="15"/>
       <c r="H81" s="6"/>
@@ -3155,7 +3065,7 @@
         <v>45</v>
       </c>
       <c r="F82" s="31" t="s">
-        <v>264</v>
+        <v>243</v>
       </c>
       <c r="G82" s="15"/>
       <c r="H82" s="6"/>
@@ -3178,7 +3088,7 @@
       <c r="H83" s="6"/>
       <c r="I83" s="8"/>
     </row>
-    <row r="84" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C84" s="14" t="s">
         <v>122</v>
       </c>
@@ -3189,13 +3099,13 @@
         <v>46</v>
       </c>
       <c r="F84" s="31" t="s">
-        <v>198</v>
+        <v>240</v>
       </c>
       <c r="G84" s="15"/>
       <c r="H84" s="6"/>
       <c r="I84" s="8"/>
     </row>
-    <row r="85" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C85" s="14" t="s">
         <v>123</v>
       </c>
@@ -3206,13 +3116,13 @@
         <v>46</v>
       </c>
       <c r="F85" s="31" t="s">
-        <v>198</v>
+        <v>244</v>
       </c>
       <c r="G85" s="15"/>
       <c r="H85" s="6"/>
       <c r="I85" s="8"/>
     </row>
-    <row r="86" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C86" s="14" t="s">
         <v>124</v>
       </c>
@@ -3222,14 +3132,12 @@
       <c r="E86" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F86" s="31" t="s">
-        <v>236</v>
-      </c>
+      <c r="F86" s="31"/>
       <c r="G86" s="15"/>
       <c r="H86" s="6"/>
       <c r="I86" s="8"/>
     </row>
-    <row r="87" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C87" s="14" t="s">
         <v>126</v>
       </c>
@@ -3239,14 +3147,12 @@
       <c r="E87" s="32" t="s">
         <v>125</v>
       </c>
-      <c r="F87" s="31" t="s">
-        <v>236</v>
-      </c>
+      <c r="F87" s="31"/>
       <c r="G87" s="15"/>
       <c r="H87" s="6"/>
       <c r="I87" s="8"/>
     </row>
-    <row r="88" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C88" s="14" t="s">
         <v>127</v>
       </c>
@@ -3257,13 +3163,13 @@
         <v>128</v>
       </c>
       <c r="F88" s="31" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="G88" s="15"/>
       <c r="H88" s="6"/>
       <c r="I88" s="8"/>
     </row>
-    <row r="89" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C89" s="14" t="s">
         <v>129</v>
       </c>
@@ -3271,10 +3177,10 @@
         <v>32</v>
       </c>
       <c r="E89" s="32" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F89" s="31" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="G89" s="15"/>
       <c r="H89" s="6"/>
@@ -3288,10 +3194,10 @@
         <v>32</v>
       </c>
       <c r="E90" s="32" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F90" s="31" t="s">
-        <v>194</v>
+        <v>188</v>
       </c>
       <c r="G90" s="15"/>
       <c r="H90" s="6"/>
@@ -3305,10 +3211,10 @@
         <v>32</v>
       </c>
       <c r="E91" s="32" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F91" s="31" t="s">
-        <v>273</v>
+        <v>227</v>
       </c>
       <c r="G91" s="15"/>
       <c r="H91" s="6"/>
@@ -3322,7 +3228,7 @@
         <v>32</v>
       </c>
       <c r="E92" s="32" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F92" s="31"/>
       <c r="G92" s="15"/>
@@ -3337,10 +3243,10 @@
         <v>32</v>
       </c>
       <c r="E93" s="32" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F93" s="31" t="s">
-        <v>272</v>
+        <v>226</v>
       </c>
       <c r="G93" s="15"/>
       <c r="H93" s="6"/>
@@ -3354,9 +3260,11 @@
         <v>32</v>
       </c>
       <c r="E94" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="F94" s="31"/>
+        <v>191</v>
+      </c>
+      <c r="F94" s="31" t="s">
+        <v>240</v>
+      </c>
       <c r="G94" s="15"/>
       <c r="H94" s="6"/>
       <c r="I94" s="8"/>
@@ -3369,7 +3277,7 @@
         <v>32</v>
       </c>
       <c r="E95" s="32" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F95" s="31"/>
       <c r="G95" s="15"/>
@@ -3384,11 +3292,9 @@
         <v>32</v>
       </c>
       <c r="E96" s="32" t="s">
-        <v>200</v>
-      </c>
-      <c r="F96" s="31" t="s">
-        <v>194</v>
-      </c>
+        <v>191</v>
+      </c>
+      <c r="F96" s="31"/>
       <c r="G96" s="15"/>
       <c r="H96" s="6"/>
       <c r="I96" s="8"/>
@@ -3401,10 +3307,10 @@
         <v>32</v>
       </c>
       <c r="E97" s="32" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="F97" s="31" t="s">
-        <v>197</v>
+        <v>190</v>
       </c>
       <c r="G97" s="15"/>
       <c r="H97" s="6"/>
@@ -3412,13 +3318,13 @@
     </row>
     <row r="98" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C98" s="14" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="D98" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E98" s="32" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="F98" s="31"/>
       <c r="G98" s="15"/>
@@ -3427,13 +3333,13 @@
     </row>
     <row r="99" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C99" s="14" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="D99" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E99" s="32" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="F99" s="31"/>
       <c r="G99" s="15"/>
@@ -3442,13 +3348,13 @@
     </row>
     <row r="100" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C100" s="14" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="D100" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E100" s="32" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="F100" s="31"/>
       <c r="G100" s="15"/>
@@ -3457,13 +3363,13 @@
     </row>
     <row r="101" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C101" s="14" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="D101" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E101" s="32" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="F101" s="31"/>
       <c r="G101" s="15"/>
@@ -3472,20 +3378,22 @@
     </row>
     <row r="102" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C102" s="14" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="D102" s="31" t="s">
         <v>32</v>
       </c>
       <c r="E102" s="32" t="s">
-        <v>226</v>
-      </c>
-      <c r="F102" s="31"/>
+        <v>217</v>
+      </c>
+      <c r="F102" s="31" t="s">
+        <v>240</v>
+      </c>
       <c r="G102" s="15"/>
       <c r="H102" s="6"/>
       <c r="I102" s="8"/>
     </row>
-    <row r="103" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C103" s="14" t="s">
         <v>138</v>
       </c>
@@ -3496,7 +3404,7 @@
         <v>20</v>
       </c>
       <c r="F103" s="31" t="s">
-        <v>259</v>
+        <v>247</v>
       </c>
       <c r="G103" s="15"/>
       <c r="H103" s="6"/>
@@ -3512,14 +3420,12 @@
       <c r="E104" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F104" s="31" t="s">
-        <v>187</v>
-      </c>
+      <c r="F104" s="31"/>
       <c r="G104" s="15"/>
       <c r="H104" s="6"/>
       <c r="I104" s="8"/>
     </row>
-    <row r="105" spans="3:9" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C105" s="14" t="s">
         <v>140</v>
       </c>
@@ -3530,7 +3436,7 @@
         <v>20</v>
       </c>
       <c r="F105" s="31" t="s">
-        <v>260</v>
+        <v>246</v>
       </c>
       <c r="G105" s="15"/>
       <c r="H105" s="6"/>
@@ -3546,14 +3452,12 @@
       <c r="E106" s="32" t="s">
         <v>20</v>
       </c>
-      <c r="F106" s="31" t="s">
-        <v>187</v>
-      </c>
+      <c r="F106" s="31"/>
       <c r="G106" s="15"/>
       <c r="H106" s="6"/>
       <c r="I106" s="8"/>
     </row>
-    <row r="107" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C107" s="14" t="s">
         <v>142</v>
       </c>
@@ -3564,7 +3468,7 @@
         <v>20</v>
       </c>
       <c r="F107" s="31" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="G107" s="15"/>
       <c r="H107" s="6"/>
@@ -3581,7 +3485,7 @@
         <v>20</v>
       </c>
       <c r="F108" s="31" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="G108" s="15"/>
       <c r="H108" s="6"/>
@@ -3592,13 +3496,13 @@
         <v>48</v>
       </c>
       <c r="D109" s="31" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E109" s="32" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="F109" s="31" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
       <c r="G109" s="15"/>
       <c r="H109" s="6"/>
@@ -3609,19 +3513,19 @@
         <v>49</v>
       </c>
       <c r="D110" s="31" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E110" s="32" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F110" s="31" t="s">
-        <v>258</v>
+        <v>250</v>
       </c>
       <c r="G110" s="15"/>
       <c r="H110" s="6"/>
       <c r="I110" s="8"/>
     </row>
-    <row r="111" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="14" t="s">
         <v>50</v>
       </c>
@@ -3632,7 +3536,7 @@
         <v>17</v>
       </c>
       <c r="F111" s="31" t="s">
-        <v>228</v>
+        <v>251</v>
       </c>
       <c r="G111" s="15"/>
       <c r="H111" s="6"/>
@@ -3648,9 +3552,7 @@
       <c r="E112" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F112" s="31" t="s">
-        <v>187</v>
-      </c>
+      <c r="F112" s="31"/>
       <c r="G112" s="15"/>
       <c r="H112" s="6"/>
       <c r="I112" s="8"/>
@@ -3665,9 +3567,7 @@
       <c r="E113" s="32" t="s">
         <v>18</v>
       </c>
-      <c r="F113" s="31" t="s">
-        <v>187</v>
-      </c>
+      <c r="F113" s="31"/>
       <c r="G113" s="15"/>
       <c r="H113" s="6"/>
       <c r="I113" s="8"/>
@@ -3682,9 +3582,7 @@
       <c r="E114" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F114" s="31" t="s">
-        <v>187</v>
-      </c>
+      <c r="F114" s="31"/>
       <c r="G114" s="15"/>
       <c r="H114" s="6"/>
       <c r="I114" s="8"/>
@@ -3699,9 +3597,7 @@
       <c r="E115" s="32" t="s">
         <v>19</v>
       </c>
-      <c r="F115" s="31" t="s">
-        <v>187</v>
-      </c>
+      <c r="F115" s="31"/>
       <c r="G115" s="15"/>
       <c r="H115" s="6"/>
       <c r="I115" s="8"/>
@@ -3717,13 +3613,13 @@
         <v>148</v>
       </c>
       <c r="F116" s="31" t="s">
-        <v>237</v>
+        <v>252</v>
       </c>
       <c r="G116" s="15"/>
       <c r="H116" s="6"/>
       <c r="I116" s="8"/>
     </row>
-    <row r="117" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C117" s="14" t="s">
         <v>149</v>
       </c>
@@ -3733,14 +3629,12 @@
       <c r="E117" s="32" t="s">
         <v>148</v>
       </c>
-      <c r="F117" s="31" t="s">
-        <v>254</v>
-      </c>
+      <c r="F117" s="31"/>
       <c r="G117" s="15"/>
       <c r="H117" s="6"/>
       <c r="I117" s="8"/>
     </row>
-    <row r="118" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C118" s="14" t="s">
         <v>150</v>
       </c>
@@ -3751,13 +3645,13 @@
         <v>148</v>
       </c>
       <c r="F118" s="31" t="s">
-        <v>234</v>
+        <v>253</v>
       </c>
       <c r="G118" s="15"/>
       <c r="H118" s="6"/>
       <c r="I118" s="8"/>
     </row>
-    <row r="119" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C119" s="14" t="s">
         <v>151</v>
       </c>
@@ -3768,13 +3662,13 @@
         <v>152</v>
       </c>
       <c r="F119" s="31" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G119" s="15"/>
       <c r="H119" s="6"/>
       <c r="I119" s="8"/>
     </row>
-    <row r="120" spans="3:9" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C120" s="14" t="s">
         <v>153</v>
       </c>
@@ -3785,13 +3679,13 @@
         <v>154</v>
       </c>
       <c r="F120" s="31" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G120" s="15"/>
       <c r="H120" s="6"/>
       <c r="I120" s="8"/>
     </row>
-    <row r="121" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C121" s="14" t="s">
         <v>155</v>
       </c>
@@ -3802,7 +3696,7 @@
         <v>156</v>
       </c>
       <c r="F121" s="31" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G121" s="15"/>
       <c r="H121" s="6"/>
@@ -3818,9 +3712,7 @@
       <c r="E122" s="32" t="s">
         <v>158</v>
       </c>
-      <c r="F122" s="31" t="s">
-        <v>187</v>
-      </c>
+      <c r="F122" s="31"/>
       <c r="G122" s="15"/>
       <c r="H122" s="6"/>
       <c r="I122" s="8"/>
@@ -3836,13 +3728,13 @@
         <v>128</v>
       </c>
       <c r="F123" s="31" t="s">
-        <v>258</v>
+        <v>248</v>
       </c>
       <c r="G123" s="15"/>
       <c r="H123" s="6"/>
       <c r="I123" s="8"/>
     </row>
-    <row r="124" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C124" s="14" t="s">
         <v>160</v>
       </c>
@@ -3852,14 +3744,12 @@
       <c r="E124" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F124" s="31" t="s">
-        <v>258</v>
-      </c>
+      <c r="F124" s="31"/>
       <c r="G124" s="15"/>
       <c r="H124" s="6"/>
       <c r="I124" s="8"/>
     </row>
-    <row r="125" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C125" s="14" t="s">
         <v>162</v>
       </c>
@@ -3869,14 +3759,12 @@
       <c r="E125" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F125" s="31" t="s">
-        <v>258</v>
-      </c>
+      <c r="F125" s="31"/>
       <c r="G125" s="15"/>
       <c r="H125" s="6"/>
       <c r="I125" s="8"/>
     </row>
-    <row r="126" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C126" s="14" t="s">
         <v>163</v>
       </c>
@@ -3886,14 +3774,12 @@
       <c r="E126" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F126" s="31" t="s">
-        <v>258</v>
-      </c>
+      <c r="F126" s="31"/>
       <c r="G126" s="15"/>
       <c r="H126" s="6"/>
       <c r="I126" s="8"/>
     </row>
-    <row r="127" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C127" s="14" t="s">
         <v>164</v>
       </c>
@@ -3903,14 +3789,12 @@
       <c r="E127" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F127" s="31" t="s">
-        <v>258</v>
-      </c>
+      <c r="F127" s="31"/>
       <c r="G127" s="15"/>
       <c r="H127" s="6"/>
       <c r="I127" s="8"/>
     </row>
-    <row r="128" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C128" s="14" t="s">
         <v>165</v>
       </c>
@@ -3920,9 +3804,7 @@
       <c r="E128" s="32" t="s">
         <v>161</v>
       </c>
-      <c r="F128" s="31" t="s">
-        <v>258</v>
-      </c>
+      <c r="F128" s="31"/>
       <c r="G128" s="15"/>
       <c r="H128" s="6"/>
       <c r="I128" s="8"/>
@@ -3932,19 +3814,19 @@
         <v>166</v>
       </c>
       <c r="D129" s="31" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="E129" s="32" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="F129" s="31" t="s">
-        <v>187</v>
+        <v>257</v>
       </c>
       <c r="G129" s="15"/>
       <c r="H129" s="6"/>
       <c r="I129" s="8"/>
     </row>
-    <row r="130" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C130" s="14" t="s">
         <v>167</v>
       </c>
@@ -3955,13 +3837,13 @@
         <v>20</v>
       </c>
       <c r="F130" s="31" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G130" s="15"/>
       <c r="H130" s="6"/>
       <c r="I130" s="8"/>
     </row>
-    <row r="131" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C131" s="14" t="s">
         <v>168</v>
       </c>
@@ -3972,13 +3854,13 @@
         <v>20</v>
       </c>
       <c r="F131" s="31" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G131" s="15"/>
       <c r="H131" s="6"/>
       <c r="I131" s="8"/>
     </row>
-    <row r="132" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C132" s="14" t="s">
         <v>169</v>
       </c>
@@ -3989,13 +3871,13 @@
         <v>20</v>
       </c>
       <c r="F132" s="31" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G132" s="15"/>
       <c r="H132" s="6"/>
       <c r="I132" s="8"/>
     </row>
-    <row r="133" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C133" s="14" t="s">
         <v>170</v>
       </c>
@@ -4006,7 +3888,7 @@
         <v>20</v>
       </c>
       <c r="F133" s="31" t="s">
-        <v>261</v>
+        <v>257</v>
       </c>
       <c r="G133" s="15"/>
       <c r="H133" s="6"/>
@@ -4020,10 +3902,10 @@
         <v>47</v>
       </c>
       <c r="E134" s="32" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F134" s="31" t="s">
-        <v>262</v>
+        <v>248</v>
       </c>
       <c r="G134" s="15"/>
       <c r="H134" s="6"/>
@@ -4037,10 +3919,10 @@
         <v>47</v>
       </c>
       <c r="E135" s="32" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="F135" s="31" t="s">
-        <v>252</v>
+        <v>225</v>
       </c>
       <c r="G135" s="15"/>
       <c r="H135" s="6"/>
@@ -4057,7 +3939,7 @@
         <v>52</v>
       </c>
       <c r="F136" s="31" t="s">
-        <v>238</v>
+        <v>258</v>
       </c>
       <c r="G136" s="15"/>
       <c r="H136" s="6"/>
@@ -4074,7 +3956,7 @@
         <v>52</v>
       </c>
       <c r="F137" s="31" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="G137" s="15"/>
       <c r="H137" s="6"/>
@@ -4091,7 +3973,7 @@
         <v>52</v>
       </c>
       <c r="F138" s="31" t="s">
-        <v>239</v>
+        <v>220</v>
       </c>
       <c r="G138" s="15"/>
       <c r="H138" s="6"/>
@@ -4108,13 +3990,13 @@
         <v>53</v>
       </c>
       <c r="F139" s="31" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="G139" s="15"/>
       <c r="H139" s="6"/>
       <c r="I139" s="8"/>
     </row>
-    <row r="140" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C140" s="14" t="s">
         <v>177</v>
       </c>
@@ -4125,13 +4007,13 @@
         <v>53</v>
       </c>
       <c r="F140" s="31" t="s">
-        <v>266</v>
+        <v>259</v>
       </c>
       <c r="G140" s="15"/>
       <c r="H140" s="6"/>
       <c r="I140" s="8"/>
     </row>
-    <row r="141" spans="3:9" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C141" s="14" t="s">
         <v>178</v>
       </c>
@@ -4142,13 +4024,13 @@
         <v>53</v>
       </c>
       <c r="F141" s="31" t="s">
-        <v>195</v>
+        <v>260</v>
       </c>
       <c r="G141" s="15"/>
       <c r="H141" s="6"/>
       <c r="I141" s="8"/>
     </row>
-    <row r="142" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C142" s="14" t="s">
         <v>179</v>
       </c>
@@ -4159,13 +4041,13 @@
         <v>53</v>
       </c>
       <c r="F142" s="31" t="s">
-        <v>229</v>
+        <v>261</v>
       </c>
       <c r="G142" s="15"/>
       <c r="H142" s="6"/>
       <c r="I142" s="8"/>
     </row>
-    <row r="143" spans="3:9" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:9" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C143" s="14" t="s">
         <v>180</v>
       </c>
@@ -4176,7 +4058,7 @@
         <v>53</v>
       </c>
       <c r="F143" s="31" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="G143" s="15"/>
       <c r="H143" s="6"/>
@@ -4193,7 +4075,7 @@
         <v>55</v>
       </c>
       <c r="F144" s="31" t="s">
-        <v>189</v>
+        <v>263</v>
       </c>
       <c r="G144" s="15"/>
       <c r="H144" s="6"/>

</xml_diff>

<commit_message>
Review RTM after linking to development
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Documents\GitHub\Internet-Banking-System\PM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\ITI\Internet-Banking-System\Internet-Banking-System\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1800" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="1800" windowWidth="20496" windowHeight="7752"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="635" uniqueCount="300">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="638" uniqueCount="302">
   <si>
     <t>Author</t>
   </si>
@@ -992,6 +992,16 @@
   </si>
   <si>
     <t>Adding Design id up on quality assurance demand</t>
+  </si>
+  <si>
+    <t>Salsabeel</t>
+  </si>
+  <si>
+    <t xml:space="preserve">(1) Reg R007,8,9,10,11,12,13,18,19,21,22,23,26,27,28 &gt;&gt; missing element ids
+(2) Log R004,5,6,7,8,11 &gt;&gt; missing element ids
+(3) PT R035 &gt;&gt; missing some files names and element id
+(4) PT R034 &gt;&gt; incorrect linking to function name
+</t>
   </si>
 </sst>
 </file>
@@ -1549,6 +1559,123 @@
     <xf numFmtId="0" fontId="6" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1558,68 +1685,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="15" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -1627,81 +1712,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="13" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="15" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="21" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="7" fillId="0" borderId="32" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1987,112 +2001,112 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y155"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="G1" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
+      <selection activeCell="M14" sqref="M14"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="2" max="2" width="9" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="34.28515625" style="4" customWidth="1"/>
-    <col min="5" max="5" width="26.28515625" style="7" customWidth="1"/>
-    <col min="6" max="6" width="27.7109375" style="7" customWidth="1"/>
-    <col min="7" max="7" width="38.42578125" style="7" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="4" customWidth="1"/>
-    <col min="9" max="9" width="31.7109375" style="7" customWidth="1"/>
-    <col min="10" max="10" width="32.140625" customWidth="1"/>
-    <col min="11" max="11" width="28.28515625" customWidth="1"/>
+    <col min="3" max="3" width="18.6640625" customWidth="1"/>
+    <col min="4" max="4" width="34.33203125" style="4" customWidth="1"/>
+    <col min="5" max="5" width="26.33203125" style="7" customWidth="1"/>
+    <col min="6" max="6" width="27.6640625" style="7" customWidth="1"/>
+    <col min="7" max="7" width="38.44140625" style="7" customWidth="1"/>
+    <col min="8" max="8" width="25.5546875" style="4" customWidth="1"/>
+    <col min="9" max="9" width="31.6640625" style="7" customWidth="1"/>
+    <col min="10" max="10" width="32.109375" customWidth="1"/>
+    <col min="11" max="11" width="28.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="2" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="38" t="s">
+    <row r="1" spans="2:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35"/>
+    <row r="2" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B2" s="55" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="39"/>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
-      <c r="G2" s="39"/>
-      <c r="H2" s="39"/>
-      <c r="I2" s="39"/>
-      <c r="J2" s="39"/>
-      <c r="K2" s="39"/>
-      <c r="L2" s="39"/>
-      <c r="M2" s="40"/>
-    </row>
-    <row r="3" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="41"/>
-      <c r="C3" s="42"/>
-      <c r="D3" s="42"/>
-      <c r="E3" s="42"/>
-      <c r="F3" s="42"/>
-      <c r="G3" s="42"/>
-      <c r="H3" s="42"/>
-      <c r="I3" s="42"/>
-      <c r="J3" s="42"/>
-      <c r="K3" s="42"/>
-      <c r="L3" s="42"/>
-      <c r="M3" s="43"/>
-    </row>
-    <row r="4" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="41"/>
-      <c r="C4" s="42"/>
-      <c r="D4" s="42"/>
-      <c r="E4" s="42"/>
-      <c r="F4" s="42"/>
-      <c r="G4" s="42"/>
-      <c r="H4" s="42"/>
-      <c r="I4" s="42"/>
-      <c r="J4" s="42"/>
-      <c r="K4" s="42"/>
-      <c r="L4" s="42"/>
-      <c r="M4" s="43"/>
-    </row>
-    <row r="5" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="41"/>
-      <c r="C5" s="42"/>
-      <c r="D5" s="42"/>
-      <c r="E5" s="42"/>
-      <c r="F5" s="42"/>
-      <c r="G5" s="42"/>
-      <c r="H5" s="42"/>
-      <c r="I5" s="42"/>
-      <c r="J5" s="42"/>
-      <c r="K5" s="42"/>
-      <c r="L5" s="42"/>
-      <c r="M5" s="43"/>
-    </row>
-    <row r="6" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="41"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
-      <c r="H6" s="42"/>
-      <c r="I6" s="42"/>
-      <c r="J6" s="42"/>
-      <c r="K6" s="42"/>
-      <c r="L6" s="42"/>
-      <c r="M6" s="43"/>
-    </row>
-    <row r="7" spans="2:13" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="44"/>
-      <c r="C7" s="45"/>
-      <c r="D7" s="45"/>
-      <c r="E7" s="45"/>
-      <c r="F7" s="45"/>
-      <c r="G7" s="45"/>
-      <c r="H7" s="45"/>
-      <c r="I7" s="45"/>
-      <c r="J7" s="45"/>
-      <c r="K7" s="45"/>
-      <c r="L7" s="45"/>
-      <c r="M7" s="46"/>
-    </row>
-    <row r="8" spans="2:13" s="9" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="C2" s="56"/>
+      <c r="D2" s="56"/>
+      <c r="E2" s="56"/>
+      <c r="F2" s="56"/>
+      <c r="G2" s="56"/>
+      <c r="H2" s="56"/>
+      <c r="I2" s="56"/>
+      <c r="J2" s="56"/>
+      <c r="K2" s="56"/>
+      <c r="L2" s="56"/>
+      <c r="M2" s="57"/>
+    </row>
+    <row r="3" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B3" s="58"/>
+      <c r="C3" s="59"/>
+      <c r="D3" s="59"/>
+      <c r="E3" s="59"/>
+      <c r="F3" s="59"/>
+      <c r="G3" s="59"/>
+      <c r="H3" s="59"/>
+      <c r="I3" s="59"/>
+      <c r="J3" s="59"/>
+      <c r="K3" s="59"/>
+      <c r="L3" s="59"/>
+      <c r="M3" s="60"/>
+    </row>
+    <row r="4" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B4" s="58"/>
+      <c r="C4" s="59"/>
+      <c r="D4" s="59"/>
+      <c r="E4" s="59"/>
+      <c r="F4" s="59"/>
+      <c r="G4" s="59"/>
+      <c r="H4" s="59"/>
+      <c r="I4" s="59"/>
+      <c r="J4" s="59"/>
+      <c r="K4" s="59"/>
+      <c r="L4" s="59"/>
+      <c r="M4" s="60"/>
+    </row>
+    <row r="5" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="58"/>
+      <c r="C5" s="59"/>
+      <c r="D5" s="59"/>
+      <c r="E5" s="59"/>
+      <c r="F5" s="59"/>
+      <c r="G5" s="59"/>
+      <c r="H5" s="59"/>
+      <c r="I5" s="59"/>
+      <c r="J5" s="59"/>
+      <c r="K5" s="59"/>
+      <c r="L5" s="59"/>
+      <c r="M5" s="60"/>
+    </row>
+    <row r="6" spans="2:13" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="58"/>
+      <c r="C6" s="59"/>
+      <c r="D6" s="59"/>
+      <c r="E6" s="59"/>
+      <c r="F6" s="59"/>
+      <c r="G6" s="59"/>
+      <c r="H6" s="59"/>
+      <c r="I6" s="59"/>
+      <c r="J6" s="59"/>
+      <c r="K6" s="59"/>
+      <c r="L6" s="59"/>
+      <c r="M6" s="60"/>
+    </row>
+    <row r="7" spans="2:13" ht="14.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B7" s="61"/>
+      <c r="C7" s="62"/>
+      <c r="D7" s="62"/>
+      <c r="E7" s="62"/>
+      <c r="F7" s="62"/>
+      <c r="G7" s="62"/>
+      <c r="H7" s="62"/>
+      <c r="I7" s="62"/>
+      <c r="J7" s="62"/>
+      <c r="K7" s="62"/>
+      <c r="L7" s="62"/>
+      <c r="M7" s="63"/>
+    </row>
+    <row r="8" spans="2:13" s="9" customFormat="1" ht="14.4" customHeight="1" x14ac:dyDescent="0.3">
       <c r="B8" s="11"/>
       <c r="C8" s="11"/>
       <c r="D8" s="11"/>
@@ -2106,233 +2120,239 @@
       <c r="L8" s="11"/>
       <c r="M8" s="11"/>
     </row>
-    <row r="9" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="9" spans="2:13" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="1"/>
-      <c r="C9" s="48" t="s">
+      <c r="C9" s="64" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="48"/>
-      <c r="E9" s="48"/>
-      <c r="F9" s="48"/>
-      <c r="G9" s="48"/>
-      <c r="H9" s="48"/>
-      <c r="I9" s="48"/>
-      <c r="J9" s="47"/>
+      <c r="D9" s="64"/>
+      <c r="E9" s="64"/>
+      <c r="F9" s="64"/>
+      <c r="G9" s="64"/>
+      <c r="H9" s="64"/>
+      <c r="I9" s="64"/>
+      <c r="J9" s="65"/>
       <c r="K9" s="1"/>
     </row>
-    <row r="10" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C10" s="49" t="s">
+    <row r="10" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C10" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="D10" s="49" t="s">
+      <c r="D10" s="34" t="s">
         <v>6</v>
       </c>
-      <c r="E10" s="64" t="s">
+      <c r="E10" s="41" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="65" t="s">
+      <c r="F10" s="66" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="50"/>
-      <c r="H10" s="51" t="s">
+      <c r="G10" s="67"/>
+      <c r="H10" s="35" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="17" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="52" t="s">
+      <c r="J10" s="68" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="50"/>
-    </row>
-    <row r="11" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C11" s="61" t="s">
+      <c r="K10" s="67"/>
+    </row>
+    <row r="11" spans="2:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C11" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="D11" s="63">
+      <c r="D11" s="40">
         <v>1</v>
       </c>
-      <c r="E11" s="62" t="s">
+      <c r="E11" s="39" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="60" t="s">
+      <c r="F11" s="69" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="56"/>
-      <c r="H11" s="55"/>
+      <c r="G11" s="70"/>
+      <c r="H11" s="36"/>
       <c r="I11" s="20"/>
-      <c r="J11" s="53"/>
-      <c r="K11" s="54"/>
-    </row>
-    <row r="12" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C12" s="55" t="s">
+      <c r="J11" s="71"/>
+      <c r="K11" s="72"/>
+    </row>
+    <row r="12" spans="2:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C12" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D12" s="67">
+      <c r="D12" s="43">
         <v>2</v>
       </c>
-      <c r="E12" s="57">
+      <c r="E12" s="37">
         <v>43529</v>
       </c>
-      <c r="F12" s="68" t="s">
+      <c r="F12" s="76" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="69"/>
-      <c r="H12" s="70" t="s">
+      <c r="G12" s="77"/>
+      <c r="H12" s="44" t="s">
         <v>58</v>
       </c>
-      <c r="I12" s="71">
+      <c r="I12" s="45">
         <v>43529</v>
       </c>
-      <c r="J12" s="72" t="s">
+      <c r="J12" s="78" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="73"/>
-    </row>
-    <row r="13" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C13" s="55" t="s">
+      <c r="K12" s="79"/>
+    </row>
+    <row r="13" spans="2:13" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C13" s="36" t="s">
         <v>10</v>
       </c>
-      <c r="D13" s="67">
+      <c r="D13" s="43">
         <v>3</v>
       </c>
-      <c r="E13" s="66" t="s">
+      <c r="E13" s="42" t="s">
         <v>298</v>
       </c>
-      <c r="F13" s="58" t="s">
+      <c r="F13" s="83" t="s">
         <v>299</v>
       </c>
-      <c r="G13" s="59"/>
-      <c r="H13" s="83"/>
-      <c r="I13" s="84"/>
-      <c r="J13" s="85"/>
-      <c r="K13" s="86"/>
-    </row>
-    <row r="14" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C14" s="79" t="s">
+      <c r="G13" s="84"/>
+      <c r="H13" s="51"/>
+      <c r="I13" s="52"/>
+      <c r="J13" s="53"/>
+      <c r="K13" s="54"/>
+    </row>
+    <row r="14" spans="2:13" ht="96.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C14" s="49" t="s">
         <v>295</v>
       </c>
-      <c r="D14" s="67">
+      <c r="D14" s="43">
         <v>4</v>
       </c>
-      <c r="E14" s="77" t="s">
+      <c r="E14" s="47" t="s">
         <v>296</v>
       </c>
-      <c r="F14" s="82" t="s">
+      <c r="F14" s="81" t="s">
         <v>297</v>
       </c>
-      <c r="G14" s="81"/>
-      <c r="H14" s="78"/>
-      <c r="I14" s="77"/>
-      <c r="J14" s="75"/>
-      <c r="K14" s="76"/>
-    </row>
-    <row r="15" spans="2:13" x14ac:dyDescent="0.25">
-      <c r="D15" s="80"/>
-      <c r="E15" s="74"/>
-    </row>
-    <row r="17" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C17" s="37" t="s">
+      <c r="G14" s="82"/>
+      <c r="H14" s="48" t="s">
+        <v>300</v>
+      </c>
+      <c r="I14" s="47" t="s">
+        <v>296</v>
+      </c>
+      <c r="J14" s="86" t="s">
+        <v>301</v>
+      </c>
+      <c r="K14" s="85"/>
+    </row>
+    <row r="15" spans="2:13" x14ac:dyDescent="0.3">
+      <c r="D15" s="50"/>
+      <c r="E15" s="46"/>
+    </row>
+    <row r="17" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C17" s="80" t="s">
         <v>61</v>
       </c>
-      <c r="D17" s="37"/>
-      <c r="E17" s="37"/>
-      <c r="F17" s="37"/>
-      <c r="G17" s="37"/>
-      <c r="H17" s="37"/>
-      <c r="I17" s="37"/>
-      <c r="J17" s="37"/>
-      <c r="K17" s="37"/>
-    </row>
-    <row r="18" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="37"/>
-      <c r="D18" s="37"/>
-      <c r="E18" s="37"/>
-      <c r="F18" s="37"/>
-      <c r="G18" s="37"/>
-      <c r="H18" s="37"/>
-      <c r="I18" s="37"/>
-      <c r="J18" s="37"/>
-      <c r="K18" s="37"/>
-    </row>
-    <row r="19" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="37"/>
-      <c r="D19" s="37"/>
-      <c r="E19" s="37"/>
-      <c r="F19" s="37"/>
-      <c r="G19" s="37"/>
-      <c r="H19" s="37"/>
-      <c r="I19" s="37"/>
-      <c r="J19" s="37"/>
-      <c r="K19" s="37"/>
-    </row>
-    <row r="20" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="37"/>
-      <c r="D20" s="37"/>
-      <c r="E20" s="37"/>
-      <c r="F20" s="37"/>
-      <c r="G20" s="37"/>
-      <c r="H20" s="37"/>
-      <c r="I20" s="37"/>
-      <c r="J20" s="37"/>
-      <c r="K20" s="37"/>
-    </row>
-    <row r="21" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="37"/>
-      <c r="D21" s="37"/>
-      <c r="E21" s="37"/>
-      <c r="F21" s="37"/>
-      <c r="G21" s="37"/>
-      <c r="H21" s="37"/>
-      <c r="I21" s="37"/>
-      <c r="J21" s="37"/>
-      <c r="K21" s="37"/>
-    </row>
-    <row r="22" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="37"/>
-      <c r="D22" s="37"/>
-      <c r="E22" s="37"/>
-      <c r="F22" s="37"/>
-      <c r="G22" s="37"/>
-      <c r="H22" s="37"/>
-      <c r="I22" s="37"/>
-      <c r="J22" s="37"/>
-      <c r="K22" s="37"/>
-    </row>
-    <row r="23" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="37"/>
-      <c r="D23" s="37"/>
-      <c r="E23" s="37"/>
-      <c r="F23" s="37"/>
-      <c r="G23" s="37"/>
-      <c r="H23" s="37"/>
-      <c r="I23" s="37"/>
-      <c r="J23" s="37"/>
-      <c r="K23" s="37"/>
-    </row>
-    <row r="24" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="37"/>
-      <c r="D24" s="37"/>
-      <c r="E24" s="37"/>
-      <c r="F24" s="37"/>
-      <c r="G24" s="37"/>
-      <c r="H24" s="37"/>
-      <c r="I24" s="37"/>
-      <c r="J24" s="37"/>
-      <c r="K24" s="37"/>
-    </row>
-    <row r="25" spans="3:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C25" s="37"/>
-      <c r="D25" s="37"/>
-      <c r="E25" s="37"/>
-      <c r="F25" s="37"/>
-      <c r="G25" s="37"/>
-      <c r="H25" s="37"/>
-      <c r="I25" s="37"/>
-      <c r="J25" s="37"/>
-      <c r="K25" s="37"/>
-    </row>
-    <row r="26" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D17" s="80"/>
+      <c r="E17" s="80"/>
+      <c r="F17" s="80"/>
+      <c r="G17" s="80"/>
+      <c r="H17" s="80"/>
+      <c r="I17" s="80"/>
+      <c r="J17" s="80"/>
+      <c r="K17" s="80"/>
+    </row>
+    <row r="18" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C18" s="80"/>
+      <c r="D18" s="80"/>
+      <c r="E18" s="80"/>
+      <c r="F18" s="80"/>
+      <c r="G18" s="80"/>
+      <c r="H18" s="80"/>
+      <c r="I18" s="80"/>
+      <c r="J18" s="80"/>
+      <c r="K18" s="80"/>
+    </row>
+    <row r="19" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C19" s="80"/>
+      <c r="D19" s="80"/>
+      <c r="E19" s="80"/>
+      <c r="F19" s="80"/>
+      <c r="G19" s="80"/>
+      <c r="H19" s="80"/>
+      <c r="I19" s="80"/>
+      <c r="J19" s="80"/>
+      <c r="K19" s="80"/>
+    </row>
+    <row r="20" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C20" s="80"/>
+      <c r="D20" s="80"/>
+      <c r="E20" s="80"/>
+      <c r="F20" s="80"/>
+      <c r="G20" s="80"/>
+      <c r="H20" s="80"/>
+      <c r="I20" s="80"/>
+      <c r="J20" s="80"/>
+      <c r="K20" s="80"/>
+    </row>
+    <row r="21" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C21" s="80"/>
+      <c r="D21" s="80"/>
+      <c r="E21" s="80"/>
+      <c r="F21" s="80"/>
+      <c r="G21" s="80"/>
+      <c r="H21" s="80"/>
+      <c r="I21" s="80"/>
+      <c r="J21" s="80"/>
+      <c r="K21" s="80"/>
+    </row>
+    <row r="22" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C22" s="80"/>
+      <c r="D22" s="80"/>
+      <c r="E22" s="80"/>
+      <c r="F22" s="80"/>
+      <c r="G22" s="80"/>
+      <c r="H22" s="80"/>
+      <c r="I22" s="80"/>
+      <c r="J22" s="80"/>
+      <c r="K22" s="80"/>
+    </row>
+    <row r="23" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C23" s="80"/>
+      <c r="D23" s="80"/>
+      <c r="E23" s="80"/>
+      <c r="F23" s="80"/>
+      <c r="G23" s="80"/>
+      <c r="H23" s="80"/>
+      <c r="I23" s="80"/>
+      <c r="J23" s="80"/>
+      <c r="K23" s="80"/>
+    </row>
+    <row r="24" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="C24" s="80"/>
+      <c r="D24" s="80"/>
+      <c r="E24" s="80"/>
+      <c r="F24" s="80"/>
+      <c r="G24" s="80"/>
+      <c r="H24" s="80"/>
+      <c r="I24" s="80"/>
+      <c r="J24" s="80"/>
+      <c r="K24" s="80"/>
+    </row>
+    <row r="25" spans="3:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="C25" s="80"/>
+      <c r="D25" s="80"/>
+      <c r="E25" s="80"/>
+      <c r="F25" s="80"/>
+      <c r="G25" s="80"/>
+      <c r="H25" s="80"/>
+      <c r="I25" s="80"/>
+      <c r="J25" s="80"/>
+      <c r="K25" s="80"/>
+    </row>
+    <row r="26" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C26" s="16"/>
       <c r="D26" s="17" t="s">
         <v>63</v>
@@ -2360,7 +2380,7 @@
       </c>
       <c r="L26" s="2"/>
     </row>
-    <row r="27" spans="3:12" s="4" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="27" spans="3:12" s="4" customFormat="1" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C27" s="12"/>
       <c r="D27" s="22" t="s">
         <v>287</v>
@@ -2386,7 +2406,7 @@
       </c>
       <c r="L27" s="3"/>
     </row>
-    <row r="28" spans="3:12" s="5" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="28" spans="3:12" s="5" customFormat="1" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C28" s="13"/>
       <c r="D28" s="19" t="s">
         <v>65</v>
@@ -2412,7 +2432,7 @@
       </c>
       <c r="L28" s="2"/>
     </row>
-    <row r="29" spans="3:12" s="5" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="29" spans="3:12" s="5" customFormat="1" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C29" s="13"/>
       <c r="D29" s="23" t="s">
         <v>67</v>
@@ -2438,7 +2458,7 @@
       </c>
       <c r="L29" s="2"/>
     </row>
-    <row r="30" spans="3:12" s="5" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="3:12" s="5" customFormat="1" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C30" s="13"/>
       <c r="D30" s="18" t="s">
         <v>68</v>
@@ -2464,7 +2484,7 @@
       </c>
       <c r="L30" s="2"/>
     </row>
-    <row r="31" spans="3:12" s="5" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="31" spans="3:12" s="5" customFormat="1" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C31" s="13"/>
       <c r="D31" s="22" t="s">
         <v>69</v>
@@ -2490,7 +2510,7 @@
       </c>
       <c r="L31" s="2"/>
     </row>
-    <row r="32" spans="3:12" s="5" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="32" spans="3:12" s="5" customFormat="1" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C32" s="13"/>
       <c r="D32" s="20" t="s">
         <v>70</v>
@@ -2514,7 +2534,7 @@
       <c r="K32" s="30"/>
       <c r="L32" s="2"/>
     </row>
-    <row r="33" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="33" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="14"/>
       <c r="D33" s="22" t="s">
         <v>71</v>
@@ -2540,7 +2560,7 @@
       </c>
       <c r="L33" s="3"/>
     </row>
-    <row r="34" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="34" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C34" s="14"/>
       <c r="D34" s="23" t="s">
         <v>72</v>
@@ -2564,7 +2584,7 @@
       </c>
       <c r="L34" s="3"/>
     </row>
-    <row r="35" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="35" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C35" s="14"/>
       <c r="D35" s="23" t="s">
         <v>62</v>
@@ -2588,7 +2608,7 @@
       </c>
       <c r="L35" s="3"/>
     </row>
-    <row r="36" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="36" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C36" s="14"/>
       <c r="D36" s="22" t="s">
         <v>73</v>
@@ -2612,7 +2632,7 @@
       </c>
       <c r="L36" s="3"/>
     </row>
-    <row r="37" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="37" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="14"/>
       <c r="D37" s="20" t="s">
         <v>75</v>
@@ -2636,7 +2656,7 @@
       </c>
       <c r="L37" s="3"/>
     </row>
-    <row r="38" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="38" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C38" s="14"/>
       <c r="D38" s="23" t="s">
         <v>76</v>
@@ -2660,7 +2680,7 @@
       </c>
       <c r="L38" s="3"/>
     </row>
-    <row r="39" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="39" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C39" s="14"/>
       <c r="D39" s="18" t="s">
         <v>77</v>
@@ -2684,7 +2704,7 @@
       </c>
       <c r="L39" s="3"/>
     </row>
-    <row r="40" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="40" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C40" s="14"/>
       <c r="D40" s="22" t="s">
         <v>78</v>
@@ -2702,7 +2722,7 @@
       <c r="K40" s="29"/>
       <c r="L40" s="3"/>
     </row>
-    <row r="41" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="41" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C41" s="14"/>
       <c r="D41" s="20" t="s">
         <v>79</v>
@@ -2726,7 +2746,7 @@
       <c r="K41" s="30"/>
       <c r="L41" s="3"/>
     </row>
-    <row r="42" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C42" s="14"/>
       <c r="D42" s="22" t="s">
         <v>80</v>
@@ -2752,7 +2772,7 @@
       </c>
       <c r="L42" s="3"/>
     </row>
-    <row r="43" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="43" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C43" s="14"/>
       <c r="D43" s="23" t="s">
         <v>81</v>
@@ -2772,7 +2792,7 @@
       <c r="K43" s="29"/>
       <c r="L43" s="3"/>
     </row>
-    <row r="44" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="44" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C44" s="14"/>
       <c r="D44" s="23" t="s">
         <v>82</v>
@@ -2796,7 +2816,7 @@
       <c r="K44" s="22"/>
       <c r="L44" s="3"/>
     </row>
-    <row r="45" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="45" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C45" s="14"/>
       <c r="D45" s="22" t="s">
         <v>83</v>
@@ -2822,7 +2842,7 @@
       </c>
       <c r="L45" s="3"/>
     </row>
-    <row r="46" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="46" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C46" s="14"/>
       <c r="D46" s="20" t="s">
         <v>22</v>
@@ -2848,7 +2868,7 @@
       </c>
       <c r="L46" s="3"/>
     </row>
-    <row r="47" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="47" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C47" s="14"/>
       <c r="D47" s="22" t="s">
         <v>23</v>
@@ -2872,7 +2892,7 @@
       </c>
       <c r="L47" s="3"/>
     </row>
-    <row r="48" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="48" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C48" s="14"/>
       <c r="D48" s="18" t="s">
         <v>25</v>
@@ -2896,7 +2916,7 @@
       </c>
       <c r="L48" s="3"/>
     </row>
-    <row r="49" spans="1:25" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:25" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C49" s="14"/>
       <c r="D49" s="22" t="s">
         <v>85</v>
@@ -2920,7 +2940,7 @@
       </c>
       <c r="L49" s="3"/>
     </row>
-    <row r="50" spans="1:25" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:25" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C50" s="14"/>
       <c r="D50" s="20" t="s">
         <v>86</v>
@@ -2946,7 +2966,7 @@
       </c>
       <c r="L50" s="3"/>
     </row>
-    <row r="51" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C51" s="14"/>
       <c r="D51" s="22" t="s">
         <v>88</v>
@@ -2972,7 +2992,7 @@
       </c>
       <c r="L51" s="3"/>
     </row>
-    <row r="52" spans="1:25" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:25" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C52" s="14"/>
       <c r="D52" s="23" t="s">
         <v>89</v>
@@ -2998,7 +3018,7 @@
       </c>
       <c r="L52" s="3"/>
     </row>
-    <row r="53" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C53" s="14"/>
       <c r="D53" s="23" t="s">
         <v>90</v>
@@ -3022,10 +3042,10 @@
       <c r="K53" s="22"/>
       <c r="L53" s="3"/>
     </row>
-    <row r="54" spans="1:25" s="6" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:25" s="6" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A54" s="10"/>
-      <c r="B54" s="35"/>
-      <c r="C54" s="36"/>
+      <c r="B54" s="74"/>
+      <c r="C54" s="75"/>
       <c r="D54" s="22" t="s">
         <v>193</v>
       </c>
@@ -3044,25 +3064,25 @@
         <v>256</v>
       </c>
       <c r="K54" s="29"/>
-      <c r="L54" s="34"/>
-      <c r="M54" s="34"/>
-      <c r="N54" s="34"/>
-      <c r="O54" s="34"/>
-      <c r="P54" s="34"/>
-      <c r="Q54" s="34"/>
-      <c r="R54" s="35"/>
-      <c r="S54" s="35"/>
-      <c r="T54" s="35"/>
-      <c r="U54" s="35"/>
-      <c r="V54" s="35"/>
-      <c r="W54" s="35"/>
-      <c r="X54" s="35"/>
+      <c r="L54" s="73"/>
+      <c r="M54" s="73"/>
+      <c r="N54" s="73"/>
+      <c r="O54" s="73"/>
+      <c r="P54" s="73"/>
+      <c r="Q54" s="73"/>
+      <c r="R54" s="74"/>
+      <c r="S54" s="74"/>
+      <c r="T54" s="74"/>
+      <c r="U54" s="74"/>
+      <c r="V54" s="74"/>
+      <c r="W54" s="74"/>
+      <c r="X54" s="74"/>
       <c r="Y54" s="8"/>
     </row>
-    <row r="55" spans="1:25" s="6" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:25" s="6" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A55" s="10"/>
-      <c r="B55" s="35"/>
-      <c r="C55" s="36"/>
+      <c r="B55" s="74"/>
+      <c r="C55" s="75"/>
       <c r="D55" s="20" t="s">
         <v>194</v>
       </c>
@@ -3083,25 +3103,25 @@
       <c r="K55" s="28" t="s">
         <v>265</v>
       </c>
-      <c r="L55" s="34"/>
-      <c r="M55" s="34"/>
-      <c r="N55" s="34"/>
-      <c r="O55" s="34"/>
-      <c r="P55" s="34"/>
-      <c r="Q55" s="34"/>
-      <c r="R55" s="35"/>
-      <c r="S55" s="35"/>
-      <c r="T55" s="35"/>
-      <c r="U55" s="35"/>
-      <c r="V55" s="35"/>
-      <c r="W55" s="35"/>
-      <c r="X55" s="35"/>
+      <c r="L55" s="73"/>
+      <c r="M55" s="73"/>
+      <c r="N55" s="73"/>
+      <c r="O55" s="73"/>
+      <c r="P55" s="73"/>
+      <c r="Q55" s="73"/>
+      <c r="R55" s="74"/>
+      <c r="S55" s="74"/>
+      <c r="T55" s="74"/>
+      <c r="U55" s="74"/>
+      <c r="V55" s="74"/>
+      <c r="W55" s="74"/>
+      <c r="X55" s="74"/>
       <c r="Y55" s="8"/>
     </row>
-    <row r="56" spans="1:25" s="6" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:25" s="6" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A56" s="10"/>
-      <c r="B56" s="35"/>
-      <c r="C56" s="36"/>
+      <c r="B56" s="74"/>
+      <c r="C56" s="75"/>
       <c r="D56" s="23" t="s">
         <v>195</v>
       </c>
@@ -3116,22 +3136,22 @@
       <c r="I56" s="29"/>
       <c r="J56" s="29"/>
       <c r="K56" s="30"/>
-      <c r="L56" s="34"/>
-      <c r="M56" s="34"/>
-      <c r="N56" s="34"/>
-      <c r="O56" s="34"/>
-      <c r="P56" s="34"/>
-      <c r="Q56" s="34"/>
-      <c r="R56" s="35"/>
-      <c r="S56" s="35"/>
-      <c r="T56" s="35"/>
-      <c r="U56" s="35"/>
-      <c r="V56" s="35"/>
-      <c r="W56" s="35"/>
-      <c r="X56" s="35"/>
+      <c r="L56" s="73"/>
+      <c r="M56" s="73"/>
+      <c r="N56" s="73"/>
+      <c r="O56" s="73"/>
+      <c r="P56" s="73"/>
+      <c r="Q56" s="73"/>
+      <c r="R56" s="74"/>
+      <c r="S56" s="74"/>
+      <c r="T56" s="74"/>
+      <c r="U56" s="74"/>
+      <c r="V56" s="74"/>
+      <c r="W56" s="74"/>
+      <c r="X56" s="74"/>
       <c r="Y56" s="8"/>
     </row>
-    <row r="57" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C57" s="14"/>
       <c r="D57" s="18" t="s">
         <v>91</v>
@@ -3157,7 +3177,7 @@
       </c>
       <c r="L57" s="3"/>
     </row>
-    <row r="58" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C58" s="14"/>
       <c r="D58" s="22" t="s">
         <v>92</v>
@@ -3183,7 +3203,7 @@
       </c>
       <c r="L58" s="3"/>
     </row>
-    <row r="59" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C59" s="14"/>
       <c r="D59" s="20" t="s">
         <v>93</v>
@@ -3209,7 +3229,7 @@
       </c>
       <c r="L59" s="3"/>
     </row>
-    <row r="60" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C60" s="14"/>
       <c r="D60" s="22" t="s">
         <v>94</v>
@@ -3233,7 +3253,7 @@
       <c r="K60" s="22"/>
       <c r="L60" s="3"/>
     </row>
-    <row r="61" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C61" s="14"/>
       <c r="D61" s="23" t="s">
         <v>95</v>
@@ -3257,7 +3277,7 @@
       </c>
       <c r="L61" s="3"/>
     </row>
-    <row r="62" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C62" s="14"/>
       <c r="D62" s="23" t="s">
         <v>96</v>
@@ -3281,7 +3301,7 @@
       </c>
       <c r="L62" s="3"/>
     </row>
-    <row r="63" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C63" s="14"/>
       <c r="D63" s="22" t="s">
         <v>97</v>
@@ -3305,7 +3325,7 @@
       </c>
       <c r="L63" s="3"/>
     </row>
-    <row r="64" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C64" s="14"/>
       <c r="D64" s="19" t="s">
         <v>98</v>
@@ -3329,7 +3349,7 @@
       </c>
       <c r="L64" s="3"/>
     </row>
-    <row r="65" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C65" s="14"/>
       <c r="D65" s="23" t="s">
         <v>99</v>
@@ -3347,7 +3367,7 @@
       <c r="K65" s="30"/>
       <c r="L65" s="3"/>
     </row>
-    <row r="66" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C66" s="14"/>
       <c r="D66" s="18" t="s">
         <v>29</v>
@@ -3373,7 +3393,7 @@
       </c>
       <c r="L66" s="3"/>
     </row>
-    <row r="67" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C67" s="14"/>
       <c r="D67" s="22" t="s">
         <v>100</v>
@@ -3397,7 +3417,7 @@
       <c r="K67" s="29"/>
       <c r="L67" s="3"/>
     </row>
-    <row r="68" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="68" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C68" s="14"/>
       <c r="D68" s="20" t="s">
         <v>32</v>
@@ -3423,7 +3443,7 @@
       </c>
       <c r="L68" s="3"/>
     </row>
-    <row r="69" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="69" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C69" s="14"/>
       <c r="D69" s="22" t="s">
         <v>34</v>
@@ -3441,7 +3461,7 @@
       <c r="K69" s="22"/>
       <c r="L69" s="3"/>
     </row>
-    <row r="70" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="70" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C70" s="14"/>
       <c r="D70" s="23" t="s">
         <v>101</v>
@@ -3467,7 +3487,7 @@
       </c>
       <c r="L70" s="3"/>
     </row>
-    <row r="71" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="71" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C71" s="14"/>
       <c r="D71" s="23" t="s">
         <v>102</v>
@@ -3493,7 +3513,7 @@
       </c>
       <c r="L71" s="3"/>
     </row>
-    <row r="72" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="72" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C72" s="14"/>
       <c r="D72" s="22" t="s">
         <v>103</v>
@@ -3519,7 +3539,7 @@
       </c>
       <c r="L72" s="3"/>
     </row>
-    <row r="73" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="73" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C73" s="14"/>
       <c r="D73" s="20" t="s">
         <v>104</v>
@@ -3545,7 +3565,7 @@
       </c>
       <c r="L73" s="3"/>
     </row>
-    <row r="74" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="74" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C74" s="14"/>
       <c r="D74" s="22" t="s">
         <v>105</v>
@@ -3571,7 +3591,7 @@
       </c>
       <c r="L74" s="3"/>
     </row>
-    <row r="75" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="75" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C75" s="14"/>
       <c r="D75" s="18" t="s">
         <v>106</v>
@@ -3597,7 +3617,7 @@
       </c>
       <c r="L75" s="3"/>
     </row>
-    <row r="76" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="76" spans="3:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C76" s="14"/>
       <c r="D76" s="22" t="s">
         <v>37</v>
@@ -3617,7 +3637,7 @@
       <c r="K76" s="29"/>
       <c r="L76" s="3"/>
     </row>
-    <row r="77" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="77" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C77" s="14"/>
       <c r="D77" s="20" t="s">
         <v>38</v>
@@ -3637,7 +3657,7 @@
       <c r="K77" s="30"/>
       <c r="L77" s="3"/>
     </row>
-    <row r="78" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="78" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C78" s="14"/>
       <c r="D78" s="22" t="s">
         <v>107</v>
@@ -3657,7 +3677,7 @@
       <c r="K78" s="22"/>
       <c r="L78" s="3"/>
     </row>
-    <row r="79" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="79" spans="3:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C79" s="14"/>
       <c r="D79" s="23" t="s">
         <v>108</v>
@@ -3677,7 +3697,7 @@
       <c r="K79" s="29"/>
       <c r="L79" s="3"/>
     </row>
-    <row r="80" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="80" spans="3:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C80" s="14"/>
       <c r="D80" s="23" t="s">
         <v>109</v>
@@ -3697,7 +3717,7 @@
       <c r="K80" s="22"/>
       <c r="L80" s="3"/>
     </row>
-    <row r="81" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C81" s="14"/>
       <c r="D81" s="22" t="s">
         <v>41</v>
@@ -3717,7 +3737,7 @@
       <c r="K81" s="29"/>
       <c r="L81" s="3"/>
     </row>
-    <row r="82" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="82" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C82" s="14"/>
       <c r="D82" s="20" t="s">
         <v>110</v>
@@ -3737,7 +3757,7 @@
       <c r="K82" s="28"/>
       <c r="L82" s="3"/>
     </row>
-    <row r="83" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C83" s="14"/>
       <c r="D83" s="23" t="s">
         <v>111</v>
@@ -3757,7 +3777,7 @@
       <c r="K83" s="30"/>
       <c r="L83" s="3"/>
     </row>
-    <row r="84" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="84" spans="3:12" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C84" s="14"/>
       <c r="D84" s="18" t="s">
         <v>112</v>
@@ -3777,7 +3797,7 @@
       <c r="K84" s="29"/>
       <c r="L84" s="3"/>
     </row>
-    <row r="85" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="85" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C85" s="14"/>
       <c r="D85" s="22" t="s">
         <v>113</v>
@@ -3797,7 +3817,7 @@
       <c r="K85" s="29"/>
       <c r="L85" s="3"/>
     </row>
-    <row r="86" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="86" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C86" s="14"/>
       <c r="D86" s="20" t="s">
         <v>114</v>
@@ -3817,7 +3837,7 @@
       <c r="K86" s="30"/>
       <c r="L86" s="3"/>
     </row>
-    <row r="87" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="87" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C87" s="14"/>
       <c r="D87" s="22" t="s">
         <v>115</v>
@@ -3837,7 +3857,7 @@
       <c r="K87" s="22"/>
       <c r="L87" s="3"/>
     </row>
-    <row r="88" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="88" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C88" s="14"/>
       <c r="D88" s="23" t="s">
         <v>116</v>
@@ -3857,7 +3877,7 @@
       <c r="K88" s="29"/>
       <c r="L88" s="3"/>
     </row>
-    <row r="89" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="89" spans="3:12" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C89" s="14"/>
       <c r="D89" s="23" t="s">
         <v>117</v>
@@ -3877,7 +3897,7 @@
       <c r="K89" s="22"/>
       <c r="L89" s="3"/>
     </row>
-    <row r="90" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="90" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C90" s="14"/>
       <c r="D90" s="22" t="s">
         <v>118</v>
@@ -3895,7 +3915,7 @@
       <c r="K90" s="29"/>
       <c r="L90" s="3"/>
     </row>
-    <row r="91" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="91" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C91" s="14"/>
       <c r="D91" s="19" t="s">
         <v>120</v>
@@ -3913,7 +3933,7 @@
       <c r="K91" s="28"/>
       <c r="L91" s="3"/>
     </row>
-    <row r="92" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="92" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C92" s="14"/>
       <c r="D92" s="23" t="s">
         <v>121</v>
@@ -3933,7 +3953,7 @@
       <c r="K92" s="30"/>
       <c r="L92" s="3"/>
     </row>
-    <row r="93" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="93" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C93" s="14"/>
       <c r="D93" s="18" t="s">
         <v>123</v>
@@ -3953,7 +3973,7 @@
       <c r="K93" s="29"/>
       <c r="L93" s="3"/>
     </row>
-    <row r="94" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="94" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C94" s="14"/>
       <c r="D94" s="22" t="s">
         <v>124</v>
@@ -3979,7 +3999,7 @@
       </c>
       <c r="L94" s="3"/>
     </row>
-    <row r="95" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="95" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C95" s="14"/>
       <c r="D95" s="20" t="s">
         <v>125</v>
@@ -4005,7 +4025,7 @@
       </c>
       <c r="L95" s="3"/>
     </row>
-    <row r="96" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="96" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C96" s="14"/>
       <c r="D96" s="22" t="s">
         <v>126</v>
@@ -4029,7 +4049,7 @@
       </c>
       <c r="L96" s="3"/>
     </row>
-    <row r="97" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="97" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C97" s="14"/>
       <c r="D97" s="23" t="s">
         <v>127</v>
@@ -4049,7 +4069,7 @@
       <c r="K97" s="29"/>
       <c r="L97" s="3"/>
     </row>
-    <row r="98" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="98" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C98" s="14"/>
       <c r="D98" s="23" t="s">
         <v>128</v>
@@ -4069,7 +4089,7 @@
       <c r="K98" s="22"/>
       <c r="L98" s="3"/>
     </row>
-    <row r="99" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="99" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C99" s="14"/>
       <c r="D99" s="22" t="s">
         <v>129</v>
@@ -4087,7 +4107,7 @@
       <c r="K99" s="29"/>
       <c r="L99" s="3"/>
     </row>
-    <row r="100" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="100" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C100" s="14"/>
       <c r="D100" s="20" t="s">
         <v>130</v>
@@ -4105,7 +4125,7 @@
       <c r="K100" s="28"/>
       <c r="L100" s="3"/>
     </row>
-    <row r="101" spans="3:12" s="9" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="101" spans="3:12" s="9" customFormat="1" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C101" s="15"/>
       <c r="D101" s="22" t="s">
         <v>131</v>
@@ -4131,7 +4151,7 @@
       </c>
       <c r="L101" s="3"/>
     </row>
-    <row r="102" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="102" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C102" s="14"/>
       <c r="D102" s="18" t="s">
         <v>200</v>
@@ -4153,7 +4173,7 @@
       <c r="K102" s="30"/>
       <c r="L102" s="3"/>
     </row>
-    <row r="103" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="103" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C103" s="14"/>
       <c r="D103" s="22" t="s">
         <v>201</v>
@@ -4171,7 +4191,7 @@
       <c r="K103" s="22"/>
       <c r="L103" s="3"/>
     </row>
-    <row r="104" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="104" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C104" s="14"/>
       <c r="D104" s="20" t="s">
         <v>202</v>
@@ -4189,7 +4209,7 @@
       <c r="K104" s="29"/>
       <c r="L104" s="3"/>
     </row>
-    <row r="105" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="105" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C105" s="14"/>
       <c r="D105" s="22" t="s">
         <v>203</v>
@@ -4207,7 +4227,7 @@
       <c r="K105" s="28"/>
       <c r="L105" s="3"/>
     </row>
-    <row r="106" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="106" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C106" s="14"/>
       <c r="D106" s="23" t="s">
         <v>204</v>
@@ -4227,7 +4247,7 @@
       <c r="K106" s="30"/>
       <c r="L106" s="3"/>
     </row>
-    <row r="107" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="107" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C107" s="14"/>
       <c r="D107" s="23" t="s">
         <v>132</v>
@@ -4247,7 +4267,7 @@
       <c r="K107" s="29"/>
       <c r="L107" s="3"/>
     </row>
-    <row r="108" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="108" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C108" s="14"/>
       <c r="D108" s="22" t="s">
         <v>133</v>
@@ -4265,7 +4285,7 @@
       <c r="K108" s="29"/>
       <c r="L108" s="3"/>
     </row>
-    <row r="109" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C109" s="14"/>
       <c r="D109" s="20" t="s">
         <v>134</v>
@@ -4285,7 +4305,7 @@
       <c r="K109" s="30"/>
       <c r="L109" s="3"/>
     </row>
-    <row r="110" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="110" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C110" s="14"/>
       <c r="D110" s="22" t="s">
         <v>135</v>
@@ -4303,7 +4323,7 @@
       <c r="K110" s="22"/>
       <c r="L110" s="3"/>
     </row>
-    <row r="111" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C111" s="14"/>
       <c r="D111" s="18" t="s">
         <v>136</v>
@@ -4323,7 +4343,7 @@
       <c r="K111" s="29"/>
       <c r="L111" s="3"/>
     </row>
-    <row r="112" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C112" s="14"/>
       <c r="D112" s="22" t="s">
         <v>137</v>
@@ -4343,7 +4363,7 @@
       <c r="K112" s="28"/>
       <c r="L112" s="3"/>
     </row>
-    <row r="113" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="113" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C113" s="14"/>
       <c r="D113" s="20" t="s">
         <v>45</v>
@@ -4363,7 +4383,7 @@
       <c r="K113" s="30"/>
       <c r="L113" s="3"/>
     </row>
-    <row r="114" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C114" s="14"/>
       <c r="D114" s="22" t="s">
         <v>46</v>
@@ -4383,7 +4403,7 @@
       <c r="K114" s="29"/>
       <c r="L114" s="3"/>
     </row>
-    <row r="115" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C115" s="14"/>
       <c r="D115" s="23" t="s">
         <v>47</v>
@@ -4403,7 +4423,7 @@
       <c r="K115" s="29"/>
       <c r="L115" s="3"/>
     </row>
-    <row r="116" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C116" s="14"/>
       <c r="D116" s="23" t="s">
         <v>138</v>
@@ -4421,7 +4441,7 @@
       <c r="K116" s="30"/>
       <c r="L116" s="3"/>
     </row>
-    <row r="117" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C117" s="14"/>
       <c r="D117" s="22" t="s">
         <v>139</v>
@@ -4439,7 +4459,7 @@
       <c r="K117" s="22"/>
       <c r="L117" s="3"/>
     </row>
-    <row r="118" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C118" s="14"/>
       <c r="D118" s="19" t="s">
         <v>140</v>
@@ -4457,7 +4477,7 @@
       <c r="K118" s="29"/>
       <c r="L118" s="3"/>
     </row>
-    <row r="119" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C119" s="14"/>
       <c r="D119" s="23" t="s">
         <v>141</v>
@@ -4475,7 +4495,7 @@
       <c r="K119" s="28"/>
       <c r="L119" s="3"/>
     </row>
-    <row r="120" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C120" s="14"/>
       <c r="D120" s="18" t="s">
         <v>48</v>
@@ -4495,7 +4515,7 @@
       <c r="K120" s="30"/>
       <c r="L120" s="3"/>
     </row>
-    <row r="121" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C121" s="14"/>
       <c r="D121" s="22" t="s">
         <v>143</v>
@@ -4513,7 +4533,7 @@
       <c r="K121" s="29"/>
       <c r="L121" s="3"/>
     </row>
-    <row r="122" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="122" spans="3:12" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C122" s="14"/>
       <c r="D122" s="20" t="s">
         <v>144</v>
@@ -4533,7 +4553,7 @@
       <c r="K122" s="29"/>
       <c r="L122" s="3"/>
     </row>
-    <row r="123" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:12" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C123" s="14"/>
       <c r="D123" s="22" t="s">
         <v>145</v>
@@ -4553,7 +4573,7 @@
       <c r="K123" s="30"/>
       <c r="L123" s="3"/>
     </row>
-    <row r="124" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="124" spans="3:12" ht="54.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C124" s="14"/>
       <c r="D124" s="23" t="s">
         <v>147</v>
@@ -4573,7 +4593,7 @@
       <c r="K124" s="22"/>
       <c r="L124" s="3"/>
     </row>
-    <row r="125" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="125" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C125" s="14"/>
       <c r="D125" s="23" t="s">
         <v>149</v>
@@ -4593,7 +4613,7 @@
       <c r="K125" s="29"/>
       <c r="L125" s="3"/>
     </row>
-    <row r="126" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="126" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C126" s="14"/>
       <c r="D126" s="22" t="s">
         <v>151</v>
@@ -4611,7 +4631,7 @@
       <c r="K126" s="28"/>
       <c r="L126" s="3"/>
     </row>
-    <row r="127" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C127" s="14"/>
       <c r="D127" s="19" t="s">
         <v>153</v>
@@ -4631,7 +4651,7 @@
       <c r="K127" s="30"/>
       <c r="L127" s="3"/>
     </row>
-    <row r="128" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="128" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C128" s="14"/>
       <c r="D128" s="23" t="s">
         <v>154</v>
@@ -4649,7 +4669,7 @@
       <c r="K128" s="29"/>
       <c r="L128" s="3"/>
     </row>
-    <row r="129" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="129" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C129" s="14"/>
       <c r="D129" s="18" t="s">
         <v>156</v>
@@ -4667,7 +4687,7 @@
       <c r="K129" s="29"/>
       <c r="L129" s="3"/>
     </row>
-    <row r="130" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C130" s="14"/>
       <c r="D130" s="22" t="s">
         <v>157</v>
@@ -4685,7 +4705,7 @@
       <c r="K130" s="30"/>
       <c r="L130" s="3"/>
     </row>
-    <row r="131" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="131" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C131" s="14"/>
       <c r="D131" s="20" t="s">
         <v>158</v>
@@ -4703,7 +4723,7 @@
       <c r="K131" s="22"/>
       <c r="L131" s="3"/>
     </row>
-    <row r="132" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="132" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C132" s="14"/>
       <c r="D132" s="22" t="s">
         <v>159</v>
@@ -4721,7 +4741,7 @@
       <c r="K132" s="29"/>
       <c r="L132" s="3"/>
     </row>
-    <row r="133" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="133" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C133" s="14"/>
       <c r="D133" s="23" t="s">
         <v>160</v>
@@ -4741,7 +4761,7 @@
       <c r="K133" s="28"/>
       <c r="L133" s="3"/>
     </row>
-    <row r="134" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C134" s="14"/>
       <c r="D134" s="23" t="s">
         <v>161</v>
@@ -4761,7 +4781,7 @@
       <c r="K134" s="29"/>
       <c r="L134" s="3"/>
     </row>
-    <row r="135" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="135" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C135" s="14"/>
       <c r="D135" s="22" t="s">
         <v>162</v>
@@ -4781,7 +4801,7 @@
       <c r="K135" s="30"/>
       <c r="L135" s="3"/>
     </row>
-    <row r="136" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="136" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C136" s="14"/>
       <c r="D136" s="20" t="s">
         <v>163</v>
@@ -4801,7 +4821,7 @@
       <c r="K136" s="22"/>
       <c r="L136" s="3"/>
     </row>
-    <row r="137" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="137" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C137" s="14"/>
       <c r="D137" s="22" t="s">
         <v>164</v>
@@ -4821,7 +4841,7 @@
       <c r="K137" s="29"/>
       <c r="L137" s="3"/>
     </row>
-    <row r="138" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="138" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C138" s="14"/>
       <c r="D138" s="18" t="s">
         <v>165</v>
@@ -4841,7 +4861,7 @@
       <c r="K138" s="28"/>
       <c r="L138" s="3"/>
     </row>
-    <row r="139" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="139" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C139" s="14"/>
       <c r="D139" s="22" t="s">
         <v>166</v>
@@ -4861,7 +4881,7 @@
       <c r="K139" s="30"/>
       <c r="L139" s="3"/>
     </row>
-    <row r="140" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="140" spans="3:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C140" s="14"/>
       <c r="D140" s="20" t="s">
         <v>167</v>
@@ -4881,7 +4901,7 @@
       <c r="K140" s="29"/>
       <c r="L140" s="3"/>
     </row>
-    <row r="141" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="141" spans="3:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C141" s="14"/>
       <c r="D141" s="22" t="s">
         <v>168</v>
@@ -4901,7 +4921,7 @@
       <c r="K141" s="30"/>
       <c r="L141" s="3"/>
     </row>
-    <row r="142" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:12" ht="72.599999999999994" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C142" s="14"/>
       <c r="D142" s="23" t="s">
         <v>169</v>
@@ -4921,7 +4941,7 @@
       <c r="K142" s="22"/>
       <c r="L142" s="3"/>
     </row>
-    <row r="143" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="143" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C143" s="14"/>
       <c r="D143" s="23" t="s">
         <v>170</v>
@@ -4941,7 +4961,7 @@
       <c r="K143" s="29"/>
       <c r="L143" s="3"/>
     </row>
-    <row r="144" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="144" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C144" s="14"/>
       <c r="D144" s="22" t="s">
         <v>171</v>
@@ -4961,7 +4981,7 @@
       <c r="K144" s="28"/>
       <c r="L144" s="3"/>
     </row>
-    <row r="145" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C145" s="14"/>
       <c r="D145" s="19" t="s">
         <v>172</v>
@@ -4981,7 +5001,7 @@
       <c r="K145" s="30"/>
       <c r="L145" s="3"/>
     </row>
-    <row r="146" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="146" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C146" s="14"/>
       <c r="D146" s="23" t="s">
         <v>173</v>
@@ -5001,7 +5021,7 @@
       <c r="K146" s="29"/>
       <c r="L146" s="3"/>
     </row>
-    <row r="147" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="147" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C147" s="14"/>
       <c r="D147" s="18" t="s">
         <v>174</v>
@@ -5021,7 +5041,7 @@
       <c r="K147" s="30"/>
       <c r="L147" s="3"/>
     </row>
-    <row r="148" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="148" spans="3:12" ht="36.6" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C148" s="14"/>
       <c r="D148" s="22" t="s">
         <v>51</v>
@@ -5041,7 +5061,7 @@
       <c r="K148" s="22"/>
       <c r="L148" s="3"/>
     </row>
-    <row r="149" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="149" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C149" s="14"/>
       <c r="D149" s="20" t="s">
         <v>175</v>
@@ -5059,7 +5079,7 @@
       <c r="K149" s="30"/>
       <c r="L149" s="3"/>
     </row>
-    <row r="150" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="150" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C150" s="14"/>
       <c r="D150" s="22" t="s">
         <v>176</v>
@@ -5077,7 +5097,7 @@
       <c r="K150" s="29"/>
       <c r="L150" s="3"/>
     </row>
-    <row r="151" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="151" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C151" s="14"/>
       <c r="D151" s="23" t="s">
         <v>177</v>
@@ -5095,7 +5115,7 @@
       <c r="K151" s="30"/>
       <c r="L151" s="3"/>
     </row>
-    <row r="152" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="152" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C152" s="14"/>
       <c r="D152" s="23" t="s">
         <v>178</v>
@@ -5113,7 +5133,7 @@
       <c r="K152" s="22"/>
       <c r="L152" s="3"/>
     </row>
-    <row r="153" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="153" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C153" s="14"/>
       <c r="D153" s="22" t="s">
         <v>55</v>
@@ -5131,7 +5151,7 @@
       <c r="K153" s="29"/>
       <c r="L153" s="3"/>
     </row>
-    <row r="154" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="154" spans="3:12" ht="18.600000000000001" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C154" s="14"/>
       <c r="D154" s="19" t="s">
         <v>56</v>
@@ -5149,17 +5169,11 @@
       <c r="K154" s="28"/>
       <c r="L154" s="3"/>
     </row>
-    <row r="155" spans="3:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="3:12" x14ac:dyDescent="0.3">
       <c r="F155" s="32"/>
     </row>
   </sheetData>
-  <mergeCells count="15">
-    <mergeCell ref="B2:M7"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
+  <mergeCells count="16">
     <mergeCell ref="L54:Q56"/>
     <mergeCell ref="B54:C56"/>
     <mergeCell ref="R54:T56"/>
@@ -5169,6 +5183,13 @@
     <mergeCell ref="C17:K25"/>
     <mergeCell ref="F14:G14"/>
     <mergeCell ref="F13:G13"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="B2:M7"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
added test cases ID related to liog in page
added test cases ID related to liog in page
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ahmed\Documents\GitHub\Internet-Banking-System\PM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="692" uniqueCount="327">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="339">
   <si>
     <t>Author</t>
   </si>
@@ -1080,6 +1080,73 @@
   </si>
   <si>
     <t>Bank_Sys_DM_ADMIN_009</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R003</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R004</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R011</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R005
+BANK_SYS_TC_Log_R006
+BANK_SYS_TC_Log_R008
+BANK_SYS_TC_Log_R009
+BANK_SYS_TC_Log_R010
+BANK_SYS_TC_Log_R011</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R012
+BANK_SYS_TC_Log_R013
+BANK_SYS_TC_Log_R014</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R005
+BANK_SYS_TC_Log_R015
+BANK_SYS_TC_Log_R016
+BANK_SYS_TC_Log_R017</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R018
+BANK_SYS_TC_Log_R019
+BANK_SYS_TC_Log_R020
+BANK_SYS_TC_Log_R021
+BANK_SYS_TC_Log_R022
+BANK_SYS_TC_Log_R023
+BANK_SYS_TC_Log_R024</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R008
+BANK_SYS_TC_Log_R009
+BANK_SYS_TC_Log_R010
+BANK_SYS_TC_Log_R016
+BANK_SYS_TC_Log_R017
+BANK_SYS_TC_Log_R019
+BANK_SYS_TC_Log_R020
+BANK_SYS_TC_Log_R021
+BANK_SYS_TC_Log_R022
+BANK_SYS_TC_Log_R023
+BANK_SYS_TC_Log_R024</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R025
+BANK_SYS_TC_Log_R026
+BANK_SYS_TC_Log_R027
+BANK_SYS_TC_Log_R028
+BANK_SYS_TC_Log_R029
+BANK_SYS_TC_Log_R030</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Log_R031</t>
   </si>
 </sst>
 </file>
@@ -1724,6 +1791,71 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1766,71 +1898,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="2" borderId="34" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2117,8 +2184,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B39" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="H139" sqref="H139"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D67" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D67" sqref="D67"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2129,7 +2196,7 @@
     <col min="5" max="5" width="26.28515625" style="6" customWidth="1"/>
     <col min="6" max="6" width="27.7109375" style="6" customWidth="1"/>
     <col min="7" max="7" width="38.42578125" style="6" customWidth="1"/>
-    <col min="8" max="8" width="25.5703125" style="3" customWidth="1"/>
+    <col min="8" max="8" width="33.85546875" style="3" customWidth="1"/>
     <col min="9" max="9" width="31.7109375" style="6" customWidth="1"/>
     <col min="10" max="10" width="32.140625" customWidth="1"/>
     <col min="11" max="11" width="28.28515625" customWidth="1"/>
@@ -2137,90 +2204,90 @@
   <sheetData>
     <row r="1" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="69" t="s">
+      <c r="B2" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="70"/>
-      <c r="D2" s="70"/>
-      <c r="E2" s="70"/>
-      <c r="F2" s="70"/>
-      <c r="G2" s="70"/>
-      <c r="H2" s="70"/>
-      <c r="I2" s="70"/>
-      <c r="J2" s="70"/>
-      <c r="K2" s="70"/>
-      <c r="L2" s="70"/>
-      <c r="M2" s="71"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="61"/>
     </row>
     <row r="3" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="72"/>
-      <c r="C3" s="73"/>
-      <c r="D3" s="73"/>
-      <c r="E3" s="73"/>
-      <c r="F3" s="73"/>
-      <c r="G3" s="73"/>
-      <c r="H3" s="73"/>
-      <c r="I3" s="73"/>
-      <c r="J3" s="73"/>
-      <c r="K3" s="73"/>
-      <c r="L3" s="73"/>
-      <c r="M3" s="74"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="72"/>
-      <c r="C4" s="73"/>
-      <c r="D4" s="73"/>
-      <c r="E4" s="73"/>
-      <c r="F4" s="73"/>
-      <c r="G4" s="73"/>
-      <c r="H4" s="73"/>
-      <c r="I4" s="73"/>
-      <c r="J4" s="73"/>
-      <c r="K4" s="73"/>
-      <c r="L4" s="73"/>
-      <c r="M4" s="74"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="64"/>
     </row>
     <row r="5" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="72"/>
-      <c r="C5" s="73"/>
-      <c r="D5" s="73"/>
-      <c r="E5" s="73"/>
-      <c r="F5" s="73"/>
-      <c r="G5" s="73"/>
-      <c r="H5" s="73"/>
-      <c r="I5" s="73"/>
-      <c r="J5" s="73"/>
-      <c r="K5" s="73"/>
-      <c r="L5" s="73"/>
-      <c r="M5" s="74"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="64"/>
     </row>
     <row r="6" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="72"/>
-      <c r="C6" s="73"/>
-      <c r="D6" s="73"/>
-      <c r="E6" s="73"/>
-      <c r="F6" s="73"/>
-      <c r="G6" s="73"/>
-      <c r="H6" s="73"/>
-      <c r="I6" s="73"/>
-      <c r="J6" s="73"/>
-      <c r="K6" s="73"/>
-      <c r="L6" s="73"/>
-      <c r="M6" s="74"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="64"/>
     </row>
     <row r="7" spans="2:13" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="75"/>
-      <c r="C7" s="76"/>
-      <c r="D7" s="76"/>
-      <c r="E7" s="76"/>
-      <c r="F7" s="76"/>
-      <c r="G7" s="76"/>
-      <c r="H7" s="76"/>
-      <c r="I7" s="76"/>
-      <c r="J7" s="76"/>
-      <c r="K7" s="76"/>
-      <c r="L7" s="76"/>
-      <c r="M7" s="77"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="67"/>
     </row>
     <row r="8" spans="2:13" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
@@ -2238,16 +2305,16 @@
     </row>
     <row r="9" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
-      <c r="C9" s="78" t="s">
+      <c r="C9" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="78"/>
-      <c r="E9" s="78"/>
-      <c r="F9" s="78"/>
-      <c r="G9" s="78"/>
-      <c r="H9" s="78"/>
-      <c r="I9" s="78"/>
-      <c r="J9" s="79"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="69"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2260,20 +2327,20 @@
       <c r="E10" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="80" t="s">
+      <c r="F10" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="81"/>
+      <c r="G10" s="71"/>
       <c r="H10" s="34" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="82" t="s">
+      <c r="J10" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="81"/>
+      <c r="K10" s="71"/>
     </row>
     <row r="11" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="37" t="s">
@@ -2285,14 +2352,14 @@
       <c r="E11" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="83" t="s">
+      <c r="F11" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="84"/>
+      <c r="G11" s="74"/>
       <c r="H11" s="35"/>
       <c r="I11" s="19"/>
-      <c r="J11" s="85"/>
-      <c r="K11" s="86"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76"/>
     </row>
     <row r="12" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="35" t="s">
@@ -2304,20 +2371,20 @@
       <c r="E12" s="36">
         <v>43529</v>
       </c>
-      <c r="F12" s="58" t="s">
+      <c r="F12" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="59"/>
+      <c r="G12" s="82"/>
       <c r="H12" s="43" t="s">
         <v>58</v>
       </c>
       <c r="I12" s="44">
         <v>43529</v>
       </c>
-      <c r="J12" s="60" t="s">
+      <c r="J12" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="61"/>
+      <c r="K12" s="84"/>
     </row>
     <row r="13" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="37" t="s">
@@ -2329,10 +2396,10 @@
       <c r="E13" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="F13" s="65" t="s">
+      <c r="F13" s="88" t="s">
         <v>293</v>
       </c>
-      <c r="G13" s="66"/>
+      <c r="G13" s="89"/>
       <c r="H13" s="50"/>
       <c r="I13" s="51"/>
       <c r="J13" s="52"/>
@@ -2348,20 +2415,20 @@
       <c r="E14" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="F14" s="63" t="s">
+      <c r="F14" s="86" t="s">
         <v>291</v>
       </c>
-      <c r="G14" s="64"/>
+      <c r="G14" s="87"/>
       <c r="H14" s="47" t="s">
         <v>294</v>
       </c>
       <c r="I14" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="J14" s="67" t="s">
+      <c r="J14" s="90" t="s">
         <v>295</v>
       </c>
-      <c r="K14" s="68"/>
+      <c r="K14" s="91"/>
     </row>
     <row r="15" spans="2:13" ht="96.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="48" t="s">
@@ -2376,116 +2443,116 @@
       <c r="F15" s="92" t="s">
         <v>324</v>
       </c>
-      <c r="G15" s="64"/>
+      <c r="G15" s="87"/>
       <c r="H15" s="48"/>
-      <c r="I15" s="89"/>
-      <c r="J15" s="91"/>
-      <c r="K15" s="90"/>
+      <c r="I15" s="56"/>
+      <c r="J15" s="58"/>
+      <c r="K15" s="57"/>
     </row>
     <row r="16" spans="2:13" x14ac:dyDescent="0.25">
       <c r="D16" s="49"/>
       <c r="E16" s="45"/>
     </row>
     <row r="18" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="62" t="s">
+      <c r="C18" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="62"/>
-      <c r="E18" s="62"/>
-      <c r="F18" s="62"/>
-      <c r="G18" s="62"/>
-      <c r="H18" s="62"/>
-      <c r="I18" s="62"/>
-      <c r="J18" s="62"/>
-      <c r="K18" s="62"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="85"/>
     </row>
     <row r="19" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="62"/>
-      <c r="D19" s="62"/>
-      <c r="E19" s="62"/>
-      <c r="F19" s="62"/>
-      <c r="G19" s="62"/>
-      <c r="H19" s="62"/>
-      <c r="I19" s="62"/>
-      <c r="J19" s="62"/>
-      <c r="K19" s="62"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="85"/>
     </row>
     <row r="20" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="62"/>
-      <c r="D20" s="62"/>
-      <c r="E20" s="62"/>
-      <c r="F20" s="62"/>
-      <c r="G20" s="62"/>
-      <c r="H20" s="62"/>
-      <c r="I20" s="62"/>
-      <c r="J20" s="62"/>
-      <c r="K20" s="62"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
     </row>
     <row r="21" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="62"/>
-      <c r="D21" s="62"/>
-      <c r="E21" s="62"/>
-      <c r="F21" s="62"/>
-      <c r="G21" s="62"/>
-      <c r="H21" s="62"/>
-      <c r="I21" s="62"/>
-      <c r="J21" s="62"/>
-      <c r="K21" s="62"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="85"/>
     </row>
     <row r="22" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="62"/>
-      <c r="D22" s="62"/>
-      <c r="E22" s="62"/>
-      <c r="F22" s="62"/>
-      <c r="G22" s="62"/>
-      <c r="H22" s="62"/>
-      <c r="I22" s="62"/>
-      <c r="J22" s="62"/>
-      <c r="K22" s="62"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
     </row>
     <row r="23" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="62"/>
-      <c r="D23" s="62"/>
-      <c r="E23" s="62"/>
-      <c r="F23" s="62"/>
-      <c r="G23" s="62"/>
-      <c r="H23" s="62"/>
-      <c r="I23" s="62"/>
-      <c r="J23" s="62"/>
-      <c r="K23" s="62"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
     </row>
     <row r="24" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="62"/>
-      <c r="D24" s="62"/>
-      <c r="E24" s="62"/>
-      <c r="F24" s="62"/>
-      <c r="G24" s="62"/>
-      <c r="H24" s="62"/>
-      <c r="I24" s="62"/>
-      <c r="J24" s="62"/>
-      <c r="K24" s="62"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="85"/>
     </row>
     <row r="25" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="62"/>
-      <c r="D25" s="62"/>
-      <c r="E25" s="62"/>
-      <c r="F25" s="62"/>
-      <c r="G25" s="62"/>
-      <c r="H25" s="62"/>
-      <c r="I25" s="62"/>
-      <c r="J25" s="62"/>
-      <c r="K25" s="62"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
     </row>
     <row r="26" spans="3:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="62"/>
-      <c r="D26" s="62"/>
-      <c r="E26" s="62"/>
-      <c r="F26" s="62"/>
-      <c r="G26" s="62"/>
-      <c r="H26" s="62"/>
-      <c r="I26" s="62"/>
-      <c r="J26" s="62"/>
-      <c r="K26" s="62"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="85"/>
     </row>
     <row r="27" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="15"/>
@@ -2788,7 +2855,7 @@
       <c r="J38" s="28" t="s">
         <v>259</v>
       </c>
-      <c r="K38" s="88" t="s">
+      <c r="K38" s="55" t="s">
         <v>266</v>
       </c>
       <c r="L38" s="54"/>
@@ -2812,7 +2879,7 @@
       <c r="J39" s="21" t="s">
         <v>259</v>
       </c>
-      <c r="K39" s="88" t="s">
+      <c r="K39" s="55" t="s">
         <v>266</v>
       </c>
       <c r="L39" s="54"/>
@@ -3187,8 +3254,8 @@
     </row>
     <row r="55" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
-      <c r="B55" s="56"/>
-      <c r="C55" s="57"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="80"/>
       <c r="D55" s="21" t="s">
         <v>193</v>
       </c>
@@ -3209,25 +3276,25 @@
       <c r="K55" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="L55" s="87"/>
-      <c r="M55" s="55"/>
-      <c r="N55" s="55"/>
-      <c r="O55" s="55"/>
-      <c r="P55" s="55"/>
-      <c r="Q55" s="55"/>
-      <c r="R55" s="56"/>
-      <c r="S55" s="56"/>
-      <c r="T55" s="56"/>
-      <c r="U55" s="56"/>
-      <c r="V55" s="56"/>
-      <c r="W55" s="56"/>
-      <c r="X55" s="56"/>
+      <c r="L55" s="77"/>
+      <c r="M55" s="78"/>
+      <c r="N55" s="78"/>
+      <c r="O55" s="78"/>
+      <c r="P55" s="78"/>
+      <c r="Q55" s="78"/>
+      <c r="R55" s="79"/>
+      <c r="S55" s="79"/>
+      <c r="T55" s="79"/>
+      <c r="U55" s="79"/>
+      <c r="V55" s="79"/>
+      <c r="W55" s="79"/>
+      <c r="X55" s="79"/>
       <c r="Y55" s="7"/>
     </row>
     <row r="56" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
-      <c r="B56" s="56"/>
-      <c r="C56" s="57"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="80"/>
       <c r="D56" s="19" t="s">
         <v>194</v>
       </c>
@@ -3248,25 +3315,25 @@
       <c r="K56" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="L56" s="87"/>
-      <c r="M56" s="55"/>
-      <c r="N56" s="55"/>
-      <c r="O56" s="55"/>
-      <c r="P56" s="55"/>
-      <c r="Q56" s="55"/>
-      <c r="R56" s="56"/>
-      <c r="S56" s="56"/>
-      <c r="T56" s="56"/>
-      <c r="U56" s="56"/>
-      <c r="V56" s="56"/>
-      <c r="W56" s="56"/>
-      <c r="X56" s="56"/>
+      <c r="L56" s="77"/>
+      <c r="M56" s="78"/>
+      <c r="N56" s="78"/>
+      <c r="O56" s="78"/>
+      <c r="P56" s="78"/>
+      <c r="Q56" s="78"/>
+      <c r="R56" s="79"/>
+      <c r="S56" s="79"/>
+      <c r="T56" s="79"/>
+      <c r="U56" s="79"/>
+      <c r="V56" s="79"/>
+      <c r="W56" s="79"/>
+      <c r="X56" s="79"/>
       <c r="Y56" s="7"/>
     </row>
     <row r="57" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
-      <c r="B57" s="56"/>
-      <c r="C57" s="57"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="80"/>
       <c r="D57" s="22" t="s">
         <v>195</v>
       </c>
@@ -3281,22 +3348,22 @@
       <c r="I57" s="28"/>
       <c r="J57" s="28"/>
       <c r="K57" s="29"/>
-      <c r="L57" s="87"/>
-      <c r="M57" s="55"/>
-      <c r="N57" s="55"/>
-      <c r="O57" s="55"/>
-      <c r="P57" s="55"/>
-      <c r="Q57" s="55"/>
-      <c r="R57" s="56"/>
-      <c r="S57" s="56"/>
-      <c r="T57" s="56"/>
-      <c r="U57" s="56"/>
-      <c r="V57" s="56"/>
-      <c r="W57" s="56"/>
-      <c r="X57" s="56"/>
+      <c r="L57" s="77"/>
+      <c r="M57" s="78"/>
+      <c r="N57" s="78"/>
+      <c r="O57" s="78"/>
+      <c r="P57" s="78"/>
+      <c r="Q57" s="78"/>
+      <c r="R57" s="79"/>
+      <c r="S57" s="79"/>
+      <c r="T57" s="79"/>
+      <c r="U57" s="79"/>
+      <c r="V57" s="79"/>
+      <c r="W57" s="79"/>
+      <c r="X57" s="79"/>
       <c r="Y57" s="7"/>
     </row>
-    <row r="58" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="13"/>
       <c r="D58" s="17" t="s">
         <v>91</v>
@@ -3310,7 +3377,9 @@
       <c r="G58" s="17" t="s">
         <v>213</v>
       </c>
-      <c r="H58" s="18"/>
+      <c r="H58" s="18" t="s">
+        <v>327</v>
+      </c>
       <c r="I58" s="29" t="s">
         <v>262</v>
       </c>
@@ -3336,7 +3405,9 @@
       <c r="G59" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="H59" s="19"/>
+      <c r="H59" s="19" t="s">
+        <v>328</v>
+      </c>
       <c r="I59" s="21" t="s">
         <v>262</v>
       </c>
@@ -3362,7 +3433,9 @@
       <c r="G60" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="H60" s="20"/>
+      <c r="H60" s="20" t="s">
+        <v>329</v>
+      </c>
       <c r="I60" s="28" t="s">
         <v>262</v>
       </c>
@@ -3388,7 +3461,9 @@
       <c r="G61" s="28" t="s">
         <v>213</v>
       </c>
-      <c r="H61" s="18"/>
+      <c r="H61" s="18" t="s">
+        <v>330</v>
+      </c>
       <c r="I61" s="21" t="s">
         <v>262</v>
       </c>
@@ -3400,7 +3475,7 @@
       </c>
       <c r="L61" s="54"/>
     </row>
-    <row r="62" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:25" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C62" s="13"/>
       <c r="D62" s="22" t="s">
         <v>95</v>
@@ -3412,7 +3487,9 @@
         <v>27</v>
       </c>
       <c r="G62" s="28"/>
-      <c r="H62" s="18"/>
+      <c r="H62" s="18" t="s">
+        <v>332</v>
+      </c>
       <c r="I62" s="28" t="s">
         <v>267</v>
       </c>
@@ -3424,7 +3501,7 @@
       </c>
       <c r="L62" s="54"/>
     </row>
-    <row r="63" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:25" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C63" s="13"/>
       <c r="D63" s="22" t="s">
         <v>96</v>
@@ -3436,7 +3513,9 @@
         <v>27</v>
       </c>
       <c r="G63" s="28"/>
-      <c r="H63" s="19"/>
+      <c r="H63" s="19" t="s">
+        <v>333</v>
+      </c>
       <c r="I63" s="21" t="s">
         <v>267</v>
       </c>
@@ -3448,7 +3527,7 @@
       </c>
       <c r="L63" s="54"/>
     </row>
-    <row r="64" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:25" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C64" s="13"/>
       <c r="D64" s="21" t="s">
         <v>97</v>
@@ -3460,7 +3539,9 @@
         <v>27</v>
       </c>
       <c r="G64" s="28"/>
-      <c r="H64" s="18"/>
+      <c r="H64" s="18" t="s">
+        <v>334</v>
+      </c>
       <c r="I64" s="28" t="s">
         <v>267</v>
       </c>
@@ -3472,7 +3553,7 @@
       </c>
       <c r="L64" s="54"/>
     </row>
-    <row r="65" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="65" spans="3:12" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C65" s="13"/>
       <c r="D65" s="18" t="s">
         <v>98</v>
@@ -3484,7 +3565,9 @@
         <v>28</v>
       </c>
       <c r="G65" s="17"/>
-      <c r="H65" s="19"/>
+      <c r="H65" s="19" t="s">
+        <v>335</v>
+      </c>
       <c r="I65" s="29" t="s">
         <v>267</v>
       </c>
@@ -3496,7 +3579,7 @@
       </c>
       <c r="L65" s="54"/>
     </row>
-    <row r="66" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="66" spans="3:12" ht="113.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C66" s="13"/>
       <c r="D66" s="22" t="s">
         <v>99</v>
@@ -3508,13 +3591,15 @@
         <v>30</v>
       </c>
       <c r="G66" s="21"/>
-      <c r="H66" s="20"/>
+      <c r="H66" s="20" t="s">
+        <v>337</v>
+      </c>
       <c r="I66" s="21"/>
       <c r="J66" s="28"/>
       <c r="K66" s="29"/>
       <c r="L66" s="54"/>
     </row>
-    <row r="67" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="67" spans="3:12" ht="207" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C67" s="13"/>
       <c r="D67" s="17" t="s">
         <v>29</v>
@@ -3528,7 +3613,9 @@
       <c r="G67" s="17" t="s">
         <v>215</v>
       </c>
-      <c r="H67" s="18"/>
+      <c r="H67" s="18" t="s">
+        <v>336</v>
+      </c>
       <c r="I67" s="28" t="s">
         <v>267</v>
       </c>
@@ -3554,7 +3641,9 @@
       <c r="G68" s="21" t="s">
         <v>213</v>
       </c>
-      <c r="H68" s="18"/>
+      <c r="H68" s="18" t="s">
+        <v>338</v>
+      </c>
       <c r="I68" s="21" t="s">
         <v>262</v>
       </c>
@@ -3580,7 +3669,9 @@
       <c r="G69" s="17" t="s">
         <v>183</v>
       </c>
-      <c r="H69" s="19"/>
+      <c r="H69" s="19" t="s">
+        <v>331</v>
+      </c>
       <c r="I69" s="28" t="s">
         <v>296</v>
       </c>
@@ -3761,7 +3852,7 @@
       <c r="J76" s="28" t="s">
         <v>274</v>
       </c>
-      <c r="K76" s="88" t="s">
+      <c r="K76" s="55" t="s">
         <v>310</v>
       </c>
       <c r="L76" s="54"/>
@@ -5411,12 +5502,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B2:M7"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
     <mergeCell ref="L55:Q57"/>
     <mergeCell ref="B55:C57"/>
     <mergeCell ref="R55:T57"/>
@@ -5428,6 +5513,12 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="F15:G15"/>
+    <mergeCell ref="B2:M7"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added test cases id related to transfer money
Added test cases id related to transfer money
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="704" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="367">
   <si>
     <t>Author</t>
   </si>
@@ -1147,6 +1147,126 @@
   </si>
   <si>
     <t>BANK_SYS_TC_Log_R031</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R001</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R006</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R002
+BANK_SYS_TC_TR_R003
+BANK_SYS_TC_TR_R004
+BANK_SYS_TC_TR_R005</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R002
+BANK_SYS_TC_TR_R007
+BANK_SYS_TC_TR_R008
+BANK_SYS_TC_TR_R009</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R010
+BANK_SYS_TC_TR_R011</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R013
+BANK_SYS_TC_TR_R014
+BANK_SYS_TC_TR_R015
+BANK_SYS_TC_TR_R016
+BANK_SYS_TC_TR_R017</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R012</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R007
+BANK_SYS_TC_TR_R008
+BANK_SYS_TC_TR_R009</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R018
+BANK_SYS_TC_TR_R019
+BANK_SYS_TC_TR_R020
+BANK_SYS_TC_TR_R021
+BANK_SYS_TC_TR_R022</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R021
+BANK_SYS_TC_TR_R022</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R023
+BANK_SYS_TC_TR_R024
+BANK_SYS_TC_TR_R025</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R026
+BANK_SYS_TC_TR_R027
+BANK_SYS_TC_TR_R028</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R029
+BANK_SYS_TC_TR_R030</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R029
+BANK_SYS_TC_TR_R030
+BANK_SYS_TC_TR_R031
+BANK_SYS_TC_TR_R032</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R013
+BANK_SYS_TC_TR_R014
+BANK_SYS_TC_TR_R015
+BANK_SYS_TC_TR_R016
+BANK_SYS_TC_TR_R017
+BANK_SYS_TC_TR_R030
+BANK_SYS_TC_TR_R032</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R031
+BANK_SYS_TC_TR_R032</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R033
+BANK_SYS_TC_TR_R034
+BANK_SYS_TC_TR_R035</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R011
+BANK_SYS_TC_TR_R036</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R037</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R038</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R039</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R040</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R041</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R042</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R043</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R044</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R045</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R046</t>
   </si>
 </sst>
 </file>
@@ -1799,6 +1919,54 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1851,54 +2019,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="32" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="19" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2184,8 +2304,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D67" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D67" sqref="D67"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C138" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H141" sqref="H141"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2204,90 +2324,90 @@
   <sheetData>
     <row r="1" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="59" t="s">
+      <c r="B2" s="75" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="60"/>
-      <c r="D2" s="60"/>
-      <c r="E2" s="60"/>
-      <c r="F2" s="60"/>
-      <c r="G2" s="60"/>
-      <c r="H2" s="60"/>
-      <c r="I2" s="60"/>
-      <c r="J2" s="60"/>
-      <c r="K2" s="60"/>
-      <c r="L2" s="60"/>
-      <c r="M2" s="61"/>
+      <c r="C2" s="76"/>
+      <c r="D2" s="76"/>
+      <c r="E2" s="76"/>
+      <c r="F2" s="76"/>
+      <c r="G2" s="76"/>
+      <c r="H2" s="76"/>
+      <c r="I2" s="76"/>
+      <c r="J2" s="76"/>
+      <c r="K2" s="76"/>
+      <c r="L2" s="76"/>
+      <c r="M2" s="77"/>
     </row>
     <row r="3" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="62"/>
-      <c r="C3" s="63"/>
-      <c r="D3" s="63"/>
-      <c r="E3" s="63"/>
-      <c r="F3" s="63"/>
-      <c r="G3" s="63"/>
-      <c r="H3" s="63"/>
-      <c r="I3" s="63"/>
-      <c r="J3" s="63"/>
-      <c r="K3" s="63"/>
-      <c r="L3" s="63"/>
-      <c r="M3" s="64"/>
+      <c r="B3" s="78"/>
+      <c r="C3" s="79"/>
+      <c r="D3" s="79"/>
+      <c r="E3" s="79"/>
+      <c r="F3" s="79"/>
+      <c r="G3" s="79"/>
+      <c r="H3" s="79"/>
+      <c r="I3" s="79"/>
+      <c r="J3" s="79"/>
+      <c r="K3" s="79"/>
+      <c r="L3" s="79"/>
+      <c r="M3" s="80"/>
     </row>
     <row r="4" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="62"/>
-      <c r="C4" s="63"/>
-      <c r="D4" s="63"/>
-      <c r="E4" s="63"/>
-      <c r="F4" s="63"/>
-      <c r="G4" s="63"/>
-      <c r="H4" s="63"/>
-      <c r="I4" s="63"/>
-      <c r="J4" s="63"/>
-      <c r="K4" s="63"/>
-      <c r="L4" s="63"/>
-      <c r="M4" s="64"/>
+      <c r="B4" s="78"/>
+      <c r="C4" s="79"/>
+      <c r="D4" s="79"/>
+      <c r="E4" s="79"/>
+      <c r="F4" s="79"/>
+      <c r="G4" s="79"/>
+      <c r="H4" s="79"/>
+      <c r="I4" s="79"/>
+      <c r="J4" s="79"/>
+      <c r="K4" s="79"/>
+      <c r="L4" s="79"/>
+      <c r="M4" s="80"/>
     </row>
     <row r="5" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="62"/>
-      <c r="C5" s="63"/>
-      <c r="D5" s="63"/>
-      <c r="E5" s="63"/>
-      <c r="F5" s="63"/>
-      <c r="G5" s="63"/>
-      <c r="H5" s="63"/>
-      <c r="I5" s="63"/>
-      <c r="J5" s="63"/>
-      <c r="K5" s="63"/>
-      <c r="L5" s="63"/>
-      <c r="M5" s="64"/>
+      <c r="B5" s="78"/>
+      <c r="C5" s="79"/>
+      <c r="D5" s="79"/>
+      <c r="E5" s="79"/>
+      <c r="F5" s="79"/>
+      <c r="G5" s="79"/>
+      <c r="H5" s="79"/>
+      <c r="I5" s="79"/>
+      <c r="J5" s="79"/>
+      <c r="K5" s="79"/>
+      <c r="L5" s="79"/>
+      <c r="M5" s="80"/>
     </row>
     <row r="6" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="62"/>
-      <c r="C6" s="63"/>
-      <c r="D6" s="63"/>
-      <c r="E6" s="63"/>
-      <c r="F6" s="63"/>
-      <c r="G6" s="63"/>
-      <c r="H6" s="63"/>
-      <c r="I6" s="63"/>
-      <c r="J6" s="63"/>
-      <c r="K6" s="63"/>
-      <c r="L6" s="63"/>
-      <c r="M6" s="64"/>
+      <c r="B6" s="78"/>
+      <c r="C6" s="79"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
+      <c r="F6" s="79"/>
+      <c r="G6" s="79"/>
+      <c r="H6" s="79"/>
+      <c r="I6" s="79"/>
+      <c r="J6" s="79"/>
+      <c r="K6" s="79"/>
+      <c r="L6" s="79"/>
+      <c r="M6" s="80"/>
     </row>
     <row r="7" spans="2:13" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="65"/>
-      <c r="C7" s="66"/>
-      <c r="D7" s="66"/>
-      <c r="E7" s="66"/>
-      <c r="F7" s="66"/>
-      <c r="G7" s="66"/>
-      <c r="H7" s="66"/>
-      <c r="I7" s="66"/>
-      <c r="J7" s="66"/>
-      <c r="K7" s="66"/>
-      <c r="L7" s="66"/>
-      <c r="M7" s="67"/>
+      <c r="B7" s="81"/>
+      <c r="C7" s="82"/>
+      <c r="D7" s="82"/>
+      <c r="E7" s="82"/>
+      <c r="F7" s="82"/>
+      <c r="G7" s="82"/>
+      <c r="H7" s="82"/>
+      <c r="I7" s="82"/>
+      <c r="J7" s="82"/>
+      <c r="K7" s="82"/>
+      <c r="L7" s="82"/>
+      <c r="M7" s="83"/>
     </row>
     <row r="8" spans="2:13" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
@@ -2305,16 +2425,16 @@
     </row>
     <row r="9" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
-      <c r="C9" s="68" t="s">
+      <c r="C9" s="84" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="68"/>
-      <c r="E9" s="68"/>
-      <c r="F9" s="68"/>
-      <c r="G9" s="68"/>
-      <c r="H9" s="68"/>
-      <c r="I9" s="68"/>
-      <c r="J9" s="69"/>
+      <c r="D9" s="84"/>
+      <c r="E9" s="84"/>
+      <c r="F9" s="84"/>
+      <c r="G9" s="84"/>
+      <c r="H9" s="84"/>
+      <c r="I9" s="84"/>
+      <c r="J9" s="85"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2327,20 +2447,20 @@
       <c r="E10" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="70" t="s">
+      <c r="F10" s="86" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="71"/>
+      <c r="G10" s="87"/>
       <c r="H10" s="34" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="72" t="s">
+      <c r="J10" s="88" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="71"/>
+      <c r="K10" s="87"/>
     </row>
     <row r="11" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="37" t="s">
@@ -2352,14 +2472,14 @@
       <c r="E11" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="73" t="s">
+      <c r="F11" s="89" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="74"/>
+      <c r="G11" s="90"/>
       <c r="H11" s="35"/>
       <c r="I11" s="19"/>
-      <c r="J11" s="75"/>
-      <c r="K11" s="76"/>
+      <c r="J11" s="91"/>
+      <c r="K11" s="92"/>
     </row>
     <row r="12" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="35" t="s">
@@ -2371,20 +2491,20 @@
       <c r="E12" s="36">
         <v>43529</v>
       </c>
-      <c r="F12" s="81" t="s">
+      <c r="F12" s="63" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="82"/>
+      <c r="G12" s="64"/>
       <c r="H12" s="43" t="s">
         <v>58</v>
       </c>
       <c r="I12" s="44">
         <v>43529</v>
       </c>
-      <c r="J12" s="83" t="s">
+      <c r="J12" s="65" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="84"/>
+      <c r="K12" s="66"/>
     </row>
     <row r="13" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="37" t="s">
@@ -2396,10 +2516,10 @@
       <c r="E13" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="F13" s="88" t="s">
+      <c r="F13" s="70" t="s">
         <v>293</v>
       </c>
-      <c r="G13" s="89"/>
+      <c r="G13" s="71"/>
       <c r="H13" s="50"/>
       <c r="I13" s="51"/>
       <c r="J13" s="52"/>
@@ -2415,20 +2535,20 @@
       <c r="E14" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="F14" s="86" t="s">
+      <c r="F14" s="68" t="s">
         <v>291</v>
       </c>
-      <c r="G14" s="87"/>
+      <c r="G14" s="69"/>
       <c r="H14" s="47" t="s">
         <v>294</v>
       </c>
       <c r="I14" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="J14" s="90" t="s">
+      <c r="J14" s="72" t="s">
         <v>295</v>
       </c>
-      <c r="K14" s="91"/>
+      <c r="K14" s="73"/>
     </row>
     <row r="15" spans="2:13" ht="96.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="48" t="s">
@@ -2440,10 +2560,10 @@
       <c r="E15" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="F15" s="92" t="s">
+      <c r="F15" s="74" t="s">
         <v>324</v>
       </c>
-      <c r="G15" s="87"/>
+      <c r="G15" s="69"/>
       <c r="H15" s="48"/>
       <c r="I15" s="56"/>
       <c r="J15" s="58"/>
@@ -2454,105 +2574,105 @@
       <c r="E16" s="45"/>
     </row>
     <row r="18" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="85" t="s">
+      <c r="C18" s="67" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="85"/>
-      <c r="E18" s="85"/>
-      <c r="F18" s="85"/>
-      <c r="G18" s="85"/>
-      <c r="H18" s="85"/>
-      <c r="I18" s="85"/>
-      <c r="J18" s="85"/>
-      <c r="K18" s="85"/>
+      <c r="D18" s="67"/>
+      <c r="E18" s="67"/>
+      <c r="F18" s="67"/>
+      <c r="G18" s="67"/>
+      <c r="H18" s="67"/>
+      <c r="I18" s="67"/>
+      <c r="J18" s="67"/>
+      <c r="K18" s="67"/>
     </row>
     <row r="19" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="85"/>
-      <c r="D19" s="85"/>
-      <c r="E19" s="85"/>
-      <c r="F19" s="85"/>
-      <c r="G19" s="85"/>
-      <c r="H19" s="85"/>
-      <c r="I19" s="85"/>
-      <c r="J19" s="85"/>
-      <c r="K19" s="85"/>
+      <c r="C19" s="67"/>
+      <c r="D19" s="67"/>
+      <c r="E19" s="67"/>
+      <c r="F19" s="67"/>
+      <c r="G19" s="67"/>
+      <c r="H19" s="67"/>
+      <c r="I19" s="67"/>
+      <c r="J19" s="67"/>
+      <c r="K19" s="67"/>
     </row>
     <row r="20" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="85"/>
-      <c r="D20" s="85"/>
-      <c r="E20" s="85"/>
-      <c r="F20" s="85"/>
-      <c r="G20" s="85"/>
-      <c r="H20" s="85"/>
-      <c r="I20" s="85"/>
-      <c r="J20" s="85"/>
-      <c r="K20" s="85"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="67"/>
+      <c r="E20" s="67"/>
+      <c r="F20" s="67"/>
+      <c r="G20" s="67"/>
+      <c r="H20" s="67"/>
+      <c r="I20" s="67"/>
+      <c r="J20" s="67"/>
+      <c r="K20" s="67"/>
     </row>
     <row r="21" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="85"/>
-      <c r="D21" s="85"/>
-      <c r="E21" s="85"/>
-      <c r="F21" s="85"/>
-      <c r="G21" s="85"/>
-      <c r="H21" s="85"/>
-      <c r="I21" s="85"/>
-      <c r="J21" s="85"/>
-      <c r="K21" s="85"/>
+      <c r="C21" s="67"/>
+      <c r="D21" s="67"/>
+      <c r="E21" s="67"/>
+      <c r="F21" s="67"/>
+      <c r="G21" s="67"/>
+      <c r="H21" s="67"/>
+      <c r="I21" s="67"/>
+      <c r="J21" s="67"/>
+      <c r="K21" s="67"/>
     </row>
     <row r="22" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="85"/>
-      <c r="D22" s="85"/>
-      <c r="E22" s="85"/>
-      <c r="F22" s="85"/>
-      <c r="G22" s="85"/>
-      <c r="H22" s="85"/>
-      <c r="I22" s="85"/>
-      <c r="J22" s="85"/>
-      <c r="K22" s="85"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="67"/>
+      <c r="E22" s="67"/>
+      <c r="F22" s="67"/>
+      <c r="G22" s="67"/>
+      <c r="H22" s="67"/>
+      <c r="I22" s="67"/>
+      <c r="J22" s="67"/>
+      <c r="K22" s="67"/>
     </row>
     <row r="23" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="85"/>
-      <c r="D23" s="85"/>
-      <c r="E23" s="85"/>
-      <c r="F23" s="85"/>
-      <c r="G23" s="85"/>
-      <c r="H23" s="85"/>
-      <c r="I23" s="85"/>
-      <c r="J23" s="85"/>
-      <c r="K23" s="85"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="67"/>
+      <c r="E23" s="67"/>
+      <c r="F23" s="67"/>
+      <c r="G23" s="67"/>
+      <c r="H23" s="67"/>
+      <c r="I23" s="67"/>
+      <c r="J23" s="67"/>
+      <c r="K23" s="67"/>
     </row>
     <row r="24" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="85"/>
-      <c r="D24" s="85"/>
-      <c r="E24" s="85"/>
-      <c r="F24" s="85"/>
-      <c r="G24" s="85"/>
-      <c r="H24" s="85"/>
-      <c r="I24" s="85"/>
-      <c r="J24" s="85"/>
-      <c r="K24" s="85"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="67"/>
+      <c r="E24" s="67"/>
+      <c r="F24" s="67"/>
+      <c r="G24" s="67"/>
+      <c r="H24" s="67"/>
+      <c r="I24" s="67"/>
+      <c r="J24" s="67"/>
+      <c r="K24" s="67"/>
     </row>
     <row r="25" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="85"/>
-      <c r="D25" s="85"/>
-      <c r="E25" s="85"/>
-      <c r="F25" s="85"/>
-      <c r="G25" s="85"/>
-      <c r="H25" s="85"/>
-      <c r="I25" s="85"/>
-      <c r="J25" s="85"/>
-      <c r="K25" s="85"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="67"/>
+      <c r="E25" s="67"/>
+      <c r="F25" s="67"/>
+      <c r="G25" s="67"/>
+      <c r="H25" s="67"/>
+      <c r="I25" s="67"/>
+      <c r="J25" s="67"/>
+      <c r="K25" s="67"/>
     </row>
     <row r="26" spans="3:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="85"/>
-      <c r="D26" s="85"/>
-      <c r="E26" s="85"/>
-      <c r="F26" s="85"/>
-      <c r="G26" s="85"/>
-      <c r="H26" s="85"/>
-      <c r="I26" s="85"/>
-      <c r="J26" s="85"/>
-      <c r="K26" s="85"/>
+      <c r="C26" s="67"/>
+      <c r="D26" s="67"/>
+      <c r="E26" s="67"/>
+      <c r="F26" s="67"/>
+      <c r="G26" s="67"/>
+      <c r="H26" s="67"/>
+      <c r="I26" s="67"/>
+      <c r="J26" s="67"/>
+      <c r="K26" s="67"/>
     </row>
     <row r="27" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="15"/>
@@ -3254,8 +3374,8 @@
     </row>
     <row r="55" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
-      <c r="B55" s="79"/>
-      <c r="C55" s="80"/>
+      <c r="B55" s="61"/>
+      <c r="C55" s="62"/>
       <c r="D55" s="21" t="s">
         <v>193</v>
       </c>
@@ -3276,25 +3396,25 @@
       <c r="K55" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="L55" s="77"/>
-      <c r="M55" s="78"/>
-      <c r="N55" s="78"/>
-      <c r="O55" s="78"/>
-      <c r="P55" s="78"/>
-      <c r="Q55" s="78"/>
-      <c r="R55" s="79"/>
-      <c r="S55" s="79"/>
-      <c r="T55" s="79"/>
-      <c r="U55" s="79"/>
-      <c r="V55" s="79"/>
-      <c r="W55" s="79"/>
-      <c r="X55" s="79"/>
+      <c r="L55" s="59"/>
+      <c r="M55" s="60"/>
+      <c r="N55" s="60"/>
+      <c r="O55" s="60"/>
+      <c r="P55" s="60"/>
+      <c r="Q55" s="60"/>
+      <c r="R55" s="61"/>
+      <c r="S55" s="61"/>
+      <c r="T55" s="61"/>
+      <c r="U55" s="61"/>
+      <c r="V55" s="61"/>
+      <c r="W55" s="61"/>
+      <c r="X55" s="61"/>
       <c r="Y55" s="7"/>
     </row>
     <row r="56" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
-      <c r="B56" s="79"/>
-      <c r="C56" s="80"/>
+      <c r="B56" s="61"/>
+      <c r="C56" s="62"/>
       <c r="D56" s="19" t="s">
         <v>194</v>
       </c>
@@ -3315,25 +3435,25 @@
       <c r="K56" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="L56" s="77"/>
-      <c r="M56" s="78"/>
-      <c r="N56" s="78"/>
-      <c r="O56" s="78"/>
-      <c r="P56" s="78"/>
-      <c r="Q56" s="78"/>
-      <c r="R56" s="79"/>
-      <c r="S56" s="79"/>
-      <c r="T56" s="79"/>
-      <c r="U56" s="79"/>
-      <c r="V56" s="79"/>
-      <c r="W56" s="79"/>
-      <c r="X56" s="79"/>
+      <c r="L56" s="59"/>
+      <c r="M56" s="60"/>
+      <c r="N56" s="60"/>
+      <c r="O56" s="60"/>
+      <c r="P56" s="60"/>
+      <c r="Q56" s="60"/>
+      <c r="R56" s="61"/>
+      <c r="S56" s="61"/>
+      <c r="T56" s="61"/>
+      <c r="U56" s="61"/>
+      <c r="V56" s="61"/>
+      <c r="W56" s="61"/>
+      <c r="X56" s="61"/>
       <c r="Y56" s="7"/>
     </row>
     <row r="57" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
-      <c r="B57" s="79"/>
-      <c r="C57" s="80"/>
+      <c r="B57" s="61"/>
+      <c r="C57" s="62"/>
       <c r="D57" s="22" t="s">
         <v>195</v>
       </c>
@@ -3348,19 +3468,19 @@
       <c r="I57" s="28"/>
       <c r="J57" s="28"/>
       <c r="K57" s="29"/>
-      <c r="L57" s="77"/>
-      <c r="M57" s="78"/>
-      <c r="N57" s="78"/>
-      <c r="O57" s="78"/>
-      <c r="P57" s="78"/>
-      <c r="Q57" s="78"/>
-      <c r="R57" s="79"/>
-      <c r="S57" s="79"/>
-      <c r="T57" s="79"/>
-      <c r="U57" s="79"/>
-      <c r="V57" s="79"/>
-      <c r="W57" s="79"/>
-      <c r="X57" s="79"/>
+      <c r="L57" s="59"/>
+      <c r="M57" s="60"/>
+      <c r="N57" s="60"/>
+      <c r="O57" s="60"/>
+      <c r="P57" s="60"/>
+      <c r="Q57" s="60"/>
+      <c r="R57" s="61"/>
+      <c r="S57" s="61"/>
+      <c r="T57" s="61"/>
+      <c r="U57" s="61"/>
+      <c r="V57" s="61"/>
+      <c r="W57" s="61"/>
+      <c r="X57" s="61"/>
       <c r="Y57" s="7"/>
     </row>
     <row r="58" spans="1:25" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -4589,13 +4709,15 @@
       <c r="G108" s="28" t="s">
         <v>279</v>
       </c>
-      <c r="H108" s="20"/>
+      <c r="H108" s="20" t="s">
+        <v>339</v>
+      </c>
       <c r="I108" s="21"/>
       <c r="J108" s="28"/>
       <c r="K108" s="28"/>
       <c r="L108" s="54"/>
     </row>
-    <row r="109" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="109" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C109" s="13"/>
       <c r="D109" s="21" t="s">
         <v>133</v>
@@ -4607,7 +4729,9 @@
         <v>20</v>
       </c>
       <c r="G109" s="17"/>
-      <c r="H109" s="18"/>
+      <c r="H109" s="18" t="s">
+        <v>341</v>
+      </c>
       <c r="I109" s="28"/>
       <c r="J109" s="21"/>
       <c r="K109" s="28"/>
@@ -4627,13 +4751,15 @@
       <c r="G110" s="21" t="s">
         <v>280</v>
       </c>
-      <c r="H110" s="19"/>
+      <c r="H110" s="19" t="s">
+        <v>340</v>
+      </c>
       <c r="I110" s="21"/>
       <c r="J110" s="28"/>
       <c r="K110" s="29"/>
       <c r="L110" s="54"/>
     </row>
-    <row r="111" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="111" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C111" s="13"/>
       <c r="D111" s="21" t="s">
         <v>135</v>
@@ -4645,13 +4771,15 @@
         <v>20</v>
       </c>
       <c r="G111" s="17"/>
-      <c r="H111" s="18"/>
+      <c r="H111" s="18" t="s">
+        <v>342</v>
+      </c>
       <c r="I111" s="28"/>
       <c r="J111" s="29"/>
       <c r="K111" s="21"/>
       <c r="L111" s="54"/>
     </row>
-    <row r="112" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="112" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C112" s="13"/>
       <c r="D112" s="17" t="s">
         <v>136</v>
@@ -4665,7 +4793,9 @@
       <c r="G112" s="21" t="s">
         <v>285</v>
       </c>
-      <c r="H112" s="18"/>
+      <c r="H112" s="18" t="s">
+        <v>343</v>
+      </c>
       <c r="I112" s="21"/>
       <c r="J112" s="21"/>
       <c r="K112" s="28"/>
@@ -4685,13 +4815,15 @@
       <c r="G113" s="17" t="s">
         <v>286</v>
       </c>
-      <c r="H113" s="19"/>
+      <c r="H113" s="19" t="s">
+        <v>345</v>
+      </c>
       <c r="I113" s="28"/>
       <c r="J113" s="28"/>
       <c r="K113" s="27"/>
       <c r="L113" s="54"/>
     </row>
-    <row r="114" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="114" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C114" s="13"/>
       <c r="D114" s="19" t="s">
         <v>45</v>
@@ -4705,13 +4837,15 @@
       <c r="G114" s="21" t="s">
         <v>287</v>
       </c>
-      <c r="H114" s="20"/>
+      <c r="H114" s="20" t="s">
+        <v>346</v>
+      </c>
       <c r="I114" s="29"/>
       <c r="J114" s="21"/>
       <c r="K114" s="29"/>
       <c r="L114" s="54"/>
     </row>
-    <row r="115" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="115" spans="3:12" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C115" s="13"/>
       <c r="D115" s="21" t="s">
         <v>46</v>
@@ -4725,13 +4859,15 @@
       <c r="G115" s="21" t="s">
         <v>288</v>
       </c>
-      <c r="H115" s="18"/>
+      <c r="H115" s="18" t="s">
+        <v>344</v>
+      </c>
       <c r="I115" s="21"/>
       <c r="J115" s="28"/>
       <c r="K115" s="28"/>
       <c r="L115" s="54"/>
     </row>
-    <row r="116" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="116" spans="3:12" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C116" s="13"/>
       <c r="D116" s="22" t="s">
         <v>47</v>
@@ -4745,13 +4881,15 @@
       <c r="G116" s="28" t="s">
         <v>237</v>
       </c>
-      <c r="H116" s="19"/>
+      <c r="H116" s="19" t="s">
+        <v>347</v>
+      </c>
       <c r="I116" s="28"/>
       <c r="J116" s="27"/>
       <c r="K116" s="28"/>
       <c r="L116" s="54"/>
     </row>
-    <row r="117" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="117" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C117" s="13"/>
       <c r="D117" s="22" t="s">
         <v>138</v>
@@ -4763,13 +4901,15 @@
         <v>18</v>
       </c>
       <c r="G117" s="28"/>
-      <c r="H117" s="18"/>
+      <c r="H117" s="18" t="s">
+        <v>349</v>
+      </c>
       <c r="I117" s="21"/>
       <c r="J117" s="29"/>
       <c r="K117" s="29"/>
       <c r="L117" s="54"/>
     </row>
-    <row r="118" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="118" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C118" s="13"/>
       <c r="D118" s="21" t="s">
         <v>139</v>
@@ -4781,13 +4921,15 @@
         <v>18</v>
       </c>
       <c r="G118" s="28"/>
-      <c r="H118" s="18"/>
+      <c r="H118" s="18" t="s">
+        <v>350</v>
+      </c>
       <c r="I118" s="28"/>
       <c r="J118" s="28"/>
       <c r="K118" s="21"/>
       <c r="L118" s="54"/>
     </row>
-    <row r="119" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="119" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C119" s="13"/>
       <c r="D119" s="18" t="s">
         <v>140</v>
@@ -4799,13 +4941,15 @@
         <v>19</v>
       </c>
       <c r="G119" s="28"/>
-      <c r="H119" s="19"/>
+      <c r="H119" s="19" t="s">
+        <v>351</v>
+      </c>
       <c r="I119" s="21"/>
       <c r="J119" s="28"/>
       <c r="K119" s="28"/>
       <c r="L119" s="54"/>
     </row>
-    <row r="120" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="120" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C120" s="13"/>
       <c r="D120" s="22" t="s">
         <v>141</v>
@@ -4817,13 +4961,15 @@
         <v>19</v>
       </c>
       <c r="G120" s="17"/>
-      <c r="H120" s="20"/>
+      <c r="H120" s="20" t="s">
+        <v>354</v>
+      </c>
       <c r="I120" s="28"/>
       <c r="J120" s="29"/>
       <c r="K120" s="27"/>
       <c r="L120" s="54"/>
     </row>
-    <row r="121" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="121" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C121" s="13"/>
       <c r="D121" s="17" t="s">
         <v>48</v>
@@ -4837,7 +4983,9 @@
       <c r="G121" s="21" t="s">
         <v>238</v>
       </c>
-      <c r="H121" s="18"/>
+      <c r="H121" s="18" t="s">
+        <v>352</v>
+      </c>
       <c r="I121" s="29"/>
       <c r="J121" s="21"/>
       <c r="K121" s="29"/>
@@ -4861,7 +5009,7 @@
       <c r="K122" s="28"/>
       <c r="L122" s="54"/>
     </row>
-    <row r="123" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="123" spans="3:12" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C123" s="13"/>
       <c r="D123" s="19" t="s">
         <v>144</v>
@@ -4875,7 +5023,9 @@
       <c r="G123" s="21" t="s">
         <v>239</v>
       </c>
-      <c r="H123" s="18"/>
+      <c r="H123" s="18" t="s">
+        <v>347</v>
+      </c>
       <c r="I123" s="28"/>
       <c r="J123" s="21"/>
       <c r="K123" s="28"/>
@@ -4941,7 +5091,7 @@
       <c r="K126" s="28"/>
       <c r="L126" s="54"/>
     </row>
-    <row r="127" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="127" spans="3:12" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C127" s="13"/>
       <c r="D127" s="21" t="s">
         <v>151</v>
@@ -4953,7 +5103,9 @@
         <v>152</v>
       </c>
       <c r="G127" s="28"/>
-      <c r="H127" s="18"/>
+      <c r="H127" s="18" t="s">
+        <v>355</v>
+      </c>
       <c r="I127" s="28"/>
       <c r="J127" s="28"/>
       <c r="K127" s="27"/>
@@ -4973,7 +5125,9 @@
       <c r="G128" s="28" t="s">
         <v>236</v>
       </c>
-      <c r="H128" s="18"/>
+      <c r="H128" s="18" t="s">
+        <v>356</v>
+      </c>
       <c r="I128" s="29"/>
       <c r="J128" s="21"/>
       <c r="K128" s="29"/>
@@ -4991,13 +5145,15 @@
         <v>155</v>
       </c>
       <c r="G129" s="28"/>
-      <c r="H129" s="19"/>
+      <c r="H129" s="19" t="s">
+        <v>357</v>
+      </c>
       <c r="I129" s="21"/>
       <c r="J129" s="28"/>
       <c r="K129" s="28"/>
       <c r="L129" s="54"/>
     </row>
-    <row r="130" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="130" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C130" s="13"/>
       <c r="D130" s="17" t="s">
         <v>156</v>
@@ -5009,7 +5165,9 @@
         <v>155</v>
       </c>
       <c r="G130" s="28"/>
-      <c r="H130" s="18"/>
+      <c r="H130" s="18" t="s">
+        <v>348</v>
+      </c>
       <c r="I130" s="28"/>
       <c r="J130" s="27"/>
       <c r="K130" s="28"/>
@@ -5027,7 +5185,9 @@
         <v>155</v>
       </c>
       <c r="G131" s="17"/>
-      <c r="H131" s="19"/>
+      <c r="H131" s="19" t="s">
+        <v>358</v>
+      </c>
       <c r="I131" s="21"/>
       <c r="J131" s="29"/>
       <c r="K131" s="29"/>
@@ -5045,7 +5205,9 @@
         <v>155</v>
       </c>
       <c r="G132" s="21"/>
-      <c r="H132" s="20"/>
+      <c r="H132" s="20" t="s">
+        <v>359</v>
+      </c>
       <c r="I132" s="28"/>
       <c r="J132" s="28"/>
       <c r="K132" s="21"/>
@@ -5063,13 +5225,15 @@
         <v>155</v>
       </c>
       <c r="G133" s="17"/>
-      <c r="H133" s="18"/>
+      <c r="H133" s="18" t="s">
+        <v>360</v>
+      </c>
       <c r="I133" s="21"/>
       <c r="J133" s="28"/>
       <c r="K133" s="28"/>
       <c r="L133" s="54"/>
     </row>
-    <row r="134" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="134" spans="3:12" ht="132" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C134" s="13"/>
       <c r="D134" s="22" t="s">
         <v>160</v>
@@ -5083,7 +5247,9 @@
       <c r="G134" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="H134" s="19"/>
+      <c r="H134" s="19" t="s">
+        <v>353</v>
+      </c>
       <c r="I134" s="28"/>
       <c r="J134" s="29"/>
       <c r="K134" s="27"/>
@@ -5103,7 +5269,9 @@
       <c r="G135" s="17" t="s">
         <v>243</v>
       </c>
-      <c r="H135" s="18"/>
+      <c r="H135" s="18" t="s">
+        <v>361</v>
+      </c>
       <c r="I135" s="29"/>
       <c r="J135" s="21"/>
       <c r="K135" s="28"/>
@@ -5123,7 +5291,9 @@
       <c r="G136" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="H136" s="18"/>
+      <c r="H136" s="18" t="s">
+        <v>362</v>
+      </c>
       <c r="I136" s="21"/>
       <c r="J136" s="28"/>
       <c r="K136" s="29"/>
@@ -5143,7 +5313,9 @@
       <c r="G137" s="21" t="s">
         <v>243</v>
       </c>
-      <c r="H137" s="19"/>
+      <c r="H137" s="19" t="s">
+        <v>363</v>
+      </c>
       <c r="I137" s="28"/>
       <c r="J137" s="21"/>
       <c r="K137" s="21"/>
@@ -5163,7 +5335,9 @@
       <c r="G138" s="28" t="s">
         <v>243</v>
       </c>
-      <c r="H138" s="20"/>
+      <c r="H138" s="20" t="s">
+        <v>364</v>
+      </c>
       <c r="I138" s="21"/>
       <c r="J138" s="28"/>
       <c r="K138" s="28"/>
@@ -5183,7 +5357,9 @@
       <c r="G139" s="28" t="s">
         <v>285</v>
       </c>
-      <c r="H139" s="18"/>
+      <c r="H139" s="18" t="s">
+        <v>365</v>
+      </c>
       <c r="I139" s="28"/>
       <c r="J139" s="29"/>
       <c r="K139" s="27"/>
@@ -5203,7 +5379,9 @@
       <c r="G140" s="28" t="s">
         <v>217</v>
       </c>
-      <c r="H140" s="19"/>
+      <c r="H140" s="19" t="s">
+        <v>366</v>
+      </c>
       <c r="I140" s="21"/>
       <c r="J140" s="21"/>
       <c r="K140" s="29"/>
@@ -5502,6 +5680,12 @@
     </row>
   </sheetData>
   <mergeCells count="17">
+    <mergeCell ref="B2:M7"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
     <mergeCell ref="L55:Q57"/>
     <mergeCell ref="B55:C57"/>
     <mergeCell ref="R55:T57"/>
@@ -5513,12 +5697,6 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="F15:G15"/>
-    <mergeCell ref="B2:M7"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added test cases ID related to admin
Added test cases ID related to admin
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="733" uniqueCount="367">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="742" uniqueCount="376">
   <si>
     <t>Author</t>
   </si>
@@ -1267,6 +1267,41 @@
   </si>
   <si>
     <t>BANK_SYS_TC_TR_R046</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R001
+BANK_SYS_TC_Admin_R002</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R003
+BANK_SYS_TC_Admin_R004
+BANK_SYS_TC_Admin_R005
+BANK_SYS_TC_Admin_R006
+BANK_SYS_TC_Admin_R007</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R008
+BANK_SYS_TC_Admin_R009
+BANK_SYS_TC_Admin_R010</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R008</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R011</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R012
+BANK_SYS_TC_Admin_R013</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R014</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R015</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_Admin_R016</t>
   </si>
 </sst>
 </file>
@@ -1919,6 +1954,60 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -1965,60 +2054,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2304,8 +2339,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y156"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C138" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="H141" sqref="H141"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C143" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H149" sqref="H149"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2324,90 +2359,90 @@
   <sheetData>
     <row r="1" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="77"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="61"/>
     </row>
     <row r="3" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="80"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="78"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="80"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="64"/>
     </row>
     <row r="5" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="80"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="64"/>
     </row>
     <row r="6" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="80"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="64"/>
     </row>
     <row r="7" spans="2:13" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="81"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="83"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="67"/>
     </row>
     <row r="8" spans="2:13" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
@@ -2425,16 +2460,16 @@
     </row>
     <row r="9" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="85"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="69"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2447,20 +2482,20 @@
       <c r="E10" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="86" t="s">
+      <c r="F10" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="87"/>
+      <c r="G10" s="71"/>
       <c r="H10" s="34" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="88" t="s">
+      <c r="J10" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="87"/>
+      <c r="K10" s="71"/>
     </row>
     <row r="11" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="37" t="s">
@@ -2472,14 +2507,14 @@
       <c r="E11" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="89" t="s">
+      <c r="F11" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="90"/>
+      <c r="G11" s="74"/>
       <c r="H11" s="35"/>
       <c r="I11" s="19"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="92"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76"/>
     </row>
     <row r="12" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="35" t="s">
@@ -2491,20 +2526,20 @@
       <c r="E12" s="36">
         <v>43529</v>
       </c>
-      <c r="F12" s="63" t="s">
+      <c r="F12" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="64"/>
+      <c r="G12" s="82"/>
       <c r="H12" s="43" t="s">
         <v>58</v>
       </c>
       <c r="I12" s="44">
         <v>43529</v>
       </c>
-      <c r="J12" s="65" t="s">
+      <c r="J12" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="66"/>
+      <c r="K12" s="84"/>
     </row>
     <row r="13" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="37" t="s">
@@ -2516,10 +2551,10 @@
       <c r="E13" s="41" t="s">
         <v>292</v>
       </c>
-      <c r="F13" s="70" t="s">
+      <c r="F13" s="88" t="s">
         <v>293</v>
       </c>
-      <c r="G13" s="71"/>
+      <c r="G13" s="89"/>
       <c r="H13" s="50"/>
       <c r="I13" s="51"/>
       <c r="J13" s="52"/>
@@ -2535,20 +2570,20 @@
       <c r="E14" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="F14" s="68" t="s">
+      <c r="F14" s="86" t="s">
         <v>291</v>
       </c>
-      <c r="G14" s="69"/>
+      <c r="G14" s="87"/>
       <c r="H14" s="47" t="s">
         <v>294</v>
       </c>
       <c r="I14" s="46" t="s">
         <v>290</v>
       </c>
-      <c r="J14" s="72" t="s">
+      <c r="J14" s="90" t="s">
         <v>295</v>
       </c>
-      <c r="K14" s="73"/>
+      <c r="K14" s="91"/>
     </row>
     <row r="15" spans="2:13" ht="96.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="48" t="s">
@@ -2560,10 +2595,10 @@
       <c r="E15" s="46" t="s">
         <v>323</v>
       </c>
-      <c r="F15" s="74" t="s">
+      <c r="F15" s="92" t="s">
         <v>324</v>
       </c>
-      <c r="G15" s="69"/>
+      <c r="G15" s="87"/>
       <c r="H15" s="48"/>
       <c r="I15" s="56"/>
       <c r="J15" s="58"/>
@@ -2574,105 +2609,105 @@
       <c r="E16" s="45"/>
     </row>
     <row r="18" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="85"/>
     </row>
     <row r="19" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="85"/>
     </row>
     <row r="20" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="67"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
     </row>
     <row r="21" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="85"/>
     </row>
     <row r="22" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="67"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
     </row>
     <row r="23" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
     </row>
     <row r="24" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="85"/>
     </row>
     <row r="25" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
     </row>
     <row r="26" spans="3:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="85"/>
     </row>
     <row r="27" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="15"/>
@@ -3374,8 +3409,8 @@
     </row>
     <row r="55" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
-      <c r="B55" s="61"/>
-      <c r="C55" s="62"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="80"/>
       <c r="D55" s="21" t="s">
         <v>193</v>
       </c>
@@ -3396,25 +3431,25 @@
       <c r="K55" s="21" t="s">
         <v>302</v>
       </c>
-      <c r="L55" s="59"/>
-      <c r="M55" s="60"/>
-      <c r="N55" s="60"/>
-      <c r="O55" s="60"/>
-      <c r="P55" s="60"/>
-      <c r="Q55" s="60"/>
-      <c r="R55" s="61"/>
-      <c r="S55" s="61"/>
-      <c r="T55" s="61"/>
-      <c r="U55" s="61"/>
-      <c r="V55" s="61"/>
-      <c r="W55" s="61"/>
-      <c r="X55" s="61"/>
+      <c r="L55" s="77"/>
+      <c r="M55" s="78"/>
+      <c r="N55" s="78"/>
+      <c r="O55" s="78"/>
+      <c r="P55" s="78"/>
+      <c r="Q55" s="78"/>
+      <c r="R55" s="79"/>
+      <c r="S55" s="79"/>
+      <c r="T55" s="79"/>
+      <c r="U55" s="79"/>
+      <c r="V55" s="79"/>
+      <c r="W55" s="79"/>
+      <c r="X55" s="79"/>
       <c r="Y55" s="7"/>
     </row>
     <row r="56" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
-      <c r="B56" s="61"/>
-      <c r="C56" s="62"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="80"/>
       <c r="D56" s="19" t="s">
         <v>194</v>
       </c>
@@ -3435,25 +3470,25 @@
       <c r="K56" s="27" t="s">
         <v>262</v>
       </c>
-      <c r="L56" s="59"/>
-      <c r="M56" s="60"/>
-      <c r="N56" s="60"/>
-      <c r="O56" s="60"/>
-      <c r="P56" s="60"/>
-      <c r="Q56" s="60"/>
-      <c r="R56" s="61"/>
-      <c r="S56" s="61"/>
-      <c r="T56" s="61"/>
-      <c r="U56" s="61"/>
-      <c r="V56" s="61"/>
-      <c r="W56" s="61"/>
-      <c r="X56" s="61"/>
+      <c r="L56" s="77"/>
+      <c r="M56" s="78"/>
+      <c r="N56" s="78"/>
+      <c r="O56" s="78"/>
+      <c r="P56" s="78"/>
+      <c r="Q56" s="78"/>
+      <c r="R56" s="79"/>
+      <c r="S56" s="79"/>
+      <c r="T56" s="79"/>
+      <c r="U56" s="79"/>
+      <c r="V56" s="79"/>
+      <c r="W56" s="79"/>
+      <c r="X56" s="79"/>
       <c r="Y56" s="7"/>
     </row>
     <row r="57" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
-      <c r="B57" s="61"/>
-      <c r="C57" s="62"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="80"/>
       <c r="D57" s="22" t="s">
         <v>195</v>
       </c>
@@ -3468,19 +3503,19 @@
       <c r="I57" s="28"/>
       <c r="J57" s="28"/>
       <c r="K57" s="29"/>
-      <c r="L57" s="59"/>
-      <c r="M57" s="60"/>
-      <c r="N57" s="60"/>
-      <c r="O57" s="60"/>
-      <c r="P57" s="60"/>
-      <c r="Q57" s="60"/>
-      <c r="R57" s="61"/>
-      <c r="S57" s="61"/>
-      <c r="T57" s="61"/>
-      <c r="U57" s="61"/>
-      <c r="V57" s="61"/>
-      <c r="W57" s="61"/>
-      <c r="X57" s="61"/>
+      <c r="L57" s="77"/>
+      <c r="M57" s="78"/>
+      <c r="N57" s="78"/>
+      <c r="O57" s="78"/>
+      <c r="P57" s="78"/>
+      <c r="Q57" s="78"/>
+      <c r="R57" s="79"/>
+      <c r="S57" s="79"/>
+      <c r="T57" s="79"/>
+      <c r="U57" s="79"/>
+      <c r="V57" s="79"/>
+      <c r="W57" s="79"/>
+      <c r="X57" s="79"/>
       <c r="Y57" s="7"/>
     </row>
     <row r="58" spans="1:25" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
@@ -5401,13 +5436,15 @@
       <c r="G141" s="28" t="s">
         <v>325</v>
       </c>
-      <c r="H141" s="18"/>
+      <c r="H141" s="18" t="s">
+        <v>367</v>
+      </c>
       <c r="I141" s="28"/>
       <c r="J141" s="28"/>
       <c r="K141" s="28"/>
       <c r="L141" s="54"/>
     </row>
-    <row r="142" spans="3:12" ht="75.75" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="142" spans="3:12" ht="94.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C142" s="13"/>
       <c r="D142" s="21" t="s">
         <v>168</v>
@@ -5421,7 +5458,9 @@
       <c r="G142" s="17" t="s">
         <v>210</v>
       </c>
-      <c r="H142" s="18"/>
+      <c r="H142" s="18" t="s">
+        <v>368</v>
+      </c>
       <c r="I142" s="29"/>
       <c r="J142" s="21"/>
       <c r="K142" s="29"/>
@@ -5441,7 +5480,9 @@
       <c r="G143" s="21" t="s">
         <v>212</v>
       </c>
-      <c r="H143" s="19"/>
+      <c r="H143" s="19" t="s">
+        <v>369</v>
+      </c>
       <c r="I143" s="21"/>
       <c r="J143" s="28"/>
       <c r="K143" s="21"/>
@@ -5461,13 +5502,15 @@
       <c r="G144" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H144" s="20"/>
+      <c r="H144" s="20" t="s">
+        <v>371</v>
+      </c>
       <c r="I144" s="28"/>
       <c r="J144" s="27"/>
       <c r="K144" s="28"/>
       <c r="L144" s="54"/>
     </row>
-    <row r="145" spans="3:12" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="145" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C145" s="13"/>
       <c r="D145" s="21" t="s">
         <v>171</v>
@@ -5481,7 +5524,9 @@
       <c r="G145" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="H145" s="18"/>
+      <c r="H145" s="18" t="s">
+        <v>372</v>
+      </c>
       <c r="I145" s="28"/>
       <c r="J145" s="28"/>
       <c r="K145" s="27"/>
@@ -5501,7 +5546,9 @@
       <c r="G146" s="30" t="s">
         <v>244</v>
       </c>
-      <c r="H146" s="19"/>
+      <c r="H146" s="19" t="s">
+        <v>370</v>
+      </c>
       <c r="I146" s="28"/>
       <c r="J146" s="28"/>
       <c r="K146" s="29"/>
@@ -5521,7 +5568,9 @@
       <c r="G147" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="H147" s="18"/>
+      <c r="H147" s="18" t="s">
+        <v>373</v>
+      </c>
       <c r="I147" s="28"/>
       <c r="J147" s="28"/>
       <c r="K147" s="28"/>
@@ -5541,7 +5590,9 @@
       <c r="G148" s="17" t="s">
         <v>246</v>
       </c>
-      <c r="H148" s="18"/>
+      <c r="H148" s="18" t="s">
+        <v>374</v>
+      </c>
       <c r="I148" s="17"/>
       <c r="J148" s="17"/>
       <c r="K148" s="29"/>
@@ -5561,7 +5612,9 @@
       <c r="G149" s="21" t="s">
         <v>326</v>
       </c>
-      <c r="H149" s="19"/>
+      <c r="H149" s="19" t="s">
+        <v>375</v>
+      </c>
       <c r="I149" s="21"/>
       <c r="J149" s="21"/>
       <c r="K149" s="21"/>
@@ -5680,12 +5733,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B2:M7"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
     <mergeCell ref="L55:Q57"/>
     <mergeCell ref="B55:C57"/>
     <mergeCell ref="R55:T57"/>
@@ -5697,6 +5744,12 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="F15:G15"/>
+    <mergeCell ref="B2:M7"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>

<commit_message>
Added test case id BANK_SYS_TC_TR_R036 for BANK_SYS_SRS_PT_R025
Added test case id BANK_SYS_TC_TR_R036 for BANK_SYS_SRS_PT_R025
</commit_message>
<xml_diff>
--- a/PM/Requirements Trcability Matrix.xlsx
+++ b/PM/Requirements Trcability Matrix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\iti\project managment\testing\Internet-Banking-System\PM\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PC\Documents\GitHub\Internet-Banking-System\PM\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="418">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="796" uniqueCount="418">
   <si>
     <t>Author</t>
   </si>
@@ -1400,10 +1400,6 @@
     <t>BANK_SYS_TC_Reg_R043</t>
   </si>
   <si>
-    <t>BANK_SYS_TC_Log_R011
-BANK_SYS_TC_ACC_R011</t>
-  </si>
-  <si>
     <t>BANK_SYS_TC_ACC_R002</t>
   </si>
   <si>
@@ -1502,6 +1498,9 @@
   </si>
   <si>
     <t>BANK_SYS_TC_ACC_R010</t>
+  </si>
+  <si>
+    <t>BANK_SYS_TC_TR_R036</t>
   </si>
 </sst>
 </file>
@@ -2154,6 +2153,60 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="30" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="33" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2200,60 +2253,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="22" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -2539,8 +2538,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:Y153"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C16" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
-      <selection activeCell="C129" sqref="C129"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="C87" zoomScale="87" zoomScaleNormal="87" workbookViewId="0">
+      <selection activeCell="H93" sqref="H93"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18.75" x14ac:dyDescent="0.25"/>
@@ -2559,90 +2558,90 @@
   <sheetData>
     <row r="1" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B2" s="75" t="s">
+      <c r="B2" s="59" t="s">
         <v>11</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-      <c r="K2" s="76"/>
-      <c r="L2" s="76"/>
-      <c r="M2" s="77"/>
+      <c r="C2" s="60"/>
+      <c r="D2" s="60"/>
+      <c r="E2" s="60"/>
+      <c r="F2" s="60"/>
+      <c r="G2" s="60"/>
+      <c r="H2" s="60"/>
+      <c r="I2" s="60"/>
+      <c r="J2" s="60"/>
+      <c r="K2" s="60"/>
+      <c r="L2" s="60"/>
+      <c r="M2" s="61"/>
     </row>
     <row r="3" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B3" s="78"/>
-      <c r="C3" s="79"/>
-      <c r="D3" s="79"/>
-      <c r="E3" s="79"/>
-      <c r="F3" s="79"/>
-      <c r="G3" s="79"/>
-      <c r="H3" s="79"/>
-      <c r="I3" s="79"/>
-      <c r="J3" s="79"/>
-      <c r="K3" s="79"/>
-      <c r="L3" s="79"/>
-      <c r="M3" s="80"/>
+      <c r="B3" s="62"/>
+      <c r="C3" s="63"/>
+      <c r="D3" s="63"/>
+      <c r="E3" s="63"/>
+      <c r="F3" s="63"/>
+      <c r="G3" s="63"/>
+      <c r="H3" s="63"/>
+      <c r="I3" s="63"/>
+      <c r="J3" s="63"/>
+      <c r="K3" s="63"/>
+      <c r="L3" s="63"/>
+      <c r="M3" s="64"/>
     </row>
     <row r="4" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="78"/>
-      <c r="C4" s="79"/>
-      <c r="D4" s="79"/>
-      <c r="E4" s="79"/>
-      <c r="F4" s="79"/>
-      <c r="G4" s="79"/>
-      <c r="H4" s="79"/>
-      <c r="I4" s="79"/>
-      <c r="J4" s="79"/>
-      <c r="K4" s="79"/>
-      <c r="L4" s="79"/>
-      <c r="M4" s="80"/>
+      <c r="B4" s="62"/>
+      <c r="C4" s="63"/>
+      <c r="D4" s="63"/>
+      <c r="E4" s="63"/>
+      <c r="F4" s="63"/>
+      <c r="G4" s="63"/>
+      <c r="H4" s="63"/>
+      <c r="I4" s="63"/>
+      <c r="J4" s="63"/>
+      <c r="K4" s="63"/>
+      <c r="L4" s="63"/>
+      <c r="M4" s="64"/>
     </row>
     <row r="5" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="78"/>
-      <c r="C5" s="79"/>
-      <c r="D5" s="79"/>
-      <c r="E5" s="79"/>
-      <c r="F5" s="79"/>
-      <c r="G5" s="79"/>
-      <c r="H5" s="79"/>
-      <c r="I5" s="79"/>
-      <c r="J5" s="79"/>
-      <c r="K5" s="79"/>
-      <c r="L5" s="79"/>
-      <c r="M5" s="80"/>
+      <c r="B5" s="62"/>
+      <c r="C5" s="63"/>
+      <c r="D5" s="63"/>
+      <c r="E5" s="63"/>
+      <c r="F5" s="63"/>
+      <c r="G5" s="63"/>
+      <c r="H5" s="63"/>
+      <c r="I5" s="63"/>
+      <c r="J5" s="63"/>
+      <c r="K5" s="63"/>
+      <c r="L5" s="63"/>
+      <c r="M5" s="64"/>
     </row>
     <row r="6" spans="2:13" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="78"/>
-      <c r="C6" s="79"/>
-      <c r="D6" s="79"/>
-      <c r="E6" s="79"/>
-      <c r="F6" s="79"/>
-      <c r="G6" s="79"/>
-      <c r="H6" s="79"/>
-      <c r="I6" s="79"/>
-      <c r="J6" s="79"/>
-      <c r="K6" s="79"/>
-      <c r="L6" s="79"/>
-      <c r="M6" s="80"/>
+      <c r="B6" s="62"/>
+      <c r="C6" s="63"/>
+      <c r="D6" s="63"/>
+      <c r="E6" s="63"/>
+      <c r="F6" s="63"/>
+      <c r="G6" s="63"/>
+      <c r="H6" s="63"/>
+      <c r="I6" s="63"/>
+      <c r="J6" s="63"/>
+      <c r="K6" s="63"/>
+      <c r="L6" s="63"/>
+      <c r="M6" s="64"/>
     </row>
     <row r="7" spans="2:13" ht="14.45" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B7" s="81"/>
-      <c r="C7" s="82"/>
-      <c r="D7" s="82"/>
-      <c r="E7" s="82"/>
-      <c r="F7" s="82"/>
-      <c r="G7" s="82"/>
-      <c r="H7" s="82"/>
-      <c r="I7" s="82"/>
-      <c r="J7" s="82"/>
-      <c r="K7" s="82"/>
-      <c r="L7" s="82"/>
-      <c r="M7" s="83"/>
+      <c r="B7" s="65"/>
+      <c r="C7" s="66"/>
+      <c r="D7" s="66"/>
+      <c r="E7" s="66"/>
+      <c r="F7" s="66"/>
+      <c r="G7" s="66"/>
+      <c r="H7" s="66"/>
+      <c r="I7" s="66"/>
+      <c r="J7" s="66"/>
+      <c r="K7" s="66"/>
+      <c r="L7" s="66"/>
+      <c r="M7" s="67"/>
     </row>
     <row r="8" spans="2:13" s="8" customFormat="1" ht="14.45" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10"/>
@@ -2660,16 +2659,16 @@
     </row>
     <row r="9" spans="2:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B9" s="1"/>
-      <c r="C9" s="84" t="s">
+      <c r="C9" s="68" t="s">
         <v>5</v>
       </c>
-      <c r="D9" s="84"/>
-      <c r="E9" s="84"/>
-      <c r="F9" s="84"/>
-      <c r="G9" s="84"/>
-      <c r="H9" s="84"/>
-      <c r="I9" s="84"/>
-      <c r="J9" s="85"/>
+      <c r="D9" s="68"/>
+      <c r="E9" s="68"/>
+      <c r="F9" s="68"/>
+      <c r="G9" s="68"/>
+      <c r="H9" s="68"/>
+      <c r="I9" s="68"/>
+      <c r="J9" s="69"/>
       <c r="K9" s="1"/>
     </row>
     <row r="10" spans="2:13" ht="15" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -2682,20 +2681,20 @@
       <c r="E10" s="40" t="s">
         <v>1</v>
       </c>
-      <c r="F10" s="86" t="s">
+      <c r="F10" s="70" t="s">
         <v>3</v>
       </c>
-      <c r="G10" s="87"/>
+      <c r="G10" s="71"/>
       <c r="H10" s="34" t="s">
         <v>7</v>
       </c>
       <c r="I10" s="16" t="s">
         <v>8</v>
       </c>
-      <c r="J10" s="88" t="s">
+      <c r="J10" s="72" t="s">
         <v>9</v>
       </c>
-      <c r="K10" s="87"/>
+      <c r="K10" s="71"/>
     </row>
     <row r="11" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C11" s="37" t="s">
@@ -2707,14 +2706,14 @@
       <c r="E11" s="38" t="s">
         <v>4</v>
       </c>
-      <c r="F11" s="89" t="s">
+      <c r="F11" s="73" t="s">
         <v>12</v>
       </c>
-      <c r="G11" s="90"/>
+      <c r="G11" s="74"/>
       <c r="H11" s="35"/>
       <c r="I11" s="19"/>
-      <c r="J11" s="91"/>
-      <c r="K11" s="92"/>
+      <c r="J11" s="75"/>
+      <c r="K11" s="76"/>
     </row>
     <row r="12" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C12" s="35" t="s">
@@ -2726,20 +2725,20 @@
       <c r="E12" s="36">
         <v>43529</v>
       </c>
-      <c r="F12" s="63" t="s">
+      <c r="F12" s="81" t="s">
         <v>59</v>
       </c>
-      <c r="G12" s="64"/>
+      <c r="G12" s="82"/>
       <c r="H12" s="43" t="s">
         <v>58</v>
       </c>
       <c r="I12" s="44">
         <v>43529</v>
       </c>
-      <c r="J12" s="65" t="s">
+      <c r="J12" s="83" t="s">
         <v>60</v>
       </c>
-      <c r="K12" s="66"/>
+      <c r="K12" s="84"/>
     </row>
     <row r="13" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C13" s="37" t="s">
@@ -2751,10 +2750,10 @@
       <c r="E13" s="41" t="s">
         <v>280</v>
       </c>
-      <c r="F13" s="70" t="s">
+      <c r="F13" s="88" t="s">
         <v>281</v>
       </c>
-      <c r="G13" s="71"/>
+      <c r="G13" s="89"/>
       <c r="H13" s="50"/>
       <c r="I13" s="51"/>
       <c r="J13" s="52"/>
@@ -2770,20 +2769,20 @@
       <c r="E14" s="46" t="s">
         <v>278</v>
       </c>
-      <c r="F14" s="68" t="s">
+      <c r="F14" s="86" t="s">
         <v>279</v>
       </c>
-      <c r="G14" s="69"/>
+      <c r="G14" s="87"/>
       <c r="H14" s="47" t="s">
         <v>282</v>
       </c>
       <c r="I14" s="46" t="s">
         <v>278</v>
       </c>
-      <c r="J14" s="72" t="s">
+      <c r="J14" s="90" t="s">
         <v>283</v>
       </c>
-      <c r="K14" s="73"/>
+      <c r="K14" s="91"/>
     </row>
     <row r="15" spans="2:13" ht="96.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C15" s="48" t="s">
@@ -2795,10 +2794,10 @@
       <c r="E15" s="46" t="s">
         <v>311</v>
       </c>
-      <c r="F15" s="74" t="s">
+      <c r="F15" s="92" t="s">
         <v>312</v>
       </c>
-      <c r="G15" s="69"/>
+      <c r="G15" s="87"/>
       <c r="H15" s="48"/>
       <c r="I15" s="56"/>
       <c r="J15" s="58"/>
@@ -2809,105 +2808,105 @@
       <c r="E16" s="45"/>
     </row>
     <row r="18" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C18" s="67" t="s">
+      <c r="C18" s="85" t="s">
         <v>61</v>
       </c>
-      <c r="D18" s="67"/>
-      <c r="E18" s="67"/>
-      <c r="F18" s="67"/>
-      <c r="G18" s="67"/>
-      <c r="H18" s="67"/>
-      <c r="I18" s="67"/>
-      <c r="J18" s="67"/>
-      <c r="K18" s="67"/>
+      <c r="D18" s="85"/>
+      <c r="E18" s="85"/>
+      <c r="F18" s="85"/>
+      <c r="G18" s="85"/>
+      <c r="H18" s="85"/>
+      <c r="I18" s="85"/>
+      <c r="J18" s="85"/>
+      <c r="K18" s="85"/>
     </row>
     <row r="19" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C19" s="67"/>
-      <c r="D19" s="67"/>
-      <c r="E19" s="67"/>
-      <c r="F19" s="67"/>
-      <c r="G19" s="67"/>
-      <c r="H19" s="67"/>
-      <c r="I19" s="67"/>
-      <c r="J19" s="67"/>
-      <c r="K19" s="67"/>
+      <c r="C19" s="85"/>
+      <c r="D19" s="85"/>
+      <c r="E19" s="85"/>
+      <c r="F19" s="85"/>
+      <c r="G19" s="85"/>
+      <c r="H19" s="85"/>
+      <c r="I19" s="85"/>
+      <c r="J19" s="85"/>
+      <c r="K19" s="85"/>
     </row>
     <row r="20" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C20" s="67"/>
-      <c r="D20" s="67"/>
-      <c r="E20" s="67"/>
-      <c r="F20" s="67"/>
-      <c r="G20" s="67"/>
-      <c r="H20" s="67"/>
-      <c r="I20" s="67"/>
-      <c r="J20" s="67"/>
-      <c r="K20" s="67"/>
+      <c r="C20" s="85"/>
+      <c r="D20" s="85"/>
+      <c r="E20" s="85"/>
+      <c r="F20" s="85"/>
+      <c r="G20" s="85"/>
+      <c r="H20" s="85"/>
+      <c r="I20" s="85"/>
+      <c r="J20" s="85"/>
+      <c r="K20" s="85"/>
     </row>
     <row r="21" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C21" s="67"/>
-      <c r="D21" s="67"/>
-      <c r="E21" s="67"/>
-      <c r="F21" s="67"/>
-      <c r="G21" s="67"/>
-      <c r="H21" s="67"/>
-      <c r="I21" s="67"/>
-      <c r="J21" s="67"/>
-      <c r="K21" s="67"/>
+      <c r="C21" s="85"/>
+      <c r="D21" s="85"/>
+      <c r="E21" s="85"/>
+      <c r="F21" s="85"/>
+      <c r="G21" s="85"/>
+      <c r="H21" s="85"/>
+      <c r="I21" s="85"/>
+      <c r="J21" s="85"/>
+      <c r="K21" s="85"/>
     </row>
     <row r="22" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C22" s="67"/>
-      <c r="D22" s="67"/>
-      <c r="E22" s="67"/>
-      <c r="F22" s="67"/>
-      <c r="G22" s="67"/>
-      <c r="H22" s="67"/>
-      <c r="I22" s="67"/>
-      <c r="J22" s="67"/>
-      <c r="K22" s="67"/>
+      <c r="C22" s="85"/>
+      <c r="D22" s="85"/>
+      <c r="E22" s="85"/>
+      <c r="F22" s="85"/>
+      <c r="G22" s="85"/>
+      <c r="H22" s="85"/>
+      <c r="I22" s="85"/>
+      <c r="J22" s="85"/>
+      <c r="K22" s="85"/>
     </row>
     <row r="23" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C23" s="67"/>
-      <c r="D23" s="67"/>
-      <c r="E23" s="67"/>
-      <c r="F23" s="67"/>
-      <c r="G23" s="67"/>
-      <c r="H23" s="67"/>
-      <c r="I23" s="67"/>
-      <c r="J23" s="67"/>
-      <c r="K23" s="67"/>
+      <c r="C23" s="85"/>
+      <c r="D23" s="85"/>
+      <c r="E23" s="85"/>
+      <c r="F23" s="85"/>
+      <c r="G23" s="85"/>
+      <c r="H23" s="85"/>
+      <c r="I23" s="85"/>
+      <c r="J23" s="85"/>
+      <c r="K23" s="85"/>
     </row>
     <row r="24" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C24" s="67"/>
-      <c r="D24" s="67"/>
-      <c r="E24" s="67"/>
-      <c r="F24" s="67"/>
-      <c r="G24" s="67"/>
-      <c r="H24" s="67"/>
-      <c r="I24" s="67"/>
-      <c r="J24" s="67"/>
-      <c r="K24" s="67"/>
+      <c r="C24" s="85"/>
+      <c r="D24" s="85"/>
+      <c r="E24" s="85"/>
+      <c r="F24" s="85"/>
+      <c r="G24" s="85"/>
+      <c r="H24" s="85"/>
+      <c r="I24" s="85"/>
+      <c r="J24" s="85"/>
+      <c r="K24" s="85"/>
     </row>
     <row r="25" spans="3:12" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="C25" s="67"/>
-      <c r="D25" s="67"/>
-      <c r="E25" s="67"/>
-      <c r="F25" s="67"/>
-      <c r="G25" s="67"/>
-      <c r="H25" s="67"/>
-      <c r="I25" s="67"/>
-      <c r="J25" s="67"/>
-      <c r="K25" s="67"/>
+      <c r="C25" s="85"/>
+      <c r="D25" s="85"/>
+      <c r="E25" s="85"/>
+      <c r="F25" s="85"/>
+      <c r="G25" s="85"/>
+      <c r="H25" s="85"/>
+      <c r="I25" s="85"/>
+      <c r="J25" s="85"/>
+      <c r="K25" s="85"/>
     </row>
     <row r="26" spans="3:12" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C26" s="67"/>
-      <c r="D26" s="67"/>
-      <c r="E26" s="67"/>
-      <c r="F26" s="67"/>
-      <c r="G26" s="67"/>
-      <c r="H26" s="67"/>
-      <c r="I26" s="67"/>
-      <c r="J26" s="67"/>
-      <c r="K26" s="67"/>
+      <c r="C26" s="85"/>
+      <c r="D26" s="85"/>
+      <c r="E26" s="85"/>
+      <c r="F26" s="85"/>
+      <c r="G26" s="85"/>
+      <c r="H26" s="85"/>
+      <c r="I26" s="85"/>
+      <c r="J26" s="85"/>
+      <c r="K26" s="85"/>
     </row>
     <row r="27" spans="3:12" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C27" s="15"/>
@@ -3663,8 +3662,8 @@
     </row>
     <row r="55" spans="1:25" s="5" customFormat="1" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="9"/>
-      <c r="B55" s="61"/>
-      <c r="C55" s="62"/>
+      <c r="B55" s="79"/>
+      <c r="C55" s="80"/>
       <c r="D55" s="21" t="s">
         <v>187</v>
       </c>
@@ -3687,25 +3686,25 @@
       <c r="K55" s="21" t="s">
         <v>290</v>
       </c>
-      <c r="L55" s="59"/>
-      <c r="M55" s="60"/>
-      <c r="N55" s="60"/>
-      <c r="O55" s="60"/>
-      <c r="P55" s="60"/>
-      <c r="Q55" s="60"/>
-      <c r="R55" s="61"/>
-      <c r="S55" s="61"/>
-      <c r="T55" s="61"/>
-      <c r="U55" s="61"/>
-      <c r="V55" s="61"/>
-      <c r="W55" s="61"/>
-      <c r="X55" s="61"/>
+      <c r="L55" s="77"/>
+      <c r="M55" s="78"/>
+      <c r="N55" s="78"/>
+      <c r="O55" s="78"/>
+      <c r="P55" s="78"/>
+      <c r="Q55" s="78"/>
+      <c r="R55" s="79"/>
+      <c r="S55" s="79"/>
+      <c r="T55" s="79"/>
+      <c r="U55" s="79"/>
+      <c r="V55" s="79"/>
+      <c r="W55" s="79"/>
+      <c r="X55" s="79"/>
       <c r="Y55" s="7"/>
     </row>
     <row r="56" spans="1:25" s="5" customFormat="1" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A56" s="9"/>
-      <c r="B56" s="61"/>
-      <c r="C56" s="62"/>
+      <c r="B56" s="79"/>
+      <c r="C56" s="80"/>
       <c r="D56" s="19" t="s">
         <v>381</v>
       </c>
@@ -3728,25 +3727,25 @@
       <c r="K56" s="27" t="s">
         <v>250</v>
       </c>
-      <c r="L56" s="59"/>
-      <c r="M56" s="60"/>
-      <c r="N56" s="60"/>
-      <c r="O56" s="60"/>
-      <c r="P56" s="60"/>
-      <c r="Q56" s="60"/>
-      <c r="R56" s="61"/>
-      <c r="S56" s="61"/>
-      <c r="T56" s="61"/>
-      <c r="U56" s="61"/>
-      <c r="V56" s="61"/>
-      <c r="W56" s="61"/>
-      <c r="X56" s="61"/>
+      <c r="L56" s="77"/>
+      <c r="M56" s="78"/>
+      <c r="N56" s="78"/>
+      <c r="O56" s="78"/>
+      <c r="P56" s="78"/>
+      <c r="Q56" s="78"/>
+      <c r="R56" s="79"/>
+      <c r="S56" s="79"/>
+      <c r="T56" s="79"/>
+      <c r="U56" s="79"/>
+      <c r="V56" s="79"/>
+      <c r="W56" s="79"/>
+      <c r="X56" s="79"/>
       <c r="Y56" s="7"/>
     </row>
     <row r="57" spans="1:25" s="5" customFormat="1" ht="169.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9"/>
-      <c r="B57" s="61"/>
-      <c r="C57" s="62"/>
+      <c r="B57" s="79"/>
+      <c r="C57" s="80"/>
       <c r="D57" s="22" t="s">
         <v>382</v>
       </c>
@@ -3763,22 +3762,22 @@
       <c r="I57" s="28"/>
       <c r="J57" s="28"/>
       <c r="K57" s="29"/>
-      <c r="L57" s="59"/>
-      <c r="M57" s="60"/>
-      <c r="N57" s="60"/>
-      <c r="O57" s="60"/>
-      <c r="P57" s="60"/>
-      <c r="Q57" s="60"/>
-      <c r="R57" s="61"/>
-      <c r="S57" s="61"/>
-      <c r="T57" s="61"/>
-      <c r="U57" s="61"/>
-      <c r="V57" s="61"/>
-      <c r="W57" s="61"/>
-      <c r="X57" s="61"/>
+      <c r="L57" s="77"/>
+      <c r="M57" s="78"/>
+      <c r="N57" s="78"/>
+      <c r="O57" s="78"/>
+      <c r="P57" s="78"/>
+      <c r="Q57" s="78"/>
+      <c r="R57" s="79"/>
+      <c r="S57" s="79"/>
+      <c r="T57" s="79"/>
+      <c r="U57" s="79"/>
+      <c r="V57" s="79"/>
+      <c r="W57" s="79"/>
+      <c r="X57" s="79"/>
       <c r="Y57" s="7"/>
     </row>
-    <row r="58" spans="1:25" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:25" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C58" s="13"/>
       <c r="D58" s="17" t="s">
         <v>91</v>
@@ -4085,7 +4084,7 @@
         <v>177</v>
       </c>
       <c r="H69" s="19" t="s">
-        <v>389</v>
+        <v>411</v>
       </c>
       <c r="I69" s="28" t="s">
         <v>284</v>
@@ -4131,7 +4130,7 @@
         <v>202</v>
       </c>
       <c r="H71" s="19" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="I71" s="28" t="s">
         <v>259</v>
@@ -4159,7 +4158,7 @@
         <v>214</v>
       </c>
       <c r="H72" s="20" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="I72" s="29" t="s">
         <v>261</v>
@@ -4187,7 +4186,7 @@
         <v>214</v>
       </c>
       <c r="H73" s="18" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I73" s="21" t="s">
         <v>250</v>
@@ -4215,7 +4214,7 @@
         <v>214</v>
       </c>
       <c r="H74" s="19" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I74" s="28" t="s">
         <v>250</v>
@@ -4243,7 +4242,7 @@
         <v>215</v>
       </c>
       <c r="H75" s="18" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="I75" s="21" t="s">
         <v>250</v>
@@ -4271,7 +4270,7 @@
         <v>216</v>
       </c>
       <c r="H76" s="18" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="I76" s="28" t="s">
         <v>250</v>
@@ -4299,7 +4298,7 @@
         <v>217</v>
       </c>
       <c r="H77" s="19" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I77" s="21" t="s">
         <v>250</v>
@@ -4327,7 +4326,7 @@
         <v>218</v>
       </c>
       <c r="H78" s="20" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="I78" s="21" t="s">
         <v>250</v>
@@ -4355,7 +4354,7 @@
         <v>219</v>
       </c>
       <c r="H79" s="18" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="I79" s="21" t="s">
         <v>302</v>
@@ -4383,7 +4382,7 @@
         <v>220</v>
       </c>
       <c r="H80" s="18" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="I80" s="21" t="s">
         <v>302</v>
@@ -4411,7 +4410,7 @@
         <v>221</v>
       </c>
       <c r="H81" s="18" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="I81" s="21" t="s">
         <v>302</v>
@@ -4439,7 +4438,7 @@
         <v>222</v>
       </c>
       <c r="H82" s="18" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="I82" s="21" t="s">
         <v>250</v>
@@ -4467,7 +4466,7 @@
         <v>178</v>
       </c>
       <c r="H83" s="19" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="I83" s="28" t="s">
         <v>303</v>
@@ -4495,7 +4494,7 @@
         <v>222</v>
       </c>
       <c r="H84" s="20" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I84" s="21" t="s">
         <v>250</v>
@@ -4523,7 +4522,7 @@
         <v>272</v>
       </c>
       <c r="H85" s="18" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="I85" s="21" t="s">
         <v>250</v>
@@ -4551,7 +4550,7 @@
         <v>223</v>
       </c>
       <c r="H86" s="19" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="I86" s="29"/>
       <c r="J86" s="21"/>
@@ -4573,7 +4572,7 @@
         <v>224</v>
       </c>
       <c r="H87" s="18" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="I87" s="21"/>
       <c r="J87" s="28"/>
@@ -4595,7 +4594,7 @@
         <v>222</v>
       </c>
       <c r="H88" s="18" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="I88" s="28"/>
       <c r="J88" s="27"/>
@@ -4617,7 +4616,7 @@
         <v>222</v>
       </c>
       <c r="H89" s="19" t="s">
-        <v>404</v>
+        <v>403</v>
       </c>
       <c r="I89" s="21"/>
       <c r="J89" s="29"/>
@@ -4639,7 +4638,7 @@
         <v>225</v>
       </c>
       <c r="H90" s="20" t="s">
-        <v>405</v>
+        <v>404</v>
       </c>
       <c r="I90" s="28"/>
       <c r="J90" s="28"/>
@@ -4696,7 +4695,9 @@
       <c r="G93" s="21" t="s">
         <v>226</v>
       </c>
-      <c r="H93" s="19"/>
+      <c r="H93" s="19" t="s">
+        <v>417</v>
+      </c>
       <c r="I93" s="29" t="s">
         <v>250</v>
       </c>
@@ -4723,7 +4724,7 @@
         <v>176</v>
       </c>
       <c r="H94" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I94" s="28" t="s">
         <v>266</v>
@@ -4751,7 +4752,7 @@
         <v>176</v>
       </c>
       <c r="H95" s="19" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I95" s="28" t="s">
         <v>266</v>
@@ -4779,7 +4780,7 @@
         <v>210</v>
       </c>
       <c r="H96" s="20" t="s">
-        <v>413</v>
+        <v>412</v>
       </c>
       <c r="I96" s="21" t="s">
         <v>250</v>
@@ -4805,7 +4806,7 @@
       </c>
       <c r="G97" s="28"/>
       <c r="H97" s="18" t="s">
-        <v>414</v>
+        <v>413</v>
       </c>
       <c r="I97" s="28" t="s">
         <v>250</v>
@@ -4833,7 +4834,7 @@
         <v>209</v>
       </c>
       <c r="H98" s="18" t="s">
-        <v>412</v>
+        <v>411</v>
       </c>
       <c r="I98" s="21" t="s">
         <v>250</v>
@@ -4861,7 +4862,7 @@
         <v>222</v>
       </c>
       <c r="H99" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I99" s="28" t="s">
         <v>250</v>
@@ -4887,7 +4888,7 @@
       </c>
       <c r="G100" s="17"/>
       <c r="H100" s="18" t="s">
-        <v>407</v>
+        <v>406</v>
       </c>
       <c r="I100" s="28" t="s">
         <v>250</v>
@@ -4913,7 +4914,7 @@
       </c>
       <c r="G101" s="21"/>
       <c r="H101" s="19" t="s">
-        <v>408</v>
+        <v>407</v>
       </c>
       <c r="I101" s="21" t="s">
         <v>250</v>
@@ -4941,7 +4942,7 @@
         <v>178</v>
       </c>
       <c r="H102" s="20" t="s">
-        <v>415</v>
+        <v>414</v>
       </c>
       <c r="I102" s="28"/>
       <c r="J102" s="27" t="s">
@@ -4965,7 +4966,7 @@
       </c>
       <c r="G103" s="21"/>
       <c r="H103" s="18" t="s">
-        <v>416</v>
+        <v>415</v>
       </c>
       <c r="I103" s="21"/>
       <c r="J103" s="29" t="s">
@@ -4989,7 +4990,7 @@
       </c>
       <c r="G104" s="21"/>
       <c r="H104" s="18" t="s">
-        <v>417</v>
+        <v>416</v>
       </c>
       <c r="I104" s="28"/>
       <c r="J104" s="28"/>
@@ -5009,7 +5010,7 @@
       </c>
       <c r="G105" s="28"/>
       <c r="H105" s="19" t="s">
-        <v>409</v>
+        <v>408</v>
       </c>
       <c r="I105" s="21"/>
       <c r="J105" s="28"/>
@@ -5029,7 +5030,7 @@
       </c>
       <c r="G106" s="28"/>
       <c r="H106" s="18" t="s">
-        <v>410</v>
+        <v>409</v>
       </c>
       <c r="I106" s="28"/>
       <c r="J106" s="29"/>
@@ -5051,7 +5052,7 @@
         <v>222</v>
       </c>
       <c r="H107" s="19" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="I107" s="29"/>
       <c r="J107" s="21"/>
@@ -5367,7 +5368,7 @@
       </c>
       <c r="G122" s="17"/>
       <c r="H122" s="19" t="s">
-        <v>411</v>
+        <v>410</v>
       </c>
       <c r="I122" s="21"/>
       <c r="J122" s="28"/>
@@ -6003,12 +6004,6 @@
     </row>
   </sheetData>
   <mergeCells count="17">
-    <mergeCell ref="B2:M7"/>
-    <mergeCell ref="C9:J9"/>
-    <mergeCell ref="F10:G10"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="F11:G11"/>
-    <mergeCell ref="J11:K11"/>
     <mergeCell ref="L55:Q57"/>
     <mergeCell ref="B55:C57"/>
     <mergeCell ref="R55:T57"/>
@@ -6020,6 +6015,12 @@
     <mergeCell ref="F13:G13"/>
     <mergeCell ref="J14:K14"/>
     <mergeCell ref="F15:G15"/>
+    <mergeCell ref="B2:M7"/>
+    <mergeCell ref="C9:J9"/>
+    <mergeCell ref="F10:G10"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="F11:G11"/>
+    <mergeCell ref="J11:K11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>